<commit_message>
Use hours, not shortcuts
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B742635B-AE3C-44D6-B090-7DC82A56DEE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AA652B-1CCC-41D4-8816-1A057F325DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="1" activeTab="2" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -21152,8 +21152,8 @@
         <v>~SPWI101~, ~Arcane~, ~1~, ~Grease~ =&gt; ~SPWI101~</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G22" si="0">_xlfn.CONCAT("~", B3, E3, "~, ~", , D3, "~, ~", C3, "~, ~", A3, "~, ~", B3, "~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~", , E3, "~ =&gt; ~", D3, "~")</f>
-        <v>~1Grease~, ~SCRL66~, ~SPWI101~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~Grease~ =&gt; ~SCRL66~</v>
+        <f t="shared" ref="G3:G22" si="0">_xlfn.CONCAT("~", B3, E3, "~, ~", , D3, "~, ~", C3, "~, ~", A3, "~, ~", B3, "~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~", , E3, "~ =&gt; ~", D3, "~")</f>
+        <v>~1Grease~, ~SCRL66~, ~SPWI101~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Grease~ =&gt; ~SCRL66~</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -21178,7 +21178,7 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>~1Armor~, ~SCRL67~, ~SPWI102~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~Armor~ =&gt; ~SCRL67~</v>
+        <v>~1Armor~, ~SCRL67~, ~SPWI102~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Armor~ =&gt; ~SCRL67~</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -21203,7 +21203,7 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>~1Burning Hands~, ~SCRL68~, ~SPWI103~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~Burning Hands~ =&gt; ~SCRL68~</v>
+        <v>~1Burning Hands~, ~SCRL68~, ~SPWI103~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Burning Hands~ =&gt; ~SCRL68~</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -21228,7 +21228,7 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>~1Charm Person~, ~SCRL69~, ~SPWI104~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~Charm Person~ =&gt; ~SCRL69~</v>
+        <v>~1Charm Person~, ~SCRL69~, ~SPWI104~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Charm Person~ =&gt; ~SCRL69~</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -21253,7 +21253,7 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>~1Color Spray~, ~SCRL70~, ~SPWI105~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~Color Spray~ =&gt; ~SCRL70~</v>
+        <v>~1Color Spray~, ~SCRL70~, ~SPWI105~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Color Spray~ =&gt; ~SCRL70~</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -21278,7 +21278,7 @@
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>~1Blindness~, ~SCRL71~, ~SPWI106~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~Blindness~ =&gt; ~SCRL71~</v>
+        <v>~1Blindness~, ~SCRL71~, ~SPWI106~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Blindness~ =&gt; ~SCRL71~</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -21303,7 +21303,7 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>~1Friends~, ~SCRL72~, ~SPWI107~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~Friends~ =&gt; ~SCRL72~</v>
+        <v>~1Friends~, ~SCRL72~, ~SPWI107~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Friends~ =&gt; ~SCRL72~</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -21328,7 +21328,7 @@
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>~1Protection from Petrification~, ~SCRL73~, ~SPWI108~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~Protection from Petrification~ =&gt; ~SCRL73~</v>
+        <v>~1Protection from Petrification~, ~SCRL73~, ~SPWI108~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Protection from Petrification~ =&gt; ~SCRL73~</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -21353,7 +21353,7 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>~1Identify~, ~SCRL75~, ~SPWI110~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~Identify~ =&gt; ~SCRL75~</v>
+        <v>~1Identify~, ~SCRL75~, ~SPWI110~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Identify~ =&gt; ~SCRL75~</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -21378,7 +21378,7 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>~1Infravision~, ~SCRL76~, ~SPWI111~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~Infravision~ =&gt; ~SCRL76~</v>
+        <v>~1Infravision~, ~SCRL76~, ~SPWI111~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Infravision~ =&gt; ~SCRL76~</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -21403,7 +21403,7 @@
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>~1Magic Missile~, ~SCRL77~, ~SPWI112~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~Magic Missile~ =&gt; ~SCRL77~</v>
+        <v>~1Magic Missile~, ~SCRL77~, ~SPWI112~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Magic Missile~ =&gt; ~SCRL77~</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -21428,7 +21428,7 @@
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>~1Protection from Evil~, ~SCRL3H, SCRL78~, ~SPWI113~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~Protection from Evil~ =&gt; ~SCRL3H, SCRL78~</v>
+        <v>~1Protection from Evil~, ~SCRL3H, SCRL78~, ~SPWI113~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Protection from Evil~ =&gt; ~SCRL3H, SCRL78~</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -21453,7 +21453,7 @@
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>~1Shield~, ~SCRL79~, ~SPWI114~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~Shield~ =&gt; ~SCRL79~</v>
+        <v>~1Shield~, ~SCRL79~, ~SPWI114~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Shield~ =&gt; ~SCRL79~</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -21478,7 +21478,7 @@
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>~1Shocking Grasp~, ~SCRL80~, ~SPWI115~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~Shocking Grasp~ =&gt; ~SCRL80~</v>
+        <v>~1Shocking Grasp~, ~SCRL80~, ~SPWI115~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Shocking Grasp~ =&gt; ~SCRL80~</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -21503,7 +21503,7 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>~1Sleep~, ~SCRL81~, ~SPWI116~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~Sleep~ =&gt; ~SCRL81~</v>
+        <v>~1Sleep~, ~SCRL81~, ~SPWI116~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Sleep~ =&gt; ~SCRL81~</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -21528,7 +21528,7 @@
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>~1Chill Touch~, ~SCRL82~, ~SPWI117~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~Chill Touch~ =&gt; ~SCRL82~</v>
+        <v>~1Chill Touch~, ~SCRL82~, ~SPWI117~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Chill Touch~ =&gt; ~SCRL82~</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -21553,7 +21553,7 @@
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>~1Chromatic Orb~, ~SCRL83~, ~SPWI118~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~Chromatic Orb~ =&gt; ~SCRL83~</v>
+        <v>~1Chromatic Orb~, ~SCRL83~, ~SPWI118~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Chromatic Orb~ =&gt; ~SCRL83~</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -21578,7 +21578,7 @@
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>~1Larloch's Minor Drain~, ~SCRL84~, ~SPWI119~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~Larloch's Minor Drain~ =&gt; ~SCRL84~</v>
+        <v>~1Larloch's Minor Drain~, ~SCRL84~, ~SPWI119~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Larloch's Minor Drain~ =&gt; ~SCRL84~</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -21603,7 +21603,7 @@
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>~1Reflected Image~, ~SCRL5U~, ~SPWI120~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~Reflected Image~ =&gt; ~SCRL5U~</v>
+        <v>~1Reflected Image~, ~SCRL5U~, ~SPWI120~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Reflected Image~ =&gt; ~SCRL5U~</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -21628,7 +21628,7 @@
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v>~1Find Familiar~, ~SCRL6D~, ~SPWI123~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~Find Familiar~ =&gt; ~SCRL6D~</v>
+        <v>~1Find Familiar~, ~SCRL6D~, ~SPWI123~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Find Familiar~ =&gt; ~SCRL6D~</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update the spell list (and just the spell list) for BG1EE
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AA652B-1CCC-41D4-8816-1A057F325DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A6C62B-862A-458D-9501-7EB123326B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="1" activeTab="2" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -4016,10 +4016,10 @@
   <dimension ref="A1:AL262"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="U266" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="O18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="T2" sqref="T2:V266"/>
+      <selection pane="bottomRight" activeCell="W280" sqref="W280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21090,8 +21090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAFBE98-3888-4E00-A1FB-56928E91D590}">
   <dimension ref="A1:G241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="G22" sqref="G3:G22"/>
+    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:F241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21148,12 +21148,12 @@
         <v>19</v>
       </c>
       <c r="F3" t="str">
-        <f>_xlfn.CONCAT("~", C3, "~, ~", A3, "~, ~", B3, "~, ~", E3, "~ =&gt; ~", C3, "~")</f>
-        <v>~SPWI101~, ~Arcane~, ~1~, ~Grease~ =&gt; ~SPWI101~</v>
+        <f>_xlfn.CONCAT("~", C3, "~, ~", A3, "~, ~", B3, "~ =&gt; ~", C3, "~    //", E3)</f>
+        <v>~SPWI101~, ~Arcane~, ~1~ =&gt; ~SPWI101~    //Grease</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G22" si="0">_xlfn.CONCAT("~", B3, E3, "~, ~", , D3, "~, ~", C3, "~, ~", A3, "~, ~", B3, "~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~", , E3, "~ =&gt; ~", D3, "~")</f>
-        <v>~1Grease~, ~SCRL66~, ~SPWI101~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Grease~ =&gt; ~SCRL66~</v>
+        <f t="shared" ref="G3:G21" si="0">_xlfn.CONCAT("~", D3, "~, ~", C3, "~, ~", A3, "~, ~", B3, "~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~", , E3, "~ =&gt; ~", D3, "~")</f>
+        <v>~SCRL66~, ~SPWI101~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Grease~ =&gt; ~SCRL66~</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -21173,12 +21173,12 @@
         <v>38</v>
       </c>
       <c r="F4" t="str">
-        <f>_xlfn.CONCAT("~", C4, "~, ~", A4, "~, ~", B4, "~, ~", E4, "~ =&gt; ~", C4, "~")</f>
-        <v>~SPWI102~, ~Arcane~, ~1~, ~Armor~ =&gt; ~SPWI102~</v>
+        <f t="shared" ref="F4:F67" si="1">_xlfn.CONCAT("~", C4, "~, ~", A4, "~, ~", B4, "~ =&gt; ~", C4, "~    //", E4)</f>
+        <v>~SPWI102~, ~Arcane~, ~1~ =&gt; ~SPWI102~    //Armor</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>~1Armor~, ~SCRL67~, ~SPWI102~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Armor~ =&gt; ~SCRL67~</v>
+        <v>~SCRL67~, ~SPWI102~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Armor~ =&gt; ~SCRL67~</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -21198,12 +21198,12 @@
         <v>39</v>
       </c>
       <c r="F5" t="str">
-        <f>_xlfn.CONCAT("~", C5, "~, ~", A5, "~, ~", B5, "~, ~", E5, "~ =&gt; ~", C5, "~")</f>
-        <v>~SPWI103~, ~Arcane~, ~1~, ~Burning Hands~ =&gt; ~SPWI103~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI103~, ~Arcane~, ~1~ =&gt; ~SPWI103~    //Burning Hands</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>~1Burning Hands~, ~SCRL68~, ~SPWI103~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Burning Hands~ =&gt; ~SCRL68~</v>
+        <v>~SCRL68~, ~SPWI103~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Burning Hands~ =&gt; ~SCRL68~</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -21223,12 +21223,12 @@
         <v>40</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" ref="F6:F10" si="1">_xlfn.CONCAT("~", C6, "~, ~", A6, "~, ~", B6, "~, ~", E6, "~ =&gt; ~", C6, "~")</f>
-        <v>~SPWI104~, ~Arcane~, ~1~, ~Charm Person~ =&gt; ~SPWI104~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI104~, ~Arcane~, ~1~ =&gt; ~SPWI104~    //Charm Person</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>~1Charm Person~, ~SCRL69~, ~SPWI104~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Charm Person~ =&gt; ~SCRL69~</v>
+        <v>~SCRL69~, ~SPWI104~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Charm Person~ =&gt; ~SCRL69~</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -21249,11 +21249,11 @@
       </c>
       <c r="F7" t="str">
         <f t="shared" si="1"/>
-        <v>~SPWI105~, ~Arcane~, ~1~, ~Color Spray~ =&gt; ~SPWI105~</v>
+        <v>~SPWI105~, ~Arcane~, ~1~ =&gt; ~SPWI105~    //Color Spray</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>~1Color Spray~, ~SCRL70~, ~SPWI105~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Color Spray~ =&gt; ~SCRL70~</v>
+        <v>~SCRL70~, ~SPWI105~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Color Spray~ =&gt; ~SCRL70~</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -21274,11 +21274,11 @@
       </c>
       <c r="F8" t="str">
         <f t="shared" si="1"/>
-        <v>~SPWI106~, ~Arcane~, ~1~, ~Blindness~ =&gt; ~SPWI106~</v>
+        <v>~SPWI106~, ~Arcane~, ~1~ =&gt; ~SPWI106~    //Blindness</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>~1Blindness~, ~SCRL71~, ~SPWI106~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Blindness~ =&gt; ~SCRL71~</v>
+        <v>~SCRL71~, ~SPWI106~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Blindness~ =&gt; ~SCRL71~</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -21299,11 +21299,11 @@
       </c>
       <c r="F9" t="str">
         <f t="shared" si="1"/>
-        <v>~SPWI107~, ~Arcane~, ~1~, ~Friends~ =&gt; ~SPWI107~</v>
+        <v>~SPWI107~, ~Arcane~, ~1~ =&gt; ~SPWI107~    //Friends</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>~1Friends~, ~SCRL72~, ~SPWI107~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Friends~ =&gt; ~SCRL72~</v>
+        <v>~SCRL72~, ~SPWI107~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Friends~ =&gt; ~SCRL72~</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -21324,11 +21324,11 @@
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
-        <v>~SPWI108~, ~Arcane~, ~1~, ~Protection from Petrification~ =&gt; ~SPWI108~</v>
+        <v>~SPWI108~, ~Arcane~, ~1~ =&gt; ~SPWI108~    //Protection from Petrification</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>~1Protection from Petrification~, ~SCRL73~, ~SPWI108~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Protection from Petrification~ =&gt; ~SCRL73~</v>
+        <v>~SCRL73~, ~SPWI108~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Protection from Petrification~ =&gt; ~SCRL73~</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -21348,12 +21348,12 @@
         <v>45</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" ref="F11:F21" si="2">_xlfn.CONCAT("~", C11, "~, ~", A11, "~, ~", B11, "~, ~", E11, "~ =&gt; ~", C11, "~")</f>
-        <v>~SPWI110~, ~Arcane~, ~1~, ~Identify~ =&gt; ~SPWI110~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI110~, ~Arcane~, ~1~ =&gt; ~SPWI110~    //Identify</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>~1Identify~, ~SCRL75~, ~SPWI110~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Identify~ =&gt; ~SCRL75~</v>
+        <v>~SCRL75~, ~SPWI110~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Identify~ =&gt; ~SCRL75~</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -21373,12 +21373,12 @@
         <v>46</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="2"/>
-        <v>~SPWI111~, ~Arcane~, ~1~, ~Infravision~ =&gt; ~SPWI111~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI111~, ~Arcane~, ~1~ =&gt; ~SPWI111~    //Infravision</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>~1Infravision~, ~SCRL76~, ~SPWI111~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Infravision~ =&gt; ~SCRL76~</v>
+        <v>~SCRL76~, ~SPWI111~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Infravision~ =&gt; ~SCRL76~</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -21398,12 +21398,12 @@
         <v>47</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="2"/>
-        <v>~SPWI112~, ~Arcane~, ~1~, ~Magic Missile~ =&gt; ~SPWI112~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI112~, ~Arcane~, ~1~ =&gt; ~SPWI112~    //Magic Missile</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>~1Magic Missile~, ~SCRL77~, ~SPWI112~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Magic Missile~ =&gt; ~SCRL77~</v>
+        <v>~SCRL77~, ~SPWI112~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Magic Missile~ =&gt; ~SCRL77~</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -21423,12 +21423,12 @@
         <v>48</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="2"/>
-        <v>~SPWI113~, ~Arcane~, ~1~, ~Protection from Evil~ =&gt; ~SPWI113~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI113~, ~Arcane~, ~1~ =&gt; ~SPWI113~    //Protection from Evil</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>~1Protection from Evil~, ~SCRL3H, SCRL78~, ~SPWI113~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Protection from Evil~ =&gt; ~SCRL3H, SCRL78~</v>
+        <v>~SCRL3H, SCRL78~, ~SPWI113~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Protection from Evil~ =&gt; ~SCRL3H, SCRL78~</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -21448,12 +21448,12 @@
         <v>49</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="2"/>
-        <v>~SPWI114~, ~Arcane~, ~1~, ~Shield~ =&gt; ~SPWI114~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI114~, ~Arcane~, ~1~ =&gt; ~SPWI114~    //Shield</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>~1Shield~, ~SCRL79~, ~SPWI114~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Shield~ =&gt; ~SCRL79~</v>
+        <v>~SCRL79~, ~SPWI114~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Shield~ =&gt; ~SCRL79~</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -21473,12 +21473,12 @@
         <v>50</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" si="2"/>
-        <v>~SPWI115~, ~Arcane~, ~1~, ~Shocking Grasp~ =&gt; ~SPWI115~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI115~, ~Arcane~, ~1~ =&gt; ~SPWI115~    //Shocking Grasp</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>~1Shocking Grasp~, ~SCRL80~, ~SPWI115~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Shocking Grasp~ =&gt; ~SCRL80~</v>
+        <v>~SCRL80~, ~SPWI115~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Shocking Grasp~ =&gt; ~SCRL80~</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -21498,12 +21498,12 @@
         <v>51</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" si="2"/>
-        <v>~SPWI116~, ~Arcane~, ~1~, ~Sleep~ =&gt; ~SPWI116~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI116~, ~Arcane~, ~1~ =&gt; ~SPWI116~    //Sleep</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>~1Sleep~, ~SCRL81~, ~SPWI116~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Sleep~ =&gt; ~SCRL81~</v>
+        <v>~SCRL81~, ~SPWI116~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Sleep~ =&gt; ~SCRL81~</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -21523,12 +21523,12 @@
         <v>52</v>
       </c>
       <c r="F18" t="str">
-        <f t="shared" si="2"/>
-        <v>~SPWI117~, ~Arcane~, ~1~, ~Chill Touch~ =&gt; ~SPWI117~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI117~, ~Arcane~, ~1~ =&gt; ~SPWI117~    //Chill Touch</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>~1Chill Touch~, ~SCRL82~, ~SPWI117~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Chill Touch~ =&gt; ~SCRL82~</v>
+        <v>~SCRL82~, ~SPWI117~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Chill Touch~ =&gt; ~SCRL82~</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -21548,12 +21548,12 @@
         <v>53</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" si="2"/>
-        <v>~SPWI118~, ~Arcane~, ~1~, ~Chromatic Orb~ =&gt; ~SPWI118~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI118~, ~Arcane~, ~1~ =&gt; ~SPWI118~    //Chromatic Orb</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>~1Chromatic Orb~, ~SCRL83~, ~SPWI118~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Chromatic Orb~ =&gt; ~SCRL83~</v>
+        <v>~SCRL83~, ~SPWI118~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Chromatic Orb~ =&gt; ~SCRL83~</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -21573,12 +21573,12 @@
         <v>54</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" si="2"/>
-        <v>~SPWI119~, ~Arcane~, ~1~, ~Larloch's Minor Drain~ =&gt; ~SPWI119~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI119~, ~Arcane~, ~1~ =&gt; ~SPWI119~    //Larloch's Minor Drain</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>~1Larloch's Minor Drain~, ~SCRL84~, ~SPWI119~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Larloch's Minor Drain~ =&gt; ~SCRL84~</v>
+        <v>~SCRL84~, ~SPWI119~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Larloch's Minor Drain~ =&gt; ~SCRL84~</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -21598,12 +21598,12 @@
         <v>552</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" si="2"/>
-        <v>~SPWI120~, ~Arcane~, ~1~, ~Reflected Image~ =&gt; ~SPWI120~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI120~, ~Arcane~, ~1~ =&gt; ~SPWI120~    //Reflected Image</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>~1Reflected Image~, ~SCRL5U~, ~SPWI120~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Reflected Image~ =&gt; ~SCRL5U~</v>
+        <v>~SCRL5U~, ~SPWI120~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Reflected Image~ =&gt; ~SCRL5U~</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -21623,12 +21623,12 @@
         <v>553</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" ref="F22:F25" si="3">_xlfn.CONCAT("~", C22, "~, ~", A22, "~, ~", B22, "~, ~", E22, "~ =&gt; ~", C22, "~")</f>
-        <v>~SPWI123~, ~Arcane~, ~1~, ~Find Familiar~ =&gt; ~SPWI123~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI123~, ~Arcane~, ~1~ =&gt; ~SPWI123~    //Find Familiar</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="0"/>
-        <v>~1Find Familiar~, ~SCRL6D~, ~SPWI123~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Find Familiar~ =&gt; ~SCRL6D~</v>
+        <f>_xlfn.CONCAT("~", D22, "~, ~", C22, "~, ~", A22, "~, ~", B22, "~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~", , E22, "~ =&gt; ~", D22, "~")</f>
+        <v>~SCRL6D~, ~SPWI123~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Find Familiar~ =&gt; ~SCRL6D~</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -21645,8 +21645,8 @@
         <v>817</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="3"/>
-        <v>~SPWI124~, ~Arcane~, ~1~, ~Nahal's Reckless Dweomer*~ =&gt; ~SPWI124~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI124~, ~Arcane~, ~1~ =&gt; ~SPWI124~    //Nahal's Reckless Dweomer*</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -21666,12 +21666,12 @@
         <v>554</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="3"/>
-        <v>~SPWI125~, ~Arcane~, ~1~, ~Spook~ =&gt; ~SPWI125~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI125~, ~Arcane~, ~1~ =&gt; ~SPWI125~    //Spook</v>
       </c>
       <c r="G24" t="str">
-        <f>_xlfn.CONCAT("~", B24, E24, "~, ~", , D24, "~, ~", C24, "~, ~", A24, "~, ~", B24, "~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~", , E24, "~ =&gt; ~", D24, "~")</f>
-        <v>~1Spook~, ~SCRLA6~, ~SPWI125~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~Spook~ =&gt; ~SCRLA6~</v>
+        <f t="shared" ref="G24:G25" si="2">_xlfn.CONCAT("~", D24, "~, ~", C24, "~, ~", A24, "~, ~", B24, "~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~", , E24, "~ =&gt; ~", D24, "~")</f>
+        <v>~SCRLA6~, ~SPWI125~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Spook~ =&gt; ~SCRLA6~</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -21691,12 +21691,18 @@
         <v>822</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="3"/>
-        <v>~SPWI126~, ~Arcane~, ~1~, ~Dancing Lights~ =&gt; ~SPWI126~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI126~, ~Arcane~, ~1~ =&gt; ~SPWI126~    //Dancing Lights</v>
       </c>
       <c r="G25" t="str">
-        <f>_xlfn.CONCAT("~", B25, E25, "~, ~", , D25, "~, ~", C25, "~, ~", A25, "~, ~", B25, "~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~", , E25, "~ =&gt; ~", D25, "~")</f>
-        <v>~1Dancing Lights~, ~BDSCRL1A~, ~SPWI126~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~SIX_HOURS~, ~0~, ~15~, ~0~, ~1~, ~Dancing Lights~ =&gt; ~BDSCRL1A~</v>
+        <f t="shared" si="2"/>
+        <v>~BDSCRL1A~, ~SPWI126~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Dancing Lights~ =&gt; ~BDSCRL1A~</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F26" t="str">
+        <f t="shared" si="1"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -21716,11 +21722,11 @@
         <v>77</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" ref="F27:F29" si="4">_xlfn.CONCAT("~", C27, "~, ~", A27, "~, ~", B27, "~, ~", E27, "~ =&gt; ~", C27, "~")</f>
-        <v>~SPWI201~, ~Arcane~, ~2~, ~Blur~ =&gt; ~SPWI201~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI201~, ~Arcane~, ~2~ =&gt; ~SPWI201~    //Blur</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" ref="G4:G49" si="5">_xlfn.CONCAT("~", B27, E27, "~, ~", , D27, "~, ~", C27, "~, ~", A27, "~, ~", B27, "~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~", " =&gt; ~", D27, "~")</f>
+        <f t="shared" ref="G27:G49" si="3">_xlfn.CONCAT("~", B27, E27, "~, ~", , D27, "~, ~", C27, "~, ~", A27, "~, ~", B27, "~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~", " =&gt; ~", D27, "~")</f>
         <v>~2Blur~, ~SCRL85~, ~SPWI201~, ~Arcane~, ~2~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL85~</v>
       </c>
     </row>
@@ -21741,11 +21747,11 @@
         <v>78</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="4"/>
-        <v>~SPWI202~, ~Arcane~, ~2~, ~Detect Evil~ =&gt; ~SPWI202~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI202~, ~Arcane~, ~2~ =&gt; ~SPWI202~    //Detect Evil</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>~2Detect Evil~, ~SCRL86~, ~SPWI202~, ~Arcane~, ~2~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL86~</v>
       </c>
     </row>
@@ -21766,11 +21772,11 @@
         <v>79</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="4"/>
-        <v>~SPWI203~, ~Arcane~, ~2~, ~Detect Invisibility~ =&gt; ~SPWI203~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI203~, ~Arcane~, ~2~ =&gt; ~SPWI203~    //Detect Invisibility</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>~2Detect Invisibility~, ~SCRL87~, ~SPWI203~, ~Arcane~, ~2~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL87~</v>
       </c>
     </row>
@@ -21791,11 +21797,11 @@
         <v>80</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" ref="F30:F40" si="6">_xlfn.CONCAT("~", C30, "~, ~", A30, "~, ~", B30, "~, ~", E30, "~ =&gt; ~", C30, "~")</f>
-        <v>~SPWI205~, ~Arcane~, ~2~, ~Horror~ =&gt; ~SPWI205~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI205~, ~Arcane~, ~2~ =&gt; ~SPWI205~    //Horror</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>~2Horror~, ~SCRL89~, ~SPWI205~, ~Arcane~, ~2~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL89~</v>
       </c>
     </row>
@@ -21816,11 +21822,11 @@
         <v>81</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="6"/>
-        <v>~SPWI206~, ~Arcane~, ~2~, ~Invisibility~ =&gt; ~SPWI206~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI206~, ~Arcane~, ~2~ =&gt; ~SPWI206~    //Invisibility</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>~2Invisibility~, ~SCRL90~, ~SPWI206~, ~Arcane~, ~2~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL90~</v>
       </c>
     </row>
@@ -21841,11 +21847,11 @@
         <v>82</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="6"/>
-        <v>~SPWI207~, ~Arcane~, ~2~, ~Knock~ =&gt; ~SPWI207~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI207~, ~Arcane~, ~2~ =&gt; ~SPWI207~    //Knock</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>~2Knock~, ~SCRL91~, ~SPWI207~, ~Arcane~, ~2~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL91~</v>
       </c>
     </row>
@@ -21866,11 +21872,11 @@
         <v>83</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="6"/>
-        <v>~SPWI208~, ~Arcane~, ~2~, ~Know Alignment~ =&gt; ~SPWI208~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI208~, ~Arcane~, ~2~ =&gt; ~SPWI208~    //Know Alignment</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>~2Know Alignment~, ~SCRL92~, ~SPWI208~, ~Arcane~, ~2~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL92~</v>
       </c>
     </row>
@@ -21891,11 +21897,11 @@
         <v>84</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="6"/>
-        <v>~SPWI209~, ~Arcane~, ~2~, ~Luck~ =&gt; ~SPWI209~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI209~, ~Arcane~, ~2~ =&gt; ~SPWI209~    //Luck</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>~2Luck~, ~SCRL93~, ~SPWI209~, ~Arcane~, ~2~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL93~</v>
       </c>
     </row>
@@ -21916,11 +21922,11 @@
         <v>85</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="6"/>
-        <v>~SPWI210~, ~Arcane~, ~2~, ~Resist Fear~ =&gt; ~SPWI210~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI210~, ~Arcane~, ~2~ =&gt; ~SPWI210~    //Resist Fear</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>~2Resist Fear~, ~SCRL94~, ~SPWI210~, ~Arcane~, ~2~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL94~</v>
       </c>
     </row>
@@ -21941,11 +21947,11 @@
         <v>86</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="6"/>
-        <v>~SPWI211~, ~Arcane~, ~2~, ~Melf's Acid Arrow~ =&gt; ~SPWI211~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI211~, ~Arcane~, ~2~ =&gt; ~SPWI211~    //Melf's Acid Arrow</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>~2Melf's Acid Arrow~, ~SCRL95~, ~SPWI211~, ~Arcane~, ~2~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL95~</v>
       </c>
     </row>
@@ -21966,11 +21972,11 @@
         <v>87</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="6"/>
-        <v>~SPWI212~, ~Arcane~, ~2~, ~Mirror Image~ =&gt; ~SPWI212~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI212~, ~Arcane~, ~2~ =&gt; ~SPWI212~    //Mirror Image</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>~2Mirror Image~, ~SCRL96~, ~SPWI212~, ~Arcane~, ~2~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL96~</v>
       </c>
     </row>
@@ -21991,11 +21997,11 @@
         <v>88</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="6"/>
-        <v>~SPWI213~, ~Arcane~, ~2~, ~Stinking Cloud~ =&gt; ~SPWI213~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI213~, ~Arcane~, ~2~ =&gt; ~SPWI213~    //Stinking Cloud</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>~2Stinking Cloud~, ~SCRL97~, ~SPWI213~, ~Arcane~, ~2~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL97~</v>
       </c>
     </row>
@@ -22016,11 +22022,11 @@
         <v>89</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="6"/>
-        <v>~SPWI214~, ~Arcane~, ~2~, ~Strength~ =&gt; ~SPWI214~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI214~, ~Arcane~, ~2~ =&gt; ~SPWI214~    //Strength</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>~2Strength~, ~SCRL98~, ~SPWI214~, ~Arcane~, ~2~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL98~</v>
       </c>
     </row>
@@ -22041,11 +22047,11 @@
         <v>90</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" si="6"/>
-        <v>~SPWI215~, ~Arcane~, ~2~, ~Web~ =&gt; ~SPWI215~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI215~, ~Arcane~, ~2~ =&gt; ~SPWI215~    //Web</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>~2Web~, ~SCRL99~, ~SPWI215~, ~Arcane~, ~2~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL99~</v>
       </c>
     </row>
@@ -22066,11 +22072,11 @@
         <v>91</v>
       </c>
       <c r="F41" t="str">
-        <f t="shared" ref="F41:F48" si="7">_xlfn.CONCAT("~", C41, "~, ~", A41, "~, ~", B41, "~, ~", E41, "~ =&gt; ~", C41, "~")</f>
-        <v>~SPWI217~, ~Arcane~, ~2~, ~Agannazar's Scorcher~ =&gt; ~SPWI217~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI217~, ~Arcane~, ~2~ =&gt; ~SPWI217~    //Agannazar's Scorcher</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>~2Agannazar's Scorcher~, ~SCRL1B~, ~SPWI217~, ~Arcane~, ~2~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1B~</v>
       </c>
     </row>
@@ -22091,11 +22097,11 @@
         <v>92</v>
       </c>
       <c r="F42" t="str">
-        <f t="shared" si="7"/>
-        <v>~SPWI218~, ~Arcane~, ~2~, ~Ghoul Touch~ =&gt; ~SPWI218~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI218~, ~Arcane~, ~2~ =&gt; ~SPWI218~    //Ghoul Touch</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>~2Ghoul Touch~, ~SCRL1C~, ~SPWI218~, ~Arcane~, ~2~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1C~</v>
       </c>
     </row>
@@ -22116,11 +22122,11 @@
         <v>93</v>
       </c>
       <c r="F43" t="str">
-        <f t="shared" si="7"/>
-        <v>~SPWI219~, ~Arcane~, ~2~, ~Vocalize~ =&gt; ~SPWI219~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI219~, ~Arcane~, ~2~ =&gt; ~SPWI219~    //Vocalize</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>~2Vocalize~, ~SCRL3G~, ~SPWI219~, ~Arcane~, ~2~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL3G~</v>
       </c>
     </row>
@@ -22141,11 +22147,11 @@
         <v>556</v>
       </c>
       <c r="F44" t="str">
-        <f t="shared" si="7"/>
-        <v>~SPWI220~, ~Arcane~, ~2~, ~Power Word Sleep~ =&gt; ~SPWI220~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI220~, ~Arcane~, ~2~ =&gt; ~SPWI220~    //Power Word Sleep</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>~2Power Word Sleep~, ~SCRL6E~, ~SPWI220~, ~Arcane~, ~2~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL6E~</v>
       </c>
     </row>
@@ -22166,11 +22172,11 @@
         <v>557</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="7"/>
-        <v>~SPWI221~, ~Arcane~, ~2~, ~Ray of Enfeeblement~ =&gt; ~SPWI221~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI221~, ~Arcane~, ~2~ =&gt; ~SPWI221~    //Ray of Enfeeblement</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>~2Ray of Enfeeblement~, ~SCRLAI~, ~SPWI221~, ~Arcane~, ~2~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRLAI~</v>
       </c>
     </row>
@@ -22188,8 +22194,8 @@
         <v>558</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="7"/>
-        <v>~SPWI222~, ~Arcane~, ~2~, ~Chaos Shield*~ =&gt; ~SPWI222~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI222~, ~Arcane~, ~2~ =&gt; ~SPWI222~    //Chaos Shield*</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
@@ -22209,11 +22215,11 @@
         <v>559</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="7"/>
-        <v>~SPWI223~, ~Arcane~, ~2~, ~Deafness~ =&gt; ~SPWI223~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI223~, ~Arcane~, ~2~ =&gt; ~SPWI223~    //Deafness</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>~2Deafness~, ~SCRLA2~, ~SPWI223~, ~Arcane~, ~2~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRLA2~</v>
       </c>
     </row>
@@ -22234,11 +22240,11 @@
         <v>560</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="7"/>
-        <v>~SPWI224~, ~Arcane~, ~2~, ~Glitterdust~ =&gt; ~SPWI224~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI224~, ~Arcane~, ~2~ =&gt; ~SPWI224~    //Glitterdust</v>
       </c>
       <c r="G48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>~2Glitterdust~, ~SCRLA3~, ~SPWI224~, ~Arcane~, ~2~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRLA3~</v>
       </c>
     </row>
@@ -22259,12 +22265,18 @@
         <v>828</v>
       </c>
       <c r="F49" t="str">
-        <f>_xlfn.CONCAT("~", C49, "~, ~", A49, "~, ~", B49, "~, ~", E49, "~ =&gt; ~", C49, "~")</f>
-        <v>~SPWI228~, ~Arcane~, ~2~, ~Darkness 15' Radius~ =&gt; ~SPWI228~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI228~, ~Arcane~, ~2~ =&gt; ~SPWI228~    //Darkness 15' Radius</v>
       </c>
       <c r="G49" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>~2Darkness 15' Radius~, ~BDSCRL2A~, ~SPWI228~, ~Arcane~, ~2~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~BDSCRL2A~</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F50" t="str">
+        <f t="shared" si="1"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
@@ -22284,11 +22296,11 @@
         <v>111</v>
       </c>
       <c r="F51" t="str">
-        <f t="shared" ref="F51:F72" si="8">_xlfn.CONCAT("~", C51, "~, ~", A51, "~, ~", B51, "~, ~", E51, "~ =&gt; ~", C51, "~")</f>
-        <v>~SPWI301~, ~Arcane~, ~3~, ~Clairvoyance~ =&gt; ~SPWI301~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI301~, ~Arcane~, ~3~ =&gt; ~SPWI301~    //Clairvoyance</v>
       </c>
       <c r="G51" t="str">
-        <f t="shared" ref="G27:G57" si="9">_xlfn.CONCAT("~", D51, "~, ~", C51, "~, ~", A51, "~, ~", B51, "~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~", " =&gt; ~", D51, "~")</f>
+        <f t="shared" ref="G51:G57" si="4">_xlfn.CONCAT("~", D51, "~, ~", C51, "~, ~", A51, "~, ~", B51, "~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~", " =&gt; ~", D51, "~")</f>
         <v>~SCRL1D~, ~SPWI301~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1D~</v>
       </c>
     </row>
@@ -22309,11 +22321,11 @@
         <v>567</v>
       </c>
       <c r="F52" t="str">
-        <f t="shared" si="8"/>
-        <v>~SPWI302~, ~Arcane~, ~3~, ~Remove Magic~ =&gt; ~SPWI302~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI302~, ~Arcane~, ~3~ =&gt; ~SPWI302~    //Remove Magic</v>
       </c>
       <c r="G52" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>~SCRLA7~, ~SPWI302~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRLA7~</v>
       </c>
     </row>
@@ -22334,11 +22346,11 @@
         <v>321</v>
       </c>
       <c r="F53" t="str">
-        <f t="shared" si="8"/>
-        <v>~SPWI303~, ~Arcane~, ~3~, ~Flame Arrow~ =&gt; ~SPWI303~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI303~, ~Arcane~, ~3~ =&gt; ~SPWI303~    //Flame Arrow</v>
       </c>
       <c r="G53" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>~SCRL1F~, ~SPWI303~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1F~</v>
       </c>
     </row>
@@ -22359,11 +22371,11 @@
         <v>113</v>
       </c>
       <c r="F54" t="str">
-        <f t="shared" si="8"/>
-        <v>~SPWI304~, ~Arcane~, ~3~, ~Fireball~ =&gt; ~SPWI304~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI304~, ~Arcane~, ~3~ =&gt; ~SPWI304~    //Fireball</v>
       </c>
       <c r="G54" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>~SCRL1G~, ~SPWI304~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1G~</v>
       </c>
     </row>
@@ -22384,11 +22396,11 @@
         <v>114</v>
       </c>
       <c r="F55" t="str">
-        <f t="shared" si="8"/>
-        <v>~SPWI305~, ~Arcane~, ~3~, ~Haste~ =&gt; ~SPWI305~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI305~, ~Arcane~, ~3~ =&gt; ~SPWI305~    //Haste</v>
       </c>
       <c r="G55" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>~SCRL1H~, ~SPWI305~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1H~</v>
       </c>
     </row>
@@ -22409,11 +22421,11 @@
         <v>115</v>
       </c>
       <c r="F56" t="str">
-        <f t="shared" si="8"/>
-        <v>~SPWI306~, ~Arcane~, ~3~, ~Hold Person~ =&gt; ~SPWI306~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI306~, ~Arcane~, ~3~ =&gt; ~SPWI306~    //Hold Person</v>
       </c>
       <c r="G56" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>~SCRL1I~, ~SPWI306~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1I~</v>
       </c>
     </row>
@@ -22434,11 +22446,11 @@
         <v>831</v>
       </c>
       <c r="F57" t="str">
-        <f t="shared" si="8"/>
-        <v>~SPWI307~, ~Arcane~, ~3~, ~Invisibility 10' Radius~ =&gt; ~SPWI307~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI307~, ~Arcane~, ~3~ =&gt; ~SPWI307~    //Invisibility 10' Radius</v>
       </c>
       <c r="G57" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>~SCRL1J~, ~SPWI307~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1J~</v>
       </c>
     </row>
@@ -22459,11 +22471,11 @@
         <v>116</v>
       </c>
       <c r="F58" t="str">
-        <f t="shared" si="8"/>
-        <v>~SPWI308~, ~Arcane~, ~3~, ~Lightning Bolt~ =&gt; ~SPWI308~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI308~, ~Arcane~, ~3~ =&gt; ~SPWI308~    //Lightning Bolt</v>
       </c>
       <c r="G58" t="str">
-        <f t="shared" ref="G58:G110" si="10">_xlfn.CONCAT("~", D58, "~, ~", C58, "~, ~", A58, "~, ~", B58, "~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~", " =&gt; ~", D58, "~")</f>
+        <f t="shared" ref="G58:G110" si="5">_xlfn.CONCAT("~", D58, "~, ~", C58, "~, ~", A58, "~, ~", B58, "~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~", " =&gt; ~", D58, "~")</f>
         <v>~SCRL1K~, ~SPWI308~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1K~</v>
       </c>
     </row>
@@ -22484,11 +22496,11 @@
         <v>117</v>
       </c>
       <c r="F59" t="str">
-        <f t="shared" si="8"/>
-        <v>~SPWI309~, ~Arcane~, ~3~, ~Monster Summoning 1~ =&gt; ~SPWI309~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI309~, ~Arcane~, ~3~ =&gt; ~SPWI309~    //Monster Summoning 1</v>
       </c>
       <c r="G59" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL1L~, ~SPWI309~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1L~</v>
       </c>
     </row>
@@ -22509,11 +22521,11 @@
         <v>830</v>
       </c>
       <c r="F60" t="str">
-        <f t="shared" si="8"/>
-        <v>~SPWI310~, ~Arcane~, ~3~, ~Non-Detection~ =&gt; ~SPWI310~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI310~, ~Arcane~, ~3~ =&gt; ~SPWI310~    //Non-Detection</v>
       </c>
       <c r="G60" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL1M~, ~SPWI310~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1M~</v>
       </c>
     </row>
@@ -22534,11 +22546,11 @@
         <v>119</v>
       </c>
       <c r="F61" t="str">
-        <f t="shared" si="8"/>
-        <v>~SPWI311~, ~Arcane~, ~3~, ~Protection from Normal Missiles~ =&gt; ~SPWI311~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI311~, ~Arcane~, ~3~ =&gt; ~SPWI311~    //Protection from Normal Missiles</v>
       </c>
       <c r="G61" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL1N~, ~SPWI311~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1N~</v>
       </c>
     </row>
@@ -22559,11 +22571,11 @@
         <v>120</v>
       </c>
       <c r="F62" t="str">
-        <f t="shared" si="8"/>
-        <v>~SPWI312~, ~Arcane~, ~3~, ~Slow~ =&gt; ~SPWI312~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI312~, ~Arcane~, ~3~ =&gt; ~SPWI312~    //Slow</v>
       </c>
       <c r="G62" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL1O~, ~SPWI312~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1O~</v>
       </c>
     </row>
@@ -22584,11 +22596,11 @@
         <v>121</v>
       </c>
       <c r="F63" t="str">
-        <f t="shared" si="8"/>
-        <v>~SPWI313~, ~Arcane~, ~3~, ~Skull Trap~ =&gt; ~SPWI313~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI313~, ~Arcane~, ~3~ =&gt; ~SPWI313~    //Skull Trap</v>
       </c>
       <c r="G63" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL1P~, ~SPWI313~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1P~</v>
       </c>
     </row>
@@ -22609,11 +22621,11 @@
         <v>122</v>
       </c>
       <c r="F64" t="str">
-        <f t="shared" si="8"/>
-        <v>~SPWI314~, ~Arcane~, ~3~, ~Vampiric Touch~ =&gt; ~SPWI314~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI314~, ~Arcane~, ~3~ =&gt; ~SPWI314~    //Vampiric Touch</v>
       </c>
       <c r="G64" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL1Q~, ~SPWI314~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1Q~</v>
       </c>
     </row>
@@ -22634,11 +22646,11 @@
         <v>123</v>
       </c>
       <c r="F65" t="str">
-        <f t="shared" si="8"/>
-        <v>~SPWI315~, ~Arcane~, ~3~, ~Wraith Form~ =&gt; ~SPWI315~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI315~, ~Arcane~, ~3~ =&gt; ~SPWI315~    //Wraith Form</v>
       </c>
       <c r="G65" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL1R~, ~SPWI315~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1R~</v>
       </c>
     </row>
@@ -22659,11 +22671,11 @@
         <v>124</v>
       </c>
       <c r="F66" t="str">
-        <f t="shared" si="8"/>
-        <v>~SPWI316~, ~Arcane~, ~3~, ~Dire Charm~ =&gt; ~SPWI316~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI316~, ~Arcane~, ~3~ =&gt; ~SPWI316~    //Dire Charm</v>
       </c>
       <c r="G66" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL1S~, ~SPWI316~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1S~</v>
       </c>
     </row>
@@ -22684,11 +22696,11 @@
         <v>125</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" si="8"/>
-        <v>~SPWI317~, ~Arcane~, ~3~, ~Ghost Armor~ =&gt; ~SPWI317~</v>
+        <f t="shared" si="1"/>
+        <v>~SPWI317~, ~Arcane~, ~3~ =&gt; ~SPWI317~    //Ghost Armor</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL1T~, ~SPWI317~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1T~</v>
       </c>
     </row>
@@ -22709,11 +22721,11 @@
         <v>561</v>
       </c>
       <c r="F68" t="str">
-        <f t="shared" si="8"/>
-        <v>~SPWI318~, ~Arcane~, ~3~, ~Minor Spell Deflection~ =&gt; ~SPWI318~</v>
+        <f t="shared" ref="F68:F131" si="6">_xlfn.CONCAT("~", C68, "~, ~", A68, "~, ~", B68, "~ =&gt; ~", C68, "~    //", E68)</f>
+        <v>~SPWI318~, ~Arcane~, ~3~ =&gt; ~SPWI318~    //Minor Spell Deflection</v>
       </c>
       <c r="G68" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL6G~, ~SPWI318~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL6G~</v>
       </c>
     </row>
@@ -22734,11 +22746,11 @@
         <v>562</v>
       </c>
       <c r="F69" t="str">
-        <f t="shared" si="8"/>
-        <v>~SPWI319~, ~Arcane~, ~3~, ~Protection from Fire~ =&gt; ~SPWI319~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI319~, ~Arcane~, ~3~ =&gt; ~SPWI319~    //Protection from Fire</v>
       </c>
       <c r="G69" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL6H~, ~SPWI319~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL6H~</v>
       </c>
     </row>
@@ -22759,11 +22771,11 @@
         <v>563</v>
       </c>
       <c r="F70" t="str">
-        <f t="shared" si="8"/>
-        <v>~SPWI320~, ~Arcane~, ~3~, ~Protection from Cold~ =&gt; ~SPWI320~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI320~, ~Arcane~, ~3~ =&gt; ~SPWI320~    //Protection from Cold</v>
       </c>
       <c r="G70" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL6I~, ~SPWI320~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL6I~</v>
       </c>
     </row>
@@ -22784,11 +22796,11 @@
         <v>564</v>
       </c>
       <c r="F71" t="str">
-        <f t="shared" si="8"/>
-        <v>~SPWI321~, ~Arcane~, ~3~, ~Spell Thrust~ =&gt; ~SPWI321~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI321~, ~Arcane~, ~3~ =&gt; ~SPWI321~    //Spell Thrust</v>
       </c>
       <c r="G71" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL6J~, ~SPWI321~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL6J~</v>
       </c>
     </row>
@@ -22809,11 +22821,11 @@
         <v>565</v>
       </c>
       <c r="F72" t="str">
-        <f t="shared" si="8"/>
-        <v>~SPWI322~, ~Arcane~, ~3~, ~Detect Illusion~ =&gt; ~SPWI322~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI322~, ~Arcane~, ~3~ =&gt; ~SPWI322~    //Detect Illusion</v>
       </c>
       <c r="G72" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL6K~, ~SPWI322~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL6K~</v>
       </c>
     </row>
@@ -22834,11 +22846,11 @@
         <v>489</v>
       </c>
       <c r="F73" t="str">
-        <f t="shared" ref="F73:F75" si="11">_xlfn.CONCAT("~", C73, "~, ~", A73, "~, ~", B73, "~, ~", E73, "~ =&gt; ~", C73, "~")</f>
-        <v>~SPWI324~, ~Arcane~, ~3~, ~Hold Undead~ =&gt; ~SPWI324~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI324~, ~Arcane~, ~3~ =&gt; ~SPWI324~    //Hold Undead</v>
       </c>
       <c r="G73" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL6L~, ~SPWI324~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL6L~</v>
       </c>
     </row>
@@ -22859,11 +22871,11 @@
         <v>566</v>
       </c>
       <c r="F74" t="str">
-        <f t="shared" si="11"/>
-        <v>~SPWI325~, ~Arcane~, ~3~, ~Melf's Minute Meteors~ =&gt; ~SPWI325~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI325~, ~Arcane~, ~3~ =&gt; ~SPWI325~    //Melf's Minute Meteors</v>
       </c>
       <c r="G74" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRLA5~, ~SPWI325~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRLA5~</v>
       </c>
     </row>
@@ -22884,12 +22896,18 @@
         <v>112</v>
       </c>
       <c r="F75" t="str">
-        <f t="shared" si="11"/>
-        <v>~SPWI326~, ~Arcane~, ~3~, ~Dispel Magic~ =&gt; ~SPWI326~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI326~, ~Arcane~, ~3~ =&gt; ~SPWI326~    //Dispel Magic</v>
       </c>
       <c r="G75" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL1E~, ~SPWI326~, ~Arcane~, ~3~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1E~</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F76" t="str">
+        <f t="shared" si="6"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
@@ -22909,11 +22927,11 @@
         <v>127</v>
       </c>
       <c r="F77" t="str">
-        <f t="shared" ref="F77:F97" si="12">_xlfn.CONCAT("~", C77, "~, ~", A77, "~, ~", B77, "~, ~", E77, "~ =&gt; ~", C77, "~")</f>
-        <v>~SPWI401~, ~Arcane~, ~4~, ~Confusion~ =&gt; ~SPWI401~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI401~, ~Arcane~, ~4~ =&gt; ~SPWI401~    //Confusion</v>
       </c>
       <c r="G77" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL1U~, ~SPWI401~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1U~</v>
       </c>
     </row>
@@ -22934,11 +22952,11 @@
         <v>143</v>
       </c>
       <c r="F78" t="str">
-        <f t="shared" si="12"/>
-        <v>~SPWI402~, ~Arcane~, ~4~, ~Dimension Door~ =&gt; ~SPWI402~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI402~, ~Arcane~, ~4~ =&gt; ~SPWI402~    //Dimension Door</v>
       </c>
       <c r="G78" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL1V~, ~SPWI402~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1V~</v>
       </c>
     </row>
@@ -22959,11 +22977,11 @@
         <v>575</v>
       </c>
       <c r="F79" t="str">
-        <f t="shared" si="12"/>
-        <v>~SPWI403~, ~Arcane~, ~4~, ~Fire Shield (Blue)~ =&gt; ~SPWI403~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI403~, ~Arcane~, ~4~ =&gt; ~SPWI403~    //Fire Shield (Blue)</v>
       </c>
       <c r="G79" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL1W~, ~SPWI403~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1W~</v>
       </c>
     </row>
@@ -22984,11 +23002,11 @@
         <v>144</v>
       </c>
       <c r="F80" t="str">
-        <f t="shared" si="12"/>
-        <v>~SPWI404~, ~Arcane~, ~4~, ~Ice Storm~ =&gt; ~SPWI404~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI404~, ~Arcane~, ~4~ =&gt; ~SPWI404~    //Ice Storm</v>
       </c>
       <c r="G80" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL1X~, ~SPWI404~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1X~</v>
       </c>
     </row>
@@ -23009,11 +23027,11 @@
         <v>145</v>
       </c>
       <c r="F81" t="str">
-        <f t="shared" si="12"/>
-        <v>~SPWI405~, ~Arcane~, ~4~, ~Improved Invisibility~ =&gt; ~SPWI405~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI405~, ~Arcane~, ~4~ =&gt; ~SPWI405~    //Improved Invisibility</v>
       </c>
       <c r="G81" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL1Y~, ~SPWI405~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1Y~</v>
       </c>
     </row>
@@ -23034,11 +23052,11 @@
         <v>146</v>
       </c>
       <c r="F82" t="str">
-        <f t="shared" si="12"/>
-        <v>~SPWI406~, ~Arcane~, ~4~, ~Minor Globe of Invulnerability~ =&gt; ~SPWI406~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI406~, ~Arcane~, ~4~ =&gt; ~SPWI406~    //Minor Globe of Invulnerability</v>
       </c>
       <c r="G82" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL1Z~, ~SPWI406~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL1Z~</v>
       </c>
     </row>
@@ -23059,11 +23077,11 @@
         <v>147</v>
       </c>
       <c r="F83" t="str">
-        <f t="shared" si="12"/>
-        <v>~SPWI407~, ~Arcane~, ~4~, ~Monster Summoning 2~ =&gt; ~SPWI407~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI407~, ~Arcane~, ~4~ =&gt; ~SPWI407~    //Monster Summoning 2</v>
       </c>
       <c r="G83" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL2A~, ~SPWI407~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL2A~</v>
       </c>
     </row>
@@ -23084,11 +23102,11 @@
         <v>183</v>
       </c>
       <c r="F84" t="str">
-        <f t="shared" si="12"/>
-        <v>~SPWI408~, ~Arcane~, ~4~, ~Stone Skin~ =&gt; ~SPWI408~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI408~, ~Arcane~, ~4~ =&gt; ~SPWI408~    //Stone Skin</v>
       </c>
       <c r="G84" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL2B~, ~SPWI408~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL2B~</v>
       </c>
     </row>
@@ -23109,11 +23127,11 @@
         <v>806</v>
       </c>
       <c r="F85" t="str">
-        <f t="shared" si="12"/>
-        <v>~SPWI409~, ~Arcane~, ~4~, ~Contagion~ =&gt; ~SPWI409~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI409~, ~Arcane~, ~4~ =&gt; ~SPWI409~    //Contagion</v>
       </c>
       <c r="G85" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRLA8~, ~SPWI409~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRLA8~</v>
       </c>
     </row>
@@ -23134,11 +23152,11 @@
         <v>149</v>
       </c>
       <c r="F86" t="str">
-        <f t="shared" si="12"/>
-        <v>~SPWI410~, ~Arcane~, ~4~, ~Remove Curse~ =&gt; ~SPWI410~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI410~, ~Arcane~, ~4~ =&gt; ~SPWI410~    //Remove Curse</v>
       </c>
       <c r="G86" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL5G, SCRLAK~, ~SPWI410~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL5G, SCRLAK~</v>
       </c>
     </row>
@@ -23159,11 +23177,11 @@
         <v>205</v>
       </c>
       <c r="F87" t="str">
-        <f t="shared" si="12"/>
-        <v>~SPWI411~, ~Arcane~, ~4~, ~Emotion: Hopelessness~ =&gt; ~SPWI411~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI411~, ~Arcane~, ~4~ =&gt; ~SPWI411~    //Emotion: Hopelessness</v>
       </c>
       <c r="G87" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL5H~, ~SPWI411~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL5H~</v>
       </c>
     </row>
@@ -23184,11 +23202,11 @@
         <v>151</v>
       </c>
       <c r="F88" t="str">
-        <f t="shared" si="12"/>
-        <v>~SPWI412~, ~Arcane~, ~4~, ~Greater Malison~ =&gt; ~SPWI412~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI412~, ~Arcane~, ~4~ =&gt; ~SPWI412~    //Greater Malison</v>
       </c>
       <c r="G88" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL5I~, ~SPWI412~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL5I~</v>
       </c>
     </row>
@@ -23209,11 +23227,11 @@
         <v>152</v>
       </c>
       <c r="F89" t="str">
-        <f t="shared" si="12"/>
-        <v>~SPWI413~, ~Arcane~, ~4~, ~Otiluke's Resilient Sphere~ =&gt; ~SPWI413~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI413~, ~Arcane~, ~4~ =&gt; ~SPWI413~    //Otiluke's Resilient Sphere</v>
       </c>
       <c r="G89" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL5J~, ~SPWI413~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL5J~</v>
       </c>
     </row>
@@ -23234,11 +23252,11 @@
         <v>153</v>
       </c>
       <c r="F90" t="str">
-        <f t="shared" si="12"/>
-        <v>~SPWI414~, ~Arcane~, ~4~, ~Spirit Armor~ =&gt; ~SPWI414~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI414~, ~Arcane~, ~4~ =&gt; ~SPWI414~    //Spirit Armor</v>
       </c>
       <c r="G90" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL5K~, ~SPWI414~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL5K~</v>
       </c>
     </row>
@@ -23259,11 +23277,11 @@
         <v>154</v>
       </c>
       <c r="F91" t="str">
-        <f t="shared" si="12"/>
-        <v>~SPWI415~, ~Arcane~, ~4~, ~Polymorph Other~ =&gt; ~SPWI415~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI415~, ~Arcane~, ~4~ =&gt; ~SPWI415~    //Polymorph Other</v>
       </c>
       <c r="G91" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL5L~, ~SPWI415~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL5L~</v>
       </c>
     </row>
@@ -23284,11 +23302,11 @@
         <v>155</v>
       </c>
       <c r="F92" t="str">
-        <f t="shared" si="12"/>
-        <v>~SPWI416~, ~Arcane~, ~4~, ~Polymorph Self~ =&gt; ~SPWI416~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI416~, ~Arcane~, ~4~ =&gt; ~SPWI416~    //Polymorph Self</v>
       </c>
       <c r="G92" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL5M~, ~SPWI416~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL5M~</v>
       </c>
     </row>
@@ -23309,11 +23327,11 @@
         <v>577</v>
       </c>
       <c r="F93" t="str">
-        <f t="shared" si="12"/>
-        <v>~SPWI417~, ~Arcane~, ~4~, ~Enchanted Weapon~ =&gt; ~SPWI417~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI417~, ~Arcane~, ~4~ =&gt; ~SPWI417~    //Enchanted Weapon</v>
       </c>
       <c r="G93" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL6M~, ~SPWI417~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL6M~</v>
       </c>
     </row>
@@ -23334,11 +23352,11 @@
         <v>578</v>
       </c>
       <c r="F94" t="str">
-        <f t="shared" si="12"/>
-        <v>~SPWI418~, ~Arcane~, ~4~, ~Fire Shield (Red)~ =&gt; ~SPWI418~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI418~, ~Arcane~, ~4~ =&gt; ~SPWI418~    //Fire Shield (Red)</v>
       </c>
       <c r="G94" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL6N~, ~SPWI418~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL6N~</v>
       </c>
     </row>
@@ -23359,11 +23377,11 @@
         <v>579</v>
       </c>
       <c r="F95" t="str">
-        <f t="shared" si="12"/>
-        <v>~SPWI419~, ~Arcane~, ~4~, ~Secret Word~ =&gt; ~SPWI419~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI419~, ~Arcane~, ~4~ =&gt; ~SPWI419~    //Secret Word</v>
       </c>
       <c r="G95" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL6O~, ~SPWI419~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL6O~</v>
       </c>
     </row>
@@ -23384,11 +23402,11 @@
         <v>580</v>
       </c>
       <c r="F96" t="str">
-        <f t="shared" si="12"/>
-        <v>~SPWI420~, ~Arcane~, ~4~, ~Minor Sequencer~ =&gt; ~SPWI420~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI420~, ~Arcane~, ~4~ =&gt; ~SPWI420~    //Minor Sequencer</v>
       </c>
       <c r="G96" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL6P~, ~SPWI420~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL6P~</v>
       </c>
     </row>
@@ -23409,11 +23427,11 @@
         <v>581</v>
       </c>
       <c r="F97" t="str">
-        <f t="shared" si="12"/>
-        <v>~SPWI421~, ~Arcane~, ~4~, ~Teleport Field~ =&gt; ~SPWI421~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI421~, ~Arcane~, ~4~ =&gt; ~SPWI421~    //Teleport Field</v>
       </c>
       <c r="G97" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL6Q~, ~SPWI421~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL6Q~</v>
       </c>
     </row>
@@ -23434,11 +23452,11 @@
         <v>582</v>
       </c>
       <c r="F98" t="str">
-        <f t="shared" ref="F98:F100" si="13">_xlfn.CONCAT("~", C98, "~, ~", A98, "~, ~", B98, "~, ~", E98, "~ =&gt; ~", C98, "~")</f>
-        <v>~SPWI423~, ~Arcane~, ~4~, ~Spider Spawn~ =&gt; ~SPWI423~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI423~, ~Arcane~, ~4~ =&gt; ~SPWI423~    //Spider Spawn</v>
       </c>
       <c r="G98" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL6R~, ~SPWI423~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL6R~</v>
       </c>
     </row>
@@ -23459,11 +23477,11 @@
         <v>583</v>
       </c>
       <c r="F99" t="str">
-        <f t="shared" si="13"/>
-        <v>~SPWI424~, ~Arcane~, ~4~, ~Farsight~ =&gt; ~SPWI424~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI424~, ~Arcane~, ~4~ =&gt; ~SPWI424~    //Farsight</v>
       </c>
       <c r="G99" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRLAJ;SCRLAQ~, ~SPWI424~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRLAJ;SCRLAQ~</v>
       </c>
     </row>
@@ -23484,12 +23502,18 @@
         <v>584</v>
       </c>
       <c r="F100" t="str">
-        <f t="shared" si="13"/>
-        <v>~SPWI425~, ~Arcane~, ~4~, ~Wizard Eye~ =&gt; ~SPWI425~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI425~, ~Arcane~, ~4~ =&gt; ~SPWI425~    //Wizard Eye</v>
       </c>
       <c r="G100" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRLA1~, ~SPWI425~, ~Arcane~, ~4~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRLA1~</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F101" t="str">
+        <f t="shared" si="6"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.35">
@@ -23509,11 +23533,11 @@
         <v>165</v>
       </c>
       <c r="F102" t="str">
-        <f t="shared" ref="F102:F124" si="14">_xlfn.CONCAT("~", C102, "~, ~", A102, "~, ~", B102, "~, ~", E102, "~ =&gt; ~", C102, "~")</f>
-        <v>~SPWI501~, ~Arcane~, ~5~, ~Animate Dead~ =&gt; ~SPWI501~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI501~, ~Arcane~, ~5~ =&gt; ~SPWI501~    //Animate Dead</v>
       </c>
       <c r="G102" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL2D~, ~SPWI501~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL2D~</v>
       </c>
     </row>
@@ -23534,11 +23558,11 @@
         <v>167</v>
       </c>
       <c r="F103" t="str">
-        <f t="shared" si="14"/>
-        <v>~SPWI502~, ~Arcane~, ~5~, ~Cloud Kill~ =&gt; ~SPWI502~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI502~, ~Arcane~, ~5~ =&gt; ~SPWI502~    //Cloud Kill</v>
       </c>
       <c r="G103" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL2E~, ~SPWI502~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL2E~</v>
       </c>
     </row>
@@ -23559,11 +23583,11 @@
         <v>168</v>
       </c>
       <c r="F104" t="str">
-        <f t="shared" si="14"/>
-        <v>~SPWI503~, ~Arcane~, ~5~, ~Cone of Cold~ =&gt; ~SPWI503~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI503~, ~Arcane~, ~5~ =&gt; ~SPWI503~    //Cone of Cold</v>
       </c>
       <c r="G104" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL2F~, ~SPWI503~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL2F~</v>
       </c>
     </row>
@@ -23584,11 +23608,11 @@
         <v>169</v>
       </c>
       <c r="F105" t="str">
-        <f t="shared" si="14"/>
-        <v>~SPWI504~, ~Arcane~, ~5~, ~Monster Summoning 3~ =&gt; ~SPWI504~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI504~, ~Arcane~, ~5~ =&gt; ~SPWI504~    //Monster Summoning 3</v>
       </c>
       <c r="G105" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL2G~, ~SPWI504~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL2G~</v>
       </c>
     </row>
@@ -23609,11 +23633,11 @@
         <v>170</v>
       </c>
       <c r="F106" t="str">
-        <f t="shared" si="14"/>
-        <v>~SPWI505~, ~Arcane~, ~5~, ~Shadow Door~ =&gt; ~SPWI505~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI505~, ~Arcane~, ~5~ =&gt; ~SPWI505~    //Shadow Door</v>
       </c>
       <c r="G106" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL2H~, ~SPWI505~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL2H~</v>
       </c>
     </row>
@@ -23634,11 +23658,11 @@
         <v>171</v>
       </c>
       <c r="F107" t="str">
-        <f t="shared" si="14"/>
-        <v>~SPWI506~, ~Arcane~, ~5~, ~Domination~ =&gt; ~SPWI506~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI506~, ~Arcane~, ~5~ =&gt; ~SPWI506~    //Domination</v>
       </c>
       <c r="G107" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL5N~, ~SPWI506~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL5N~</v>
       </c>
     </row>
@@ -23659,11 +23683,11 @@
         <v>172</v>
       </c>
       <c r="F108" t="str">
-        <f t="shared" si="14"/>
-        <v>~SPWI507~, ~Arcane~, ~5~, ~Hold Monster~ =&gt; ~SPWI507~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI507~, ~Arcane~, ~5~ =&gt; ~SPWI507~    //Hold Monster</v>
       </c>
       <c r="G108" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL5O~, ~SPWI507~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL5O~</v>
       </c>
     </row>
@@ -23684,11 +23708,11 @@
         <v>173</v>
       </c>
       <c r="F109" t="str">
-        <f t="shared" si="14"/>
-        <v>~SPWI508~, ~Arcane~, ~5~, ~Chaos~ =&gt; ~SPWI508~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI508~, ~Arcane~, ~5~ =&gt; ~SPWI508~    //Chaos</v>
       </c>
       <c r="G109" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL5P~, ~SPWI508~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL5P~</v>
       </c>
     </row>
@@ -23709,11 +23733,11 @@
         <v>174</v>
       </c>
       <c r="F110" t="str">
-        <f t="shared" si="14"/>
-        <v>~SPWI509~, ~Arcane~, ~5~, ~Feeblemind~ =&gt; ~SPWI509~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI509~, ~Arcane~, ~5~ =&gt; ~SPWI509~    //Feeblemind</v>
       </c>
       <c r="G110" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>~SCRL5Q~, ~SPWI509~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL5Q~</v>
       </c>
     </row>
@@ -23734,11 +23758,11 @@
         <v>585</v>
       </c>
       <c r="F111" t="str">
-        <f t="shared" si="14"/>
-        <v>~SPWI510~, ~Arcane~, ~5~, ~Spell Immunity~ =&gt; ~SPWI510~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI510~, ~Arcane~, ~5~ =&gt; ~SPWI510~    //Spell Immunity</v>
       </c>
       <c r="G111" t="str">
-        <f t="shared" ref="G111:G174" si="15">_xlfn.CONCAT("~", D111, "~, ~", C111, "~, ~", A111, "~, ~", B111, "~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~", " =&gt; ~", D111, "~")</f>
+        <f t="shared" ref="G111:G174" si="7">_xlfn.CONCAT("~", D111, "~, ~", C111, "~, ~", A111, "~, ~", B111, "~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~", " =&gt; ~", D111, "~")</f>
         <v>~SCRL6S~, ~SPWI510~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL6S~</v>
       </c>
     </row>
@@ -23759,11 +23783,11 @@
         <v>586</v>
       </c>
       <c r="F112" t="str">
-        <f t="shared" si="14"/>
-        <v>~SPWI511~, ~Arcane~, ~5~, ~Protection from Normal Weapons~ =&gt; ~SPWI511~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI511~, ~Arcane~, ~5~ =&gt; ~SPWI511~    //Protection from Normal Weapons</v>
       </c>
       <c r="G112" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL6T~, ~SPWI511~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL6T~</v>
       </c>
     </row>
@@ -23784,11 +23808,11 @@
         <v>587</v>
       </c>
       <c r="F113" t="str">
-        <f t="shared" si="14"/>
-        <v>~SPWI512~, ~Arcane~, ~5~, ~Protection from Electricity~ =&gt; ~SPWI512~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI512~, ~Arcane~, ~5~ =&gt; ~SPWI512~    //Protection from Electricity</v>
       </c>
       <c r="G113" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL5T~, ~SPWI512~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL5T~</v>
       </c>
     </row>
@@ -23809,11 +23833,11 @@
         <v>588</v>
       </c>
       <c r="F114" t="str">
-        <f t="shared" si="14"/>
-        <v>~SPWI513~, ~Arcane~, ~5~, ~Breach~ =&gt; ~SPWI513~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI513~, ~Arcane~, ~5~ =&gt; ~SPWI513~    //Breach</v>
       </c>
       <c r="G114" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL6U~, ~SPWI513~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL6U~</v>
       </c>
     </row>
@@ -23834,11 +23858,11 @@
         <v>241</v>
       </c>
       <c r="F115" t="str">
-        <f t="shared" si="14"/>
-        <v>~SPWI514~, ~Arcane~, ~5~, ~Lower Resistance~ =&gt; ~SPWI514~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI514~, ~Arcane~, ~5~ =&gt; ~SPWI514~    //Lower Resistance</v>
       </c>
       <c r="G115" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL6V~, ~SPWI514~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL6V~</v>
       </c>
     </row>
@@ -23859,11 +23883,11 @@
         <v>593</v>
       </c>
       <c r="F116" t="str">
-        <f t="shared" si="14"/>
-        <v>~SPWI515~, ~Arcane~, ~5~, ~Oracle~ =&gt; ~SPWI515~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI515~, ~Arcane~, ~5~ =&gt; ~SPWI515~    //Oracle</v>
       </c>
       <c r="G116" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL6W~, ~SPWI515~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL6W~</v>
       </c>
     </row>
@@ -23884,11 +23908,11 @@
         <v>594</v>
       </c>
       <c r="F117" t="str">
-        <f t="shared" si="14"/>
-        <v>~SPWI516~, ~Arcane~, ~5~, ~Conjure Lesser Fire Elemental~ =&gt; ~SPWI516~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI516~, ~Arcane~, ~5~ =&gt; ~SPWI516~    //Conjure Lesser Fire Elemental</v>
       </c>
       <c r="G117" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL6X~, ~SPWI516~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL6X~</v>
       </c>
     </row>
@@ -23909,11 +23933,11 @@
         <v>599</v>
       </c>
       <c r="F118" t="str">
-        <f t="shared" si="14"/>
-        <v>~SPWI517~, ~Arcane~, ~5~, ~Protection from Acid~ =&gt; ~SPWI517~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI517~, ~Arcane~, ~5~ =&gt; ~SPWI517~    //Protection from Acid</v>
       </c>
       <c r="G118" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL6Y~, ~SPWI517~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL6Y~</v>
       </c>
     </row>
@@ -23934,11 +23958,11 @@
         <v>596</v>
       </c>
       <c r="F119" t="str">
-        <f t="shared" si="14"/>
-        <v>~SPWI518~, ~Arcane~, ~5~, ~Phantom Blade~ =&gt; ~SPWI518~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI518~, ~Arcane~, ~5~ =&gt; ~SPWI518~    //Phantom Blade</v>
       </c>
       <c r="G119" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL6Z~, ~SPWI518~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL6Z~</v>
       </c>
     </row>
@@ -23959,11 +23983,11 @@
         <v>597</v>
       </c>
       <c r="F120" t="str">
-        <f t="shared" si="14"/>
-        <v>~SPWI519~, ~Arcane~, ~5~, ~Spell Shield~ =&gt; ~SPWI519~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI519~, ~Arcane~, ~5~ =&gt; ~SPWI519~    //Spell Shield</v>
       </c>
       <c r="G120" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL8X~, ~SPWI519~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8X~</v>
       </c>
     </row>
@@ -23984,11 +24008,11 @@
         <v>598</v>
       </c>
       <c r="F121" t="str">
-        <f t="shared" si="14"/>
-        <v>~SPWI520~, ~Arcane~, ~5~, ~Conjure Lesser Air Elemental~ =&gt; ~SPWI520~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI520~, ~Arcane~, ~5~ =&gt; ~SPWI520~    //Conjure Lesser Air Elemental</v>
       </c>
       <c r="G121" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7B~, ~SPWI520~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7B~</v>
       </c>
     </row>
@@ -24009,11 +24033,11 @@
         <v>595</v>
       </c>
       <c r="F122" t="str">
-        <f t="shared" si="14"/>
-        <v>~SPWI521~, ~Arcane~, ~5~, ~Conjure Lesser Earth Elemental~ =&gt; ~SPWI521~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI521~, ~Arcane~, ~5~ =&gt; ~SPWI521~    //Conjure Lesser Earth Elemental</v>
       </c>
       <c r="G122" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7C~, ~SPWI521~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7C~</v>
       </c>
     </row>
@@ -24034,11 +24058,11 @@
         <v>600</v>
       </c>
       <c r="F123" t="str">
-        <f t="shared" si="14"/>
-        <v>~SPWI522~, ~Arcane~, ~5~, ~Minor Spell Turning~ =&gt; ~SPWI522~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI522~, ~Arcane~, ~5~ =&gt; ~SPWI522~    //Minor Spell Turning</v>
       </c>
       <c r="G123" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7D~, ~SPWI522~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7D~</v>
       </c>
     </row>
@@ -24059,83 +24083,131 @@
         <v>242</v>
       </c>
       <c r="F124" t="str">
-        <f t="shared" si="14"/>
-        <v>~SPWI523~, ~Arcane~, ~5~, ~Sunfire~ =&gt; ~SPWI523~</v>
+        <f t="shared" si="6"/>
+        <v>~SPWI523~, ~Arcane~, ~5~ =&gt; ~SPWI523~    //Sunfire</v>
       </c>
       <c r="G124" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRLAL;SCRLAR~, ~SPWI523~, ~Arcane~, ~5~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRLAL;SCRLAR~</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F125" t="str">
+        <f t="shared" si="6"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G125" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F126" t="str">
+        <f t="shared" si="6"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G126" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F127" t="str">
+        <f t="shared" si="6"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G127" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F128" t="str">
+        <f t="shared" si="6"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G128" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F129" t="str">
+        <f t="shared" si="6"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G129" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F130" t="str">
+        <f t="shared" si="6"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G130" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F131" t="str">
+        <f t="shared" si="6"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G131" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F132" t="str">
+        <f t="shared" ref="F132:F195" si="8">_xlfn.CONCAT("~", C132, "~, ~", A132, "~, ~", B132, "~ =&gt; ~", C132, "~    //", E132)</f>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G132" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F133" t="str">
+        <f t="shared" si="8"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G133" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F134" t="str">
+        <f t="shared" si="8"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G134" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F135" t="str">
+        <f t="shared" si="8"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G135" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F136" t="str">
+        <f t="shared" si="8"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G136" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
@@ -24156,11 +24228,11 @@
         <v>189</v>
       </c>
       <c r="F137" t="str">
-        <f t="shared" ref="F137:F145" si="16">_xlfn.CONCAT("~", C137, "~, ~", A137, "~, ~", B137, "~, ~", E137, "~ =&gt; ~", C137, "~")</f>
-        <v>~SPWI601~, ~Arcane~, ~6~, ~Invisible Stalker~ =&gt; ~SPWI601~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI601~, ~Arcane~, ~6~ =&gt; ~SPWI601~    //Invisible Stalker</v>
       </c>
       <c r="G137" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7E~, ~SPWI601~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7E~</v>
       </c>
     </row>
@@ -24181,11 +24253,11 @@
         <v>190</v>
       </c>
       <c r="F138" t="str">
-        <f t="shared" si="16"/>
-        <v>~SPWI602~, ~Arcane~, ~6~, ~Globe of Invulnerability~ =&gt; ~SPWI602~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI602~, ~Arcane~, ~6~ =&gt; ~SPWI602~    //Globe of Invulnerability</v>
       </c>
       <c r="G138" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7F~, ~SPWI602~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7F~</v>
       </c>
     </row>
@@ -24206,11 +24278,11 @@
         <v>315</v>
       </c>
       <c r="F139" t="str">
-        <f t="shared" si="16"/>
-        <v>~SPWI603~, ~Arcane~, ~6~, ~Tenser's Transformation~ =&gt; ~SPWI603~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI603~, ~Arcane~, ~6~ =&gt; ~SPWI603~    //Tenser's Transformation</v>
       </c>
       <c r="G139" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7G~, ~SPWI603~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7G~</v>
       </c>
     </row>
@@ -24231,11 +24303,11 @@
         <v>191</v>
       </c>
       <c r="F140" t="str">
-        <f t="shared" si="16"/>
-        <v>~SPWI604~, ~Arcane~, ~6~, ~Flesh to Stone~ =&gt; ~SPWI604~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI604~, ~Arcane~, ~6~ =&gt; ~SPWI604~    //Flesh to Stone</v>
       </c>
       <c r="G140" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7H~, ~SPWI604~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7H~</v>
       </c>
     </row>
@@ -24256,11 +24328,11 @@
         <v>192</v>
       </c>
       <c r="F141" t="str">
-        <f t="shared" si="16"/>
-        <v>~SPWI605~, ~Arcane~, ~6~, ~Death Spell~ =&gt; ~SPWI605~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI605~, ~Arcane~, ~6~ =&gt; ~SPWI605~    //Death Spell</v>
       </c>
       <c r="G141" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7I~, ~SPWI605~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7I~</v>
       </c>
     </row>
@@ -24281,11 +24353,11 @@
         <v>601</v>
       </c>
       <c r="F142" t="str">
-        <f t="shared" si="16"/>
-        <v>~SPWI606~, ~Arcane~, ~6~, ~Protection from Magical Energy~ =&gt; ~SPWI606~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI606~, ~Arcane~, ~6~ =&gt; ~SPWI606~    //Protection from Magical Energy</v>
       </c>
       <c r="G142" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7J~, ~SPWI606~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7J~</v>
       </c>
     </row>
@@ -24306,11 +24378,11 @@
         <v>602</v>
       </c>
       <c r="F143" t="str">
-        <f t="shared" si="16"/>
-        <v>~SPWI607~, ~Arcane~, ~6~, ~Mislead~ =&gt; ~SPWI607~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI607~, ~Arcane~, ~6~ =&gt; ~SPWI607~    //Mislead</v>
       </c>
       <c r="G143" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7K~, ~SPWI607~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7K~</v>
       </c>
     </row>
@@ -24331,11 +24403,11 @@
         <v>603</v>
       </c>
       <c r="F144" t="str">
-        <f t="shared" si="16"/>
-        <v>~SPWI608~, ~Arcane~, ~6~, ~Pierce Magic~ =&gt; ~SPWI608~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI608~, ~Arcane~, ~6~ =&gt; ~SPWI608~    //Pierce Magic</v>
       </c>
       <c r="G144" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7L~, ~SPWI608~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7L~</v>
       </c>
     </row>
@@ -24356,11 +24428,11 @@
         <v>604</v>
       </c>
       <c r="F145" t="str">
-        <f t="shared" si="16"/>
-        <v>~SPWI609~, ~Arcane~, ~6~, ~True Sight~ =&gt; ~SPWI609~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI609~, ~Arcane~, ~6~ =&gt; ~SPWI609~    //True Sight</v>
       </c>
       <c r="G145" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7M~, ~SPWI609~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7M~</v>
       </c>
     </row>
@@ -24368,8 +24440,12 @@
       <c r="C146" s="3"/>
       <c r="D146" s="3"/>
       <c r="E146" s="3"/>
+      <c r="F146" t="str">
+        <f t="shared" si="8"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G146" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
@@ -24390,11 +24466,11 @@
         <v>605</v>
       </c>
       <c r="F147" t="str">
-        <f t="shared" ref="F147:F161" si="17">_xlfn.CONCAT("~", C147, "~, ~", A147, "~, ~", B147, "~, ~", E147, "~ =&gt; ~", C147, "~")</f>
-        <v>~SPWI611~, ~Arcane~, ~6~, ~Protection from Magical Weapons~ =&gt; ~SPWI611~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI611~, ~Arcane~, ~6~ =&gt; ~SPWI611~    //Protection from Magical Weapons</v>
       </c>
       <c r="G147" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7O~, ~SPWI611~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7O~</v>
       </c>
     </row>
@@ -24415,11 +24491,11 @@
         <v>266</v>
       </c>
       <c r="F148" t="str">
-        <f t="shared" si="17"/>
-        <v>~SPWI612~, ~Arcane~, ~6~, ~Power Word Silence~ =&gt; ~SPWI612~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI612~, ~Arcane~, ~6~ =&gt; ~SPWI612~    //Power Word Silence</v>
       </c>
       <c r="G148" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7P~, ~SPWI612~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7P~</v>
       </c>
     </row>
@@ -24440,11 +24516,11 @@
         <v>606</v>
       </c>
       <c r="F149" t="str">
-        <f t="shared" si="17"/>
-        <v>~SPWI613~, ~Arcane~, ~6~, ~Improved Haste~ =&gt; ~SPWI613~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI613~, ~Arcane~, ~6~ =&gt; ~SPWI613~    //Improved Haste</v>
       </c>
       <c r="G149" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7Q~, ~SPWI613~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7Q~</v>
       </c>
     </row>
@@ -24465,11 +24541,11 @@
         <v>260</v>
       </c>
       <c r="F150" t="str">
-        <f t="shared" si="17"/>
-        <v>~SPWI614~, ~Arcane~, ~6~, ~Death Fog~ =&gt; ~SPWI614~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI614~, ~Arcane~, ~6~ =&gt; ~SPWI614~    //Death Fog</v>
       </c>
       <c r="G150" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7R~, ~SPWI614~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7R~</v>
       </c>
     </row>
@@ -24490,11 +24566,11 @@
         <v>259</v>
       </c>
       <c r="F151" t="str">
-        <f t="shared" si="17"/>
-        <v>~SPWI615~, ~Arcane~, ~6~, ~Chain Lightning~ =&gt; ~SPWI615~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI615~, ~Arcane~, ~6~ =&gt; ~SPWI615~    //Chain Lightning</v>
       </c>
       <c r="G151" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7S~, ~SPWI615~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7S~</v>
       </c>
     </row>
@@ -24515,11 +24591,11 @@
         <v>261</v>
       </c>
       <c r="F152" t="str">
-        <f t="shared" si="17"/>
-        <v>~SPWI616~, ~Arcane~, ~6~, ~Disintigrate~ =&gt; ~SPWI616~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI616~, ~Arcane~, ~6~ =&gt; ~SPWI616~    //Disintigrate</v>
       </c>
       <c r="G152" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7T~, ~SPWI616~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7T~</v>
       </c>
     </row>
@@ -24540,11 +24616,11 @@
         <v>607</v>
       </c>
       <c r="F153" t="str">
-        <f t="shared" si="17"/>
-        <v>~SPWI617~, ~Arcane~, ~6~, ~Contingency~ =&gt; ~SPWI617~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI617~, ~Arcane~, ~6~ =&gt; ~SPWI617~    //Contingency</v>
       </c>
       <c r="G153" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7U~, ~SPWI617~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7U~</v>
       </c>
     </row>
@@ -24565,11 +24641,11 @@
         <v>608</v>
       </c>
       <c r="F154" t="str">
-        <f t="shared" si="17"/>
-        <v>~SPWI618~, ~Arcane~, ~6~, ~Spell Deflection~ =&gt; ~SPWI618~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI618~, ~Arcane~, ~6~ =&gt; ~SPWI618~    //Spell Deflection</v>
       </c>
       <c r="G154" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7V~, ~SPWI618~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7V~</v>
       </c>
     </row>
@@ -24590,11 +24666,11 @@
         <v>609</v>
       </c>
       <c r="F155" t="str">
-        <f t="shared" si="17"/>
-        <v>~SPWI619~, ~Arcane~, ~6~, ~Wyvern Call~ =&gt; ~SPWI619~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI619~, ~Arcane~, ~6~ =&gt; ~SPWI619~    //Wyvern Call</v>
       </c>
       <c r="G155" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7W~, ~SPWI619~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7W~</v>
       </c>
     </row>
@@ -24615,11 +24691,11 @@
         <v>237</v>
       </c>
       <c r="F156" t="str">
-        <f t="shared" si="17"/>
-        <v>~SPWI620~, ~Arcane~, ~6~, ~Conjure Fire Elemental~ =&gt; ~SPWI620~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI620~, ~Arcane~, ~6~ =&gt; ~SPWI620~    //Conjure Fire Elemental</v>
       </c>
       <c r="G156" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7X~, ~SPWI620~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7X~</v>
       </c>
     </row>
@@ -24640,11 +24716,11 @@
         <v>610</v>
       </c>
       <c r="F157" t="str">
-        <f t="shared" si="17"/>
-        <v>~SPWI621~, ~Arcane~, ~6~, ~Conjure Air Elemental~ =&gt; ~SPWI621~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI621~, ~Arcane~, ~6~ =&gt; ~SPWI621~    //Conjure Air Elemental</v>
       </c>
       <c r="G157" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7Y~, ~SPWI621~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7Y~</v>
       </c>
     </row>
@@ -24665,11 +24741,11 @@
         <v>238</v>
       </c>
       <c r="F158" t="str">
-        <f t="shared" si="17"/>
-        <v>~SPWI622~, ~Arcane~, ~6~, ~Conjure Earth Elemental~ =&gt; ~SPWI622~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI622~, ~Arcane~, ~6~ =&gt; ~SPWI622~    //Conjure Earth Elemental</v>
       </c>
       <c r="G158" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL7Z~, ~SPWI622~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL7Z~</v>
       </c>
     </row>
@@ -24690,11 +24766,11 @@
         <v>616</v>
       </c>
       <c r="F159" t="str">
-        <f t="shared" si="17"/>
-        <v>~SPWI623~, ~Arcane~, ~6~, ~Carrion Summons~ =&gt; ~SPWI623~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI623~, ~Arcane~, ~6~ =&gt; ~SPWI623~    //Carrion Summons</v>
       </c>
       <c r="G159" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL8A~, ~SPWI623~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8A~</v>
       </c>
     </row>
@@ -24715,11 +24791,11 @@
         <v>617</v>
       </c>
       <c r="F160" t="str">
-        <f t="shared" si="17"/>
-        <v>~SPWI624~, ~Arcane~, ~6~, ~Summon Nishruu~ =&gt; ~SPWI624~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI624~, ~Arcane~, ~6~ =&gt; ~SPWI624~    //Summon Nishruu</v>
       </c>
       <c r="G160" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL8B~, ~SPWI624~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8B~</v>
       </c>
     </row>
@@ -24740,59 +24816,91 @@
         <v>314</v>
       </c>
       <c r="F161" t="str">
-        <f t="shared" si="17"/>
-        <v>~SPWI625~, ~Arcane~, ~6~, ~Stone to Flesh~ =&gt; ~SPWI625~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI625~, ~Arcane~, ~6~ =&gt; ~SPWI625~    //Stone to Flesh</v>
       </c>
       <c r="G161" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL8C~, ~SPWI625~, ~Arcane~, ~6~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8C~</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F162" t="str">
+        <f t="shared" si="8"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G162" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F163" t="str">
+        <f t="shared" si="8"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G163" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F164" t="str">
+        <f t="shared" si="8"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G164" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F165" t="str">
+        <f t="shared" si="8"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G165" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F166" t="str">
+        <f t="shared" si="8"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G166" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F167" t="str">
+        <f t="shared" si="8"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G167" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F168" t="str">
+        <f t="shared" si="8"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G168" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F169" t="str">
+        <f t="shared" si="8"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G169" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
@@ -24813,11 +24921,11 @@
         <v>630</v>
       </c>
       <c r="F170" t="str">
-        <f t="shared" ref="F170:F174" si="18">_xlfn.CONCAT("~", C170, "~, ~", A170, "~, ~", B170, "~, ~", E170, "~ =&gt; ~", C170, "~")</f>
-        <v>~SPWI701~, ~Arcane~, ~7~, ~Spell Turning~ =&gt; ~SPWI701~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI701~, ~Arcane~, ~7~ =&gt; ~SPWI701~    //Spell Turning</v>
       </c>
       <c r="G170" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL8D~, ~SPWI701~, ~Arcane~, ~7~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8D~</v>
       </c>
     </row>
@@ -24838,11 +24946,11 @@
         <v>832</v>
       </c>
       <c r="F171" t="str">
-        <f t="shared" si="18"/>
-        <v>~SPWI702~, ~Arcane~, ~7~, ~Protection From The Elements~ =&gt; ~SPWI702~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI702~, ~Arcane~, ~7~ =&gt; ~SPWI702~    //Protection From The Elements</v>
       </c>
       <c r="G171" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL8E~, ~SPWI702~, ~Arcane~, ~7~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8E~</v>
       </c>
     </row>
@@ -24863,11 +24971,11 @@
         <v>632</v>
       </c>
       <c r="F172" t="str">
-        <f t="shared" si="18"/>
-        <v>~SPWI703~, ~Arcane~, ~7~, ~Project Image~ =&gt; ~SPWI703~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI703~, ~Arcane~, ~7~ =&gt; ~SPWI703~    //Project Image</v>
       </c>
       <c r="G172" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL8F~, ~SPWI703~, ~Arcane~, ~7~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8F~</v>
       </c>
     </row>
@@ -24888,11 +24996,11 @@
         <v>633</v>
       </c>
       <c r="F173" t="str">
-        <f t="shared" si="18"/>
-        <v>~SPWI704~, ~Arcane~, ~7~, ~Ruby Ray of Reversal~ =&gt; ~SPWI704~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI704~, ~Arcane~, ~7~ =&gt; ~SPWI704~    //Ruby Ray of Reversal</v>
       </c>
       <c r="G173" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL8G~, ~SPWI704~, ~Arcane~, ~7~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8G~</v>
       </c>
     </row>
@@ -24913,11 +25021,11 @@
         <v>634</v>
       </c>
       <c r="F174" t="str">
-        <f t="shared" si="18"/>
-        <v>~SPWI705~, ~Arcane~, ~7~, ~Khelben's Warding Whip~ =&gt; ~SPWI705~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI705~, ~Arcane~, ~7~ =&gt; ~SPWI705~    //Khelben's Warding Whip</v>
       </c>
       <c r="G174" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>~SCRL8H~, ~SPWI705~, ~Arcane~, ~7~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8H~</v>
       </c>
     </row>
@@ -24925,8 +25033,12 @@
       <c r="C175" s="3"/>
       <c r="D175" s="3"/>
       <c r="E175" s="3"/>
+      <c r="F175" t="str">
+        <f t="shared" si="8"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G175" t="str">
-        <f t="shared" ref="G175:G238" si="19">_xlfn.CONCAT("~", D175, "~, ~", C175, "~, ~", A175, "~, ~", B175, "~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~", " =&gt; ~", D175, "~")</f>
+        <f t="shared" ref="G175:G238" si="9">_xlfn.CONCAT("~", D175, "~, ~", C175, "~, ~", A175, "~, ~", B175, "~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~", " =&gt; ~", D175, "~")</f>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
@@ -24947,11 +25059,11 @@
         <v>635</v>
       </c>
       <c r="F176" t="str">
-        <f t="shared" ref="F176:F177" si="20">_xlfn.CONCAT("~", C176, "~, ~", A176, "~, ~", B176, "~, ~", E176, "~ =&gt; ~", C176, "~")</f>
-        <v>~SPWI707~, ~Arcane~, ~7~, ~Cacofiend~ =&gt; ~SPWI707~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI707~, ~Arcane~, ~7~ =&gt; ~SPWI707~    //Cacofiend</v>
       </c>
       <c r="G176" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL8I~, ~SPWI707~, ~Arcane~, ~7~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8I~</v>
       </c>
     </row>
@@ -24972,11 +25084,11 @@
         <v>636</v>
       </c>
       <c r="F177" t="str">
-        <f t="shared" si="20"/>
-        <v>~SPWI708~, ~Arcane~, ~7~, ~Mantle~ =&gt; ~SPWI708~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI708~, ~Arcane~, ~7~ =&gt; ~SPWI708~    //Mantle</v>
       </c>
       <c r="G177" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL8J~, ~SPWI708~, ~Arcane~, ~7~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8J~</v>
       </c>
     </row>
@@ -24984,8 +25096,12 @@
       <c r="C178" s="3"/>
       <c r="D178" s="3"/>
       <c r="E178" s="3"/>
+      <c r="F178" t="str">
+        <f t="shared" si="8"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G178" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
@@ -25006,11 +25122,11 @@
         <v>637</v>
       </c>
       <c r="F179" t="str">
-        <f t="shared" ref="F179:F192" si="21">_xlfn.CONCAT("~", C179, "~, ~", A179, "~, ~", B179, "~, ~", E179, "~ =&gt; ~", C179, "~")</f>
-        <v>~SPWI710~, ~Arcane~, ~7~, ~Spell Sequencer~ =&gt; ~SPWI710~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI710~, ~Arcane~, ~7~ =&gt; ~SPWI710~    //Spell Sequencer</v>
       </c>
       <c r="G179" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL8L~, ~SPWI710~, ~Arcane~, ~7~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8L~</v>
       </c>
     </row>
@@ -25031,11 +25147,11 @@
         <v>638</v>
       </c>
       <c r="F180" t="str">
-        <f t="shared" si="21"/>
-        <v>~SPWI711~, ~Arcane~, ~7~, ~Sphere of Chaos~ =&gt; ~SPWI711~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI711~, ~Arcane~, ~7~ =&gt; ~SPWI711~    //Sphere of Chaos</v>
       </c>
       <c r="G180" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL8M~, ~SPWI711~, ~Arcane~, ~7~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8M~</v>
       </c>
     </row>
@@ -25056,11 +25172,11 @@
         <v>639</v>
       </c>
       <c r="F181" t="str">
-        <f t="shared" si="21"/>
-        <v>~SPWI712~, ~Arcane~, ~7~, ~Delayed Blast Fireball~ =&gt; ~SPWI712~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI712~, ~Arcane~, ~7~ =&gt; ~SPWI712~    //Delayed Blast Fireball</v>
       </c>
       <c r="G181" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL8N~, ~SPWI712~, ~Arcane~, ~7~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8N~</v>
       </c>
     </row>
@@ -25081,11 +25197,11 @@
         <v>281</v>
       </c>
       <c r="F182" t="str">
-        <f t="shared" si="21"/>
-        <v>~SPWI713~, ~Arcane~, ~7~, ~Finger of Death~ =&gt; ~SPWI713~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI713~, ~Arcane~, ~7~ =&gt; ~SPWI713~    //Finger of Death</v>
       </c>
       <c r="G182" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL8O~, ~SPWI713~, ~Arcane~, ~7~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8O~</v>
       </c>
     </row>
@@ -25106,11 +25222,11 @@
         <v>285</v>
       </c>
       <c r="F183" t="str">
-        <f t="shared" si="21"/>
-        <v>~SPWI714~, ~Arcane~, ~7~, ~Prismatic Spray~ =&gt; ~SPWI714~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI714~, ~Arcane~, ~7~ =&gt; ~SPWI714~    //Prismatic Spray</v>
       </c>
       <c r="G183" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL8P~, ~SPWI714~, ~Arcane~, ~7~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8P~</v>
       </c>
     </row>
@@ -25131,11 +25247,11 @@
         <v>284</v>
       </c>
       <c r="F184" t="str">
-        <f t="shared" si="21"/>
-        <v>~SPWI715~, ~Arcane~, ~7~, ~Power Word, Stun~ =&gt; ~SPWI715~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI715~, ~Arcane~, ~7~ =&gt; ~SPWI715~    //Power Word, Stun</v>
       </c>
       <c r="G184" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL8Q~, ~SPWI715~, ~Arcane~, ~7~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8Q~</v>
       </c>
     </row>
@@ -25156,11 +25272,11 @@
         <v>283</v>
       </c>
       <c r="F185" t="str">
-        <f t="shared" si="21"/>
-        <v>~SPWI716~, ~Arcane~, ~7~, ~Mordenkainen's Sword~ =&gt; ~SPWI716~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI716~, ~Arcane~, ~7~ =&gt; ~SPWI716~    //Mordenkainen's Sword</v>
       </c>
       <c r="G185" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL8R~, ~SPWI716~, ~Arcane~, ~7~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8R~</v>
       </c>
     </row>
@@ -25181,11 +25297,11 @@
         <v>640</v>
       </c>
       <c r="F186" t="str">
-        <f t="shared" si="21"/>
-        <v>~SPWI717~, ~Arcane~, ~7~, ~Summon Efreeti~ =&gt; ~SPWI717~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI717~, ~Arcane~, ~7~ =&gt; ~SPWI717~    //Summon Efreeti</v>
       </c>
       <c r="G186" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL8S~, ~SPWI717~, ~Arcane~, ~7~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8S~</v>
       </c>
     </row>
@@ -25206,11 +25322,11 @@
         <v>641</v>
       </c>
       <c r="F187" t="str">
-        <f t="shared" si="21"/>
-        <v>~SPWI718~, ~Arcane~, ~7~, ~Summon Djinni~ =&gt; ~SPWI718~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI718~, ~Arcane~, ~7~ =&gt; ~SPWI718~    //Summon Djinni</v>
       </c>
       <c r="G187" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL8T~, ~SPWI718~, ~Arcane~, ~7~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8T~</v>
       </c>
     </row>
@@ -25231,11 +25347,11 @@
         <v>642</v>
       </c>
       <c r="F188" t="str">
-        <f t="shared" si="21"/>
-        <v>~SPWI719~, ~Arcane~, ~7~, ~Summon Hakeashar~ =&gt; ~SPWI719~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI719~, ~Arcane~, ~7~ =&gt; ~SPWI719~    //Summon Hakeashar</v>
       </c>
       <c r="G188" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL8U~, ~SPWI719~, ~Arcane~, ~7~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8U~</v>
       </c>
     </row>
@@ -25256,11 +25372,11 @@
         <v>643</v>
       </c>
       <c r="F189" t="str">
-        <f t="shared" si="21"/>
-        <v>~SPWI720~, ~Arcane~, ~7~, ~Control Undead~ =&gt; ~SPWI720~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI720~, ~Arcane~, ~7~ =&gt; ~SPWI720~    //Control Undead</v>
       </c>
       <c r="G189" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL8V~, ~SPWI720~, ~Arcane~, ~7~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8V~</v>
       </c>
     </row>
@@ -25281,11 +25397,11 @@
         <v>288</v>
       </c>
       <c r="F190" t="str">
-        <f t="shared" si="21"/>
-        <v>~SPWI721~, ~Arcane~, ~7~, ~Mass Invisibility~ =&gt; ~SPWI721~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI721~, ~Arcane~, ~7~ =&gt; ~SPWI721~    //Mass Invisibility</v>
       </c>
       <c r="G190" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL8W~, ~SPWI721~, ~Arcane~, ~7~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8W~</v>
       </c>
     </row>
@@ -25306,11 +25422,11 @@
         <v>644</v>
       </c>
       <c r="F191" t="str">
-        <f t="shared" si="21"/>
-        <v>~SPWI722~, ~Arcane~, ~7~, ~Limited Wish~ =&gt; ~SPWI722~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI722~, ~Arcane~, ~7~ =&gt; ~SPWI722~    //Limited Wish</v>
       </c>
       <c r="G191" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRLA4~, ~SPWI722~, ~Arcane~, ~7~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRLA4~</v>
       </c>
     </row>
@@ -25328,35 +25444,51 @@
         <v>645</v>
       </c>
       <c r="F192" t="str">
-        <f t="shared" si="21"/>
-        <v>~SPWI723~, ~Arcane~, ~7~, ~Improved Chaos Shield*~ =&gt; ~SPWI723~</v>
+        <f t="shared" si="8"/>
+        <v>~SPWI723~, ~Arcane~, ~7~ =&gt; ~SPWI723~    //Improved Chaos Shield*</v>
       </c>
       <c r="G192" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~~, ~SPWI723~, ~Arcane~, ~7~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F193" t="str">
+        <f t="shared" si="8"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G193" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F194" t="str">
+        <f t="shared" si="8"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G194" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F195" t="str">
+        <f t="shared" si="8"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G195" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F196" t="str">
+        <f t="shared" ref="F196:F241" si="10">_xlfn.CONCAT("~", C196, "~, ~", A196, "~, ~", B196, "~ =&gt; ~", C196, "~    //", E196)</f>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G196" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
@@ -25364,8 +25496,12 @@
       <c r="C197" s="3"/>
       <c r="D197" s="3"/>
       <c r="E197" s="3"/>
+      <c r="F197" t="str">
+        <f t="shared" si="10"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G197" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
@@ -25384,11 +25520,11 @@
         <v>608</v>
       </c>
       <c r="F198" t="str">
-        <f t="shared" ref="F198:F202" si="22">_xlfn.CONCAT("~", C198, "~, ~", A198, "~, ~", B198, "~, ~", E198, "~ =&gt; ~", C198, "~")</f>
-        <v>~SPWI802~, ~Arcane~, ~8~, ~Spell Deflection~ =&gt; ~SPWI802~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI802~, ~Arcane~, ~8~ =&gt; ~SPWI802~    //Spell Deflection</v>
       </c>
       <c r="G198" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~~, ~SPWI802~, ~Arcane~, ~8~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
@@ -25409,11 +25545,11 @@
         <v>656</v>
       </c>
       <c r="F199" t="str">
-        <f t="shared" si="22"/>
-        <v>~SPWI803~, ~Arcane~, ~8~, ~Protection from Energy~ =&gt; ~SPWI803~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI803~, ~Arcane~, ~8~ =&gt; ~SPWI803~    //Protection from Energy</v>
       </c>
       <c r="G199" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL8Y~, ~SPWI803~, ~Arcane~, ~8~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8Y~</v>
       </c>
     </row>
@@ -25434,11 +25570,11 @@
         <v>657</v>
       </c>
       <c r="F200" t="str">
-        <f t="shared" si="22"/>
-        <v>~SPWI804~, ~Arcane~, ~8~, ~Simulacrum~ =&gt; ~SPWI804~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI804~, ~Arcane~, ~8~ =&gt; ~SPWI804~    //Simulacrum</v>
       </c>
       <c r="G200" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL8Z~, ~SPWI804~, ~Arcane~, ~8~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL8Z~</v>
       </c>
     </row>
@@ -25459,11 +25595,11 @@
         <v>658</v>
       </c>
       <c r="F201" t="str">
-        <f t="shared" si="22"/>
-        <v>~SPWI805~, ~Arcane~, ~8~, ~Pierce Shield~ =&gt; ~SPWI805~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI805~, ~Arcane~, ~8~ =&gt; ~SPWI805~    //Pierce Shield</v>
       </c>
       <c r="G201" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9A~, ~SPWI805~, ~Arcane~, ~8~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9A~</v>
       </c>
     </row>
@@ -25484,11 +25620,11 @@
         <v>659</v>
       </c>
       <c r="F202" t="str">
-        <f t="shared" si="22"/>
-        <v>~SPWI806~, ~Arcane~, ~8~, ~Summon Fiend~ =&gt; ~SPWI806~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI806~, ~Arcane~, ~8~ =&gt; ~SPWI806~    //Summon Fiend</v>
       </c>
       <c r="G202" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9B~, ~SPWI806~, ~Arcane~, ~8~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9B~</v>
       </c>
     </row>
@@ -25496,8 +25632,12 @@
       <c r="C203" s="3"/>
       <c r="D203" s="3"/>
       <c r="E203" s="3"/>
+      <c r="F203" t="str">
+        <f t="shared" si="10"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G203" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
@@ -25518,11 +25658,11 @@
         <v>660</v>
       </c>
       <c r="F204" t="str">
-        <f t="shared" ref="F204:F209" si="23">_xlfn.CONCAT("~", C204, "~, ~", A204, "~, ~", B204, "~, ~", E204, "~ =&gt; ~", C204, "~")</f>
-        <v>~SPWI808~, ~Arcane~, ~8~, ~Improved Mantle~ =&gt; ~SPWI808~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI808~, ~Arcane~, ~8~ =&gt; ~SPWI808~    //Improved Mantle</v>
       </c>
       <c r="G204" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9C~, ~SPWI808~, ~Arcane~, ~8~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9C~</v>
       </c>
     </row>
@@ -25543,11 +25683,11 @@
         <v>661</v>
       </c>
       <c r="F205" t="str">
-        <f t="shared" si="23"/>
-        <v>~SPWI809~, ~Arcane~, ~8~, ~Spell Trigger~ =&gt; ~SPWI809~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI809~, ~Arcane~, ~8~ =&gt; ~SPWI809~    //Spell Trigger</v>
       </c>
       <c r="G205" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9D~, ~SPWI809~, ~Arcane~, ~8~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9D~</v>
       </c>
     </row>
@@ -25568,11 +25708,11 @@
         <v>299</v>
       </c>
       <c r="F206" t="str">
-        <f t="shared" si="23"/>
-        <v>~SPWI810~, ~Arcane~, ~8~, ~Incendiary Cloud~ =&gt; ~SPWI810~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI810~, ~Arcane~, ~8~ =&gt; ~SPWI810~    //Incendiary Cloud</v>
       </c>
       <c r="G206" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9E~, ~SPWI810~, ~Arcane~, ~8~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9E~</v>
       </c>
     </row>
@@ -25593,11 +25733,11 @@
         <v>662</v>
       </c>
       <c r="F207" t="str">
-        <f t="shared" si="23"/>
-        <v>~SPWI811~, ~Arcane~, ~8~, ~Symbol, Fear~ =&gt; ~SPWI811~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI811~, ~Arcane~, ~8~ =&gt; ~SPWI811~    //Symbol, Fear</v>
       </c>
       <c r="G207" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9F~, ~SPWI811~, ~Arcane~, ~8~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9F~</v>
       </c>
     </row>
@@ -25618,11 +25758,11 @@
         <v>302</v>
       </c>
       <c r="F208" t="str">
-        <f t="shared" si="23"/>
-        <v>~SPWI812~, ~Arcane~, ~8~, ~Abi-Dalzim's Horrid Wilting~ =&gt; ~SPWI812~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI812~, ~Arcane~, ~8~ =&gt; ~SPWI812~    //Abi-Dalzim's Horrid Wilting</v>
       </c>
       <c r="G208" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9G~, ~SPWI812~, ~Arcane~, ~8~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9G~</v>
       </c>
     </row>
@@ -25643,11 +25783,11 @@
         <v>663</v>
       </c>
       <c r="F209" t="str">
-        <f t="shared" si="23"/>
-        <v>~SPWI813~, ~Arcane~, ~8~, ~Maze~ =&gt; ~SPWI813~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI813~, ~Arcane~, ~8~ =&gt; ~SPWI813~    //Maze</v>
       </c>
       <c r="G209" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9H~, ~SPWI813~, ~Arcane~, ~8~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9H~</v>
       </c>
     </row>
@@ -25655,8 +25795,12 @@
       <c r="C210" s="3"/>
       <c r="D210" s="3"/>
       <c r="E210" s="3"/>
+      <c r="F210" t="str">
+        <f t="shared" si="10"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G210" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
@@ -25677,11 +25821,11 @@
         <v>664</v>
       </c>
       <c r="F211" t="str">
-        <f t="shared" ref="F211:F214" si="24">_xlfn.CONCAT("~", C211, "~, ~", A211, "~, ~", B211, "~, ~", E211, "~ =&gt; ~", C211, "~")</f>
-        <v>~SPWI815~, ~Arcane~, ~8~, ~Power Word Blind~ =&gt; ~SPWI815~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI815~, ~Arcane~, ~8~ =&gt; ~SPWI815~    //Power Word Blind</v>
       </c>
       <c r="G211" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9J~, ~SPWI815~, ~Arcane~, ~8~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9J~</v>
       </c>
     </row>
@@ -25702,11 +25846,11 @@
         <v>666</v>
       </c>
       <c r="F212" t="str">
-        <f t="shared" si="24"/>
-        <v>~SPWI816~, ~Arcane~, ~8~, ~Symbol, Stun~ =&gt; ~SPWI816~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI816~, ~Arcane~, ~8~ =&gt; ~SPWI816~    //Symbol, Stun</v>
       </c>
       <c r="G212" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRLAN;SCRLAP~, ~SPWI816~, ~Arcane~, ~8~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRLAN;SCRLAP~</v>
       </c>
     </row>
@@ -25727,11 +25871,11 @@
         <v>665</v>
       </c>
       <c r="F213" t="str">
-        <f t="shared" si="24"/>
-        <v>~SPWI817~, ~Arcane~, ~8~, ~Symbol, Death~ =&gt; ~SPWI817~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI817~, ~Arcane~, ~8~ =&gt; ~SPWI817~    //Symbol, Death</v>
       </c>
       <c r="G213" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRLAM;SCRLAO~, ~SPWI817~, ~Arcane~, ~8~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRLAM;SCRLAO~</v>
       </c>
     </row>
@@ -25752,23 +25896,31 @@
         <v>667</v>
       </c>
       <c r="F214" t="str">
-        <f t="shared" si="24"/>
-        <v>~SPWI818~, ~Arcane~, ~8~, ~Bigby's Clenched Fist~ =&gt; ~SPWI818~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI818~, ~Arcane~, ~8~ =&gt; ~SPWI818~    //Bigby's Clenched Fist</v>
       </c>
       <c r="G214" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRLB1~, ~SPWI818~, ~Arcane~, ~8~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRLB1~</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F215" t="str">
+        <f t="shared" si="10"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G215" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F216" t="str">
+        <f t="shared" si="10"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G216" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
@@ -25776,8 +25928,12 @@
       <c r="C217" s="3"/>
       <c r="D217" s="3"/>
       <c r="E217" s="3"/>
+      <c r="F217" t="str">
+        <f t="shared" si="10"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G217" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
@@ -25798,11 +25954,11 @@
         <v>679</v>
       </c>
       <c r="F218" t="str">
-        <f t="shared" ref="F218:F219" si="25">_xlfn.CONCAT("~", C218, "~, ~", A218, "~, ~", B218, "~, ~", E218, "~ =&gt; ~", C218, "~")</f>
-        <v>~SPWI902~, ~Arcane~, ~9~, ~Spell Trap~ =&gt; ~SPWI902~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI902~, ~Arcane~, ~9~ =&gt; ~SPWI902~    //Spell Trap</v>
       </c>
       <c r="G218" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9L~, ~SPWI902~, ~Arcane~, ~9~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9L~</v>
       </c>
     </row>
@@ -25823,11 +25979,11 @@
         <v>680</v>
       </c>
       <c r="F219" t="str">
-        <f t="shared" si="25"/>
-        <v>~SPWI903~, ~Arcane~, ~9~, ~Spellstrike~ =&gt; ~SPWI903~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI903~, ~Arcane~, ~9~ =&gt; ~SPWI903~    //Spellstrike</v>
       </c>
       <c r="G219" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9M~, ~SPWI903~, ~Arcane~, ~9~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9M~</v>
       </c>
     </row>
@@ -25835,8 +25991,12 @@
       <c r="C220" s="3"/>
       <c r="D220" s="3"/>
       <c r="E220" s="3"/>
+      <c r="F220" t="str">
+        <f t="shared" si="10"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G220" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
@@ -25857,11 +26017,11 @@
         <v>681</v>
       </c>
       <c r="F221" t="str">
-        <f>_xlfn.CONCAT("~", C221, "~, ~", A221, "~, ~", B221, "~, ~", E221, "~ =&gt; ~", C221, "~")</f>
-        <v>~SPWI905~, ~Arcane~, ~9~, ~Gate~ =&gt; ~SPWI905~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI905~, ~Arcane~, ~9~ =&gt; ~SPWI905~    //Gate</v>
       </c>
       <c r="G221" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9N~, ~SPWI905~, ~Arcane~, ~9~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9N~</v>
       </c>
     </row>
@@ -25869,8 +26029,12 @@
       <c r="C222" s="3"/>
       <c r="D222" s="3"/>
       <c r="E222" s="3"/>
+      <c r="F222" t="str">
+        <f t="shared" si="10"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
       <c r="G222" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~~, ~~, ~~, ~~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~~</v>
       </c>
     </row>
@@ -25891,11 +26055,11 @@
         <v>682</v>
       </c>
       <c r="F223" t="str">
-        <f t="shared" ref="F223:F241" si="26">_xlfn.CONCAT("~", C223, "~, ~", A223, "~, ~", B223, "~, ~", E223, "~ =&gt; ~", C223, "~")</f>
-        <v>~SPWI907~, ~Arcane~, ~9~, ~Absolute Immunity~ =&gt; ~SPWI907~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI907~, ~Arcane~, ~9~ =&gt; ~SPWI907~    //Absolute Immunity</v>
       </c>
       <c r="G223" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9P~, ~SPWI907~, ~Arcane~, ~9~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9P~</v>
       </c>
     </row>
@@ -25916,11 +26080,11 @@
         <v>683</v>
       </c>
       <c r="F224" t="str">
-        <f t="shared" si="26"/>
-        <v>~SPWI908~, ~Arcane~, ~9~, ~Chain Contingency~ =&gt; ~SPWI908~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI908~, ~Arcane~, ~9~ =&gt; ~SPWI908~    //Chain Contingency</v>
       </c>
       <c r="G224" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9Q~, ~SPWI908~, ~Arcane~, ~9~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9Q~</v>
       </c>
     </row>
@@ -25941,11 +26105,11 @@
         <v>684</v>
       </c>
       <c r="F225" t="str">
-        <f t="shared" si="26"/>
-        <v>~SPWI909~, ~Arcane~, ~9~, ~Time Stop~ =&gt; ~SPWI909~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI909~, ~Arcane~, ~9~ =&gt; ~SPWI909~    //Time Stop</v>
       </c>
       <c r="G225" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9R~, ~SPWI909~, ~Arcane~, ~9~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9R~</v>
       </c>
     </row>
@@ -25966,11 +26130,11 @@
         <v>685</v>
       </c>
       <c r="F226" t="str">
-        <f t="shared" si="26"/>
-        <v>~SPWI910~, ~Arcane~, ~9~, ~Imprisonment~ =&gt; ~SPWI910~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI910~, ~Arcane~, ~9~ =&gt; ~SPWI910~    //Imprisonment</v>
       </c>
       <c r="G226" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9S~, ~SPWI910~, ~Arcane~, ~9~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9S~</v>
       </c>
     </row>
@@ -25991,11 +26155,11 @@
         <v>686</v>
       </c>
       <c r="F227" t="str">
-        <f t="shared" si="26"/>
-        <v>~SPWI911~, ~Arcane~, ~9~, ~Meteor Swarm~ =&gt; ~SPWI911~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI911~, ~Arcane~, ~9~ =&gt; ~SPWI911~    //Meteor Swarm</v>
       </c>
       <c r="G227" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9T~, ~SPWI911~, ~Arcane~, ~9~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9T~</v>
       </c>
     </row>
@@ -26016,11 +26180,11 @@
         <v>311</v>
       </c>
       <c r="F228" t="str">
-        <f t="shared" si="26"/>
-        <v>~SPWI912~, ~Arcane~, ~9~, ~Power Word, Kill~ =&gt; ~SPWI912~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI912~, ~Arcane~, ~9~ =&gt; ~SPWI912~    //Power Word, Kill</v>
       </c>
       <c r="G228" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9U~, ~SPWI912~, ~Arcane~, ~9~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9U~</v>
       </c>
     </row>
@@ -26041,11 +26205,11 @@
         <v>687</v>
       </c>
       <c r="F229" t="str">
-        <f t="shared" si="26"/>
-        <v>~SPWI913~, ~Arcane~, ~9~, ~Wail of the Banshee~ =&gt; ~SPWI913~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI913~, ~Arcane~, ~9~ =&gt; ~SPWI913~    //Wail of the Banshee</v>
       </c>
       <c r="G229" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9V~, ~SPWI913~, ~Arcane~, ~9~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9V~</v>
       </c>
     </row>
@@ -26066,11 +26230,11 @@
         <v>688</v>
       </c>
       <c r="F230" t="str">
-        <f t="shared" si="26"/>
-        <v>~SPWI914~, ~Arcane~, ~9~, ~Energy Drain~ =&gt; ~SPWI914~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI914~, ~Arcane~, ~9~ =&gt; ~SPWI914~    //Energy Drain</v>
       </c>
       <c r="G230" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9W~, ~SPWI914~, ~Arcane~, ~9~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9W~</v>
       </c>
     </row>
@@ -26091,11 +26255,11 @@
         <v>689</v>
       </c>
       <c r="F231" t="str">
-        <f t="shared" si="26"/>
-        <v>~SPWI915~, ~Arcane~, ~9~, ~Black Blade of Disaster~ =&gt; ~SPWI915~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI915~, ~Arcane~, ~9~ =&gt; ~SPWI915~    //Black Blade of Disaster</v>
       </c>
       <c r="G231" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9X~, ~SPWI915~, ~Arcane~, ~9~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9X~</v>
       </c>
     </row>
@@ -26116,11 +26280,11 @@
         <v>690</v>
       </c>
       <c r="F232" t="str">
-        <f t="shared" si="26"/>
-        <v>~SPWI916~, ~Arcane~, ~9~, ~Shapechange~ =&gt; ~SPWI916~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI916~, ~Arcane~, ~9~ =&gt; ~SPWI916~    //Shapechange</v>
       </c>
       <c r="G232" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9Y~, ~SPWI916~, ~Arcane~, ~9~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9Y~</v>
       </c>
     </row>
@@ -26141,11 +26305,11 @@
         <v>691</v>
       </c>
       <c r="F233" t="str">
-        <f t="shared" si="26"/>
-        <v>~SPWI917~, ~Arcane~, ~9~, ~Freedom~ =&gt; ~SPWI917~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI917~, ~Arcane~, ~9~ =&gt; ~SPWI917~    //Freedom</v>
       </c>
       <c r="G233" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRL9Z~, ~SPWI917~, ~Arcane~, ~9~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRL9Z~</v>
       </c>
     </row>
@@ -26166,11 +26330,11 @@
         <v>692</v>
       </c>
       <c r="F234" t="str">
-        <f t="shared" si="26"/>
-        <v>~SPWI918~, ~Arcane~, ~9~, ~Bigby's Crushing Hand~ =&gt; ~SPWI918~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI918~, ~Arcane~, ~9~ =&gt; ~SPWI918~    //Bigby's Crushing Hand</v>
       </c>
       <c r="G234" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRLB2~, ~SPWI918~, ~Arcane~, ~9~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRLB2~</v>
       </c>
     </row>
@@ -26191,11 +26355,11 @@
         <v>693</v>
       </c>
       <c r="F235" t="str">
-        <f t="shared" si="26"/>
-        <v>~SPWI919~, ~Arcane~, ~9~, ~Wish~ =&gt; ~SPWI919~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI919~, ~Arcane~, ~9~ =&gt; ~SPWI919~    //Wish</v>
       </c>
       <c r="G235" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~SCRLB4~, ~SPWI919~, ~Arcane~, ~9~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~SCRLB4~</v>
       </c>
     </row>
@@ -26216,11 +26380,11 @@
         <v>694</v>
       </c>
       <c r="F236" t="str">
-        <f t="shared" si="26"/>
-        <v>~SPWI920~, ~Arcane~, ~10~, ~Energy Blades~ =&gt; ~SPWI920~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI920~, ~Arcane~, ~10~ =&gt; ~SPWI920~    //Energy Blades</v>
       </c>
       <c r="G236" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~--HLA--~, ~SPWI920~, ~Arcane~, ~10~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~--HLA--~</v>
       </c>
     </row>
@@ -26241,11 +26405,11 @@
         <v>695</v>
       </c>
       <c r="F237" t="str">
-        <f t="shared" si="26"/>
-        <v>~SPWI921~, ~Arcane~, ~10~, ~Improved Alacrity~ =&gt; ~SPWI921~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI921~, ~Arcane~, ~10~ =&gt; ~SPWI921~    //Improved Alacrity</v>
       </c>
       <c r="G237" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~--HLA--~, ~SPWI921~, ~Arcane~, ~10~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~--HLA--~</v>
       </c>
     </row>
@@ -26266,11 +26430,11 @@
         <v>696</v>
       </c>
       <c r="F238" t="str">
-        <f t="shared" si="26"/>
-        <v>~SPWI922~, ~Arcane~, ~10~, ~Dragon's Breath~ =&gt; ~SPWI922~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI922~, ~Arcane~, ~10~ =&gt; ~SPWI922~    //Dragon's Breath</v>
       </c>
       <c r="G238" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="9"/>
         <v>~--HLA--~, ~SPWI922~, ~Arcane~, ~10~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~--HLA--~</v>
       </c>
     </row>
@@ -26291,11 +26455,11 @@
         <v>697</v>
       </c>
       <c r="F239" t="str">
-        <f t="shared" si="26"/>
-        <v>~SPWI923~, ~Arcane~, ~10~, ~Summon Planetar~ =&gt; ~SPWI923~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI923~, ~Arcane~, ~10~ =&gt; ~SPWI923~    //Summon Planetar</v>
       </c>
       <c r="G239" t="str">
-        <f t="shared" ref="G239:G241" si="27">_xlfn.CONCAT("~", D239, "~, ~", C239, "~, ~", A239, "~, ~", B239, "~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~", " =&gt; ~", D239, "~")</f>
+        <f t="shared" ref="G239:G241" si="11">_xlfn.CONCAT("~", D239, "~, ~", C239, "~, ~", A239, "~, ~", B239, "~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~", " =&gt; ~", D239, "~")</f>
         <v>~--HLA--~, ~SPWI923~, ~Arcane~, ~10~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~--HLA--~</v>
       </c>
     </row>
@@ -26316,11 +26480,11 @@
         <v>698</v>
       </c>
       <c r="F240" t="str">
-        <f t="shared" si="26"/>
-        <v>~SPWI924~, ~Arcane~, ~10~, ~Summon Dark Planetar~ =&gt; ~SPWI924~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI924~, ~Arcane~, ~10~ =&gt; ~SPWI924~    //Summon Dark Planetar</v>
       </c>
       <c r="G240" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="11"/>
         <v>~--HLA--~, ~SPWI924~, ~Arcane~, ~10~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~--HLA--~</v>
       </c>
     </row>
@@ -26341,11 +26505,11 @@
         <v>699</v>
       </c>
       <c r="F241" t="str">
-        <f t="shared" si="26"/>
-        <v>~SPWI925~, ~Arcane~, ~10~, ~Comet~ =&gt; ~SPWI925~</v>
+        <f t="shared" si="10"/>
+        <v>~SPWI925~, ~Arcane~, ~10~ =&gt; ~SPWI925~    //Comet</v>
       </c>
       <c r="G241" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="11"/>
         <v>~--HLA--~, ~SPWI925~, ~Arcane~, ~10~, ~1~, ~100~, ~0~, ~0~, ~15~, ~0~, ~1~ =&gt; ~--HLA--~</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixes for level 10 spells missing from BG1EE core
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793451D7-3915-46B1-B278-B84618F8F904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9859862-B0B7-4B39-8A1C-6F78C71E7DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="1" activeTab="2" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="1" activeTab="1" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
   <sheets>
     <sheet name="Bullshit scroll price tinkering" sheetId="1" r:id="rId1"/>
@@ -2820,7 +2820,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2871,8 +2871,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2894,6 +2901,11 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2904,13 +2916,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2924,8 +2937,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="4" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Accent2" xfId="4" builtinId="33"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
@@ -4018,11 +4035,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A58FEB-71E1-4ACD-8B85-E92BCBF62977}">
   <dimension ref="A1:AL262"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C149" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="R248" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AH146" sqref="AH146"/>
+      <selection pane="bottomRight" activeCell="V263" sqref="V263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20867,13 +20884,13 @@
       <c r="R258" t="s">
         <v>695</v>
       </c>
-      <c r="T258" t="s">
+      <c r="T258" s="3" t="s">
         <v>674</v>
       </c>
-      <c r="U258" s="2" t="s">
+      <c r="U258" s="9" t="s">
         <v>818</v>
       </c>
-      <c r="V258" t="s">
+      <c r="V258" s="3" t="s">
         <v>695</v>
       </c>
       <c r="X258" t="s">
@@ -20955,13 +20972,13 @@
       <c r="R260" t="s">
         <v>697</v>
       </c>
-      <c r="T260" t="s">
+      <c r="T260" s="3" t="s">
         <v>676</v>
       </c>
-      <c r="U260" s="2" t="s">
+      <c r="U260" s="9" t="s">
         <v>818</v>
       </c>
-      <c r="V260" t="s">
+      <c r="V260" s="3" t="s">
         <v>697</v>
       </c>
       <c r="X260" t="s">
@@ -20999,13 +21016,13 @@
       <c r="R261" t="s">
         <v>698</v>
       </c>
-      <c r="T261" t="s">
+      <c r="T261" s="10" t="s">
         <v>677</v>
       </c>
-      <c r="U261" s="2" t="s">
+      <c r="U261" s="11" t="s">
         <v>818</v>
       </c>
-      <c r="V261" t="s">
+      <c r="V261" s="10" t="s">
         <v>698</v>
       </c>
       <c r="X261" t="s">
@@ -21093,7 +21110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAFBE98-3888-4E00-A1FB-56928E91D590}">
   <dimension ref="A1:H241"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
+    <sheetView zoomScale="82" workbookViewId="0">
       <selection activeCell="G3" sqref="G3:G241"/>
     </sheetView>
   </sheetViews>
@@ -21193,7 +21210,7 @@
         <v>~SCRL67~, ~SPWI102~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~SCRL67~    //Armor</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" ref="H3:H21" si="2">_xlfn.CONCAT("~", D4, "~, ~", C4, "~, ~", A4, "~, ~", B4, "~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~", , E4, "~ =&gt; ~", D4, "~")</f>
+        <f t="shared" ref="H4:H21" si="2">_xlfn.CONCAT("~", D4, "~, ~", C4, "~, ~", A4, "~, ~", B4, "~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~", , E4, "~ =&gt; ~", D4, "~")</f>
         <v>~SCRL67~, ~SPWI102~, ~Arcane~, ~1~, ~1~, ~100~, ~0~, ~6~, ~0~, ~15~, ~0~, ~1~, ~Armor~ =&gt; ~SCRL67~</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More tweaking to research file
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C371AA-4D0E-4DD9-B0C4-4E2C815F7393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C20364-07A4-404B-9848-507AD24A6A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="1" activeTab="3" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -26593,8 +26593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA6EE01-45F2-4B9F-A391-530E73E3233F}">
   <dimension ref="A1:G247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" zoomScale="82" workbookViewId="0">
-      <selection activeCell="A229" sqref="A229:XFD229"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="82" workbookViewId="0">
+      <selection activeCell="G151" sqref="G151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -29616,7 +29616,7 @@
         <v>585</v>
       </c>
       <c r="F126" t="str">
-        <f t="shared" ref="F126:F181" si="4">_xlfn.CONCAT("~", C126, "~, ~", A126, "~, ~", B126, "~ =&gt; ~", C126, "~    //", E126)</f>
+        <f t="shared" ref="F126:G181" si="4">_xlfn.CONCAT("~", C126, "~, ~", A126, "~, ~", B126, "~ =&gt; ~", C126, "~    //", E126)</f>
         <v>~SPWI510~, ~Arcane~, ~5~ =&gt; ~SPWI510~    //Spell Immunity</v>
       </c>
       <c r="G126" t="str">
@@ -30225,13 +30225,13 @@
       <c r="E151" t="s">
         <v>192</v>
       </c>
-      <c r="F151" t="e">
-        <f>_xlfn.CONCAT("~", C151, "~, ~",#REF!, "~, ~",#REF!, "~ =&gt; ~", C151, "~    //", E151)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G151" t="e">
-        <f>_xlfn.CONCAT("~", D151, "~, ~", C151, "~, ~",#REF!, "~, ~",#REF!, "~, ~1~, ~0~ =&gt; ~", D151, "~    //", E151)</f>
-        <v>#REF!</v>
+      <c r="F151" t="str">
+        <f t="shared" si="4"/>
+        <v>~SPWI605~, ~Arcane~, ~6~ =&gt; ~SPWI605~    //Death Spell</v>
+      </c>
+      <c r="G151" t="str">
+        <f t="shared" si="4"/>
+        <v>~SCDSPEL~, ~6~, ~SPWI605~ =&gt; ~SCDSPEL~    //~SPWI605~, ~Arcane~, ~6~ =&gt; ~SPWI605~    //Death Spell</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updating scrolls in IWD
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C20364-07A4-404B-9848-507AD24A6A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA7AF88-A1D9-4F9F-AA42-04B8C2000829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="1" activeTab="3" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="1" activeTab="1" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
   <sheets>
     <sheet name="Bullshit scroll price tinkering" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6650" uniqueCount="937">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6650" uniqueCount="938">
   <si>
     <t>Caster Level</t>
   </si>
@@ -2839,6 +2839,9 @@
   </si>
   <si>
     <t>SCRLAM</t>
+  </si>
+  <si>
+    <t>SCMSIV</t>
   </si>
 </sst>
 </file>
@@ -4060,11 +4063,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A58FEB-71E1-4ACD-8B85-E92BCBF62977}">
   <dimension ref="A1:AL262"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AC220" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="AC170" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AG235" sqref="AG235"/>
+      <selection pane="bottomRight" activeCell="AG185" sqref="AG185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11514,7 +11517,7 @@
         <v>130</v>
       </c>
       <c r="AG93" t="s">
-        <v>701</v>
+        <v>387</v>
       </c>
       <c r="AH93" t="s">
         <v>144</v>
@@ -16992,7 +16995,7 @@
         <v>860</v>
       </c>
       <c r="AG184" t="s">
-        <v>438</v>
+        <v>937</v>
       </c>
       <c r="AH184" t="s">
         <v>263</v>
@@ -26593,8 +26596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA6EE01-45F2-4B9F-A391-530E73E3233F}">
   <dimension ref="A1:G247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="82" workbookViewId="0">
-      <selection activeCell="G151" sqref="G151"/>
+    <sheetView topLeftCell="A80" zoomScale="82" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -28650,7 +28653,7 @@
         <v>130</v>
       </c>
       <c r="D87" t="s">
-        <v>701</v>
+        <v>387</v>
       </c>
       <c r="E87" t="s">
         <v>144</v>
@@ -28661,7 +28664,7 @@
       </c>
       <c r="G87" t="str">
         <f t="shared" si="3"/>
-        <v>~SCRL1X~, ~SPWI404~, ~Arcane~, ~4~, ~1~, ~0~ =&gt; ~SCRL1X~    //Ice Storm</v>
+        <v>~SCSTOR~, ~SPWI404~, ~Arcane~, ~4~, ~1~, ~0~ =&gt; ~SCSTOR~    //Ice Storm</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
@@ -30230,8 +30233,8 @@
         <v>~SPWI605~, ~Arcane~, ~6~ =&gt; ~SPWI605~    //Death Spell</v>
       </c>
       <c r="G151" t="str">
-        <f t="shared" si="4"/>
-        <v>~SCDSPEL~, ~6~, ~SPWI605~ =&gt; ~SCDSPEL~    //~SPWI605~, ~Arcane~, ~6~ =&gt; ~SPWI605~    //Death Spell</v>
+        <f t="shared" si="5"/>
+        <v>~SCDSPEL~, ~SPWI605~, ~Arcane~, ~6~, ~1~, ~0~ =&gt; ~SCDSPEL~    //Death Spell</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.35">
@@ -30695,7 +30698,7 @@
         <v>860</v>
       </c>
       <c r="D170" t="s">
-        <v>438</v>
+        <v>937</v>
       </c>
       <c r="E170" t="s">
         <v>263</v>
@@ -30706,7 +30709,7 @@
       </c>
       <c r="G170" t="str">
         <f t="shared" si="5"/>
-        <v>~SCMONIV~, ~SPWI627~, ~Arcane~, ~6~, ~1~, ~0~ =&gt; ~SCMONIV~    //Monster Summoning 4</v>
+        <v>~SCMSIV~, ~SPWI627~, ~Arcane~, ~6~, ~1~, ~0~ =&gt; ~SCMSIV~    //Monster Summoning 4</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Adding in spell list for PST:EE
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA7AF88-A1D9-4F9F-AA42-04B8C2000829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BDDAEF-A2B1-4BDA-BFDB-85AD31A9961E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="1" activeTab="1" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="1" activeTab="4" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
   <sheets>
     <sheet name="Bullshit scroll price tinkering" sheetId="1" r:id="rId1"/>
     <sheet name="Spells" sheetId="2" r:id="rId2"/>
     <sheet name="Arrays BG1" sheetId="3" r:id="rId3"/>
     <sheet name="Arrays IWD" sheetId="4" r:id="rId4"/>
+    <sheet name="Arrays PST" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6650" uniqueCount="938">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6957" uniqueCount="938">
   <si>
     <t>Caster Level</t>
   </si>
@@ -4063,11 +4064,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A58FEB-71E1-4ACD-8B85-E92BCBF62977}">
   <dimension ref="A1:AL262"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AC170" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="95" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="Z251" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AG185" sqref="AG185"/>
+      <selection pane="bottomRight" activeCell="AB2" sqref="AB2:AD251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32578,4 +32579,2011 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ADE92CE-2EB5-472A-B31C-F9EF9D9789C2}">
+  <dimension ref="A1:G85"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="82" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86:XFD99"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>925</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>533</v>
+      </c>
+      <c r="E3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" t="str">
+        <f>_xlfn.CONCAT("~", C3, "~, ~", A3, "~, ~", B3, "~ =&gt; ~", C3, "~    //", E3)</f>
+        <v>~SPWI101~, ~Arcane~, ~1~ =&gt; ~SPWI101~    //Chromatic Orb</v>
+      </c>
+      <c r="G3" t="str">
+        <f>_xlfn.CONCAT("~", D3, "~, ~", C3, "~, ~", A3, "~, ~", B3, "~, ~1~, ~0~ =&gt; ~", D3, "~    //", E3)</f>
+        <v>~RECIPE01, SPWI101~, ~SPWI101~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~RECIPE01, SPWI101~    //Chromatic Orb</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>546</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" ref="F4:F46" si="0">_xlfn.CONCAT("~", C4, "~, ~", A4, "~, ~", B4, "~ =&gt; ~", C4, "~    //", E4)</f>
+        <v>~SPWI102~, ~Arcane~, ~1~ =&gt; ~SPWI102~    //Armor</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" ref="G4:G46" si="1">_xlfn.CONCAT("~", D4, "~, ~", C4, "~, ~", A4, "~, ~", B4, "~, ~1~, ~0~ =&gt; ~", D4, "~    //", E4)</f>
+        <v>~SPWI102, BREAST1/2~, ~SPWI102~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~SPWI102, BREAST1/2~    //Armor</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>465</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI103~, ~Arcane~, ~1~ =&gt; ~SPWI103~    //Minor Embalming</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI103~, ~SPWI103~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~SPWI103~    //Minor Embalming</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>466</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI104~, ~Arcane~, ~1~ =&gt; ~SPWI104~    //Fist of Iron</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI104~, ~SPWI104~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~SPWI104~    //Fist of Iron</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>532</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI105~, ~Arcane~, ~1~ =&gt; ~SPWI105~    //Identify</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v>~RECIPE02~, ~SPWI105~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~RECIPE02~    //Identify</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI107~, ~Arcane~, ~1~ =&gt; ~SPWI107~    //Magic Missile</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI107~, ~SPWI107~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~SPWI107~    //Magic Missile</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>467</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI108~, ~Arcane~, ~1~ =&gt; ~SPWI108~    //Pacify</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI108~, ~SPWI108~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~SPWI108~    //Pacify</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI111~, ~Arcane~, ~1~ =&gt; ~SPWI111~    //Shield</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI111~, ~SPWI111~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~SPWI111~    //Shield</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>468</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI113~, ~Arcane~, ~1~ =&gt; ~SPWI113~    //Missile of Patience</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI113~, ~SPWI113~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~SPWI113~    //Missile of Patience</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI114~, ~Arcane~, ~1~ =&gt; ~SPWI114~    //Friends</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI114~, ~SPWI114~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~SPWI114~    //Friends</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI115~, ~Arcane~, ~1~ =&gt; ~SPWI115~    //Blindness</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI115~, ~SPWI115~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~SPWI115~    //Blindness</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="E14" t="s">
+        <v>469</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI116~, ~Arcane~, ~1~ =&gt; ~SPWI116~    //Tongues of Flame</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v>~ --ignus only~, ~SPWI116~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~ --ignus only~    //Tongues of Flame</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>535</v>
+      </c>
+      <c r="E15" t="s">
+        <v>470</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI117~, ~Arcane~, ~1~ =&gt; ~SPWI117~    //Seeking Flames</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
+        <v>~IGNUS01~, ~SPWI117~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~IGNUS01~    //Seeking Flames</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>536</v>
+      </c>
+      <c r="E16" t="s">
+        <v>471</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI118~, ~Arcane~, ~1~ =&gt; ~SPWI118~    //Scripture of Steel</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v>~CIRCLE02~, ~SPWI118~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~CIRCLE02~    //Scripture of Steel</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
+        <v>537</v>
+      </c>
+      <c r="E17" t="s">
+        <v>474</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI119~, ~Arcane~, ~1~ =&gt; ~SPWI119~    //Submerge the Will</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="1"/>
+        <v>~CIRCLE03~, ~SPWI119~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~CIRCLE03~    //Submerge the Will</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>463</v>
+      </c>
+      <c r="D18" t="s">
+        <v>538</v>
+      </c>
+      <c r="E18" t="s">
+        <v>472</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI120~, ~Arcane~, ~1~ =&gt; ~SPWI120~    //Vilquar's Eye</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="1"/>
+        <v>~CIRCLE04~, ~SPWI120~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~CIRCLE04~    //Vilquar's Eye</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>464</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="E19" t="s">
+        <v>473</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI121~, ~Arcane~, ~1~ =&gt; ~SPWI121~    //Reign of Anger</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
+        <v>~ --dak'kon only~, ~SPWI121~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~ --dak'kon only~    //Reign of Anger</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="1"/>
+        <v>~~, ~~, ~~, ~~, ~1~, ~0~ =&gt; ~~    //</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" t="s">
+        <v>475</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI201~, ~Arcane~, ~2~ =&gt; ~SPWI201~    //Adder's Kiss</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI201~, ~SPWI201~, ~Arcane~, ~2~, ~1~, ~0~ =&gt; ~SPWI201~    //Adder's Kiss</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" t="s">
+        <v>476</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI202~, ~Arcane~, ~2~ =&gt; ~SPWI202~    //Black-Barbed Curse</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI202~, ~SPWI202~, ~Arcane~, ~2~, ~1~, ~0~ =&gt; ~SPWI202~    //Black-Barbed Curse</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" t="s">
+        <v>477</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI203~, ~Arcane~, ~2~ =&gt; ~SPWI203~    //Black-Barbed Shield</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI203~, ~SPWI203~, ~Arcane~, ~2~, ~1~, ~0~ =&gt; ~SPWI203~    //Black-Barbed Shield</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" t="s">
+        <v>534</v>
+      </c>
+      <c r="E24" t="s">
+        <v>478</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI204~, ~Arcane~, ~2~ =&gt; ~SPWI204~    //Blood Bridge</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="1"/>
+        <v>~RECIPE03, SPWI204~, ~SPWI204~, ~Arcane~, ~2~, ~1~, ~0~ =&gt; ~RECIPE03, SPWI204~    //Blood Bridge</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" t="s">
+        <v>479</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI205~, ~Arcane~, ~2~ =&gt; ~SPWI205~    //Greater Embalming</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI205~, ~SPWI205~, ~Arcane~, ~2~, ~1~, ~0~ =&gt; ~SPWI205~    //Greater Embalming</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" t="s">
+        <v>480</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI207~, ~Arcane~, ~2~ =&gt; ~SPWI207~    //Ice Knife</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI207~, ~SPWI207~, ~Arcane~, ~2~, ~1~, ~0~ =&gt; ~SPWI207~    //Ice Knife</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" t="s">
+        <v>481</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI209~, ~Arcane~, ~2~ =&gt; ~SPWI209~    //Pain Mirror</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI209~, ~SPWI209~, ~Arcane~, ~2~, ~1~, ~0~ =&gt; ~SPWI209~    //Pain Mirror</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI211~, ~Arcane~, ~2~ =&gt; ~SPWI211~    //Strength</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI211~, ~SPWI211~, ~Arcane~, ~2~, ~1~, ~0~ =&gt; ~SPWI211~    //Strength</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" t="s">
+        <v>482</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI212~, ~Arcane~, ~2~ =&gt; ~SPWI212~    //Swarm Curse</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI212~, ~SPWI212~, ~Arcane~, ~2~, ~1~, ~0~ =&gt; ~SPWI212~    //Swarm Curse</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" t="s">
+        <v>80</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI213~, ~Arcane~, ~2~ =&gt; ~SPWI213~    //Horror</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI213~, ~SPWI213~, ~Arcane~, ~2~, ~1~, ~0~ =&gt; ~SPWI213~    //Horror</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI214~, ~Arcane~, ~2~ =&gt; ~SPWI214~    //Luck</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI214~, ~SPWI214~, ~Arcane~, ~2~, ~1~, ~0~ =&gt; ~SPWI214~    //Luck</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI215~, ~Arcane~, ~2~ =&gt; ~SPWI215~    //Knock</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI215~, ~SPWI215~, ~Arcane~, ~2~, ~1~, ~0~ =&gt; ~SPWI215~    //Knock</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" t="s">
+        <v>77</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI216~, ~Arcane~, ~2~ =&gt; ~SPWI216~    //Blur</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI216~, ~SPWI216~, ~Arcane~, ~2~, ~1~, ~0~ =&gt; ~SPWI216~    //Blur</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" t="s">
+        <v>541</v>
+      </c>
+      <c r="E34" t="s">
+        <v>483</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI217~, ~Arcane~, ~2~ =&gt; ~SPWI217~    //Ignus' Terror</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="1"/>
+        <v>~IGNUS02~, ~SPWI217~, ~Arcane~, ~2~, ~1~, ~0~ =&gt; ~IGNUS02~    //Ignus' Terror</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35" t="s">
+        <v>542</v>
+      </c>
+      <c r="E35" t="s">
+        <v>484</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI218~, ~Arcane~, ~2~ =&gt; ~SPWI218~    //Infernal Orb</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="1"/>
+        <v>~IGNUS04~, ~SPWI218~, ~Arcane~, ~2~, ~1~, ~0~ =&gt; ~IGNUS04~    //Infernal Orb</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" t="s">
+        <v>543</v>
+      </c>
+      <c r="E36" t="s">
+        <v>485</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI219~, ~Arcane~, ~2~ =&gt; ~SPWI219~    //Power of One</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="1"/>
+        <v>~CIRCLE05~, ~SPWI219~, ~Arcane~, ~2~, ~1~, ~0~ =&gt; ~CIRCLE05~    //Power of One</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="1"/>
+        <v>~~, ~~, ~~, ~~, ~1~, ~0~ =&gt; ~~    //</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>94</v>
+      </c>
+      <c r="D38" t="s">
+        <v>94</v>
+      </c>
+      <c r="E38" t="s">
+        <v>486</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI301~, ~Arcane~, ~3~ =&gt; ~SPWI301~    //Ball Lightning</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI301~, ~SPWI301~, ~Arcane~, ~3~, ~1~, ~0~ =&gt; ~SPWI301~    //Ball Lightning</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" t="s">
+        <v>97</v>
+      </c>
+      <c r="E39" t="s">
+        <v>487</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI304~, ~Arcane~, ~3~ =&gt; ~SPWI304~    //Cloak of Warding</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI304~, ~SPWI304~, ~Arcane~, ~3~, ~1~, ~0~ =&gt; ~SPWI304~    //Cloak of Warding</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" t="s">
+        <v>98</v>
+      </c>
+      <c r="E40" t="s">
+        <v>488</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI305~, ~Arcane~, ~3~ =&gt; ~SPWI305~    //Elysium's Tears</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI305~, ~SPWI305~, ~Arcane~, ~3~, ~1~, ~0~ =&gt; ~SPWI305~    //Elysium's Tears</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" t="s">
+        <v>100</v>
+      </c>
+      <c r="E41" t="s">
+        <v>489</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI307~, ~Arcane~, ~3~ =&gt; ~SPWI307~    //Hold Undead</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI307~, ~SPWI307~, ~Arcane~, ~3~, ~1~, ~0~ =&gt; ~SPWI307~    //Hold Undead</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>101</v>
+      </c>
+      <c r="D42" t="s">
+        <v>101</v>
+      </c>
+      <c r="E42" t="s">
+        <v>490</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI308~, ~Arcane~, ~3~ =&gt; ~SPWI308~    //Tasha's Unbearable Derisive Laughter</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI308~, ~SPWI308~, ~Arcane~, ~3~, ~1~, ~0~ =&gt; ~SPWI308~    //Tasha's Unbearable Derisive Laughter</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
+        <v>102</v>
+      </c>
+      <c r="D43" t="s">
+        <v>102</v>
+      </c>
+      <c r="E43" t="s">
+        <v>122</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI309~, ~Arcane~, ~3~ =&gt; ~SPWI309~    //Vampiric Touch</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI309~, ~SPWI309~, ~Arcane~, ~3~, ~1~, ~0~ =&gt; ~SPWI309~    //Vampiric Touch</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>103</v>
+      </c>
+      <c r="D44" t="s">
+        <v>103</v>
+      </c>
+      <c r="E44" t="s">
+        <v>491</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI310~, ~Arcane~, ~3~ =&gt; ~SPWI310~    //Ax of Torment</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI310~, ~SPWI310~, ~Arcane~, ~3~, ~1~, ~0~ =&gt; ~SPWI310~    //Ax of Torment</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>104</v>
+      </c>
+      <c r="D45" t="s">
+        <v>104</v>
+      </c>
+      <c r="E45" t="s">
+        <v>492</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI311~, ~Arcane~, ~3~ =&gt; ~SPWI311~    //Zerthimon's Focus</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="1"/>
+        <v>~SPWI311~, ~SPWI311~, ~Arcane~, ~3~, ~1~, ~0~ =&gt; ~SPWI311~    //Zerthimon's Focus</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>105</v>
+      </c>
+      <c r="D46" t="s">
+        <v>544</v>
+      </c>
+      <c r="E46" t="s">
+        <v>493</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="0"/>
+        <v>~SPWI312~, ~Arcane~, ~3~ =&gt; ~SPWI312~    //Infernal Shield</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="1"/>
+        <v>~IGNU03~, ~SPWI312~, ~Arcane~, ~3~, ~1~, ~0~ =&gt; ~IGNU03~    //Infernal Shield</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47" t="s">
+        <v>106</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="E47" t="s">
+        <v>494</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" ref="F47:F62" si="2">_xlfn.CONCAT("~", C47, "~, ~", A47, "~, ~", B47, "~ =&gt; ~", C47, "~    //", E47)</f>
+        <v>~SPWI313~, ~Arcane~, ~3~ =&gt; ~SPWI313~    //Fiery Rain</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" ref="G47:G62" si="3">_xlfn.CONCAT("~", D47, "~, ~", C47, "~, ~", A47, "~, ~", B47, "~, ~1~, ~0~ =&gt; ~", D47, "~    //", E47)</f>
+        <v>~ --ignus only~, ~SPWI313~, ~Arcane~, ~3~, ~1~, ~0~ =&gt; ~ --ignus only~    //Fiery Rain</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48" t="s">
+        <v>107</v>
+      </c>
+      <c r="D48" t="s">
+        <v>545</v>
+      </c>
+      <c r="E48" t="s">
+        <v>495</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="2"/>
+        <v>~SPWI314~, ~Arcane~, ~3~ =&gt; ~SPWI314~    //Balance In All Things</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="3"/>
+        <v>~CIRCLE06~, ~SPWI314~, ~Arcane~, ~3~, ~1~, ~0~ =&gt; ~CIRCLE06~    //Balance In All Things</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F49" t="str">
+        <f t="shared" si="2"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="3"/>
+        <v>~~, ~~, ~~, ~~, ~1~, ~0~ =&gt; ~~    //</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>17</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50" t="s">
+        <v>126</v>
+      </c>
+      <c r="D50" t="s">
+        <v>126</v>
+      </c>
+      <c r="E50" t="s">
+        <v>496</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="2"/>
+        <v>~SPWI401~, ~Arcane~, ~4~ =&gt; ~SPWI401~    //Blacksphere</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="3"/>
+        <v>~SPWI401~, ~SPWI401~, ~Arcane~, ~4~, ~1~, ~0~ =&gt; ~SPWI401~    //Blacksphere</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>17</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51" t="s">
+        <v>128</v>
+      </c>
+      <c r="D51" t="s">
+        <v>128</v>
+      </c>
+      <c r="E51" t="s">
+        <v>127</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" si="2"/>
+        <v>~SPWI402~, ~Arcane~, ~4~ =&gt; ~SPWI402~    //Confusion</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="3"/>
+        <v>~SPWI402~, ~SPWI402~, ~Arcane~, ~4~, ~1~, ~0~ =&gt; ~SPWI402~    //Confusion</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>131</v>
+      </c>
+      <c r="D52" t="s">
+        <v>131</v>
+      </c>
+      <c r="E52" t="s">
+        <v>497</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="2"/>
+        <v>~SPWI405~, ~Arcane~, ~4~ =&gt; ~SPWI405~    //Force Missiles</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="3"/>
+        <v>~SPWI405~, ~SPWI405~, ~Arcane~, ~4~, ~1~, ~0~ =&gt; ~SPWI405~    //Force Missiles</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53" t="s">
+        <v>132</v>
+      </c>
+      <c r="D53" t="s">
+        <v>132</v>
+      </c>
+      <c r="E53" t="s">
+        <v>498</v>
+      </c>
+      <c r="F53" t="str">
+        <f t="shared" si="2"/>
+        <v>~SPWI406~, ~Arcane~, ~4~ =&gt; ~SPWI406~    //Improved Strength</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="3"/>
+        <v>~SPWI406~, ~SPWI406~, ~Arcane~, ~4~, ~1~, ~0~ =&gt; ~SPWI406~    //Improved Strength</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>17</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54" t="s">
+        <v>134</v>
+      </c>
+      <c r="D54" t="s">
+        <v>134</v>
+      </c>
+      <c r="E54" t="s">
+        <v>499</v>
+      </c>
+      <c r="F54" t="str">
+        <f t="shared" si="2"/>
+        <v>~SPWI408~, ~Arcane~, ~4~ =&gt; ~SPWI408~    //Shroud of Shadows</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="3"/>
+        <v>~SPWI408~, ~SPWI408~, ~Arcane~, ~4~, ~1~, ~0~ =&gt; ~SPWI408~    //Shroud of Shadows</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55" t="s">
+        <v>135</v>
+      </c>
+      <c r="D55" t="s">
+        <v>135</v>
+      </c>
+      <c r="E55" t="s">
+        <v>149</v>
+      </c>
+      <c r="F55" t="str">
+        <f t="shared" si="2"/>
+        <v>~SPWI409~, ~Arcane~, ~4~ =&gt; ~SPWI409~    //Remove Curse</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="3"/>
+        <v>~SPWI409~, ~SPWI409~, ~Arcane~, ~4~, ~1~, ~0~ =&gt; ~SPWI409~    //Remove Curse</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56">
+        <v>4</v>
+      </c>
+      <c r="C56" t="s">
+        <v>136</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="E56" t="s">
+        <v>500</v>
+      </c>
+      <c r="F56" t="str">
+        <f t="shared" si="2"/>
+        <v>~SPWI410~, ~Arcane~, ~4~ =&gt; ~SPWI410~    //Elemental Strike</v>
+      </c>
+      <c r="G56" t="str">
+        <f t="shared" si="3"/>
+        <v>~ --ignus only~, ~SPWI410~, ~Arcane~, ~4~, ~1~, ~0~ =&gt; ~ --ignus only~    //Elemental Strike</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F57" t="str">
+        <f t="shared" si="2"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="3"/>
+        <v>~~, ~~, ~~, ~~, ~1~, ~0~ =&gt; ~~    //</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>17</v>
+      </c>
+      <c r="B58">
+        <v>5</v>
+      </c>
+      <c r="C58" t="s">
+        <v>156</v>
+      </c>
+      <c r="D58" t="s">
+        <v>156</v>
+      </c>
+      <c r="E58" t="s">
+        <v>166</v>
+      </c>
+      <c r="F58" t="str">
+        <f t="shared" si="2"/>
+        <v>~SPWI501~, ~Arcane~, ~5~ =&gt; ~SPWI501~    //Cloudkill</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="3"/>
+        <v>~SPWI501~, ~SPWI501~, ~Arcane~, ~5~, ~1~, ~0~ =&gt; ~SPWI501~    //Cloudkill</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>17</v>
+      </c>
+      <c r="B59">
+        <v>5</v>
+      </c>
+      <c r="C59" t="s">
+        <v>157</v>
+      </c>
+      <c r="D59" t="s">
+        <v>157</v>
+      </c>
+      <c r="E59" t="s">
+        <v>168</v>
+      </c>
+      <c r="F59" t="str">
+        <f t="shared" si="2"/>
+        <v>~SPWI502~, ~Arcane~, ~5~ =&gt; ~SPWI502~    //Cone of Cold</v>
+      </c>
+      <c r="G59" t="str">
+        <f t="shared" si="3"/>
+        <v>~SPWI502~, ~SPWI502~, ~Arcane~, ~5~, ~1~, ~0~ =&gt; ~SPWI502~    //Cone of Cold</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>17</v>
+      </c>
+      <c r="B60">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s">
+        <v>159</v>
+      </c>
+      <c r="D60" t="s">
+        <v>159</v>
+      </c>
+      <c r="E60" t="s">
+        <v>501</v>
+      </c>
+      <c r="F60" t="str">
+        <f t="shared" si="2"/>
+        <v>~SPWI504~, ~Arcane~, ~5~ =&gt; ~SPWI504~    //Enoll Eva's Duplication</v>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="3"/>
+        <v>~SPWI504~, ~SPWI504~, ~Arcane~, ~5~, ~1~, ~0~ =&gt; ~SPWI504~    //Enoll Eva's Duplication</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>17</v>
+      </c>
+      <c r="B61">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>160</v>
+      </c>
+      <c r="D61" t="s">
+        <v>160</v>
+      </c>
+      <c r="E61" t="s">
+        <v>502</v>
+      </c>
+      <c r="F61" t="str">
+        <f t="shared" si="2"/>
+        <v>~SPWI505~, ~Arcane~, ~5~ =&gt; ~SPWI505~    //Desert Hell</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" si="3"/>
+        <v>~SPWI505~, ~SPWI505~, ~Arcane~, ~5~, ~1~, ~0~ =&gt; ~SPWI505~    //Desert Hell</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>17</v>
+      </c>
+      <c r="B62">
+        <v>5</v>
+      </c>
+      <c r="C62" t="s">
+        <v>161</v>
+      </c>
+      <c r="D62" t="s">
+        <v>161</v>
+      </c>
+      <c r="E62" t="s">
+        <v>503</v>
+      </c>
+      <c r="F62" t="str">
+        <f t="shared" si="2"/>
+        <v>~SPWI506~, ~Arcane~, ~5~ =&gt; ~SPWI506~    //Fire and Ice</v>
+      </c>
+      <c r="G62" t="str">
+        <f t="shared" si="3"/>
+        <v>~SPWI506~, ~SPWI506~, ~Arcane~, ~5~, ~1~, ~0~ =&gt; ~SPWI506~    //Fire and Ice</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F63" t="str">
+        <f t="shared" ref="F63:F72" si="4">_xlfn.CONCAT("~", C63, "~, ~", A63, "~, ~", B63, "~ =&gt; ~", C63, "~    //", E63)</f>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
+      <c r="G63" t="str">
+        <f t="shared" ref="G63:G72" si="5">_xlfn.CONCAT("~", D63, "~, ~", C63, "~, ~", A63, "~, ~", B63, "~, ~1~, ~0~ =&gt; ~", D63, "~    //", E63)</f>
+        <v>~~, ~~, ~~, ~~, ~1~, ~0~ =&gt; ~~    //</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>17</v>
+      </c>
+      <c r="B64">
+        <v>6</v>
+      </c>
+      <c r="C64" t="s">
+        <v>184</v>
+      </c>
+      <c r="D64" t="s">
+        <v>184</v>
+      </c>
+      <c r="E64" t="s">
+        <v>258</v>
+      </c>
+      <c r="F64" t="str">
+        <f t="shared" si="4"/>
+        <v>~SPWI601~, ~Arcane~, ~6~ =&gt; ~SPWI601~    //Antimagic Shell</v>
+      </c>
+      <c r="G64" t="str">
+        <f t="shared" si="5"/>
+        <v>~SPWI601~, ~SPWI601~, ~Arcane~, ~6~, ~1~, ~0~ =&gt; ~SPWI601~    //Antimagic Shell</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>17</v>
+      </c>
+      <c r="B65">
+        <v>6</v>
+      </c>
+      <c r="C65" t="s">
+        <v>185</v>
+      </c>
+      <c r="D65" t="s">
+        <v>185</v>
+      </c>
+      <c r="E65" t="s">
+        <v>190</v>
+      </c>
+      <c r="F65" t="str">
+        <f t="shared" si="4"/>
+        <v>~SPWI602~, ~Arcane~, ~6~ =&gt; ~SPWI602~    //Globe of Invulnerability</v>
+      </c>
+      <c r="G65" t="str">
+        <f t="shared" si="5"/>
+        <v>~SPWI602~, ~SPWI602~, ~Arcane~, ~6~, ~1~, ~0~ =&gt; ~SPWI602~    //Globe of Invulnerability</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>17</v>
+      </c>
+      <c r="B66">
+        <v>6</v>
+      </c>
+      <c r="C66" t="s">
+        <v>186</v>
+      </c>
+      <c r="D66" t="s">
+        <v>186</v>
+      </c>
+      <c r="E66" t="s">
+        <v>504</v>
+      </c>
+      <c r="F66" t="str">
+        <f t="shared" si="4"/>
+        <v>~SPWI603~, ~Arcane~, ~6~ =&gt; ~SPWI603~    //Howl of Pandemonium</v>
+      </c>
+      <c r="G66" t="str">
+        <f t="shared" si="5"/>
+        <v>~SPWI603~, ~SPWI603~, ~Arcane~, ~6~, ~1~, ~0~ =&gt; ~SPWI603~    //Howl of Pandemonium</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>17</v>
+      </c>
+      <c r="B67">
+        <v>6</v>
+      </c>
+      <c r="C67" t="s">
+        <v>187</v>
+      </c>
+      <c r="D67" t="s">
+        <v>187</v>
+      </c>
+      <c r="E67" t="s">
+        <v>505</v>
+      </c>
+      <c r="F67" t="str">
+        <f t="shared" si="4"/>
+        <v>~SPWI604~, ~Arcane~, ~6~ =&gt; ~SPWI604~    //Chain Lightning Storm</v>
+      </c>
+      <c r="G67" t="str">
+        <f t="shared" si="5"/>
+        <v>~SPWI604~, ~SPWI604~, ~Arcane~, ~6~, ~1~, ~0~ =&gt; ~SPWI604~    //Chain Lightning Storm</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F68" t="str">
+        <f t="shared" si="4"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
+      <c r="G68" t="str">
+        <f t="shared" si="5"/>
+        <v>~~, ~~, ~~, ~~, ~1~, ~0~ =&gt; ~~    //</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>17</v>
+      </c>
+      <c r="B69">
+        <v>7</v>
+      </c>
+      <c r="C69" t="s">
+        <v>270</v>
+      </c>
+      <c r="D69" t="s">
+        <v>270</v>
+      </c>
+      <c r="E69" t="s">
+        <v>287</v>
+      </c>
+      <c r="F69" t="str">
+        <f t="shared" si="4"/>
+        <v>~SPWI701~, ~Arcane~, ~7~ =&gt; ~SPWI701~    //Acid Storm</v>
+      </c>
+      <c r="G69" t="str">
+        <f t="shared" si="5"/>
+        <v>~SPWI701~, ~SPWI701~, ~Arcane~, ~7~, ~1~, ~0~ =&gt; ~SPWI701~    //Acid Storm</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>17</v>
+      </c>
+      <c r="B70">
+        <v>7</v>
+      </c>
+      <c r="C70" t="s">
+        <v>271</v>
+      </c>
+      <c r="D70" t="s">
+        <v>271</v>
+      </c>
+      <c r="E70" t="s">
+        <v>506</v>
+      </c>
+      <c r="F70" t="str">
+        <f t="shared" si="4"/>
+        <v>~SPWI702~, ~Arcane~, ~7~ =&gt; ~SPWI702~    //Blade Storm</v>
+      </c>
+      <c r="G70" t="str">
+        <f t="shared" si="5"/>
+        <v>~SPWI702~, ~SPWI702~, ~Arcane~, ~7~, ~1~, ~0~ =&gt; ~SPWI702~    //Blade Storm</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>17</v>
+      </c>
+      <c r="B71">
+        <v>7</v>
+      </c>
+      <c r="C71" t="s">
+        <v>273</v>
+      </c>
+      <c r="D71" t="s">
+        <v>273</v>
+      </c>
+      <c r="E71" t="s">
+        <v>507</v>
+      </c>
+      <c r="F71" t="str">
+        <f t="shared" si="4"/>
+        <v>~SPWI704~, ~Arcane~, ~7~ =&gt; ~SPWI704~    //Guardian Mantle</v>
+      </c>
+      <c r="G71" t="str">
+        <f t="shared" si="5"/>
+        <v>~SPWI704~, ~SPWI704~, ~Arcane~, ~7~, ~1~, ~0~ =&gt; ~SPWI704~    //Guardian Mantle</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>17</v>
+      </c>
+      <c r="B72">
+        <v>7</v>
+      </c>
+      <c r="C72" t="s">
+        <v>274</v>
+      </c>
+      <c r="D72" t="s">
+        <v>274</v>
+      </c>
+      <c r="E72" t="s">
+        <v>508</v>
+      </c>
+      <c r="F72" t="str">
+        <f t="shared" si="4"/>
+        <v>~SPWI705~, ~Arcane~, ~7~ =&gt; ~SPWI705~    //Stygian Ice Storm</v>
+      </c>
+      <c r="G72" t="str">
+        <f t="shared" si="5"/>
+        <v>~SPWI705~, ~SPWI705~, ~Arcane~, ~7~, ~1~, ~0~ =&gt; ~SPWI705~    //Stygian Ice Storm</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F73" t="str">
+        <f t="shared" ref="F73:F85" si="6">_xlfn.CONCAT("~", C73, "~, ~", A73, "~, ~", B73, "~ =&gt; ~", C73, "~    //", E73)</f>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
+      <c r="G73" t="str">
+        <f t="shared" ref="G73:G85" si="7">_xlfn.CONCAT("~", D73, "~, ~", C73, "~, ~", A73, "~, ~", B73, "~, ~1~, ~0~ =&gt; ~", D73, "~    //", E73)</f>
+        <v>~~, ~~, ~~, ~~, ~1~, ~0~ =&gt; ~~    //</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>17</v>
+      </c>
+      <c r="B74">
+        <v>8</v>
+      </c>
+      <c r="C74" t="s">
+        <v>292</v>
+      </c>
+      <c r="D74" t="s">
+        <v>292</v>
+      </c>
+      <c r="E74" t="s">
+        <v>509</v>
+      </c>
+      <c r="F74" t="str">
+        <f t="shared" si="6"/>
+        <v>~SPWI802~, ~Arcane~, ~8~ =&gt; ~SPWI802~    //Meteor Storm Bombardment</v>
+      </c>
+      <c r="G74" t="str">
+        <f t="shared" si="7"/>
+        <v>~SPWI802~, ~SPWI802~, ~Arcane~, ~8~, ~1~, ~0~ =&gt; ~SPWI802~    //Meteor Storm Bombardment</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>17</v>
+      </c>
+      <c r="B75">
+        <v>8</v>
+      </c>
+      <c r="C75" t="s">
+        <v>293</v>
+      </c>
+      <c r="D75" t="s">
+        <v>293</v>
+      </c>
+      <c r="E75" t="s">
+        <v>510</v>
+      </c>
+      <c r="F75" t="str">
+        <f t="shared" si="6"/>
+        <v>~SPWI803~, ~Arcane~, ~8~ =&gt; ~SPWI803~    //Deathbolt</v>
+      </c>
+      <c r="G75" t="str">
+        <f t="shared" si="7"/>
+        <v>~SPWI803~, ~SPWI803~, ~Arcane~, ~8~, ~1~, ~0~ =&gt; ~SPWI803~    //Deathbolt</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>17</v>
+      </c>
+      <c r="B76">
+        <v>8</v>
+      </c>
+      <c r="C76" t="s">
+        <v>294</v>
+      </c>
+      <c r="D76" t="s">
+        <v>294</v>
+      </c>
+      <c r="E76" t="s">
+        <v>511</v>
+      </c>
+      <c r="F76" t="str">
+        <f t="shared" si="6"/>
+        <v>~SPWI804~, ~Arcane~, ~8~ =&gt; ~SPWI804~    //Ignus' Fury</v>
+      </c>
+      <c r="G76" t="str">
+        <f t="shared" si="7"/>
+        <v>~SPWI804~, ~SPWI804~, ~Arcane~, ~8~, ~1~, ~0~ =&gt; ~SPWI804~    //Ignus' Fury</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>17</v>
+      </c>
+      <c r="B77">
+        <v>8</v>
+      </c>
+      <c r="C77" t="s">
+        <v>295</v>
+      </c>
+      <c r="D77" t="s">
+        <v>295</v>
+      </c>
+      <c r="E77" t="s">
+        <v>305</v>
+      </c>
+      <c r="F77" t="str">
+        <f t="shared" si="6"/>
+        <v>~SPWI805~, ~Arcane~, ~8~ =&gt; ~SPWI805~    //Power Word, Blind</v>
+      </c>
+      <c r="G77" t="str">
+        <f t="shared" si="7"/>
+        <v>~SPWI805~, ~SPWI805~, ~Arcane~, ~8~, ~1~, ~0~ =&gt; ~SPWI805~    //Power Word, Blind</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>17</v>
+      </c>
+      <c r="B78">
+        <v>8</v>
+      </c>
+      <c r="C78" t="s">
+        <v>297</v>
+      </c>
+      <c r="D78" t="s">
+        <v>297</v>
+      </c>
+      <c r="E78" t="s">
+        <v>512</v>
+      </c>
+      <c r="F78" t="str">
+        <f t="shared" si="6"/>
+        <v>~SPWI807~, ~Arcane~, ~8~ =&gt; ~SPWI807~    //Mechanus' Cannon</v>
+      </c>
+      <c r="G78" t="str">
+        <f t="shared" si="7"/>
+        <v>~SPWI807~, ~SPWI807~, ~Arcane~, ~8~, ~1~, ~0~ =&gt; ~SPWI807~    //Mechanus' Cannon</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F79" t="str">
+        <f t="shared" si="6"/>
+        <v>~~, ~~, ~~ =&gt; ~~    //</v>
+      </c>
+      <c r="G79" t="str">
+        <f t="shared" si="7"/>
+        <v>~~, ~~, ~~, ~~, ~1~, ~0~ =&gt; ~~    //</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>17</v>
+      </c>
+      <c r="B80">
+        <v>9</v>
+      </c>
+      <c r="C80" t="s">
+        <v>513</v>
+      </c>
+      <c r="D80" t="s">
+        <v>513</v>
+      </c>
+      <c r="E80" t="s">
+        <v>527</v>
+      </c>
+      <c r="F80" t="str">
+        <f t="shared" si="6"/>
+        <v>~SPWI901~, ~Arcane~, ~9~ =&gt; ~SPWI901~    //Celestial Host</v>
+      </c>
+      <c r="G80" t="str">
+        <f t="shared" si="7"/>
+        <v>~SPWI901~, ~SPWI901~, ~Arcane~, ~9~, ~1~, ~0~ =&gt; ~SPWI901~    //Celestial Host</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>17</v>
+      </c>
+      <c r="B81">
+        <v>9</v>
+      </c>
+      <c r="C81" t="s">
+        <v>514</v>
+      </c>
+      <c r="D81" t="s">
+        <v>514</v>
+      </c>
+      <c r="E81" t="s">
+        <v>528</v>
+      </c>
+      <c r="F81" t="str">
+        <f t="shared" si="6"/>
+        <v>~SPWI902~, ~Arcane~, ~9~ =&gt; ~SPWI902~    //Conflagration</v>
+      </c>
+      <c r="G81" t="str">
+        <f t="shared" si="7"/>
+        <v>~SPWI902~, ~SPWI902~, ~Arcane~, ~9~, ~1~, ~0~ =&gt; ~SPWI902~    //Conflagration</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>17</v>
+      </c>
+      <c r="B82">
+        <v>9</v>
+      </c>
+      <c r="C82" t="s">
+        <v>517</v>
+      </c>
+      <c r="D82" t="s">
+        <v>517</v>
+      </c>
+      <c r="E82" t="s">
+        <v>529</v>
+      </c>
+      <c r="F82" t="str">
+        <f t="shared" si="6"/>
+        <v>~SPWI905~, ~Arcane~, ~9~ =&gt; ~SPWI905~    //Elysium's Fires</v>
+      </c>
+      <c r="G82" t="str">
+        <f t="shared" si="7"/>
+        <v>~SPWI905~, ~SPWI905~, ~Arcane~, ~9~, ~1~, ~0~ =&gt; ~SPWI905~    //Elysium's Fires</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>17</v>
+      </c>
+      <c r="B83">
+        <v>9</v>
+      </c>
+      <c r="C83" t="s">
+        <v>521</v>
+      </c>
+      <c r="D83" t="s">
+        <v>521</v>
+      </c>
+      <c r="E83" t="s">
+        <v>311</v>
+      </c>
+      <c r="F83" t="str">
+        <f t="shared" si="6"/>
+        <v>~SPWI909~, ~Arcane~, ~9~ =&gt; ~SPWI909~    //Power Word, Kill</v>
+      </c>
+      <c r="G83" t="str">
+        <f t="shared" si="7"/>
+        <v>~SPWI909~, ~SPWI909~, ~Arcane~, ~9~, ~1~, ~0~ =&gt; ~SPWI909~    //Power Word, Kill</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>17</v>
+      </c>
+      <c r="B84">
+        <v>9</v>
+      </c>
+      <c r="C84" t="s">
+        <v>524</v>
+      </c>
+      <c r="D84" t="s">
+        <v>524</v>
+      </c>
+      <c r="E84" t="s">
+        <v>530</v>
+      </c>
+      <c r="F84" t="str">
+        <f t="shared" si="6"/>
+        <v>~SPWI912~, ~Arcane~, ~9~ =&gt; ~SPWI912~    //Abyssal Fury</v>
+      </c>
+      <c r="G84" t="str">
+        <f t="shared" si="7"/>
+        <v>~SPWI912~, ~SPWI912~, ~Arcane~, ~9~, ~1~, ~0~ =&gt; ~SPWI912~    //Abyssal Fury</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>17</v>
+      </c>
+      <c r="B85">
+        <v>9</v>
+      </c>
+      <c r="C85" t="s">
+        <v>526</v>
+      </c>
+      <c r="D85" t="s">
+        <v>526</v>
+      </c>
+      <c r="E85" t="s">
+        <v>531</v>
+      </c>
+      <c r="F85" t="str">
+        <f t="shared" si="6"/>
+        <v>~SPWI914~, ~Arcane~, ~9~ =&gt; ~SPWI914~    //Rune of Torment</v>
+      </c>
+      <c r="G85" t="str">
+        <f t="shared" si="7"/>
+        <v>~SPWI914~, ~SPWI914~, ~Arcane~, ~9~, ~1~, ~0~ =&gt; ~SPWI914~    //Rune of Torment</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding in arcane scroll list for arcane spell items
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BDDAEF-A2B1-4BDA-BFDB-85AD31A9961E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A2997B-AABF-4948-95D3-B40A05D78C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="1" activeTab="4" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -2952,7 +2952,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2969,6 +2969,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent2" xfId="4" builtinId="33"/>
@@ -32585,8 +32586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ADE92CE-2EB5-472A-B31C-F9EF9D9789C2}">
   <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="82" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86:XFD99"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32638,7 +32639,7 @@
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>533</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
         <v>53</v>
@@ -32649,7 +32650,7 @@
       </c>
       <c r="G3" t="str">
         <f>_xlfn.CONCAT("~", D3, "~, ~", C3, "~, ~", A3, "~, ~", B3, "~, ~1~, ~0~ =&gt; ~", D3, "~    //", E3)</f>
-        <v>~RECIPE01, SPWI101~, ~SPWI101~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~RECIPE01, SPWI101~    //Chromatic Orb</v>
+        <v>~SPWI101~, ~SPWI101~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~SPWI101~    //Chromatic Orb</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -32663,7 +32664,7 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>546</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>38</v>
@@ -32674,7 +32675,7 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" ref="G4:G46" si="1">_xlfn.CONCAT("~", D4, "~, ~", C4, "~, ~", A4, "~, ~", B4, "~, ~1~, ~0~ =&gt; ~", D4, "~    //", E4)</f>
-        <v>~SPWI102, BREAST1/2~, ~SPWI102~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~SPWI102, BREAST1/2~    //Armor</v>
+        <v>~SPWI102~, ~SPWI102~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~SPWI102~    //Armor</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -32738,7 +32739,7 @@
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>532</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
         <v>45</v>
@@ -32749,7 +32750,7 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" si="1"/>
-        <v>~RECIPE02~, ~SPWI105~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~RECIPE02~    //Identify</v>
+        <v>~SPWI105~, ~SPWI105~, ~Arcane~, ~1~, ~1~, ~0~ =&gt; ~SPWI105~    //Identify</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -32912,7 +32913,7 @@
       <c r="C14" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="12" t="s">
         <v>539</v>
       </c>
       <c r="E14" t="s">
@@ -32937,7 +32938,7 @@
       <c r="C15" t="s">
         <v>35</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="6" t="s">
         <v>535</v>
       </c>
       <c r="E15" t="s">
@@ -32962,7 +32963,7 @@
       <c r="C16" t="s">
         <v>36</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="6" t="s">
         <v>536</v>
       </c>
       <c r="E16" t="s">
@@ -32987,7 +32988,7 @@
       <c r="C17" t="s">
         <v>37</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="6" t="s">
         <v>537</v>
       </c>
       <c r="E17" t="s">
@@ -33012,7 +33013,7 @@
       <c r="C18" t="s">
         <v>463</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="6" t="s">
         <v>538</v>
       </c>
       <c r="E18" t="s">
@@ -33037,7 +33038,7 @@
       <c r="C19" t="s">
         <v>464</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="12" t="s">
         <v>540</v>
       </c>
       <c r="E19" t="s">
@@ -33148,7 +33149,7 @@
         <v>61</v>
       </c>
       <c r="D24" t="s">
-        <v>534</v>
+        <v>61</v>
       </c>
       <c r="E24" t="s">
         <v>478</v>
@@ -33159,7 +33160,7 @@
       </c>
       <c r="G24" t="str">
         <f t="shared" si="1"/>
-        <v>~RECIPE03, SPWI204~, ~SPWI204~, ~Arcane~, ~2~, ~1~, ~0~ =&gt; ~RECIPE03, SPWI204~    //Blood Bridge</v>
+        <v>~SPWI204~, ~SPWI204~, ~Arcane~, ~2~, ~1~, ~0~ =&gt; ~SPWI204~    //Blood Bridge</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -33397,7 +33398,7 @@
       <c r="C34" t="s">
         <v>74</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="6" t="s">
         <v>541</v>
       </c>
       <c r="E34" t="s">
@@ -33422,7 +33423,7 @@
       <c r="C35" t="s">
         <v>75</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="6" t="s">
         <v>542</v>
       </c>
       <c r="E35" t="s">
@@ -33447,7 +33448,7 @@
       <c r="C36" t="s">
         <v>76</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="6" t="s">
         <v>543</v>
       </c>
       <c r="E36" t="s">
@@ -33682,7 +33683,7 @@
       <c r="C46" t="s">
         <v>105</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="6" t="s">
         <v>544</v>
       </c>
       <c r="E46" t="s">
@@ -33707,7 +33708,7 @@
       <c r="C47" t="s">
         <v>106</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="12" t="s">
         <v>539</v>
       </c>
       <c r="E47" t="s">
@@ -33732,7 +33733,7 @@
       <c r="C48" t="s">
         <v>107</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="6" t="s">
         <v>545</v>
       </c>
       <c r="E48" t="s">
@@ -33917,7 +33918,7 @@
       <c r="C56" t="s">
         <v>136</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D56" s="12" t="s">
         <v>539</v>
       </c>
       <c r="E56" t="s">
@@ -34583,6 +34584,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Making array formulas for priest scrolls
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FECA7A-C324-42B9-AC91-C6CD42742642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7006BB15-EE35-4161-B53B-6AF1A2A1BACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="3" activeTab="6" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="3" activeTab="5" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
   <sheets>
     <sheet name="Bullshit scroll price tinkering" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9805" uniqueCount="1399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9804" uniqueCount="1400">
   <si>
     <t>Caster Level</t>
   </si>
@@ -4228,6 +4228,9 @@
   </si>
   <si>
     <t>Wizard</t>
+  </si>
+  <si>
+    <t>Q</t>
   </si>
 </sst>
 </file>
@@ -39988,11 +39991,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8D663FA-7A19-48F5-9205-7E8EC0237793}">
   <dimension ref="A1:BB247"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="T234" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="T190" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Y2" sqref="W1:Y1048576"/>
+      <selection pane="bottomRight" activeCell="X196" sqref="X196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -53965,9 +53968,6 @@
       <c r="W196" s="18" t="s">
         <v>1170</v>
       </c>
-      <c r="X196" t="s">
-        <v>1381</v>
-      </c>
       <c r="Y196" t="s">
         <v>1160</v>
       </c>
@@ -56505,8 +56505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF15ABCD-FC5C-493C-97CD-DCC4602D4EAD}">
   <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="82" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141:XFD154"/>
+    <sheetView topLeftCell="A93" zoomScale="82" workbookViewId="0">
+      <selection activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -59299,7 +59299,7 @@
         <v>939</v>
       </c>
       <c r="B129" t="s">
-        <v>1214</v>
+        <v>1399</v>
       </c>
       <c r="C129" s="18" t="s">
         <v>1181</v>
@@ -59309,11 +59309,11 @@
       </c>
       <c r="F129" t="str">
         <f t="shared" si="6"/>
-        <v>~SPPR721~, ~Divine~, ~Quest~ =&gt; ~SPPR721~    //Energy Blades</v>
+        <v>~SPPR721~, ~Divine~, ~Q~ =&gt; ~SPPR721~    //Energy Blades</v>
       </c>
       <c r="G129" t="str">
         <f t="shared" si="7"/>
-        <v>~~, ~SPPR721~, ~Divine~, ~Quest~, ~1~, ~0~ =&gt; ~~    //Energy Blades</v>
+        <v>~~, ~SPPR721~, ~Divine~, ~Q~, ~1~, ~0~ =&gt; ~~    //Energy Blades</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.35">
@@ -59321,7 +59321,7 @@
         <v>939</v>
       </c>
       <c r="B130" t="s">
-        <v>1214</v>
+        <v>1399</v>
       </c>
       <c r="C130" s="19" t="s">
         <v>1182</v>
@@ -59332,11 +59332,11 @@
       </c>
       <c r="F130" t="str">
         <f t="shared" si="6"/>
-        <v>~SPPR722~, ~Divine~, ~Quest~ =&gt; ~SPPR722~    //Storm of Vengeance</v>
+        <v>~SPPR722~, ~Divine~, ~Q~ =&gt; ~SPPR722~    //Storm of Vengeance</v>
       </c>
       <c r="G130" t="str">
         <f t="shared" si="7"/>
-        <v>~~, ~SPPR722~, ~Divine~, ~Quest~, ~1~, ~0~ =&gt; ~~    //Storm of Vengeance</v>
+        <v>~~, ~SPPR722~, ~Divine~, ~Q~, ~1~, ~0~ =&gt; ~~    //Storm of Vengeance</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.35">
@@ -59344,7 +59344,7 @@
         <v>939</v>
       </c>
       <c r="B131" t="s">
-        <v>1214</v>
+        <v>1399</v>
       </c>
       <c r="C131" s="19" t="s">
         <v>1183</v>
@@ -59355,11 +59355,11 @@
       </c>
       <c r="F131" t="str">
         <f t="shared" si="6"/>
-        <v>~SPPR723~, ~Divine~, ~Quest~ =&gt; ~SPPR723~    //Elemental Summoning</v>
+        <v>~SPPR723~, ~Divine~, ~Q~ =&gt; ~SPPR723~    //Elemental Summoning</v>
       </c>
       <c r="G131" t="str">
         <f t="shared" si="7"/>
-        <v>~~, ~SPPR723~, ~Divine~, ~Quest~, ~1~, ~0~ =&gt; ~~    //Elemental Summoning</v>
+        <v>~~, ~SPPR723~, ~Divine~, ~Q~, ~1~, ~0~ =&gt; ~~    //Elemental Summoning</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.35">
@@ -59367,7 +59367,7 @@
         <v>939</v>
       </c>
       <c r="B132" t="s">
-        <v>1214</v>
+        <v>1399</v>
       </c>
       <c r="C132" s="19" t="s">
         <v>1226</v>
@@ -59378,11 +59378,11 @@
       </c>
       <c r="F132" t="str">
         <f t="shared" si="6"/>
-        <v>~SPPR724~, ~Divine~, ~Quest~ =&gt; ~SPPR724~    //Greater Elemental Summoning</v>
+        <v>~SPPR724~, ~Divine~, ~Q~ =&gt; ~SPPR724~    //Greater Elemental Summoning</v>
       </c>
       <c r="G132" t="str">
         <f t="shared" si="7"/>
-        <v>~~, ~SPPR724~, ~Divine~, ~Quest~, ~1~, ~0~ =&gt; ~~    //Greater Elemental Summoning</v>
+        <v>~~, ~SPPR724~, ~Divine~, ~Q~, ~1~, ~0~ =&gt; ~~    //Greater Elemental Summoning</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.35">
@@ -59390,7 +59390,7 @@
         <v>939</v>
       </c>
       <c r="B133" t="s">
-        <v>1214</v>
+        <v>1399</v>
       </c>
       <c r="C133" s="18" t="s">
         <v>1227</v>
@@ -59400,11 +59400,11 @@
       </c>
       <c r="F133" t="str">
         <f t="shared" si="6"/>
-        <v>~SPPR725~, ~Divine~, ~Quest~ =&gt; ~SPPR725~    //Globe of Blades</v>
+        <v>~SPPR725~, ~Divine~, ~Q~ =&gt; ~SPPR725~    //Globe of Blades</v>
       </c>
       <c r="G133" t="str">
         <f t="shared" si="7"/>
-        <v>~~, ~SPPR725~, ~Divine~, ~Quest~, ~1~, ~0~ =&gt; ~~    //Globe of Blades</v>
+        <v>~~, ~SPPR725~, ~Divine~, ~Q~, ~1~, ~0~ =&gt; ~~    //Globe of Blades</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.35">
@@ -59412,7 +59412,7 @@
         <v>939</v>
       </c>
       <c r="B134" t="s">
-        <v>1214</v>
+        <v>1399</v>
       </c>
       <c r="C134" s="19" t="s">
         <v>1228</v>
@@ -59423,11 +59423,11 @@
       </c>
       <c r="F134" t="str">
         <f t="shared" si="6"/>
-        <v>~SPPR726~, ~Divine~, ~Quest~ =&gt; ~SPPR726~    //Summon Deva</v>
+        <v>~SPPR726~, ~Divine~, ~Q~ =&gt; ~SPPR726~    //Summon Deva</v>
       </c>
       <c r="G134" t="str">
         <f t="shared" si="7"/>
-        <v>~~, ~SPPR726~, ~Divine~, ~Quest~, ~1~, ~0~ =&gt; ~~    //Summon Deva</v>
+        <v>~~, ~SPPR726~, ~Divine~, ~Q~, ~1~, ~0~ =&gt; ~~    //Summon Deva</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.35">
@@ -59435,7 +59435,7 @@
         <v>939</v>
       </c>
       <c r="B135" t="s">
-        <v>1214</v>
+        <v>1399</v>
       </c>
       <c r="C135" s="19" t="s">
         <v>1229</v>
@@ -59446,11 +59446,11 @@
       </c>
       <c r="F135" t="str">
         <f t="shared" si="6"/>
-        <v>~SPPR727~, ~Divine~, ~Quest~ =&gt; ~SPPR727~    //Summon Fallen Deva</v>
+        <v>~SPPR727~, ~Divine~, ~Q~ =&gt; ~SPPR727~    //Summon Fallen Deva</v>
       </c>
       <c r="G135" t="str">
         <f t="shared" si="7"/>
-        <v>~~, ~SPPR727~, ~Divine~, ~Quest~, ~1~, ~0~ =&gt; ~~    //Summon Fallen Deva</v>
+        <v>~~, ~SPPR727~, ~Divine~, ~Q~, ~1~, ~0~ =&gt; ~~    //Summon Fallen Deva</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.35">
@@ -59458,7 +59458,7 @@
         <v>939</v>
       </c>
       <c r="B136" t="s">
-        <v>1214</v>
+        <v>1399</v>
       </c>
       <c r="C136" s="19" t="s">
         <v>1230</v>
@@ -59469,11 +59469,11 @@
       </c>
       <c r="F136" t="str">
         <f t="shared" si="6"/>
-        <v>~SPPR728~, ~Divine~, ~Quest~ =&gt; ~SPPR728~    //Implosion</v>
+        <v>~SPPR728~, ~Divine~, ~Q~ =&gt; ~SPPR728~    //Implosion</v>
       </c>
       <c r="G136" t="str">
         <f t="shared" si="7"/>
-        <v>~~, ~SPPR728~, ~Divine~, ~Quest~, ~1~, ~0~ =&gt; ~~    //Implosion</v>
+        <v>~~, ~SPPR728~, ~Divine~, ~Q~, ~1~, ~0~ =&gt; ~~    //Implosion</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.35">
@@ -59481,7 +59481,7 @@
         <v>939</v>
       </c>
       <c r="B137" t="s">
-        <v>1214</v>
+        <v>1399</v>
       </c>
       <c r="C137" s="19" t="s">
         <v>1232</v>
@@ -59492,11 +59492,11 @@
       </c>
       <c r="F137" t="str">
         <f t="shared" si="6"/>
-        <v>~SPPR730~, ~Divine~, ~Quest~ =&gt; ~SPPR730~    //Aura of Flaming Death</v>
+        <v>~SPPR730~, ~Divine~, ~Q~ =&gt; ~SPPR730~    //Aura of Flaming Death</v>
       </c>
       <c r="G137" t="str">
         <f t="shared" si="7"/>
-        <v>~~, ~SPPR730~, ~Divine~, ~Quest~, ~1~, ~0~ =&gt; ~~    //Aura of Flaming Death</v>
+        <v>~~, ~SPPR730~, ~Divine~, ~Q~, ~1~, ~0~ =&gt; ~~    //Aura of Flaming Death</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.35">
@@ -59504,7 +59504,7 @@
         <v>939</v>
       </c>
       <c r="B138" t="s">
-        <v>1214</v>
+        <v>1399</v>
       </c>
       <c r="C138" s="19" t="s">
         <v>1233</v>
@@ -59515,11 +59515,11 @@
       </c>
       <c r="F138" t="str">
         <f t="shared" si="6"/>
-        <v>~SPPR731~, ~Divine~, ~Quest~ =&gt; ~SPPR731~    //Fire Elemental Transformation</v>
+        <v>~SPPR731~, ~Divine~, ~Q~ =&gt; ~SPPR731~    //Fire Elemental Transformation</v>
       </c>
       <c r="G138" t="str">
         <f t="shared" si="7"/>
-        <v>~~, ~SPPR731~, ~Divine~, ~Quest~, ~1~, ~0~ =&gt; ~~    //Fire Elemental Transformation</v>
+        <v>~~, ~SPPR731~, ~Divine~, ~Q~, ~1~, ~0~ =&gt; ~~    //Fire Elemental Transformation</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.35">
@@ -59527,7 +59527,7 @@
         <v>939</v>
       </c>
       <c r="B139" t="s">
-        <v>1214</v>
+        <v>1399</v>
       </c>
       <c r="C139" s="19" t="s">
         <v>1234</v>
@@ -59538,11 +59538,11 @@
       </c>
       <c r="F139" t="str">
         <f t="shared" si="6"/>
-        <v>~SPPR732~, ~Divine~, ~Quest~ =&gt; ~SPPR732~    //Earth Elemental Transformation</v>
+        <v>~SPPR732~, ~Divine~, ~Q~ =&gt; ~SPPR732~    //Earth Elemental Transformation</v>
       </c>
       <c r="G139" t="str">
         <f t="shared" si="7"/>
-        <v>~~, ~SPPR732~, ~Divine~, ~Quest~, ~1~, ~0~ =&gt; ~~    //Earth Elemental Transformation</v>
+        <v>~~, ~SPPR732~, ~Divine~, ~Q~, ~1~, ~0~ =&gt; ~~    //Earth Elemental Transformation</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.35">
@@ -59550,7 +59550,7 @@
         <v>939</v>
       </c>
       <c r="B140" t="s">
-        <v>1214</v>
+        <v>1399</v>
       </c>
       <c r="C140" s="18" t="s">
         <v>1260</v>
@@ -59560,11 +59560,11 @@
       </c>
       <c r="F140" t="str">
         <f t="shared" si="6"/>
-        <v>~SPPR751~, ~Divine~, ~Quest~ =&gt; ~SPPR751~    //Ethereal Retribution</v>
+        <v>~SPPR751~, ~Divine~, ~Q~ =&gt; ~SPPR751~    //Ethereal Retribution</v>
       </c>
       <c r="G140" t="str">
         <f t="shared" si="7"/>
-        <v>~~, ~SPPR751~, ~Divine~, ~Quest~, ~1~, ~0~ =&gt; ~~    //Ethereal Retribution</v>
+        <v>~~, ~SPPR751~, ~Divine~, ~Q~, ~1~, ~0~ =&gt; ~~    //Ethereal Retribution</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Error in negative plane protection for BG1:EE
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A58BA9B-9453-4129-87FE-3106FE8E42E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097AD8EC-0A20-45DE-B8D0-FF686CDEAEE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="5" activeTab="6" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -40004,10 +40004,10 @@
   <dimension ref="A1:BB247"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="X3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="Q87" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="W18" sqref="W18:Y18"/>
+      <selection pane="bottomRight" activeCell="W99" sqref="W99:W100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -48253,7 +48253,7 @@
         <v>1</v>
       </c>
       <c r="W100" s="20" t="s">
-        <v>1091</v>
+        <v>1093</v>
       </c>
       <c r="Y100" t="s">
         <v>1196</v>
@@ -56519,8 +56519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF15ABCD-FC5C-493C-97CD-DCC4602D4EAD}">
   <dimension ref="A1:J132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H106" zoomScale="82" workbookViewId="0">
-      <selection activeCell="J122" sqref="J122"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="82" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -58456,7 +58456,7 @@
         <v>4</v>
       </c>
       <c r="C71" s="20" t="s">
-        <v>1091</v>
+        <v>1093</v>
       </c>
       <c r="E71" t="s">
         <v>1196</v>
@@ -58469,11 +58469,11 @@
       </c>
       <c r="I71" t="str">
         <f>_xlfn.CONCAT("~", C71, "~, ~", A71, "~, ~", B71, "~ =&gt; ~", C71, "~    //", E71)</f>
-        <v>~SPPR411~, ~Divine~, ~4~ =&gt; ~SPPR411~    //Negative Plane Protection</v>
+        <v>~SPPR413~, ~Divine~, ~4~ =&gt; ~SPPR413~    //Negative Plane Protection</v>
       </c>
       <c r="J71" t="str">
         <f t="shared" si="3"/>
-        <v>~BZ!E1101~, ~SPPR411~, ~Divine~, ~4~, ~1~, ~BZ!E11I~, ~0~, ~0~, ~1~, ~1~, ~0~, ~1~, ~1~, ~1~, ~1~, ~1~, ~1~, ~1~, ~1~ =&gt; ~~    //Negative Plane Protection</v>
+        <v>~BZ!E1301~, ~SPPR413~, ~Divine~, ~4~, ~1~, ~BZ!E13I~, ~0~, ~0~, ~1~, ~1~, ~0~, ~1~, ~1~, ~1~, ~1~, ~1~, ~1~, ~1~, ~1~ =&gt; ~~    //Negative Plane Protection</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Go through Core spells to identify "missing" potions
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5544EC8-2C81-494D-9C91-A5F424671D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97B3D23-7CC7-4C37-97B9-F5C6BB7DF64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9720" yWindow="0" windowWidth="9480" windowHeight="11400" firstSheet="7" activeTab="7" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -60702,7 +60702,7 @@
   <dimension ref="A1:L68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F49" workbookViewId="0">
-      <selection activeCell="L69" sqref="L69"/>
+      <selection activeCell="K65" sqref="K65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Looking at all the potions I want to make from base, IWD, Olvyn
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97B3D23-7CC7-4C37-97B9-F5C6BB7DF64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509CAE27-749A-441B-964F-E173B67B4251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9720" yWindow="0" windowWidth="9480" windowHeight="11400" firstSheet="7" activeTab="7" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="4" activeTab="7" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
   <sheets>
     <sheet name="Bullshit scroll price tinkering" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10036" uniqueCount="1585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10063" uniqueCount="1611">
   <si>
     <t>Caster Level</t>
   </si>
@@ -4788,6 +4788,84 @@
   </si>
   <si>
     <t>Champions Strength</t>
+  </si>
+  <si>
+    <t>Reflect Attack</t>
+  </si>
+  <si>
+    <t>Ghostwalk</t>
+  </si>
+  <si>
+    <t>Fly</t>
+  </si>
+  <si>
+    <t>Displacement</t>
+  </si>
+  <si>
+    <t>Legend Lore</t>
+  </si>
+  <si>
+    <t>Major Mirror Image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ghostform </t>
+  </si>
+  <si>
+    <t>Gedlee's Electric Barrier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Omnipresence </t>
+  </si>
+  <si>
+    <t>Extend Vision</t>
+  </si>
+  <si>
+    <t>Perfect Invisibility</t>
+  </si>
+  <si>
+    <t>Attain Perfection</t>
+  </si>
+  <si>
+    <t>Eclectic Recall</t>
+  </si>
+  <si>
+    <t>Mental Agility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camouflage </t>
+  </si>
+  <si>
+    <t>Snake's Swiftness</t>
+  </si>
+  <si>
+    <t>Turning Weapon</t>
+  </si>
+  <si>
+    <t>Searing Smite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ghostwalk </t>
+  </si>
+  <si>
+    <t>Wind Shots</t>
+  </si>
+  <si>
+    <t>Piercing Shots</t>
+  </si>
+  <si>
+    <t>Expose to the Elements</t>
+  </si>
+  <si>
+    <t>Sphere of Security</t>
+  </si>
+  <si>
+    <t>Antiharm Shell</t>
+  </si>
+  <si>
+    <t>Protection From Non-Silver Weapons</t>
+  </si>
+  <si>
+    <t>Colossal Growth</t>
   </si>
 </sst>
 </file>
@@ -4975,6 +5053,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4989,10 +5071,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -6090,10 +6168,10 @@
   <dimension ref="A1:AT262"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AE195" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="V2" sqref="V1:V1048576"/>
+      <selection pane="bottomRight" activeCell="AH262" sqref="AF240:AH262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6137,60 +6215,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" s="5" customFormat="1">
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25" t="s">
         <v>193</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23" t="s">
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25" t="s">
         <v>316</v>
       </c>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23" t="s">
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25" t="s">
         <v>547</v>
       </c>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23" t="s">
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25" t="s">
         <v>819</v>
       </c>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23" t="s">
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25" t="s">
         <v>833</v>
       </c>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23" t="s">
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25" t="s">
         <v>834</v>
       </c>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="23"/>
-      <c r="AD1" s="23"/>
-      <c r="AE1" s="23" t="s">
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25" t="s">
         <v>835</v>
       </c>
-      <c r="AF1" s="23"/>
-      <c r="AG1" s="23"/>
-      <c r="AH1" s="23"/>
-      <c r="AI1" s="23" t="s">
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25" t="s">
         <v>869</v>
       </c>
-      <c r="AJ1" s="23"/>
-      <c r="AK1" s="23"/>
-      <c r="AL1" s="23"/>
+      <c r="AJ1" s="25"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="25"/>
       <c r="AM1" s="11"/>
       <c r="AN1" s="11"/>
       <c r="AO1" s="11"/>
@@ -40622,76 +40700,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" s="5" customFormat="1">
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="25" t="s">
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="24" t="s">
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="26" t="s">
         <v>316</v>
       </c>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24" t="s">
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26" t="s">
         <v>547</v>
       </c>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24" t="s">
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26" t="s">
         <v>819</v>
       </c>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24" t="s">
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26" t="s">
         <v>833</v>
       </c>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="24"/>
-      <c r="AH1" s="24"/>
-      <c r="AI1" s="24" t="s">
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26" t="s">
         <v>834</v>
       </c>
-      <c r="AJ1" s="24"/>
-      <c r="AK1" s="24"/>
-      <c r="AL1" s="24" t="s">
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26" t="s">
         <v>835</v>
       </c>
-      <c r="AM1" s="24"/>
-      <c r="AN1" s="24"/>
-      <c r="AO1" s="24"/>
-      <c r="AP1" s="24"/>
-      <c r="AQ1" s="24"/>
-      <c r="AR1" s="24" t="s">
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="26" t="s">
         <v>869</v>
       </c>
-      <c r="AS1" s="24"/>
-      <c r="AT1" s="24"/>
-      <c r="AU1" s="24"/>
-      <c r="AV1" s="24"/>
-      <c r="AW1" s="24"/>
-      <c r="AX1" s="24"/>
-      <c r="AY1" s="24"/>
-      <c r="AZ1" s="24"/>
-      <c r="BA1" s="24"/>
-      <c r="BB1" s="25"/>
+      <c r="AS1" s="26"/>
+      <c r="AT1" s="26"/>
+      <c r="AU1" s="26"/>
+      <c r="AV1" s="26"/>
+      <c r="AW1" s="26"/>
+      <c r="AX1" s="26"/>
+      <c r="AY1" s="26"/>
+      <c r="AZ1" s="26"/>
+      <c r="BA1" s="26"/>
+      <c r="BB1" s="27"/>
     </row>
     <row r="2" spans="1:54">
       <c r="A2" s="4" t="s">
@@ -60699,10 +60777,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A6DB01-2873-4025-8F60-A17DF1993631}">
-  <dimension ref="A1:L68"/>
+  <dimension ref="A1:L96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F49" workbookViewId="0">
-      <selection activeCell="K65" sqref="K65"/>
+    <sheetView tabSelected="1" topLeftCell="F75" workbookViewId="0">
+      <selection activeCell="L97" sqref="L97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -60720,35 +60798,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>1404</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="23"/>
       <c r="L1" t="s">
         <v>1566</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="27" t="s">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="29" t="s">
         <v>1406</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="4" t="s">
@@ -61599,7 +61677,7 @@
       </c>
     </row>
     <row r="67" spans="1:12">
-      <c r="A67" s="29" t="s">
+      <c r="A67" s="24" t="s">
         <v>1562</v>
       </c>
       <c r="B67" t="s">
@@ -61621,6 +61699,141 @@
       </c>
       <c r="L68" t="s">
         <v>1155</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="L70" t="s">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="L71" t="s">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="L72" t="s">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="L73" t="s">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="L74" t="s">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="L75" t="s">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
+      <c r="L76" t="s">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
+      <c r="L77" t="s">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
+      <c r="L78" t="s">
+        <v>1593</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
+      <c r="L79" t="s">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
+      <c r="L80" t="s">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="81" spans="12:12">
+      <c r="L81" t="s">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="82" spans="12:12">
+      <c r="L82" t="s">
+        <v>1597</v>
+      </c>
+    </row>
+    <row r="83" spans="12:12">
+      <c r="L83" t="s">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="84" spans="12:12">
+      <c r="L84" t="s">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="85" spans="12:12">
+      <c r="L85" t="s">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="86" spans="12:12">
+      <c r="L86" t="s">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="87" spans="12:12">
+      <c r="L87" t="s">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="88" spans="12:12">
+      <c r="L88" t="s">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="89" spans="12:12">
+      <c r="L89" t="s">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="90" spans="12:12">
+      <c r="L90" t="s">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="91" spans="12:12">
+      <c r="L91" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="92" spans="12:12">
+      <c r="L92" t="s">
+        <v>1606</v>
+      </c>
+    </row>
+    <row r="93" spans="12:12">
+      <c r="L93" t="s">
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="94" spans="12:12">
+      <c r="L94" t="s">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="95" spans="12:12">
+      <c r="L95" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="96" spans="12:12">
+      <c r="L96" t="s">
+        <v>1610</v>
       </c>
     </row>
   </sheetData>
@@ -61655,32 +61868,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>1404</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="27" t="s">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="29" t="s">
         <v>1406</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="4" t="s">
@@ -61718,7 +61931,7 @@
       <c r="C10" s="2"/>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="29"/>
+      <c r="A67" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Identifying potions by game component, tradition
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509CAE27-749A-441B-964F-E173B67B4251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726C3FB0-60A6-47F0-B635-148320653562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="4" activeTab="7" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10063" uniqueCount="1611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10225" uniqueCount="1615">
   <si>
     <t>Caster Level</t>
   </si>
@@ -4866,6 +4866,18 @@
   </si>
   <si>
     <t>Colossal Growth</t>
+  </si>
+  <si>
+    <t>Mod</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>Tradition</t>
+  </si>
+  <si>
+    <t>Ovlyn</t>
   </si>
 </sst>
 </file>
@@ -60777,10 +60789,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A6DB01-2873-4025-8F60-A17DF1993631}">
-  <dimension ref="A1:L96"/>
+  <dimension ref="A1:N98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F75" workbookViewId="0">
-      <selection activeCell="L97" sqref="L97"/>
+    <sheetView tabSelected="1" topLeftCell="F68" workbookViewId="0">
+      <selection activeCell="M72" sqref="M72:M98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -60794,10 +60806,10 @@
     <col min="8" max="8" width="5.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.453125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14">
       <c r="A1" s="29" t="s">
         <v>1404</v>
       </c>
@@ -60813,8 +60825,14 @@
       <c r="L1" t="s">
         <v>1566</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" t="s">
+        <v>1611</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1613</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -60828,7 +60846,7 @@
       <c r="I2" s="29"/>
       <c r="J2" s="29"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="4" t="s">
         <v>1405</v>
       </c>
@@ -60863,7 +60881,7 @@
         <v>1567</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>1410</v>
       </c>
@@ -60876,8 +60894,14 @@
       <c r="L4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>1411</v>
       </c>
@@ -60890,8 +60914,14 @@
       <c r="L5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>1412</v>
       </c>
@@ -60904,8 +60934,14 @@
       <c r="L6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>1413</v>
       </c>
@@ -60918,8 +60954,14 @@
       <c r="L7" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>1414</v>
       </c>
@@ -60932,8 +60974,14 @@
       <c r="L8" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>1415</v>
       </c>
@@ -60946,8 +60994,14 @@
       <c r="L9" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>1416</v>
       </c>
@@ -60960,8 +61014,14 @@
       <c r="L10" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>1417</v>
       </c>
@@ -60974,8 +61034,14 @@
       <c r="L11" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>1418</v>
       </c>
@@ -60988,8 +61054,14 @@
       <c r="L12" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>1419</v>
       </c>
@@ -61002,8 +61074,14 @@
       <c r="L13" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="M13" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>1420</v>
       </c>
@@ -61016,8 +61094,14 @@
       <c r="L14" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>1421</v>
       </c>
@@ -61030,8 +61114,14 @@
       <c r="L15" t="s">
         <v>1568</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>1422</v>
       </c>
@@ -61044,8 +61134,14 @@
       <c r="L16" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>1423</v>
       </c>
@@ -61058,8 +61154,14 @@
       <c r="L17" t="s">
         <v>1569</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="M17" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>1424</v>
       </c>
@@ -61072,8 +61174,14 @@
       <c r="L18" t="s">
         <v>1570</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="M18" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>1425</v>
       </c>
@@ -61086,8 +61194,14 @@
       <c r="L19" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="M19" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>1426</v>
       </c>
@@ -61100,8 +61214,14 @@
       <c r="L20" t="s">
         <v>1571</v>
       </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="M20" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>1427</v>
       </c>
@@ -61114,8 +61234,14 @@
       <c r="L21" t="s">
         <v>1572</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="M21" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>1428</v>
       </c>
@@ -61128,8 +61254,14 @@
       <c r="L22" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="M22" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>1429</v>
       </c>
@@ -61145,8 +61277,14 @@
       <c r="L23" t="s">
         <v>1573</v>
       </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="M23" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
         <v>1430</v>
       </c>
@@ -61159,8 +61297,14 @@
       <c r="L24" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="M24" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" t="s">
         <v>1431</v>
       </c>
@@ -61176,8 +61320,14 @@
       <c r="L25" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="M25" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" t="s">
         <v>1432</v>
       </c>
@@ -61190,8 +61340,14 @@
       <c r="L26" t="s">
         <v>1574</v>
       </c>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="M26" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
         <v>1433</v>
       </c>
@@ -61207,8 +61363,14 @@
       <c r="L27" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="M27" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" t="s">
         <v>1434</v>
       </c>
@@ -61221,8 +61383,14 @@
       <c r="L28" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="M28" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
         <v>1435</v>
       </c>
@@ -61235,8 +61403,14 @@
       <c r="L29" t="s">
         <v>1575</v>
       </c>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="M29" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
         <v>1436</v>
       </c>
@@ -61249,8 +61423,14 @@
       <c r="L30" t="s">
         <v>1576</v>
       </c>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="M30" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
         <v>1437</v>
       </c>
@@ -61263,8 +61443,14 @@
       <c r="L31" t="s">
         <v>604</v>
       </c>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="M31" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" t="s">
         <v>1438</v>
       </c>
@@ -61277,8 +61463,14 @@
       <c r="L32" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="M32" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" t="s">
         <v>1439</v>
       </c>
@@ -61291,8 +61483,14 @@
       <c r="L33" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="M33" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" t="s">
         <v>1440</v>
       </c>
@@ -61308,8 +61506,14 @@
       <c r="L34" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="35" spans="1:12">
+      <c r="M34" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
         <v>1441</v>
       </c>
@@ -61322,8 +61526,14 @@
       <c r="L35" t="s">
         <v>1577</v>
       </c>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="M35" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" t="s">
         <v>1442</v>
       </c>
@@ -61336,8 +61546,14 @@
       <c r="L36" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="37" spans="1:12">
+      <c r="M36" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" t="s">
         <v>1443</v>
       </c>
@@ -61350,8 +61566,14 @@
       <c r="L37" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="38" spans="1:12">
+      <c r="M37" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N37" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
         <v>1444</v>
       </c>
@@ -61364,8 +61586,14 @@
       <c r="L38" t="s">
         <v>1578</v>
       </c>
-    </row>
-    <row r="39" spans="1:12">
+      <c r="M38" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
         <v>1445</v>
       </c>
@@ -61378,8 +61606,14 @@
       <c r="L39" t="s">
         <v>1579</v>
       </c>
-    </row>
-    <row r="40" spans="1:12">
+      <c r="M39" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" t="s">
         <v>1446</v>
       </c>
@@ -61392,8 +61626,14 @@
       <c r="L40" t="s">
         <v>1580</v>
       </c>
-    </row>
-    <row r="41" spans="1:12">
+      <c r="M40" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N40" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
         <v>1447</v>
       </c>
@@ -61406,8 +61646,14 @@
       <c r="L41" t="s">
         <v>940</v>
       </c>
-    </row>
-    <row r="42" spans="1:12">
+      <c r="M41" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N41" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
         <v>1448</v>
       </c>
@@ -61423,8 +61669,14 @@
       <c r="L42" t="s">
         <v>946</v>
       </c>
-    </row>
-    <row r="43" spans="1:12">
+      <c r="M42" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N42" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
       <c r="A43" t="s">
         <v>1449</v>
       </c>
@@ -61437,8 +61689,14 @@
       <c r="L43" t="s">
         <v>1188</v>
       </c>
-    </row>
-    <row r="44" spans="1:12">
+      <c r="M43" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N43" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
       <c r="A44" t="s">
         <v>1450</v>
       </c>
@@ -61451,8 +61709,14 @@
       <c r="L44" t="s">
         <v>957</v>
       </c>
-    </row>
-    <row r="45" spans="1:12">
+      <c r="M44" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N44" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
       <c r="A45" t="s">
         <v>1451</v>
       </c>
@@ -61465,8 +61729,14 @@
       <c r="L45" t="s">
         <v>960</v>
       </c>
-    </row>
-    <row r="46" spans="1:12">
+      <c r="M45" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N45" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
       <c r="A46" t="s">
         <v>1452</v>
       </c>
@@ -61479,8 +61749,14 @@
       <c r="L46" t="s">
         <v>1267</v>
       </c>
-    </row>
-    <row r="47" spans="1:12">
+      <c r="M46" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N46" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
       <c r="A47" t="s">
         <v>1453</v>
       </c>
@@ -61493,8 +61769,14 @@
       <c r="L47" t="s">
         <v>968</v>
       </c>
-    </row>
-    <row r="48" spans="1:12">
+      <c r="M47" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N47" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
       <c r="A48" t="s">
         <v>1454</v>
       </c>
@@ -61507,8 +61789,14 @@
       <c r="L48" t="s">
         <v>1316</v>
       </c>
-    </row>
-    <row r="49" spans="1:12">
+      <c r="M48" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N48" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
       <c r="A49" t="s">
         <v>1455</v>
       </c>
@@ -61521,8 +61809,14 @@
       <c r="L49" t="s">
         <v>1581</v>
       </c>
-    </row>
-    <row r="50" spans="1:12">
+      <c r="M49" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N49" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
       <c r="A50" t="s">
         <v>1456</v>
       </c>
@@ -61535,32 +61829,56 @@
       <c r="L50" t="s">
         <v>1193</v>
       </c>
-    </row>
-    <row r="51" spans="1:12">
+      <c r="M50" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N50" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
       <c r="A51" t="s">
         <v>1457</v>
       </c>
       <c r="L51" t="s">
         <v>1196</v>
       </c>
-    </row>
-    <row r="52" spans="1:12">
+      <c r="M51" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N51" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
       <c r="A52" t="s">
         <v>1458</v>
       </c>
       <c r="L52" t="s">
         <v>1081</v>
       </c>
-    </row>
-    <row r="53" spans="1:12">
+      <c r="M52" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N52" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
       <c r="A53" t="s">
         <v>1459</v>
       </c>
       <c r="L53" t="s">
         <v>1109</v>
       </c>
-    </row>
-    <row r="54" spans="1:12">
+      <c r="M53" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N53" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
       <c r="A54" t="s">
         <v>1460</v>
       </c>
@@ -61573,24 +61891,42 @@
       <c r="L54" t="s">
         <v>1128</v>
       </c>
-    </row>
-    <row r="55" spans="1:12">
+      <c r="M54" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N54" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
       <c r="A55" t="s">
         <v>1508</v>
       </c>
       <c r="L55" t="s">
         <v>1132</v>
       </c>
-    </row>
-    <row r="56" spans="1:12">
+      <c r="M55" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N55" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
       <c r="A56" t="s">
         <v>1509</v>
       </c>
       <c r="L56" t="s">
         <v>1207</v>
       </c>
-    </row>
-    <row r="57" spans="1:12">
+      <c r="M56" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N56" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
       <c r="A57" t="s">
         <v>1510</v>
       </c>
@@ -61603,40 +61939,61 @@
       <c r="L57" t="s">
         <v>1582</v>
       </c>
-    </row>
-    <row r="58" spans="1:12">
+      <c r="M57" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N57" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
       <c r="A58" t="s">
         <v>1511</v>
       </c>
       <c r="L58" t="s">
         <v>1583</v>
       </c>
-    </row>
-    <row r="59" spans="1:12">
+      <c r="M58" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N58" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
       <c r="A59" t="s">
         <v>1512</v>
       </c>
       <c r="L59" t="s">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12">
+        <v>1197</v>
+      </c>
+      <c r="M59" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N59" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
       <c r="A60" t="s">
         <v>1513</v>
       </c>
       <c r="L60" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12">
+        <v>9</v>
+      </c>
+      <c r="M60" t="s">
+        <v>1612</v>
+      </c>
+      <c r="N60" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
       <c r="A61" t="s">
         <v>1514</v>
       </c>
-      <c r="L61" t="s">
-        <v>1271</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12">
+    </row>
+    <row r="62" spans="1:14">
       <c r="A62" t="s">
         <v>1515</v>
       </c>
@@ -61647,25 +62004,49 @@
         <v>1561</v>
       </c>
       <c r="L62" t="s">
-        <v>1197</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12">
+        <v>1045</v>
+      </c>
+      <c r="M62" t="s">
+        <v>1408</v>
+      </c>
+      <c r="N62" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
       <c r="L63" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12">
+        <v>1043</v>
+      </c>
+      <c r="M63" t="s">
+        <v>1408</v>
+      </c>
+      <c r="N63" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
       <c r="L64" t="s">
-        <v>1584</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12">
+        <v>1046</v>
+      </c>
+      <c r="M64" t="s">
+        <v>1408</v>
+      </c>
+      <c r="N64" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14">
       <c r="L65" t="s">
-        <v>1199</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12">
+        <v>1271</v>
+      </c>
+      <c r="M65" t="s">
+        <v>1408</v>
+      </c>
+      <c r="N65" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14">
       <c r="A66" t="s">
         <v>1519</v>
       </c>
@@ -61673,10 +62054,16 @@
         <v>1518</v>
       </c>
       <c r="L66" t="s">
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12">
+        <v>1584</v>
+      </c>
+      <c r="M66" t="s">
+        <v>1408</v>
+      </c>
+      <c r="N66" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14">
       <c r="A67" s="24" t="s">
         <v>1562</v>
       </c>
@@ -61687,10 +62074,16 @@
         <v>1051</v>
       </c>
       <c r="L67" t="s">
-        <v>1108</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12">
+        <v>1199</v>
+      </c>
+      <c r="M67" t="s">
+        <v>1408</v>
+      </c>
+      <c r="N67" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14">
       <c r="A68" t="s">
         <v>1564</v>
       </c>
@@ -61698,142 +62091,251 @@
         <v>1565</v>
       </c>
       <c r="L68" t="s">
+        <v>1105</v>
+      </c>
+      <c r="M68" t="s">
+        <v>1408</v>
+      </c>
+      <c r="N68" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14">
+      <c r="L69" t="s">
+        <v>1108</v>
+      </c>
+      <c r="M69" t="s">
+        <v>1408</v>
+      </c>
+      <c r="N69" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14">
+      <c r="L70" t="s">
         <v>1155</v>
       </c>
-    </row>
-    <row r="70" spans="1:12">
-      <c r="L70" t="s">
+      <c r="M70" t="s">
+        <v>1408</v>
+      </c>
+      <c r="N70" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14">
+      <c r="L72" t="s">
         <v>1585</v>
       </c>
-    </row>
-    <row r="71" spans="1:12">
-      <c r="L71" t="s">
+      <c r="M72" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14">
+      <c r="L73" t="s">
         <v>1586</v>
       </c>
-    </row>
-    <row r="72" spans="1:12">
-      <c r="L72" t="s">
+      <c r="M73" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14">
+      <c r="L74" t="s">
         <v>1587</v>
       </c>
-    </row>
-    <row r="73" spans="1:12">
-      <c r="L73" t="s">
+      <c r="M74" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14">
+      <c r="L75" t="s">
         <v>1588</v>
       </c>
-    </row>
-    <row r="74" spans="1:12">
-      <c r="L74" t="s">
+      <c r="M75" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14">
+      <c r="L76" t="s">
         <v>1589</v>
       </c>
-    </row>
-    <row r="75" spans="1:12">
-      <c r="L75" t="s">
+      <c r="M76" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14">
+      <c r="L77" t="s">
         <v>1590</v>
       </c>
-    </row>
-    <row r="76" spans="1:12">
-      <c r="L76" t="s">
+      <c r="M77" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14">
+      <c r="L78" t="s">
         <v>1591</v>
       </c>
-    </row>
-    <row r="77" spans="1:12">
-      <c r="L77" t="s">
+      <c r="M78" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14">
+      <c r="L79" t="s">
         <v>1592</v>
       </c>
-    </row>
-    <row r="78" spans="1:12">
-      <c r="L78" t="s">
+      <c r="M79" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14">
+      <c r="L80" t="s">
         <v>1593</v>
       </c>
-    </row>
-    <row r="79" spans="1:12">
-      <c r="L79" t="s">
+      <c r="M80" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="81" spans="12:13">
+      <c r="L81" t="s">
         <v>1594</v>
       </c>
-    </row>
-    <row r="80" spans="1:12">
-      <c r="L80" t="s">
+      <c r="M81" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="82" spans="12:13">
+      <c r="L82" t="s">
         <v>1595</v>
       </c>
-    </row>
-    <row r="81" spans="12:12">
-      <c r="L81" t="s">
+      <c r="M82" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="83" spans="12:13">
+      <c r="L83" t="s">
         <v>1596</v>
       </c>
-    </row>
-    <row r="82" spans="12:12">
-      <c r="L82" t="s">
+      <c r="M83" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="84" spans="12:13">
+      <c r="L84" t="s">
         <v>1597</v>
       </c>
-    </row>
-    <row r="83" spans="12:12">
-      <c r="L83" t="s">
+      <c r="M84" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="85" spans="12:13">
+      <c r="L85" t="s">
         <v>1598</v>
       </c>
-    </row>
-    <row r="84" spans="12:12">
-      <c r="L84" t="s">
+      <c r="M85" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="86" spans="12:13">
+      <c r="L86" t="s">
         <v>1599</v>
       </c>
-    </row>
-    <row r="85" spans="12:12">
-      <c r="L85" t="s">
+      <c r="M86" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="87" spans="12:13">
+      <c r="L87" t="s">
         <v>1600</v>
       </c>
-    </row>
-    <row r="86" spans="12:12">
-      <c r="L86" t="s">
+      <c r="M87" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="88" spans="12:13">
+      <c r="L88" t="s">
         <v>1601</v>
       </c>
-    </row>
-    <row r="87" spans="12:12">
-      <c r="L87" t="s">
+      <c r="M88" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="89" spans="12:13">
+      <c r="L89" t="s">
         <v>1602</v>
       </c>
-    </row>
-    <row r="88" spans="12:12">
-      <c r="L88" t="s">
+      <c r="M89" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="90" spans="12:13">
+      <c r="L90" t="s">
         <v>1603</v>
       </c>
-    </row>
-    <row r="89" spans="12:12">
-      <c r="L89" t="s">
+      <c r="M90" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="91" spans="12:13">
+      <c r="L91" t="s">
         <v>1604</v>
       </c>
-    </row>
-    <row r="90" spans="12:12">
-      <c r="L90" t="s">
+      <c r="M91" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="92" spans="12:13">
+      <c r="L92" t="s">
         <v>1605</v>
       </c>
-    </row>
-    <row r="91" spans="12:12">
-      <c r="L91" t="s">
+      <c r="M92" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="93" spans="12:13">
+      <c r="L93" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="92" spans="12:12">
-      <c r="L92" t="s">
+      <c r="M93" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="94" spans="12:13">
+      <c r="L94" t="s">
         <v>1606</v>
       </c>
-    </row>
-    <row r="93" spans="12:12">
-      <c r="L93" t="s">
+      <c r="M94" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="95" spans="12:13">
+      <c r="L95" t="s">
         <v>1607</v>
       </c>
-    </row>
-    <row r="94" spans="12:12">
-      <c r="L94" t="s">
+      <c r="M95" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="96" spans="12:13">
+      <c r="L96" t="s">
         <v>1608</v>
       </c>
-    </row>
-    <row r="95" spans="12:12">
-      <c r="L95" t="s">
+      <c r="M96" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="97" spans="12:13">
+      <c r="L97" t="s">
         <v>1609</v>
       </c>
-    </row>
-    <row r="96" spans="12:12">
-      <c r="L96" t="s">
+      <c r="M97" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="98" spans="12:13">
+      <c r="L98" t="s">
         <v>1610</v>
+      </c>
+      <c r="M98" t="s">
+        <v>1614</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Roughing in spell recipes for brewing potions
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726C3FB0-60A6-47F0-B635-148320653562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E23141-8C33-447F-A9D9-9FB305A64F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="4" activeTab="7" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10225" uniqueCount="1615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10280" uniqueCount="1652">
   <si>
     <t>Caster Level</t>
   </si>
@@ -4878,6 +4878,117 @@
   </si>
   <si>
     <t>Ovlyn</t>
+  </si>
+  <si>
+    <t>Protection from fire, etc.</t>
+  </si>
+  <si>
+    <t>Cure light wounds</t>
+  </si>
+  <si>
+    <t>Cure Disease/Cure Medium wounds</t>
+  </si>
+  <si>
+    <t>A's Scorcher</t>
+  </si>
+  <si>
+    <t>Protection from Electricity, others</t>
+  </si>
+  <si>
+    <t>Cure Critical Wounds + Cure Serious</t>
+  </si>
+  <si>
+    <t>Champion's Strength + level</t>
+  </si>
+  <si>
+    <t>Magic resistance + level (20)</t>
+  </si>
+  <si>
+    <t>Find Traps + Knock + Luck</t>
+  </si>
+  <si>
+    <t>Mage Armor + Spirit Armor + Ghost Armor</t>
+  </si>
+  <si>
+    <t>Champion's Strength + level + cause disease + Contagion</t>
+  </si>
+  <si>
+    <t>Magic resistance + Ray of enfeeblement + rigid thinking + champions strength + confusion + feeblemind</t>
+  </si>
+  <si>
+    <t>Detect Illusion + True Sight</t>
+  </si>
+  <si>
+    <t>Protection from Petrification + Stone to Flesh</t>
+  </si>
+  <si>
+    <t>Saves +3/DEX -3</t>
+  </si>
+  <si>
+    <t>Stoneskin + Emotion</t>
+  </si>
+  <si>
+    <t>Cat's Grace * or Draw Upon Holy Might</t>
+  </si>
+  <si>
+    <t>Trollish Fortitude * or Draw Upon Holy Might</t>
+  </si>
+  <si>
+    <t>Fox's Cunning*</t>
+  </si>
+  <si>
+    <t>Burning hands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Draw Upon Holy Might + </t>
+  </si>
+  <si>
+    <t>; DUHM + level; DUHM</t>
+  </si>
+  <si>
+    <t>; DUHMh + level; DUHM</t>
+  </si>
+  <si>
+    <t>; DUHM; DUHM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stength or Chamption's Strength or </t>
+  </si>
+  <si>
+    <t>Shield + prtoection from (magical) energy</t>
+  </si>
+  <si>
+    <t>Aid / Knock / Find Traps / Bless</t>
+  </si>
+  <si>
+    <t>Rogue's Potion of Frost Giant</t>
+  </si>
+  <si>
+    <t>protection from normal weapons; Armor of faith; protect elec</t>
+  </si>
+  <si>
+    <t>WAND16</t>
+  </si>
+  <si>
+    <t>Potion of Icedust</t>
+  </si>
+  <si>
+    <t>Prot. Fire</t>
+  </si>
+  <si>
+    <t>OHDPotn1</t>
+  </si>
+  <si>
+    <t>Potion of clairvoyance</t>
+  </si>
+  <si>
+    <t>See invisible</t>
+  </si>
+  <si>
+    <t>Detect Invisible; true seeing; invisibility purge</t>
+  </si>
+  <si>
+    <t>Chant; Barkskin!</t>
   </si>
 </sst>
 </file>
@@ -4964,7 +5075,7 @@
       <name val="Monospaced"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4989,6 +5100,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -5037,7 +5160,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -5084,6 +5207,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent2" xfId="4" builtinId="33"/>
@@ -60791,16 +60916,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A6DB01-2873-4025-8F60-A17DF1993631}">
   <dimension ref="A1:N98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F68" workbookViewId="0">
-      <selection activeCell="M72" sqref="M72:M98"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.54296875" customWidth="1"/>
     <col min="5" max="5" width="8.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="4.90625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.1796875" bestFit="1" customWidth="1"/>
@@ -60891,6 +61016,9 @@
       <c r="C4" t="s">
         <v>1520</v>
       </c>
+      <c r="D4" t="s">
+        <v>1615</v>
+      </c>
       <c r="L4" t="s">
         <v>19</v>
       </c>
@@ -60911,6 +61039,9 @@
       <c r="C5" t="s">
         <v>1521</v>
       </c>
+      <c r="D5" t="s">
+        <v>1636</v>
+      </c>
       <c r="L5" t="s">
         <v>38</v>
       </c>
@@ -60931,6 +61062,9 @@
       <c r="C6" t="s">
         <v>1522</v>
       </c>
+      <c r="D6" t="s">
+        <v>1636</v>
+      </c>
       <c r="L6" t="s">
         <v>43</v>
       </c>
@@ -60951,6 +61085,9 @@
       <c r="C7" t="s">
         <v>1523</v>
       </c>
+      <c r="D7" t="s">
+        <v>1636</v>
+      </c>
       <c r="L7" t="s">
         <v>49</v>
       </c>
@@ -60971,6 +61108,9 @@
       <c r="C8" t="s">
         <v>1524</v>
       </c>
+      <c r="D8" t="s">
+        <v>1637</v>
+      </c>
       <c r="L8" t="s">
         <v>52</v>
       </c>
@@ -60991,6 +61131,9 @@
       <c r="C9" t="s">
         <v>1525</v>
       </c>
+      <c r="D9" t="s">
+        <v>1638</v>
+      </c>
       <c r="L9" t="s">
         <v>77</v>
       </c>
@@ -61011,6 +61154,9 @@
       <c r="C10" s="2" t="s">
         <v>1527</v>
       </c>
+      <c r="D10" t="s">
+        <v>1616</v>
+      </c>
       <c r="L10" t="s">
         <v>84</v>
       </c>
@@ -61031,6 +61177,9 @@
       <c r="C11" t="s">
         <v>1528</v>
       </c>
+      <c r="D11" t="s">
+        <v>315</v>
+      </c>
       <c r="L11" t="s">
         <v>85</v>
       </c>
@@ -61051,6 +61200,9 @@
       <c r="C12" t="s">
         <v>81</v>
       </c>
+      <c r="D12" t="s">
+        <v>81</v>
+      </c>
       <c r="L12" t="s">
         <v>87</v>
       </c>
@@ -61071,6 +61223,9 @@
       <c r="C13" t="s">
         <v>1529</v>
       </c>
+      <c r="D13" t="s">
+        <v>1651</v>
+      </c>
       <c r="L13" t="s">
         <v>92</v>
       </c>
@@ -61091,6 +61246,9 @@
       <c r="C14" t="s">
         <v>1526</v>
       </c>
+      <c r="D14" t="s">
+        <v>1621</v>
+      </c>
       <c r="L14" t="s">
         <v>93</v>
       </c>
@@ -61111,6 +61269,9 @@
       <c r="C15" t="s">
         <v>113</v>
       </c>
+      <c r="D15" t="s">
+        <v>113</v>
+      </c>
       <c r="L15" t="s">
         <v>1568</v>
       </c>
@@ -61131,6 +61292,9 @@
       <c r="C16" t="s">
         <v>114</v>
       </c>
+      <c r="D16" t="s">
+        <v>114</v>
+      </c>
       <c r="L16" t="s">
         <v>125</v>
       </c>
@@ -61151,6 +61315,9 @@
       <c r="C17" t="s">
         <v>1530</v>
       </c>
+      <c r="D17" t="s">
+        <v>1626</v>
+      </c>
       <c r="L17" t="s">
         <v>1569</v>
       </c>
@@ -61171,6 +61338,9 @@
       <c r="C18" t="s">
         <v>1530</v>
       </c>
+      <c r="D18" t="s">
+        <v>1625</v>
+      </c>
       <c r="L18" t="s">
         <v>1570</v>
       </c>
@@ -61191,6 +61361,9 @@
       <c r="C19" t="s">
         <v>1531</v>
       </c>
+      <c r="D19" t="s">
+        <v>1617</v>
+      </c>
       <c r="L19" t="s">
         <v>145</v>
       </c>
@@ -61211,6 +61384,9 @@
       <c r="C20" t="s">
         <v>1532</v>
       </c>
+      <c r="D20" t="s">
+        <v>1643</v>
+      </c>
       <c r="L20" t="s">
         <v>1571</v>
       </c>
@@ -61231,6 +61407,9 @@
       <c r="C21" t="s">
         <v>1533</v>
       </c>
+      <c r="D21" s="31" t="s">
+        <v>1631</v>
+      </c>
       <c r="L21" t="s">
         <v>1572</v>
       </c>
@@ -61251,6 +61430,9 @@
       <c r="C22" t="s">
         <v>1534</v>
       </c>
+      <c r="D22" t="s">
+        <v>1007</v>
+      </c>
       <c r="L22" t="s">
         <v>149</v>
       </c>
@@ -61294,6 +61476,9 @@
       <c r="C24" t="s">
         <v>1536</v>
       </c>
+      <c r="D24" t="s">
+        <v>563</v>
+      </c>
       <c r="L24" t="s">
         <v>153</v>
       </c>
@@ -61337,6 +61522,9 @@
       <c r="C26" t="s">
         <v>1538</v>
       </c>
+      <c r="D26" t="s">
+        <v>1624</v>
+      </c>
       <c r="L26" t="s">
         <v>1574</v>
       </c>
@@ -61380,6 +61568,9 @@
       <c r="C28" t="s">
         <v>113</v>
       </c>
+      <c r="D28" t="s">
+        <v>113</v>
+      </c>
       <c r="L28" t="s">
         <v>600</v>
       </c>
@@ -61400,6 +61591,9 @@
       <c r="C29" t="s">
         <v>1540</v>
       </c>
+      <c r="D29" t="s">
+        <v>1618</v>
+      </c>
       <c r="L29" t="s">
         <v>1575</v>
       </c>
@@ -61420,6 +61614,9 @@
       <c r="C30" t="s">
         <v>1541</v>
       </c>
+      <c r="D30" s="31" t="s">
+        <v>1632</v>
+      </c>
       <c r="L30" t="s">
         <v>1576</v>
       </c>
@@ -61440,6 +61637,9 @@
       <c r="C31" t="s">
         <v>1542</v>
       </c>
+      <c r="D31" s="30" t="s">
+        <v>1633</v>
+      </c>
       <c r="L31" t="s">
         <v>604</v>
       </c>
@@ -61460,6 +61660,9 @@
       <c r="C32" t="s">
         <v>46</v>
       </c>
+      <c r="D32" t="s">
+        <v>46</v>
+      </c>
       <c r="L32" t="s">
         <v>606</v>
       </c>
@@ -61480,6 +61683,9 @@
       <c r="C33" t="s">
         <v>1543</v>
       </c>
+      <c r="D33" t="s">
+        <v>1619</v>
+      </c>
       <c r="L33" t="s">
         <v>608</v>
       </c>
@@ -61523,6 +61729,9 @@
       <c r="C35" t="s">
         <v>1545</v>
       </c>
+      <c r="D35" t="s">
+        <v>190</v>
+      </c>
       <c r="L35" t="s">
         <v>1577</v>
       </c>
@@ -61543,6 +61752,9 @@
       <c r="C36" t="s">
         <v>1544</v>
       </c>
+      <c r="D36" t="s">
+        <v>1622</v>
+      </c>
       <c r="L36" t="s">
         <v>636</v>
       </c>
@@ -61563,6 +61775,9 @@
       <c r="C37" t="s">
         <v>1546</v>
       </c>
+      <c r="D37" t="s">
+        <v>1640</v>
+      </c>
       <c r="L37" t="s">
         <v>660</v>
       </c>
@@ -61583,6 +61798,9 @@
       <c r="C38" t="s">
         <v>1547</v>
       </c>
+      <c r="D38" t="s">
+        <v>1623</v>
+      </c>
       <c r="L38" t="s">
         <v>1578</v>
       </c>
@@ -61603,6 +61821,9 @@
       <c r="C39" t="s">
         <v>1548</v>
       </c>
+      <c r="D39" t="s">
+        <v>1635</v>
+      </c>
       <c r="L39" t="s">
         <v>1579</v>
       </c>
@@ -61623,6 +61844,9 @@
       <c r="C40" t="s">
         <v>1549</v>
       </c>
+      <c r="D40" t="s">
+        <v>1628</v>
+      </c>
       <c r="L40" t="s">
         <v>1580</v>
       </c>
@@ -61643,6 +61867,9 @@
       <c r="C41" t="s">
         <v>1550</v>
       </c>
+      <c r="D41" t="s">
+        <v>84</v>
+      </c>
       <c r="L41" t="s">
         <v>940</v>
       </c>
@@ -61686,6 +61913,9 @@
       <c r="C43" t="s">
         <v>1552</v>
       </c>
+      <c r="D43" t="s">
+        <v>1641</v>
+      </c>
       <c r="L43" t="s">
         <v>1188</v>
       </c>
@@ -61706,6 +61936,9 @@
       <c r="C44" t="s">
         <v>1553</v>
       </c>
+      <c r="D44" t="s">
+        <v>1213</v>
+      </c>
       <c r="L44" t="s">
         <v>957</v>
       </c>
@@ -61726,6 +61959,9 @@
       <c r="C45" t="s">
         <v>1554</v>
       </c>
+      <c r="D45" t="s">
+        <v>1627</v>
+      </c>
       <c r="L45" t="s">
         <v>960</v>
       </c>
@@ -61746,6 +61982,9 @@
       <c r="C46" t="s">
         <v>1555</v>
       </c>
+      <c r="D46" t="s">
+        <v>1639</v>
+      </c>
       <c r="L46" t="s">
         <v>1267</v>
       </c>
@@ -61766,6 +62005,9 @@
       <c r="C47" t="s">
         <v>1556</v>
       </c>
+      <c r="D47" t="s">
+        <v>1333</v>
+      </c>
       <c r="L47" t="s">
         <v>968</v>
       </c>
@@ -61784,7 +62026,10 @@
         <v>1504</v>
       </c>
       <c r="C48" t="s">
-        <v>1530</v>
+        <v>1629</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1630</v>
       </c>
       <c r="L48" t="s">
         <v>1316</v>
@@ -61800,10 +62045,10 @@
       <c r="A49" t="s">
         <v>1455</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="30" t="s">
         <v>1505</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="30" t="s">
         <v>1557</v>
       </c>
       <c r="L49" t="s">
@@ -61820,11 +62065,14 @@
       <c r="A50" t="s">
         <v>1456</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="30" t="s">
         <v>1506</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="30" t="s">
         <v>1558</v>
+      </c>
+      <c r="E50" t="b">
+        <v>1</v>
       </c>
       <c r="L50" t="s">
         <v>1193</v>
@@ -61888,6 +62136,9 @@
       <c r="C54" t="s">
         <v>1559</v>
       </c>
+      <c r="D54" t="s">
+        <v>1020</v>
+      </c>
       <c r="L54" t="s">
         <v>1128</v>
       </c>
@@ -61936,6 +62187,9 @@
       <c r="C57" t="s">
         <v>1560</v>
       </c>
+      <c r="D57" t="s">
+        <v>1620</v>
+      </c>
       <c r="L57" t="s">
         <v>1582</v>
       </c>
@@ -61950,6 +62204,12 @@
       <c r="A58" t="s">
         <v>1511</v>
       </c>
+      <c r="B58" s="30" t="s">
+        <v>1642</v>
+      </c>
+      <c r="C58" s="30" t="s">
+        <v>1522</v>
+      </c>
       <c r="L58" t="s">
         <v>1583</v>
       </c>
@@ -62003,6 +62263,9 @@
       <c r="C62" t="s">
         <v>1561</v>
       </c>
+      <c r="D62" t="s">
+        <v>43</v>
+      </c>
       <c r="L62" t="s">
         <v>1045</v>
       </c>
@@ -62014,6 +62277,15 @@
       </c>
     </row>
     <row r="63" spans="1:14">
+      <c r="A63" t="s">
+        <v>1644</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1646</v>
+      </c>
       <c r="L63" t="s">
         <v>1043</v>
       </c>
@@ -62025,6 +62297,18 @@
       </c>
     </row>
     <row r="64" spans="1:14">
+      <c r="A64" t="s">
+        <v>1647</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1648</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1649</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1650</v>
+      </c>
       <c r="L64" t="s">
         <v>1046</v>
       </c>
@@ -62053,6 +62337,9 @@
       <c r="B66" t="s">
         <v>1518</v>
       </c>
+      <c r="D66" t="s">
+        <v>42</v>
+      </c>
       <c r="L66" t="s">
         <v>1584</v>
       </c>
@@ -62073,6 +62360,9 @@
       <c r="C67" t="s">
         <v>1051</v>
       </c>
+      <c r="D67" t="s">
+        <v>1051</v>
+      </c>
       <c r="L67" t="s">
         <v>1199</v>
       </c>
@@ -62089,6 +62379,9 @@
       </c>
       <c r="B68" t="s">
         <v>1565</v>
+      </c>
+      <c r="D68" t="s">
+        <v>1634</v>
       </c>
       <c r="L68" t="s">
         <v>1105</v>

</xml_diff>

<commit_message>
Initial potion recipes for base game
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBE965A-1E7F-473C-98BC-FD8A21DEC913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79382A69-A65F-4DA8-B98F-D59DD7907F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="6" activeTab="7" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="6" activeTab="9" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
   <sheets>
     <sheet name="Bullshit scroll price tinkering" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="25" r:id="rId13"/>
+    <pivotCache cacheId="29" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10416" uniqueCount="1679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10419" uniqueCount="1679">
   <si>
     <t>Caster Level</t>
   </si>
@@ -5323,13 +5323,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Bardez" refreshedDate="45244.406474421296" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="47" xr:uid="{A926483A-2931-4F10-ADCD-E1C45E8F4C10}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Bardez" refreshedDate="45244.429949537036" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="47" xr:uid="{A926483A-2931-4F10-ADCD-E1C45E8F4C10}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:B123" sheet="Spell Boosts"/>
   </cacheSource>
   <cacheFields count="2">
     <cacheField name="Spell" numFmtId="0">
-      <sharedItems containsBlank="1" count="24">
+      <sharedItems containsBlank="1" count="25">
         <s v="Bless"/>
         <s v="Armor of faith"/>
         <s v="Aid"/>
@@ -5340,6 +5340,7 @@
         <s v="Holy Power"/>
         <s v="Champion's Strength"/>
         <s v="Righteous Magic"/>
+        <s v="Magic Resistance"/>
         <m/>
         <s v="Armor"/>
         <s v="Friends"/>
@@ -5369,10 +5370,10 @@
         <s v="DEX +X"/>
         <s v="CON +X"/>
         <s v="Thac0 bonus"/>
+        <s v="MR +X%"/>
         <m/>
         <s v="CHA +X"/>
         <s v="Thieving skills +5%"/>
-        <s v="MR +X%"/>
         <s v="CR + X%"/>
         <s v="FR + X%"/>
       </sharedItems>
@@ -5489,126 +5490,127 @@
     <x v="11"/>
   </r>
   <r>
-    <x v="10"/>
+    <x v="11"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="14"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="17"/>
     <x v="11"/>
   </r>
   <r>
+    <x v="18"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <x v="16"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="22"/>
     <x v="10"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="23"/>
     <x v="11"/>
   </r>
   <r>
     <x v="11"/>
-    <x v="5"/>
-  </r>
-  <r>
     <x v="12"/>
-    <x v="12"/>
-  </r>
-  <r>
-    <x v="13"/>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="14"/>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="14"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="14"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="14"/>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="15"/>
-    <x v="7"/>
-  </r>
-  <r>
-    <x v="16"/>
-    <x v="14"/>
-  </r>
-  <r>
-    <x v="17"/>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="18"/>
-    <x v="15"/>
-  </r>
-  <r>
-    <x v="19"/>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="20"/>
-    <x v="16"/>
-  </r>
-  <r>
-    <x v="21"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="21"/>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="21"/>
-    <x v="10"/>
-  </r>
-  <r>
-    <x v="21"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="21"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="22"/>
-    <x v="14"/>
-  </r>
-  <r>
-    <x v="10"/>
-    <x v="11"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F3C0FD81-EC5D-4C31-9DDA-F8F6B464BBF6}" name="PivotTable1" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:R27" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F3C0FD81-EC5D-4C31-9DDA-F8F6B464BBF6}" name="PivotTable1" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:R28" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="25">
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="26">
         <item x="2"/>
-        <item x="11"/>
+        <item x="12"/>
         <item x="1"/>
         <item x="3"/>
         <item x="0"/>
         <item x="8"/>
         <item x="4"/>
         <item x="5"/>
+        <item x="19"/>
+        <item x="21"/>
+        <item x="13"/>
         <item x="18"/>
+        <item x="7"/>
+        <item x="15"/>
+        <item x="10"/>
+        <item x="23"/>
+        <item m="1" x="24"/>
+        <item x="9"/>
+        <item x="14"/>
         <item x="20"/>
-        <item x="12"/>
+        <item x="16"/>
+        <item x="6"/>
+        <item x="22"/>
         <item x="17"/>
-        <item x="7"/>
-        <item x="14"/>
-        <item x="9"/>
-        <item x="13"/>
-        <item x="19"/>
-        <item x="15"/>
-        <item x="6"/>
-        <item x="21"/>
-        <item x="16"/>
-        <item h="1" x="10"/>
-        <item m="1" x="23"/>
-        <item x="22"/>
+        <item h="1" x="11"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -5616,21 +5618,21 @@
       <items count="18">
         <item x="4"/>
         <item x="5"/>
-        <item x="12"/>
+        <item x="13"/>
         <item x="3"/>
         <item x="6"/>
         <item x="7"/>
-        <item h="1" x="11"/>
+        <item h="1" x="12"/>
         <item x="0"/>
         <item x="1"/>
-        <item x="14"/>
+        <item x="11"/>
         <item x="15"/>
         <item x="16"/>
         <item x="2"/>
         <item x="8"/>
         <item x="9"/>
         <item x="10"/>
-        <item x="13"/>
+        <item x="14"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -5638,7 +5640,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="23">
+  <rowItems count="24">
     <i>
       <x/>
     </i>
@@ -5688,9 +5690,6 @@
       <x v="15"/>
     </i>
     <i>
-      <x v="16"/>
-    </i>
-    <i>
       <x v="17"/>
     </i>
     <i>
@@ -5701,6 +5700,12 @@
     </i>
     <i>
       <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
     </i>
     <i>
       <x v="23"/>
@@ -6854,8 +6859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A6DB01-2873-4025-8F60-A17DF1993631}">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6952,6 +6957,9 @@
       </c>
     </row>
     <row r="5" spans="1:11">
+      <c r="A5" t="b">
+        <v>1</v>
+      </c>
       <c r="B5" t="s">
         <v>1452</v>
       </c>
@@ -6966,6 +6974,9 @@
       </c>
     </row>
     <row r="6" spans="1:11">
+      <c r="A6" t="b">
+        <v>1</v>
+      </c>
       <c r="B6" t="s">
         <v>1411</v>
       </c>
@@ -6980,129 +6991,153 @@
       </c>
     </row>
     <row r="7" spans="1:11">
+      <c r="A7" t="b">
+        <v>1</v>
+      </c>
       <c r="B7" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1473</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1526</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="b">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
         <v>1412</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>1463</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>1522</v>
-      </c>
-      <c r="E7" t="s">
-        <v>1634</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="B8" t="s">
-        <v>1413</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1464</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1523</v>
       </c>
       <c r="E8" t="s">
         <v>1634</v>
       </c>
     </row>
     <row r="9" spans="1:11">
+      <c r="A9" t="b">
+        <v>1</v>
+      </c>
       <c r="B9" t="s">
+        <v>1413</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1464</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1523</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="b">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
         <v>1414</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>1465</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>1524</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>1635</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
-      <c r="B10" t="s">
+    <row r="11" spans="1:11">
+      <c r="A11" t="b">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
         <v>1415</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>1466</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>1525</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>1636</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
-      <c r="B11" t="s">
+    <row r="12" spans="1:11">
+      <c r="A12" t="b">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
         <v>1416</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>1467</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>1527</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>1615</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
-      <c r="B12" t="s">
+    <row r="13" spans="1:11">
+      <c r="A13" t="b">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
         <v>1417</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>1468</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>1528</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
-      <c r="B13" t="s">
+    <row r="14" spans="1:11">
+      <c r="A14" t="b">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
         <v>1418</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>1469</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>81</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="B14" t="s">
-        <v>1419</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1472</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1529</v>
-      </c>
-      <c r="E14" t="s">
-        <v>1649</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="B15" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="C15" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="D15" t="s">
-        <v>1526</v>
+        <v>1529</v>
       </c>
       <c r="E15" t="s">
-        <v>1620</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -63458,10 +63493,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E951067-FB38-4555-BDE6-E253C2F03B6A}">
-  <dimension ref="A3:R27"/>
+  <dimension ref="A3:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -63948,21 +63983,19 @@
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="33" t="s">
-        <v>1199</v>
-      </c>
-      <c r="B19" s="34">
-        <v>1</v>
-      </c>
+        <v>1113</v>
+      </c>
+      <c r="B19" s="34"/>
       <c r="C19" s="34"/>
       <c r="D19" s="34"/>
       <c r="E19" s="34"/>
       <c r="F19" s="34"/>
-      <c r="G19" s="34">
-        <v>1</v>
-      </c>
+      <c r="G19" s="34"/>
       <c r="H19" s="34"/>
       <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="J19" s="34">
+        <v>1</v>
+      </c>
       <c r="K19" s="34"/>
       <c r="L19" s="34"/>
       <c r="M19" s="34"/>
@@ -63971,24 +64004,24 @@
       <c r="P19" s="34"/>
       <c r="Q19" s="34"/>
       <c r="R19" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="33" t="s">
-        <v>49</v>
+        <v>1678</v>
       </c>
       <c r="B20" s="34"/>
-      <c r="C20" s="34">
-        <v>1</v>
-      </c>
+      <c r="C20" s="34"/>
       <c r="D20" s="34"/>
       <c r="E20" s="34"/>
       <c r="F20" s="34"/>
       <c r="G20" s="34"/>
       <c r="H20" s="34"/>
       <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
+      <c r="J20" s="34">
+        <v>1</v>
+      </c>
       <c r="K20" s="34"/>
       <c r="L20" s="34"/>
       <c r="M20" s="34"/>
@@ -64002,16 +64035,18 @@
     </row>
     <row r="21" spans="1:18">
       <c r="A21" s="33" t="s">
-        <v>153</v>
-      </c>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34">
-        <v>1</v>
-      </c>
+        <v>1199</v>
+      </c>
+      <c r="B21" s="34">
+        <v>1</v>
+      </c>
+      <c r="C21" s="34"/>
       <c r="D21" s="34"/>
       <c r="E21" s="34"/>
       <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
+      <c r="G21" s="34">
+        <v>1</v>
+      </c>
       <c r="H21" s="34"/>
       <c r="I21" s="34"/>
       <c r="J21" s="34"/>
@@ -64023,21 +64058,21 @@
       <c r="P21" s="34"/>
       <c r="Q21" s="34"/>
       <c r="R21" s="34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="33" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
+      <c r="C22" s="34">
+        <v>1</v>
+      </c>
       <c r="D22" s="34"/>
       <c r="E22" s="34"/>
       <c r="F22" s="34"/>
-      <c r="G22" s="34">
-        <v>1</v>
-      </c>
+      <c r="G22" s="34"/>
       <c r="H22" s="34"/>
       <c r="I22" s="34"/>
       <c r="J22" s="34"/>
@@ -64054,16 +64089,16 @@
     </row>
     <row r="23" spans="1:18">
       <c r="A23" s="33" t="s">
-        <v>990</v>
+        <v>153</v>
       </c>
       <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
+      <c r="C23" s="34">
+        <v>1</v>
+      </c>
       <c r="D23" s="34"/>
       <c r="E23" s="34"/>
       <c r="F23" s="34"/>
-      <c r="G23" s="34">
-        <v>1</v>
-      </c>
+      <c r="G23" s="34"/>
       <c r="H23" s="34"/>
       <c r="I23" s="34"/>
       <c r="J23" s="34"/>
@@ -64080,53 +64115,45 @@
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="33" t="s">
-        <v>315</v>
-      </c>
-      <c r="B24" s="34">
-        <v>1</v>
-      </c>
-      <c r="C24" s="34">
-        <v>1</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
       <c r="D24" s="34"/>
       <c r="E24" s="34"/>
       <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
+      <c r="G24" s="34">
+        <v>1</v>
+      </c>
       <c r="H24" s="34"/>
-      <c r="I24" s="34">
-        <v>1</v>
-      </c>
+      <c r="I24" s="34"/>
       <c r="J24" s="34"/>
       <c r="K24" s="34"/>
       <c r="L24" s="34"/>
-      <c r="M24" s="34">
-        <v>1</v>
-      </c>
+      <c r="M24" s="34"/>
       <c r="N24" s="34"/>
       <c r="O24" s="34"/>
-      <c r="P24" s="34">
-        <v>1</v>
-      </c>
+      <c r="P24" s="34"/>
       <c r="Q24" s="34"/>
       <c r="R24" s="34">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="33" t="s">
-        <v>1665</v>
+        <v>990</v>
       </c>
       <c r="B25" s="34"/>
       <c r="C25" s="34"/>
       <c r="D25" s="34"/>
       <c r="E25" s="34"/>
       <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
+      <c r="G25" s="34">
+        <v>1</v>
+      </c>
       <c r="H25" s="34"/>
       <c r="I25" s="34"/>
-      <c r="J25" s="34">
-        <v>1</v>
-      </c>
+      <c r="J25" s="34"/>
       <c r="K25" s="34"/>
       <c r="L25" s="34"/>
       <c r="M25" s="34"/>
@@ -64140,88 +64167,123 @@
     </row>
     <row r="26" spans="1:18">
       <c r="A26" s="33" t="s">
-        <v>1678</v>
-      </c>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
+        <v>315</v>
+      </c>
+      <c r="B26" s="34">
+        <v>1</v>
+      </c>
+      <c r="C26" s="34">
+        <v>1</v>
+      </c>
       <c r="D26" s="34"/>
       <c r="E26" s="34"/>
       <c r="F26" s="34"/>
       <c r="G26" s="34"/>
       <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34">
-        <v>1</v>
-      </c>
+      <c r="I26" s="34">
+        <v>1</v>
+      </c>
+      <c r="J26" s="34"/>
       <c r="K26" s="34"/>
       <c r="L26" s="34"/>
-      <c r="M26" s="34"/>
+      <c r="M26" s="34">
+        <v>1</v>
+      </c>
       <c r="N26" s="34"/>
       <c r="O26" s="34"/>
-      <c r="P26" s="34"/>
+      <c r="P26" s="34">
+        <v>1</v>
+      </c>
       <c r="Q26" s="34"/>
       <c r="R26" s="34">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:18">
       <c r="A27" s="33" t="s">
+        <v>1665</v>
+      </c>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34">
+        <v>1</v>
+      </c>
+      <c r="K27" s="34"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="34"/>
+      <c r="N27" s="34"/>
+      <c r="O27" s="34"/>
+      <c r="P27" s="34"/>
+      <c r="Q27" s="34"/>
+      <c r="R27" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="A28" s="33" t="s">
         <v>1669</v>
       </c>
-      <c r="B27" s="34">
+      <c r="B28" s="34">
         <v>4</v>
       </c>
-      <c r="C27" s="34">
+      <c r="C28" s="34">
         <v>6</v>
       </c>
-      <c r="D27" s="34">
-        <v>1</v>
-      </c>
-      <c r="E27" s="34">
-        <v>1</v>
-      </c>
-      <c r="F27" s="34">
+      <c r="D28" s="34">
+        <v>1</v>
+      </c>
+      <c r="E28" s="34">
+        <v>1</v>
+      </c>
+      <c r="F28" s="34">
         <v>3</v>
       </c>
-      <c r="G27" s="34">
+      <c r="G28" s="34">
         <v>6</v>
       </c>
-      <c r="H27" s="34">
+      <c r="H28" s="34">
         <v>2</v>
       </c>
-      <c r="I27" s="34">
+      <c r="I28" s="34">
         <v>5</v>
       </c>
-      <c r="J27" s="34">
-        <v>2</v>
-      </c>
-      <c r="K27" s="34">
-        <v>1</v>
-      </c>
-      <c r="L27" s="34">
-        <v>1</v>
-      </c>
-      <c r="M27" s="34">
+      <c r="J28" s="34">
+        <v>3</v>
+      </c>
+      <c r="K28" s="34">
+        <v>1</v>
+      </c>
+      <c r="L28" s="34">
+        <v>1</v>
+      </c>
+      <c r="M28" s="34">
         <v>5</v>
       </c>
-      <c r="N27" s="34">
-        <v>1</v>
-      </c>
-      <c r="O27" s="34">
-        <v>1</v>
-      </c>
-      <c r="P27" s="34">
+      <c r="N28" s="34">
+        <v>1</v>
+      </c>
+      <c r="O28" s="34">
+        <v>1</v>
+      </c>
+      <c r="P28" s="34">
         <v>3</v>
       </c>
-      <c r="Q27" s="34">
-        <v>1</v>
-      </c>
-      <c r="R27" s="34">
-        <v>43</v>
+      <c r="Q28" s="34">
+        <v>1</v>
+      </c>
+      <c r="R28" s="34">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -64229,8 +64291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D4DEF77-0A73-437F-AF61-6691330407EF}">
   <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7265625" defaultRowHeight="14.5"/>
@@ -64439,6 +64501,14 @@
         <v>1660</v>
       </c>
     </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="4" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1672</v>
+      </c>
+    </row>
     <row r="29" spans="1:2">
       <c r="A29" s="4" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Several potions in to creation recipes
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79382A69-A65F-4DA8-B98F-D59DD7907F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB722A6-1F76-46F3-B588-2378EAF2A54E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="6" activeTab="9" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="6" activeTab="10" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
   <sheets>
     <sheet name="Bullshit scroll price tinkering" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10419" uniqueCount="1679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10422" uniqueCount="1679">
   <si>
     <t>Caster Level</t>
   </si>
@@ -6859,8 +6859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A6DB01-2873-4025-8F60-A17DF1993631}">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6870,7 +6870,8 @@
     <col min="4" max="4" width="25.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.54296875" customWidth="1"/>
     <col min="6" max="6" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.90625" customWidth="1"/>
+    <col min="8" max="8" width="4.90625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.1796875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.1796875" bestFit="1" customWidth="1"/>
@@ -7127,6 +7128,9 @@
       </c>
     </row>
     <row r="15" spans="1:11">
+      <c r="A15" t="b">
+        <v>1</v>
+      </c>
       <c r="B15" t="s">
         <v>1419</v>
       </c>
@@ -7141,6 +7145,9 @@
       </c>
     </row>
     <row r="16" spans="1:11">
+      <c r="A16" t="b">
+        <v>1</v>
+      </c>
       <c r="B16" t="s">
         <v>1421</v>
       </c>
@@ -7154,7 +7161,10 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="1:6">
+      <c r="A17" t="b">
+        <v>1</v>
+      </c>
       <c r="B17" t="s">
         <v>1422</v>
       </c>
@@ -7168,7 +7178,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="1:6">
       <c r="B18" t="s">
         <v>1423</v>
       </c>
@@ -7185,7 +7195,7 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="1:6">
       <c r="B19" t="s">
         <v>1424</v>
       </c>
@@ -7202,7 +7212,10 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="1:6">
+      <c r="A20" t="b">
+        <v>1</v>
+      </c>
       <c r="B20" t="s">
         <v>1425</v>
       </c>
@@ -7216,7 +7229,10 @@
         <v>1616</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="1:6">
+      <c r="A21" t="b">
+        <v>1</v>
+      </c>
       <c r="B21" t="s">
         <v>1426</v>
       </c>
@@ -7230,7 +7246,10 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="1:6">
+      <c r="A22" t="b">
+        <v>1</v>
+      </c>
       <c r="B22" t="s">
         <v>1427</v>
       </c>
@@ -7244,7 +7263,10 @@
         <v>1629</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="1:6">
+      <c r="A23" t="b">
+        <v>1</v>
+      </c>
       <c r="B23" t="s">
         <v>1428</v>
       </c>
@@ -7258,7 +7280,10 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="1:6">
+      <c r="A24" t="b">
+        <v>1</v>
+      </c>
       <c r="B24" t="s">
         <v>1429</v>
       </c>
@@ -7272,7 +7297,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="1:6">
       <c r="B25" t="s">
         <v>1430</v>
       </c>
@@ -7286,7 +7311,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="1:6">
       <c r="B26" t="s">
         <v>1431</v>
       </c>
@@ -7300,7 +7325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:6">
+    <row r="27" spans="1:6">
       <c r="B27" t="s">
         <v>1432</v>
       </c>
@@ -7314,7 +7339,7 @@
         <v>1623</v>
       </c>
     </row>
-    <row r="28" spans="2:6">
+    <row r="28" spans="1:6">
       <c r="B28" t="s">
         <v>1433</v>
       </c>
@@ -7328,7 +7353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:6">
+    <row r="29" spans="1:6">
       <c r="B29" t="s">
         <v>1434</v>
       </c>
@@ -7342,7 +7367,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="2:6">
+    <row r="30" spans="1:6">
       <c r="B30" t="s">
         <v>1435</v>
       </c>
@@ -7356,7 +7381,7 @@
         <v>1617</v>
       </c>
     </row>
-    <row r="31" spans="2:6">
+    <row r="31" spans="1:6">
       <c r="B31" t="s">
         <v>1436</v>
       </c>
@@ -7370,7 +7395,7 @@
         <v>1630</v>
       </c>
     </row>
-    <row r="32" spans="2:6">
+    <row r="32" spans="1:6">
       <c r="B32" t="s">
         <v>1437</v>
       </c>
@@ -7800,11 +7825,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97994022-E0D3-4848-B3E3-1B87FDCE7E6E}">
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:C98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40:C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -8146,7 +8171,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>608</v>
+        <v>259</v>
       </c>
       <c r="B31" t="s">
         <v>1611</v>
@@ -8157,7 +8182,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>630</v>
+        <v>608</v>
       </c>
       <c r="B32" t="s">
         <v>1611</v>
@@ -8168,7 +8193,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>1576</v>
+        <v>630</v>
       </c>
       <c r="B33" t="s">
         <v>1611</v>
@@ -8179,7 +8204,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>636</v>
+        <v>1576</v>
       </c>
       <c r="B34" t="s">
         <v>1611</v>
@@ -8190,7 +8215,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>660</v>
+        <v>636</v>
       </c>
       <c r="B35" t="s">
         <v>1611</v>
@@ -8201,7 +8226,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>1577</v>
+        <v>660</v>
       </c>
       <c r="B36" t="s">
         <v>1611</v>
@@ -8212,7 +8237,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="B37" t="s">
         <v>1611</v>
@@ -8223,7 +8248,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="B38" t="s">
         <v>1611</v>
@@ -8234,18 +8259,18 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>940</v>
+        <v>1579</v>
       </c>
       <c r="B39" t="s">
         <v>1611</v>
       </c>
       <c r="C39" t="s">
-        <v>939</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="B40" t="s">
         <v>1611</v>
@@ -8256,7 +8281,7 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="B41" t="s">
         <v>1611</v>
@@ -8267,7 +8292,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>1188</v>
+        <v>946</v>
       </c>
       <c r="B42" t="s">
         <v>1611</v>
@@ -8278,7 +8303,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>957</v>
+        <v>1188</v>
       </c>
       <c r="B43" t="s">
         <v>1611</v>
@@ -8289,7 +8314,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="B44" t="s">
         <v>1611</v>
@@ -8300,7 +8325,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>1267</v>
+        <v>960</v>
       </c>
       <c r="B45" t="s">
         <v>1611</v>
@@ -8311,7 +8336,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>968</v>
+        <v>1267</v>
       </c>
       <c r="B46" t="s">
         <v>1611</v>
@@ -8322,7 +8347,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>1316</v>
+        <v>968</v>
       </c>
       <c r="B47" t="s">
         <v>1611</v>
@@ -8333,7 +8358,7 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>1580</v>
+        <v>1316</v>
       </c>
       <c r="B48" t="s">
         <v>1611</v>
@@ -8344,7 +8369,7 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>1193</v>
+        <v>1580</v>
       </c>
       <c r="B49" t="s">
         <v>1611</v>
@@ -8355,7 +8380,7 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>1196</v>
+        <v>1193</v>
       </c>
       <c r="B50" t="s">
         <v>1611</v>
@@ -8366,7 +8391,7 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>1081</v>
+        <v>1196</v>
       </c>
       <c r="B51" t="s">
         <v>1611</v>
@@ -8377,7 +8402,7 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>1109</v>
+        <v>1081</v>
       </c>
       <c r="B52" t="s">
         <v>1611</v>
@@ -8388,7 +8413,7 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>1128</v>
+        <v>1109</v>
       </c>
       <c r="B53" t="s">
         <v>1611</v>
@@ -8399,7 +8424,7 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>1132</v>
+        <v>1128</v>
       </c>
       <c r="B54" t="s">
         <v>1611</v>
@@ -8410,7 +8435,7 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>1207</v>
+        <v>1132</v>
       </c>
       <c r="B55" t="s">
         <v>1611</v>
@@ -8421,7 +8446,7 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>1581</v>
+        <v>1207</v>
       </c>
       <c r="B56" t="s">
         <v>1611</v>
@@ -8432,7 +8457,7 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="B57" t="s">
         <v>1611</v>
@@ -8443,7 +8468,7 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>1197</v>
+        <v>1582</v>
       </c>
       <c r="B58" t="s">
         <v>1611</v>
@@ -8454,7 +8479,7 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>9</v>
+        <v>1197</v>
       </c>
       <c r="B59" t="s">
         <v>1611</v>
@@ -8463,20 +8488,20 @@
         <v>939</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
-      <c r="A61" t="s">
-        <v>1045</v>
-      </c>
-      <c r="B61" t="s">
-        <v>1408</v>
-      </c>
-      <c r="C61" t="s">
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1611</v>
+      </c>
+      <c r="C60" t="s">
         <v>939</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="B62" t="s">
         <v>1408</v>
@@ -8487,7 +8512,7 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
       <c r="B63" t="s">
         <v>1408</v>
@@ -8498,7 +8523,7 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>1271</v>
+        <v>1046</v>
       </c>
       <c r="B64" t="s">
         <v>1408</v>
@@ -8509,7 +8534,7 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>1583</v>
+        <v>1271</v>
       </c>
       <c r="B65" t="s">
         <v>1408</v>
@@ -8520,7 +8545,7 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>1199</v>
+        <v>1583</v>
       </c>
       <c r="B66" t="s">
         <v>1408</v>
@@ -8531,7 +8556,7 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>1105</v>
+        <v>1199</v>
       </c>
       <c r="B67" t="s">
         <v>1408</v>
@@ -8542,7 +8567,7 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
       <c r="B68" t="s">
         <v>1408</v>
@@ -8553,7 +8578,7 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>1155</v>
+        <v>1108</v>
       </c>
       <c r="B69" t="s">
         <v>1408</v>
@@ -8562,17 +8587,20 @@
         <v>939</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
-      <c r="A71" t="s">
-        <v>1584</v>
-      </c>
-      <c r="B71" t="s">
-        <v>1613</v>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1408</v>
+      </c>
+      <c r="C70" t="s">
+        <v>939</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="B72" t="s">
         <v>1613</v>
@@ -8580,7 +8608,7 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="B73" t="s">
         <v>1613</v>
@@ -8588,7 +8616,7 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="B74" t="s">
         <v>1613</v>
@@ -8596,7 +8624,7 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="B75" t="s">
         <v>1613</v>
@@ -8604,7 +8632,7 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="B76" t="s">
         <v>1613</v>
@@ -8612,7 +8640,7 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="B77" t="s">
         <v>1613</v>
@@ -8620,7 +8648,7 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="B78" t="s">
         <v>1613</v>
@@ -8628,7 +8656,7 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="B79" t="s">
         <v>1613</v>
@@ -8636,7 +8664,7 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="B80" t="s">
         <v>1613</v>
@@ -8644,7 +8672,7 @@
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="B81" t="s">
         <v>1613</v>
@@ -8652,7 +8680,7 @@
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="B82" t="s">
         <v>1613</v>
@@ -8660,7 +8688,7 @@
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="B83" t="s">
         <v>1613</v>
@@ -8668,7 +8696,7 @@
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="B84" t="s">
         <v>1613</v>
@@ -8676,7 +8704,7 @@
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="B85" t="s">
         <v>1613</v>
@@ -8684,7 +8712,7 @@
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="B86" t="s">
         <v>1613</v>
@@ -8692,7 +8720,7 @@
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="B87" t="s">
         <v>1613</v>
@@ -8700,7 +8728,7 @@
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="B88" t="s">
         <v>1613</v>
@@ -8708,7 +8736,7 @@
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="B89" t="s">
         <v>1613</v>
@@ -8716,7 +8744,7 @@
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="B90" t="s">
         <v>1613</v>
@@ -8724,7 +8752,7 @@
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="B91" t="s">
         <v>1613</v>
@@ -8732,7 +8760,7 @@
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>631</v>
+        <v>1604</v>
       </c>
       <c r="B92" t="s">
         <v>1613</v>
@@ -8740,7 +8768,7 @@
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>1605</v>
+        <v>631</v>
       </c>
       <c r="B93" t="s">
         <v>1613</v>
@@ -8748,7 +8776,7 @@
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
       <c r="B94" t="s">
         <v>1613</v>
@@ -8756,7 +8784,7 @@
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="B95" t="s">
         <v>1613</v>
@@ -8764,7 +8792,7 @@
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="B96" t="s">
         <v>1613</v>
@@ -8772,9 +8800,17 @@
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
+        <v>1608</v>
+      </c>
+      <c r="B97" t="s">
+        <v>1613</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
         <v>1609</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B98" t="s">
         <v>1613</v>
       </c>
     </row>
@@ -63496,7 +63532,7 @@
   <dimension ref="A3:R28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -64291,8 +64327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D4DEF77-0A73-437F-AF61-6691330407EF}">
   <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7265625" defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Finish out most potion recipies in base game
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF746B5-558D-4DC6-8C1F-60B13A892A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474430A6-E378-47BA-A3F7-13BEAEFED714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="6" activeTab="9" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -6880,8 +6880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A6DB01-2873-4025-8F60-A17DF1993631}">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -7655,6 +7655,9 @@
       </c>
     </row>
     <row r="41" spans="1:7">
+      <c r="A41" t="b">
+        <v>1</v>
+      </c>
       <c r="B41" t="s">
         <v>1446</v>
       </c>
@@ -7672,6 +7675,9 @@
       </c>
     </row>
     <row r="42" spans="1:7">
+      <c r="A42" t="b">
+        <v>1</v>
+      </c>
       <c r="B42" t="s">
         <v>1447</v>
       </c>
@@ -7703,6 +7709,9 @@
       </c>
     </row>
     <row r="44" spans="1:7">
+      <c r="A44" t="b">
+        <v>1</v>
+      </c>
       <c r="B44" t="s">
         <v>1449</v>
       </c>
@@ -7720,6 +7729,9 @@
       </c>
     </row>
     <row r="45" spans="1:7">
+      <c r="A45" t="b">
+        <v>1</v>
+      </c>
       <c r="B45" t="s">
         <v>1450</v>
       </c>
@@ -7737,6 +7749,9 @@
       </c>
     </row>
     <row r="46" spans="1:7">
+      <c r="A46" t="b">
+        <v>1</v>
+      </c>
       <c r="B46" t="s">
         <v>1451</v>
       </c>
@@ -7754,6 +7769,9 @@
       </c>
     </row>
     <row r="47" spans="1:7">
+      <c r="A47" t="b">
+        <v>1</v>
+      </c>
       <c r="B47" t="s">
         <v>1453</v>
       </c>
@@ -7771,6 +7789,9 @@
       </c>
     </row>
     <row r="48" spans="1:7">
+      <c r="A48" t="b">
+        <v>1</v>
+      </c>
       <c r="B48" t="s">
         <v>1454</v>
       </c>
@@ -7787,7 +7808,7 @@
         <v>1681</v>
       </c>
     </row>
-    <row r="49" spans="2:7">
+    <row r="49" spans="1:7">
       <c r="B49" t="s">
         <v>1455</v>
       </c>
@@ -7798,7 +7819,7 @@
         <v>1557</v>
       </c>
     </row>
-    <row r="50" spans="2:7">
+    <row r="50" spans="1:7">
       <c r="B50" t="s">
         <v>1456</v>
       </c>
@@ -7812,22 +7833,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:7">
+    <row r="51" spans="1:7">
       <c r="B51" t="s">
         <v>1457</v>
       </c>
     </row>
-    <row r="52" spans="2:7">
+    <row r="52" spans="1:7">
       <c r="B52" t="s">
         <v>1458</v>
       </c>
     </row>
-    <row r="53" spans="2:7">
+    <row r="53" spans="1:7">
       <c r="B53" t="s">
         <v>1459</v>
       </c>
     </row>
-    <row r="54" spans="2:7">
+    <row r="54" spans="1:7">
+      <c r="A54" t="b">
+        <v>1</v>
+      </c>
       <c r="B54" t="s">
         <v>1460</v>
       </c>
@@ -7844,17 +7868,20 @@
         <v>1679</v>
       </c>
     </row>
-    <row r="55" spans="2:7">
+    <row r="55" spans="1:7">
       <c r="B55" t="s">
         <v>1508</v>
       </c>
     </row>
-    <row r="56" spans="2:7">
+    <row r="56" spans="1:7">
       <c r="B56" t="s">
         <v>1509</v>
       </c>
     </row>
-    <row r="57" spans="2:7">
+    <row r="57" spans="1:7">
+      <c r="A57" t="b">
+        <v>1</v>
+      </c>
       <c r="B57" t="s">
         <v>1510</v>
       </c>
@@ -7871,7 +7898,7 @@
         <v>1679</v>
       </c>
     </row>
-    <row r="58" spans="2:7">
+    <row r="58" spans="1:7">
       <c r="B58" t="s">
         <v>1511</v>
       </c>
@@ -7882,22 +7909,25 @@
         <v>1522</v>
       </c>
     </row>
-    <row r="59" spans="2:7">
+    <row r="59" spans="1:7">
       <c r="B59" t="s">
         <v>1512</v>
       </c>
     </row>
-    <row r="60" spans="2:7">
+    <row r="60" spans="1:7">
       <c r="B60" t="s">
         <v>1513</v>
       </c>
     </row>
-    <row r="61" spans="2:7">
+    <row r="61" spans="1:7">
       <c r="B61" t="s">
         <v>1514</v>
       </c>
     </row>
-    <row r="62" spans="2:7">
+    <row r="62" spans="1:7">
+      <c r="A62" t="b">
+        <v>1</v>
+      </c>
       <c r="B62" t="s">
         <v>1515</v>
       </c>
@@ -7914,7 +7944,7 @@
         <v>1677</v>
       </c>
     </row>
-    <row r="63" spans="2:7">
+    <row r="63" spans="1:7">
       <c r="B63" t="s">
         <v>1640</v>
       </c>
@@ -7928,7 +7958,10 @@
         <v>1678</v>
       </c>
     </row>
-    <row r="64" spans="2:7">
+    <row r="64" spans="1:7">
+      <c r="A64" t="b">
+        <v>1</v>
+      </c>
       <c r="B64" t="s">
         <v>1643</v>
       </c>

</xml_diff>

<commit_message>
Annotate desire for Snilloc's snowball
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687AC18B-C991-4740-8613-99248407FD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7847FAFD-F30C-4704-ACAA-108C0ED269D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="6" activeTab="9" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="6" activeTab="10" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
   <sheets>
     <sheet name="Bullshit scroll price tinkering" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,9 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="29" r:id="rId13"/>
+    <pivotCache cacheId="0" r:id="rId13"/>
   </pivotCaches>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10468" uniqueCount="1686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10471" uniqueCount="1687">
   <si>
     <t>Caster Level</t>
   </si>
@@ -5097,6 +5098,9 @@
   </si>
   <si>
     <t>Stoneskin or Barkskin or Iron skins; flesh to stone</t>
+  </si>
+  <si>
+    <t>Snowball</t>
   </si>
 </sst>
 </file>
@@ -5268,7 +5272,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -5300,6 +5304,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5315,13 +5325,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent2" xfId="4" builtinId="33"/>
@@ -5602,7 +5605,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F3C0FD81-EC5D-4C31-9DDA-F8F6B464BBF6}" name="PivotTable1" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F3C0FD81-EC5D-4C31-9DDA-F8F6B464BBF6}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:R28" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
@@ -6880,8 +6883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A6DB01-2873-4025-8F60-A17DF1993631}">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6894,13 +6897,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="33" t="s">
         <v>1404</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" s="23"/>
@@ -7305,7 +7308,7 @@
       <c r="D22" t="s">
         <v>1533</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E22" s="26" t="s">
         <v>1628</v>
       </c>
       <c r="G22" t="s">
@@ -7473,7 +7476,7 @@
       <c r="D31" t="s">
         <v>1541</v>
       </c>
-      <c r="E31" s="31" t="s">
+      <c r="E31" s="26" t="s">
         <v>1629</v>
       </c>
       <c r="G31" t="s">
@@ -7493,7 +7496,7 @@
       <c r="D32" t="s">
         <v>1542</v>
       </c>
-      <c r="E32" s="31" t="s">
+      <c r="E32" s="26" t="s">
         <v>1682</v>
       </c>
       <c r="G32" t="s">
@@ -7812,10 +7815,10 @@
       <c r="B49" t="s">
         <v>1455</v>
       </c>
-      <c r="C49" s="30" t="s">
+      <c r="C49" s="25" t="s">
         <v>1505</v>
       </c>
-      <c r="D49" s="30" t="s">
+      <c r="D49" s="25" t="s">
         <v>1557</v>
       </c>
     </row>
@@ -7823,10 +7826,10 @@
       <c r="B50" t="s">
         <v>1456</v>
       </c>
-      <c r="C50" s="30" t="s">
+      <c r="C50" s="25" t="s">
         <v>1506</v>
       </c>
-      <c r="D50" s="30" t="s">
+      <c r="D50" s="25" t="s">
         <v>1558</v>
       </c>
       <c r="F50" t="b">
@@ -7902,10 +7905,10 @@
       <c r="B58" t="s">
         <v>1511</v>
       </c>
-      <c r="C58" s="30" t="s">
+      <c r="C58" s="25" t="s">
         <v>1638</v>
       </c>
-      <c r="D58" s="30" t="s">
+      <c r="D58" s="25" t="s">
         <v>1522</v>
       </c>
     </row>
@@ -8035,11 +8038,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97994022-E0D3-4848-B3E3-1B87FDCE7E6E}">
-  <dimension ref="A1:C99"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B98" sqref="B72:B98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -8808,17 +8811,20 @@
         <v>939</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
-      <c r="A72" t="s">
-        <v>1584</v>
-      </c>
-      <c r="B72" t="s">
-        <v>1684</v>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1408</v>
+      </c>
+      <c r="C71" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="B73" t="s">
         <v>1684</v>
@@ -8826,7 +8832,7 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="B74" t="s">
         <v>1684</v>
@@ -8834,7 +8840,7 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="B75" t="s">
         <v>1684</v>
@@ -8842,7 +8848,7 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="B76" t="s">
         <v>1684</v>
@@ -8850,7 +8856,7 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="B77" t="s">
         <v>1684</v>
@@ -8858,7 +8864,7 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="B78" t="s">
         <v>1684</v>
@@ -8866,7 +8872,7 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="B79" t="s">
         <v>1684</v>
@@ -8874,7 +8880,7 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="B80" t="s">
         <v>1684</v>
@@ -8882,7 +8888,7 @@
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="B81" t="s">
         <v>1684</v>
@@ -8890,7 +8896,7 @@
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="B82" t="s">
         <v>1684</v>
@@ -8898,7 +8904,7 @@
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="B83" t="s">
         <v>1684</v>
@@ -8906,7 +8912,7 @@
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="B84" t="s">
         <v>1684</v>
@@ -8914,7 +8920,7 @@
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="B85" t="s">
         <v>1684</v>
@@ -8922,7 +8928,7 @@
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="B86" t="s">
         <v>1684</v>
@@ -8930,7 +8936,7 @@
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="B87" t="s">
         <v>1684</v>
@@ -8938,7 +8944,7 @@
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="B88" t="s">
         <v>1684</v>
@@ -8946,7 +8952,7 @@
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="B89" t="s">
         <v>1684</v>
@@ -8954,7 +8960,7 @@
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="B90" t="s">
         <v>1684</v>
@@ -8962,7 +8968,7 @@
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="B91" t="s">
         <v>1684</v>
@@ -8970,7 +8976,7 @@
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="B92" t="s">
         <v>1684</v>
@@ -8978,7 +8984,7 @@
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>631</v>
+        <v>1604</v>
       </c>
       <c r="B93" t="s">
         <v>1684</v>
@@ -8986,7 +8992,7 @@
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>1605</v>
+        <v>631</v>
       </c>
       <c r="B94" t="s">
         <v>1684</v>
@@ -8994,7 +9000,7 @@
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
       <c r="B95" t="s">
         <v>1684</v>
@@ -9002,7 +9008,7 @@
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="B96" t="s">
         <v>1684</v>
@@ -9010,7 +9016,7 @@
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="B97" t="s">
         <v>1684</v>
@@ -9018,7 +9024,7 @@
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="B98" t="s">
         <v>1684</v>
@@ -9026,9 +9032,17 @@
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
+        <v>1609</v>
+      </c>
+      <c r="B99" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
         <v>1683</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B100" t="s">
         <v>1684</v>
       </c>
     </row>
@@ -9059,17 +9073,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="33" t="s">
         <v>1404</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
       <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10">
@@ -9078,13 +9092,13 @@
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="33" t="s">
         <v>1406</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="4" t="s">
@@ -9185,60 +9199,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" s="5" customFormat="1">
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25" t="s">
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29" t="s">
         <v>193</v>
       </c>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25" t="s">
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29" t="s">
         <v>316</v>
       </c>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25" t="s">
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29" t="s">
         <v>547</v>
       </c>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25" t="s">
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29" t="s">
         <v>819</v>
       </c>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25" t="s">
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29" t="s">
         <v>833</v>
       </c>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25" t="s">
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29" t="s">
         <v>834</v>
       </c>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25" t="s">
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29" t="s">
         <v>835</v>
       </c>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25" t="s">
+      <c r="AF1" s="29"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29" t="s">
         <v>869</v>
       </c>
-      <c r="AJ1" s="25"/>
-      <c r="AK1" s="25"/>
-      <c r="AL1" s="25"/>
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="29"/>
       <c r="AM1" s="11"/>
       <c r="AN1" s="11"/>
       <c r="AO1" s="11"/>
@@ -43670,76 +43684,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" s="5" customFormat="1">
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="30" t="s">
         <v>175</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="27" t="s">
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="26" t="s">
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26" t="s">
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30" t="s">
         <v>547</v>
       </c>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26" t="s">
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30" t="s">
         <v>819</v>
       </c>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="26" t="s">
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30" t="s">
         <v>833</v>
       </c>
-      <c r="AD1" s="26"/>
-      <c r="AE1" s="26"/>
-      <c r="AF1" s="26"/>
-      <c r="AG1" s="26"/>
-      <c r="AH1" s="26"/>
-      <c r="AI1" s="26" t="s">
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30" t="s">
         <v>834</v>
       </c>
-      <c r="AJ1" s="26"/>
-      <c r="AK1" s="26"/>
-      <c r="AL1" s="26" t="s">
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="30"/>
+      <c r="AL1" s="30" t="s">
         <v>835</v>
       </c>
-      <c r="AM1" s="26"/>
-      <c r="AN1" s="26"/>
-      <c r="AO1" s="26"/>
-      <c r="AP1" s="26"/>
-      <c r="AQ1" s="26"/>
-      <c r="AR1" s="26" t="s">
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
+      <c r="AO1" s="30"/>
+      <c r="AP1" s="30"/>
+      <c r="AQ1" s="30"/>
+      <c r="AR1" s="30" t="s">
         <v>869</v>
       </c>
-      <c r="AS1" s="26"/>
-      <c r="AT1" s="26"/>
-      <c r="AU1" s="26"/>
-      <c r="AV1" s="26"/>
-      <c r="AW1" s="26"/>
-      <c r="AX1" s="26"/>
-      <c r="AY1" s="26"/>
-      <c r="AZ1" s="26"/>
-      <c r="BA1" s="26"/>
-      <c r="BB1" s="27"/>
+      <c r="AS1" s="30"/>
+      <c r="AT1" s="30"/>
+      <c r="AU1" s="30"/>
+      <c r="AV1" s="30"/>
+      <c r="AW1" s="30"/>
+      <c r="AX1" s="30"/>
+      <c r="AY1" s="30"/>
+      <c r="AZ1" s="30"/>
+      <c r="BA1" s="30"/>
+      <c r="BB1" s="31"/>
     </row>
     <row r="2" spans="1:54">
       <c r="A2" s="4" t="s">
@@ -63776,15 +63790,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="27" t="s">
         <v>1668</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="27" t="s">
         <v>1667</v>
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="27" t="s">
         <v>1665</v>
       </c>
       <c r="B4" t="s">
@@ -63840,698 +63854,374 @@
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="28" t="s">
         <v>957</v>
       </c>
-      <c r="B5" s="34">
-        <v>1</v>
-      </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34">
-        <v>1</v>
-      </c>
-      <c r="I5" s="34">
-        <v>1</v>
-      </c>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34">
-        <v>1</v>
-      </c>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="34">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="R5">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34">
-        <v>1</v>
-      </c>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
-      <c r="Q6" s="34"/>
-      <c r="R6" s="34">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="R6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="28" t="s">
         <v>1651</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34">
-        <v>1</v>
-      </c>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="34"/>
-      <c r="P7" s="34"/>
-      <c r="Q7" s="34"/>
-      <c r="R7" s="34">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="R7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="28" t="s">
         <v>960</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34">
-        <v>1</v>
-      </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34">
-        <v>1</v>
-      </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="34"/>
-      <c r="P8" s="34"/>
-      <c r="Q8" s="34"/>
-      <c r="R8" s="34">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="R8">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="28" t="s">
         <v>940</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34">
-        <v>1</v>
-      </c>
-      <c r="I9" s="34">
-        <v>1</v>
-      </c>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34">
-        <v>1</v>
-      </c>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="34"/>
-      <c r="R9" s="34">
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="R9">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="28" t="s">
         <v>1023</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34">
-        <v>1</v>
-      </c>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="34">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="34"/>
-      <c r="R10" s="34">
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="R10">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="28" t="s">
         <v>961</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34">
-        <v>1</v>
-      </c>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34">
-        <v>1</v>
-      </c>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34">
-        <v>1</v>
-      </c>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
-      <c r="P11" s="34"/>
-      <c r="Q11" s="34"/>
-      <c r="R11" s="34">
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="R11">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="28" t="s">
         <v>968</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34">
-        <v>1</v>
-      </c>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34">
-        <v>1</v>
-      </c>
-      <c r="O12" s="34">
-        <v>1</v>
-      </c>
-      <c r="P12" s="34"/>
-      <c r="Q12" s="34"/>
-      <c r="R12" s="34">
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="R12">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="28" t="s">
         <v>1663</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34">
-        <v>1</v>
-      </c>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="34"/>
-      <c r="P13" s="34"/>
-      <c r="Q13" s="34"/>
-      <c r="R13" s="34">
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="R13">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="28" t="s">
         <v>1664</v>
       </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34">
-        <v>1</v>
-      </c>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="34"/>
-      <c r="P14" s="34"/>
-      <c r="Q14" s="34"/>
-      <c r="R14" s="34">
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="R14">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34">
-        <v>1</v>
-      </c>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
-      <c r="P15" s="34"/>
-      <c r="Q15" s="34"/>
-      <c r="R15" s="34">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="R15">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34">
-        <v>1</v>
-      </c>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="34"/>
-      <c r="P16" s="34"/>
-      <c r="Q16" s="34"/>
-      <c r="R16" s="34">
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="R16">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:18">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="28" t="s">
         <v>1195</v>
       </c>
-      <c r="B17" s="34">
-        <v>1</v>
-      </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34">
-        <v>1</v>
-      </c>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="34"/>
-      <c r="P17" s="34">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="34"/>
-      <c r="R17" s="34">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="R17">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:18">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34">
-        <v>1</v>
-      </c>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34">
-        <v>1</v>
-      </c>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="34">
-        <v>1</v>
-      </c>
-      <c r="N18" s="34"/>
-      <c r="O18" s="34"/>
-      <c r="P18" s="34"/>
-      <c r="Q18" s="34">
-        <v>1</v>
-      </c>
-      <c r="R18" s="34">
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:18">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="28" t="s">
         <v>1113</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34">
-        <v>1</v>
-      </c>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="34"/>
-      <c r="P19" s="34"/>
-      <c r="Q19" s="34"/>
-      <c r="R19" s="34">
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="R19">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:18">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="28" t="s">
         <v>1675</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34">
-        <v>1</v>
-      </c>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="34"/>
-      <c r="P20" s="34"/>
-      <c r="Q20" s="34"/>
-      <c r="R20" s="34">
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="R20">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:18">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="28" t="s">
         <v>1199</v>
       </c>
-      <c r="B21" s="34">
-        <v>1</v>
-      </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34">
-        <v>1</v>
-      </c>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="34"/>
-      <c r="P21" s="34"/>
-      <c r="Q21" s="34"/>
-      <c r="R21" s="34">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="R21">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:18">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34">
-        <v>1</v>
-      </c>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
-      <c r="O22" s="34"/>
-      <c r="P22" s="34"/>
-      <c r="Q22" s="34"/>
-      <c r="R22" s="34">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="R22">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:18">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34">
-        <v>1</v>
-      </c>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
-      <c r="M23" s="34"/>
-      <c r="N23" s="34"/>
-      <c r="O23" s="34"/>
-      <c r="P23" s="34"/>
-      <c r="Q23" s="34"/>
-      <c r="R23" s="34">
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="R23">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34">
-        <v>1</v>
-      </c>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="34"/>
-      <c r="P24" s="34"/>
-      <c r="Q24" s="34"/>
-      <c r="R24" s="34">
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="R24">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:18">
-      <c r="A25" s="33" t="s">
+      <c r="A25" s="28" t="s">
         <v>990</v>
       </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34">
-        <v>1</v>
-      </c>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="34"/>
-      <c r="M25" s="34"/>
-      <c r="N25" s="34"/>
-      <c r="O25" s="34"/>
-      <c r="P25" s="34"/>
-      <c r="Q25" s="34"/>
-      <c r="R25" s="34">
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="R25">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:18">
-      <c r="A26" s="33" t="s">
+      <c r="A26" s="28" t="s">
         <v>315</v>
       </c>
-      <c r="B26" s="34">
-        <v>1</v>
-      </c>
-      <c r="C26" s="34">
-        <v>1</v>
-      </c>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34">
-        <v>1</v>
-      </c>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="34">
-        <v>1</v>
-      </c>
-      <c r="N26" s="34"/>
-      <c r="O26" s="34"/>
-      <c r="P26" s="34">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="34"/>
-      <c r="R26" s="34">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="R26">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:18">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="28" t="s">
         <v>1662</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34">
-        <v>1</v>
-      </c>
-      <c r="K27" s="34"/>
-      <c r="L27" s="34"/>
-      <c r="M27" s="34"/>
-      <c r="N27" s="34"/>
-      <c r="O27" s="34"/>
-      <c r="P27" s="34"/>
-      <c r="Q27" s="34"/>
-      <c r="R27" s="34">
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="R27">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:18">
-      <c r="A28" s="33" t="s">
+      <c r="A28" s="28" t="s">
         <v>1666</v>
       </c>
-      <c r="B28" s="34">
+      <c r="B28">
         <v>4</v>
       </c>
-      <c r="C28" s="34">
+      <c r="C28">
         <v>6</v>
       </c>
-      <c r="D28" s="34">
-        <v>1</v>
-      </c>
-      <c r="E28" s="34">
-        <v>1</v>
-      </c>
-      <c r="F28" s="34">
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
         <v>3</v>
       </c>
-      <c r="G28" s="34">
+      <c r="G28">
         <v>6</v>
       </c>
-      <c r="H28" s="34">
+      <c r="H28">
         <v>2</v>
       </c>
-      <c r="I28" s="34">
+      <c r="I28">
         <v>5</v>
       </c>
-      <c r="J28" s="34">
+      <c r="J28">
         <v>3</v>
       </c>
-      <c r="K28" s="34">
-        <v>1</v>
-      </c>
-      <c r="L28" s="34">
-        <v>1</v>
-      </c>
-      <c r="M28" s="34">
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
         <v>5</v>
       </c>
-      <c r="N28" s="34">
-        <v>1</v>
-      </c>
-      <c r="O28" s="34">
-        <v>1</v>
-      </c>
-      <c r="P28" s="34">
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28">
         <v>3</v>
       </c>
-      <c r="Q28" s="34">
-        <v>1</v>
-      </c>
-      <c r="R28" s="34">
+      <c r="Q28">
+        <v>1</v>
+      </c>
+      <c r="R28">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Spell mapping to images
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7847FAFD-F30C-4704-ACAA-108C0ED269D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A58C2D8-9CCB-4806-B76D-5A03FEB115FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="6" activeTab="10" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="10" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
   <sheets>
     <sheet name="Bullshit scroll price tinkering" sheetId="1" r:id="rId1"/>
@@ -24,13 +24,13 @@
     <sheet name="Spell Boosts" sheetId="11" r:id="rId9"/>
     <sheet name="Potions" sheetId="8" r:id="rId10"/>
     <sheet name="Missing Potions" sheetId="10" r:id="rId11"/>
-    <sheet name="Potions (IWD2)" sheetId="9" r:id="rId12"/>
+    <sheet name="Mapping Potion Art to Spells" sheetId="13" r:id="rId12"/>
+    <sheet name="Potions (IWD2)" sheetId="9" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId13"/>
+    <pivotCache cacheId="1" r:id="rId14"/>
   </pivotCaches>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10471" uniqueCount="1687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11125" uniqueCount="1874">
   <si>
     <t>Caster Level</t>
   </si>
@@ -5101,6 +5101,567 @@
   </si>
   <si>
     <t>Snowball</t>
+  </si>
+  <si>
+    <t>potion-ai-001.png</t>
+  </si>
+  <si>
+    <t>potion-ai-002.png</t>
+  </si>
+  <si>
+    <t>potion-ai-003.png</t>
+  </si>
+  <si>
+    <t>potion-ai-004.png</t>
+  </si>
+  <si>
+    <t>potion-ai-004a.png</t>
+  </si>
+  <si>
+    <t>potion-ai-004b.png</t>
+  </si>
+  <si>
+    <t>potion-ai-004c.png</t>
+  </si>
+  <si>
+    <t>potion-ai-004d.png</t>
+  </si>
+  <si>
+    <t>potion-ai-005.png</t>
+  </si>
+  <si>
+    <t>potion-ai-006.png</t>
+  </si>
+  <si>
+    <t>potion-ai-007.png</t>
+  </si>
+  <si>
+    <t>potion-ai-007a.png</t>
+  </si>
+  <si>
+    <t>potion-ai-007b.png</t>
+  </si>
+  <si>
+    <t>potion-ai-007c.png</t>
+  </si>
+  <si>
+    <t>potion-ai-008.png</t>
+  </si>
+  <si>
+    <t>potion-ai-009.png</t>
+  </si>
+  <si>
+    <t>potion-ai-010.png</t>
+  </si>
+  <si>
+    <t>potion-ai-011.png</t>
+  </si>
+  <si>
+    <t>potion-ai-012.png</t>
+  </si>
+  <si>
+    <t>potion-ai-013.png</t>
+  </si>
+  <si>
+    <t>potion-ai-013a.png</t>
+  </si>
+  <si>
+    <t>potion-ai-013b.png</t>
+  </si>
+  <si>
+    <t>potion-ai-013c.png</t>
+  </si>
+  <si>
+    <t>potion-ai-014.png</t>
+  </si>
+  <si>
+    <t>potion-ai-015.png</t>
+  </si>
+  <si>
+    <t>potion-ai-016.png</t>
+  </si>
+  <si>
+    <t>potion-ai-017.png</t>
+  </si>
+  <si>
+    <t>potion-ai-018.png</t>
+  </si>
+  <si>
+    <t>potion-ai-019.png</t>
+  </si>
+  <si>
+    <t>potion-ai-020.png</t>
+  </si>
+  <si>
+    <t>potion-ai-021.png</t>
+  </si>
+  <si>
+    <t>potion-ai-022.png</t>
+  </si>
+  <si>
+    <t>potion-ai-023.png</t>
+  </si>
+  <si>
+    <t>potion-ai-024.png</t>
+  </si>
+  <si>
+    <t>potion-ai-025.png</t>
+  </si>
+  <si>
+    <t>potion-ai-026.png</t>
+  </si>
+  <si>
+    <t>potion-ai-027.png</t>
+  </si>
+  <si>
+    <t>potion-ai-028.png</t>
+  </si>
+  <si>
+    <t>potion-ai-029.png</t>
+  </si>
+  <si>
+    <t>potion-ai-030.png</t>
+  </si>
+  <si>
+    <t>potion-ai-031.png</t>
+  </si>
+  <si>
+    <t>potion-ai-032.png</t>
+  </si>
+  <si>
+    <t>potion-ai-033.png</t>
+  </si>
+  <si>
+    <t>potion-ai-034.png</t>
+  </si>
+  <si>
+    <t>potion-ai-035.png</t>
+  </si>
+  <si>
+    <t>potion-ai-036.png</t>
+  </si>
+  <si>
+    <t>potion-ai-037.png</t>
+  </si>
+  <si>
+    <t>potion-ai-038.png</t>
+  </si>
+  <si>
+    <t>potion-ai-039.png</t>
+  </si>
+  <si>
+    <t>potion-ai-040.png</t>
+  </si>
+  <si>
+    <t>potion-ai-041.png</t>
+  </si>
+  <si>
+    <t>potion-ai-042.png</t>
+  </si>
+  <si>
+    <t>potion-ai-043.png</t>
+  </si>
+  <si>
+    <t>potion-ai-044.png</t>
+  </si>
+  <si>
+    <t>potion-ai-045.png</t>
+  </si>
+  <si>
+    <t>potion-ai-046.png</t>
+  </si>
+  <si>
+    <t>potion-ai-047.png</t>
+  </si>
+  <si>
+    <t>potion-ai-048.png</t>
+  </si>
+  <si>
+    <t>potion-ai-049.png</t>
+  </si>
+  <si>
+    <t>potion-ai-050.png</t>
+  </si>
+  <si>
+    <t>potion-ai-051.png</t>
+  </si>
+  <si>
+    <t>potion-ai-052.png</t>
+  </si>
+  <si>
+    <t>potion-ai-053.png</t>
+  </si>
+  <si>
+    <t>potion-ai-054.png</t>
+  </si>
+  <si>
+    <t>potion-ai-055.png</t>
+  </si>
+  <si>
+    <t>potion-ai-056.png</t>
+  </si>
+  <si>
+    <t>potion-ai-057.png</t>
+  </si>
+  <si>
+    <t>potion-ai-058.png</t>
+  </si>
+  <si>
+    <t>potion-ai-059.png</t>
+  </si>
+  <si>
+    <t>potion-ai-060.png</t>
+  </si>
+  <si>
+    <t>potion-ai-061.png</t>
+  </si>
+  <si>
+    <t>potion-ai-062.png</t>
+  </si>
+  <si>
+    <t>potion-ai-063.png</t>
+  </si>
+  <si>
+    <t>potion-ai-064.png</t>
+  </si>
+  <si>
+    <t>potion-ai-065.png</t>
+  </si>
+  <si>
+    <t>potion-ai-066.png</t>
+  </si>
+  <si>
+    <t>potion-ai-070.png</t>
+  </si>
+  <si>
+    <t>potion-ai-071.png</t>
+  </si>
+  <si>
+    <t>potion-ai-072.png</t>
+  </si>
+  <si>
+    <t>potion-ai-073.png</t>
+  </si>
+  <si>
+    <t>potion-ai-074.png</t>
+  </si>
+  <si>
+    <t>potion-ai-075.png</t>
+  </si>
+  <si>
+    <t>potion-ai-076.png</t>
+  </si>
+  <si>
+    <t>potion-ai-077.png</t>
+  </si>
+  <si>
+    <t>potion-ai-078.png</t>
+  </si>
+  <si>
+    <t>potion-ai-079.png</t>
+  </si>
+  <si>
+    <t>potion-ai-080.png</t>
+  </si>
+  <si>
+    <t>potion-ai-081.png</t>
+  </si>
+  <si>
+    <t>potion-ai-082.png</t>
+  </si>
+  <si>
+    <t>potion-ai-083.png</t>
+  </si>
+  <si>
+    <t>potion-ai-084.png</t>
+  </si>
+  <si>
+    <t>potion-ai-085.png</t>
+  </si>
+  <si>
+    <t>potion-ai-086.png</t>
+  </si>
+  <si>
+    <t>potion-ai-087.png</t>
+  </si>
+  <si>
+    <t>potion-ai-088.png</t>
+  </si>
+  <si>
+    <t>potion-ai-089.png</t>
+  </si>
+  <si>
+    <t>potion-ai-090.png</t>
+  </si>
+  <si>
+    <t>potion-ai-091.png</t>
+  </si>
+  <si>
+    <t>potion-ai-092.png</t>
+  </si>
+  <si>
+    <t>potion-ai-093.png</t>
+  </si>
+  <si>
+    <t>potion-ai-094.png</t>
+  </si>
+  <si>
+    <t>potion-ai-095.png</t>
+  </si>
+  <si>
+    <t>potion-ai-096.png</t>
+  </si>
+  <si>
+    <t>potion-ai-097.png</t>
+  </si>
+  <si>
+    <t>potion-ai-098.png</t>
+  </si>
+  <si>
+    <t>potion-ai-099.png</t>
+  </si>
+  <si>
+    <t>potion-ai-100.png</t>
+  </si>
+  <si>
+    <t>potion-ai-101.png</t>
+  </si>
+  <si>
+    <t>potion-ai-102.png</t>
+  </si>
+  <si>
+    <t>potion-ai-103.png</t>
+  </si>
+  <si>
+    <t>potion-ai-104.png</t>
+  </si>
+  <si>
+    <t>potion-ai-105.png</t>
+  </si>
+  <si>
+    <t>potion-ai-106.png</t>
+  </si>
+  <si>
+    <t>potion-ai-107.png</t>
+  </si>
+  <si>
+    <t>potion-ai-108.png</t>
+  </si>
+  <si>
+    <t>potion-ai-109.png</t>
+  </si>
+  <si>
+    <t>potion-ai-110.png</t>
+  </si>
+  <si>
+    <t>potion-ai-111.png</t>
+  </si>
+  <si>
+    <t>potion-ai-112.png</t>
+  </si>
+  <si>
+    <t>potion-ai-113.png</t>
+  </si>
+  <si>
+    <t>potion-ai-114.png</t>
+  </si>
+  <si>
+    <t>potion-ai-115.png</t>
+  </si>
+  <si>
+    <t>potion-ai-116.png</t>
+  </si>
+  <si>
+    <t>potion-ai-117.png</t>
+  </si>
+  <si>
+    <t>potion-ai-118.png</t>
+  </si>
+  <si>
+    <t>potion-ai-119.png</t>
+  </si>
+  <si>
+    <t>potion-ai-31a.png</t>
+  </si>
+  <si>
+    <t>Art Asset</t>
+  </si>
+  <si>
+    <t>Variable CL effects</t>
+  </si>
+  <si>
+    <t>SPWI113;SPPR107</t>
+  </si>
+  <si>
+    <t>Spell Code</t>
+  </si>
+  <si>
+    <t>Descrption BAM</t>
+  </si>
+  <si>
+    <t>BZPN001I</t>
+  </si>
+  <si>
+    <t>BZPN005I</t>
+  </si>
+  <si>
+    <t>BZPN008I</t>
+  </si>
+  <si>
+    <t>BZPN013I</t>
+  </si>
+  <si>
+    <t>BZPN019I</t>
+  </si>
+  <si>
+    <t>BZPN026I</t>
+  </si>
+  <si>
+    <t>BZPN032I</t>
+  </si>
+  <si>
+    <t>BZPN040I</t>
+  </si>
+  <si>
+    <t>BZPN049I</t>
+  </si>
+  <si>
+    <t>BZPN058I</t>
+  </si>
+  <si>
+    <t>BZPN070I</t>
+  </si>
+  <si>
+    <t>BZPN080I</t>
+  </si>
+  <si>
+    <t>BZPN090I</t>
+  </si>
+  <si>
+    <t>BZPN100I</t>
+  </si>
+  <si>
+    <t>BZPN110I</t>
+  </si>
+  <si>
+    <t>IWDification</t>
+  </si>
+  <si>
+    <t>SPPR303;SPWI326</t>
+  </si>
+  <si>
+    <t>Protection From Fire</t>
+  </si>
+  <si>
+    <t>SPPR307;SPWI410</t>
+  </si>
+  <si>
+    <t>Storm Shield</t>
+  </si>
+  <si>
+    <t>IWD?</t>
+  </si>
+  <si>
+    <t>SPPR505;SPWI609</t>
+  </si>
+  <si>
+    <t>StoneSkin</t>
+  </si>
+  <si>
+    <t>SPWI408;SPPR506</t>
+  </si>
+  <si>
+    <t>not evil</t>
+  </si>
+  <si>
+    <t>Protection From Petrification</t>
+  </si>
+  <si>
+    <t>spwi111</t>
+  </si>
+  <si>
+    <t>olvyn</t>
+  </si>
+  <si>
+    <t>bomb</t>
+  </si>
+  <si>
+    <t>Protection From Normal Missiles</t>
+  </si>
+  <si>
+    <t>Fireshield Blue</t>
+  </si>
+  <si>
+    <t>Spell Immunity: Abjuration</t>
+  </si>
+  <si>
+    <t>SPWI590</t>
+  </si>
+  <si>
+    <t>Spell Immunity: Divination</t>
+  </si>
+  <si>
+    <t>SPWI592</t>
+  </si>
+  <si>
+    <t>Spell Immunity: Conjuration</t>
+  </si>
+  <si>
+    <t>SPWI591</t>
+  </si>
+  <si>
+    <t>Spell Immunity: Enchantment</t>
+  </si>
+  <si>
+    <t>SPWI593</t>
+  </si>
+  <si>
+    <t>Spell Immunity: Illusion</t>
+  </si>
+  <si>
+    <t>SPWI594</t>
+  </si>
+  <si>
+    <t>Spell Immunity: Evocation</t>
+  </si>
+  <si>
+    <t>SPWI595</t>
+  </si>
+  <si>
+    <t>Spell Immunity: Necromancy</t>
+  </si>
+  <si>
+    <t>SPWI596</t>
+  </si>
+  <si>
+    <t>SPWI597</t>
+  </si>
+  <si>
+    <t>Spell Immunity: Alteration</t>
+  </si>
+  <si>
+    <t>Protection From Normal Weapons</t>
+  </si>
+  <si>
+    <t>Protection From Electricity</t>
+  </si>
+  <si>
+    <t>Protection From Acid</t>
+  </si>
+  <si>
+    <t>Protection From Magic Energy</t>
+  </si>
+  <si>
+    <t>Protection From Magical Weapons</t>
+  </si>
+  <si>
+    <t>SPPR701;SPWI618</t>
+  </si>
+  <si>
+    <t>Spell Defelection</t>
+  </si>
+  <si>
+    <t>Protection From the Elements</t>
   </si>
 </sst>
 </file>
@@ -5605,7 +6166,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F3C0FD81-EC5D-4C31-9DDA-F8F6B464BBF6}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F3C0FD81-EC5D-4C31-9DDA-F8F6B464BBF6}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:R28" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
@@ -8041,8 +8602,8 @@
   <dimension ref="A1:C100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C72" sqref="C72"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A100" sqref="A73:A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -9052,6 +9613,2619 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90FF5842-5F39-42CA-813E-70DCD245FAB4}">
+  <dimension ref="A1:G128"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B129" sqref="B129"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="23" t="s">
+        <v>1814</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1566</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>1817</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>1676</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>1815</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>1818</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>1687</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1679</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>1689</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1866</v>
+      </c>
+      <c r="C4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>1690</v>
+      </c>
+      <c r="B5" t="s">
+        <v>940</v>
+      </c>
+      <c r="C5" t="s">
+        <v>938</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1679</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1011</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1677</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1850</v>
+      </c>
+      <c r="C8" t="s">
+        <v>224</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1819</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B11" t="s">
+        <v>656</v>
+      </c>
+      <c r="C11" t="s">
+        <v>293</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>1697</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C12" t="s">
+        <v>977</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>1698</v>
+      </c>
+      <c r="B13" t="s">
+        <v>269</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>1699</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1835</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1680</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>1701</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1867</v>
+      </c>
+      <c r="C16" t="s">
+        <v>226</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>1702</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1836</v>
+      </c>
+      <c r="C17" t="s">
+        <v>996</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>1703</v>
+      </c>
+      <c r="B18" t="s">
+        <v>947</v>
+      </c>
+      <c r="C18" t="s">
+        <v>955</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E18" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>1704</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1868</v>
+      </c>
+      <c r="C19" t="s">
+        <v>231</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>1705</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>1706</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1847</v>
+      </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>1707</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E22" t="b">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>1708</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>1709</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1247</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>1710</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B26" t="s">
+        <v>943</v>
+      </c>
+      <c r="C26" t="s">
+        <v>951</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1680</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>1712</v>
+      </c>
+      <c r="B27" t="s">
+        <v>259</v>
+      </c>
+      <c r="C27" t="s">
+        <v>252</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1251</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>1714</v>
+      </c>
+      <c r="B29" t="s">
+        <v>197</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B30" t="s">
+        <v>960</v>
+      </c>
+      <c r="C30" t="s">
+        <v>969</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>1716</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1245</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E32" t="b">
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1823</v>
+      </c>
+      <c r="G32" t="s">
+        <v>1843</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B33" t="s">
+        <v>198</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E34" t="b">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1852</v>
+      </c>
+      <c r="C35" t="s">
+        <v>224</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1823</v>
+      </c>
+      <c r="G35" t="s">
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>1721</v>
+      </c>
+      <c r="B36" t="s">
+        <v>315</v>
+      </c>
+      <c r="C36" t="s">
+        <v>186</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>1722</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>1723</v>
+      </c>
+      <c r="B38" t="s">
+        <v>636</v>
+      </c>
+      <c r="C38" t="s">
+        <v>277</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E38" t="b">
+        <v>0</v>
+      </c>
+      <c r="F38" t="s">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1838</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E39" t="b">
+        <v>0</v>
+      </c>
+      <c r="F39" t="s">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>1725</v>
+      </c>
+      <c r="B40" t="s">
+        <v>957</v>
+      </c>
+      <c r="C40" t="s">
+        <v>959</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E40" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1869</v>
+      </c>
+      <c r="C41" t="s">
+        <v>243</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>1727</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E42" t="b">
+        <v>0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>1813</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E43" t="b">
+        <v>0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>1824</v>
+      </c>
+      <c r="G43" t="s">
+        <v>1834</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>1728</v>
+      </c>
+      <c r="B44" t="s">
+        <v>630</v>
+      </c>
+      <c r="C44" t="s">
+        <v>270</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E44" t="b">
+        <v>1</v>
+      </c>
+      <c r="F44" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>1729</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E45" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>1730</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1860</v>
+      </c>
+      <c r="C46" t="s">
+        <v>224</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E46" t="b">
+        <v>1</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1825</v>
+      </c>
+      <c r="G46" t="s">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
+        <v>1731</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E47" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" t="s">
+        <v>1732</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E48" t="b">
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>1733</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1839</v>
+      </c>
+      <c r="D49" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E49" t="b">
+        <v>0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>1734</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1842</v>
+      </c>
+      <c r="D50" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E50" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>1735</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D51" t="s">
+        <v>1679</v>
+      </c>
+      <c r="E51" t="b">
+        <v>0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>1736</v>
+      </c>
+      <c r="B52" t="s">
+        <v>968</v>
+      </c>
+      <c r="C52" t="s">
+        <v>982</v>
+      </c>
+      <c r="D52" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E52" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>1737</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1569</v>
+      </c>
+      <c r="C53" t="s">
+        <v>207</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E53" t="b">
+        <v>1</v>
+      </c>
+      <c r="F53" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1844</v>
+      </c>
+      <c r="C54" t="s">
+        <v>26</v>
+      </c>
+      <c r="D54" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E54" t="b">
+        <v>0</v>
+      </c>
+      <c r="F54" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
+        <v>1739</v>
+      </c>
+      <c r="B55" t="s">
+        <v>216</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D55" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>1740</v>
+      </c>
+      <c r="B56" t="s">
+        <v>77</v>
+      </c>
+      <c r="C56" t="s">
+        <v>58</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E56" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
+        <v>1741</v>
+      </c>
+      <c r="B57" t="s">
+        <v>577</v>
+      </c>
+      <c r="C57" t="s">
+        <v>206</v>
+      </c>
+      <c r="D57" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E57" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" t="s">
+        <v>1742</v>
+      </c>
+      <c r="B58" t="s">
+        <v>260</v>
+      </c>
+      <c r="C58" t="s">
+        <v>251</v>
+      </c>
+      <c r="D58" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E58" t="b">
+        <v>0</v>
+      </c>
+      <c r="F58" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B59" t="s">
+        <v>604</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1840</v>
+      </c>
+      <c r="D59" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E59" t="b">
+        <v>0</v>
+      </c>
+      <c r="F59" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D60" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E60" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" t="s">
+        <v>1745</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D61" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E61" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>1746</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D62" t="s">
+        <v>1679</v>
+      </c>
+      <c r="E62" t="b">
+        <v>0</v>
+      </c>
+      <c r="F62" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>1747</v>
+      </c>
+      <c r="B63" t="s">
+        <v>606</v>
+      </c>
+      <c r="C63" t="s">
+        <v>250</v>
+      </c>
+      <c r="D63" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E63" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B64" t="s">
+        <v>218</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E64" t="b">
+        <v>0</v>
+      </c>
+      <c r="F64" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" t="s">
+        <v>1749</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D65" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E65" t="b">
+        <v>0</v>
+      </c>
+      <c r="F65" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" t="s">
+        <v>1750</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1870</v>
+      </c>
+      <c r="C66" t="s">
+        <v>248</v>
+      </c>
+      <c r="D66" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E66" t="b">
+        <v>0</v>
+      </c>
+      <c r="F66" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" t="s">
+        <v>1751</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1092</v>
+      </c>
+      <c r="D67" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E67" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" t="s">
+        <v>1752</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1845</v>
+      </c>
+      <c r="D68" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E68" t="b">
+        <v>0</v>
+      </c>
+      <c r="F68" t="s">
+        <v>1827</v>
+      </c>
+      <c r="G68" t="s">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
+        <v>1753</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1662</v>
+      </c>
+      <c r="C69" t="s">
+        <v>108</v>
+      </c>
+      <c r="D69" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E69" t="b">
+        <v>1</v>
+      </c>
+      <c r="F69" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" t="s">
+        <v>1754</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1858</v>
+      </c>
+      <c r="C70" t="s">
+        <v>224</v>
+      </c>
+      <c r="D70" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E70" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" t="s">
+        <v>1828</v>
+      </c>
+      <c r="G70" t="s">
+        <v>1859</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" t="s">
+        <v>1755</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1164</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E71" t="b">
+        <v>0</v>
+      </c>
+      <c r="F71" t="s">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" t="s">
+        <v>1756</v>
+      </c>
+      <c r="B72" t="s">
+        <v>125</v>
+      </c>
+      <c r="C72" t="s">
+        <v>110</v>
+      </c>
+      <c r="D72" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E72" t="b">
+        <v>0</v>
+      </c>
+      <c r="F72" t="s">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" t="s">
+        <v>1757</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D73" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E73" t="b">
+        <v>0</v>
+      </c>
+      <c r="F73" t="s">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" t="s">
+        <v>1758</v>
+      </c>
+      <c r="B74" t="s">
+        <v>961</v>
+      </c>
+      <c r="C74" t="s">
+        <v>970</v>
+      </c>
+      <c r="D74" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E74" t="b">
+        <v>0</v>
+      </c>
+      <c r="F74" t="s">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" t="s">
+        <v>1759</v>
+      </c>
+      <c r="B75" t="s">
+        <v>600</v>
+      </c>
+      <c r="C75" t="s">
+        <v>591</v>
+      </c>
+      <c r="D75" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E75" t="b">
+        <v>1</v>
+      </c>
+      <c r="F75" t="s">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" t="s">
+        <v>1760</v>
+      </c>
+      <c r="B76" t="s">
+        <v>152</v>
+      </c>
+      <c r="C76" t="s">
+        <v>139</v>
+      </c>
+      <c r="D76" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E76" t="b">
+        <v>0</v>
+      </c>
+      <c r="F76" t="s">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" t="s">
+        <v>1761</v>
+      </c>
+      <c r="B77" t="s">
+        <v>79</v>
+      </c>
+      <c r="C77" t="s">
+        <v>60</v>
+      </c>
+      <c r="D77" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E77" t="b">
+        <v>0</v>
+      </c>
+      <c r="F77" t="s">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" t="s">
+        <v>1762</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1873</v>
+      </c>
+      <c r="C78" t="s">
+        <v>271</v>
+      </c>
+      <c r="D78" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E78" t="b">
+        <v>1</v>
+      </c>
+      <c r="F78" t="s">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" t="s">
+        <v>1763</v>
+      </c>
+      <c r="B79" t="s">
+        <v>49</v>
+      </c>
+      <c r="C79" t="s">
+        <v>32</v>
+      </c>
+      <c r="D79" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E79" t="b">
+        <v>0</v>
+      </c>
+      <c r="F79" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" t="s">
+        <v>1764</v>
+      </c>
+      <c r="B80" t="s">
+        <v>682</v>
+      </c>
+      <c r="C80" t="s">
+        <v>519</v>
+      </c>
+      <c r="D80" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E80" t="b">
+        <v>0</v>
+      </c>
+      <c r="F80" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" t="s">
+        <v>1765</v>
+      </c>
+      <c r="B81" t="s">
+        <v>146</v>
+      </c>
+      <c r="C81" t="s">
+        <v>132</v>
+      </c>
+      <c r="D81" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E81" t="b">
+        <v>1</v>
+      </c>
+      <c r="F81" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" t="s">
+        <v>1766</v>
+      </c>
+      <c r="B82" t="s">
+        <v>82</v>
+      </c>
+      <c r="C82" t="s">
+        <v>64</v>
+      </c>
+      <c r="D82" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E82" t="b">
+        <v>0</v>
+      </c>
+      <c r="F82" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" t="s">
+        <v>1767</v>
+      </c>
+      <c r="B83" t="s">
+        <v>153</v>
+      </c>
+      <c r="C83" t="s">
+        <v>140</v>
+      </c>
+      <c r="D83" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E83" t="b">
+        <v>0</v>
+      </c>
+      <c r="F83" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" t="s">
+        <v>1768</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1872</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1871</v>
+      </c>
+      <c r="D84" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E84" t="b">
+        <v>1</v>
+      </c>
+      <c r="F84" t="s">
+        <v>1829</v>
+      </c>
+      <c r="G84" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" t="s">
+        <v>1769</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1839</v>
+      </c>
+      <c r="D85" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E85" t="b">
+        <v>0</v>
+      </c>
+      <c r="F85" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" t="s">
+        <v>1770</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D86" t="s">
+        <v>1679</v>
+      </c>
+      <c r="E86" t="b">
+        <v>0</v>
+      </c>
+      <c r="F86" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" t="s">
+        <v>1771</v>
+      </c>
+      <c r="B87" t="s">
+        <v>149</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1837</v>
+      </c>
+      <c r="D87" t="s">
+        <v>1679</v>
+      </c>
+      <c r="E87" t="b">
+        <v>0</v>
+      </c>
+      <c r="F87" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" t="s">
+        <v>1772</v>
+      </c>
+      <c r="B88" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C88" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D88" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E88" t="b">
+        <v>0</v>
+      </c>
+      <c r="F88" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" t="s">
+        <v>1773</v>
+      </c>
+      <c r="B89" t="s">
+        <v>1865</v>
+      </c>
+      <c r="C89" t="s">
+        <v>224</v>
+      </c>
+      <c r="D89" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E89" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" t="s">
+        <v>1830</v>
+      </c>
+      <c r="G89" t="s">
+        <v>1864</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B90" t="s">
+        <v>1849</v>
+      </c>
+      <c r="C90" t="s">
+        <v>129</v>
+      </c>
+      <c r="D90" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E90" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" t="s">
+        <v>1775</v>
+      </c>
+      <c r="B91" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C91" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D91" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E91" t="b">
+        <v>0</v>
+      </c>
+      <c r="F91" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B92" t="s">
+        <v>562</v>
+      </c>
+      <c r="C92" t="s">
+        <v>204</v>
+      </c>
+      <c r="D92" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E92" t="b">
+        <v>1</v>
+      </c>
+      <c r="F92" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B93" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C93" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D93" t="s">
+        <v>1679</v>
+      </c>
+      <c r="E93" t="b">
+        <v>0</v>
+      </c>
+      <c r="F93" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B94" t="s">
+        <v>990</v>
+      </c>
+      <c r="C94" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D94" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E94" t="b">
+        <v>0</v>
+      </c>
+      <c r="F94" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B95" t="s">
+        <v>679</v>
+      </c>
+      <c r="C95" t="s">
+        <v>514</v>
+      </c>
+      <c r="D95" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E95" t="b">
+        <v>0</v>
+      </c>
+      <c r="F95" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" t="s">
+        <v>1780</v>
+      </c>
+      <c r="B96" t="s">
+        <v>84</v>
+      </c>
+      <c r="C96" t="s">
+        <v>66</v>
+      </c>
+      <c r="D96" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E96" t="b">
+        <v>0</v>
+      </c>
+      <c r="F96" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" t="s">
+        <v>1781</v>
+      </c>
+      <c r="B97" t="s">
+        <v>48</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1816</v>
+      </c>
+      <c r="D97" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E97" t="b">
+        <v>1</v>
+      </c>
+      <c r="F97" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" t="s">
+        <v>1782</v>
+      </c>
+      <c r="B98" t="s">
+        <v>145</v>
+      </c>
+      <c r="C98" t="s">
+        <v>131</v>
+      </c>
+      <c r="D98" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E98" t="b">
+        <v>1</v>
+      </c>
+      <c r="F98" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" t="s">
+        <v>1783</v>
+      </c>
+      <c r="B99" t="s">
+        <v>830</v>
+      </c>
+      <c r="C99" t="s">
+        <v>103</v>
+      </c>
+      <c r="D99" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E99" t="b">
+        <v>0</v>
+      </c>
+      <c r="F99" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" t="s">
+        <v>1784</v>
+      </c>
+      <c r="B100" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C100" t="s">
+        <v>1232</v>
+      </c>
+      <c r="D100" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E100" t="b">
+        <v>1</v>
+      </c>
+      <c r="F100" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101" t="s">
+        <v>1785</v>
+      </c>
+      <c r="B101" t="s">
+        <v>88</v>
+      </c>
+      <c r="C101" t="s">
+        <v>70</v>
+      </c>
+      <c r="D101" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E101" t="b">
+        <v>0</v>
+      </c>
+      <c r="F101" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B102" t="s">
+        <v>9</v>
+      </c>
+      <c r="C102" t="s">
+        <v>1173</v>
+      </c>
+      <c r="D102" t="s">
+        <v>1679</v>
+      </c>
+      <c r="E102" t="b">
+        <v>0</v>
+      </c>
+      <c r="F102" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" t="s">
+        <v>1787</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1856</v>
+      </c>
+      <c r="C103" t="s">
+        <v>224</v>
+      </c>
+      <c r="D103" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E103" t="b">
+        <v>1</v>
+      </c>
+      <c r="F103" t="s">
+        <v>1831</v>
+      </c>
+      <c r="G103" t="s">
+        <v>1857</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" t="s">
+        <v>1788</v>
+      </c>
+      <c r="B104" t="s">
+        <v>1848</v>
+      </c>
+      <c r="C104" t="s">
+        <v>104</v>
+      </c>
+      <c r="D104" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E104" t="b">
+        <v>0</v>
+      </c>
+      <c r="F104" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" t="s">
+        <v>1789</v>
+      </c>
+      <c r="B105" t="s">
+        <v>963</v>
+      </c>
+      <c r="C105" t="s">
+        <v>972</v>
+      </c>
+      <c r="D105" t="s">
+        <v>1677</v>
+      </c>
+      <c r="F105" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" t="s">
+        <v>1790</v>
+      </c>
+      <c r="B106" t="s">
+        <v>1854</v>
+      </c>
+      <c r="C106" t="s">
+        <v>224</v>
+      </c>
+      <c r="D106" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E106" t="b">
+        <v>1</v>
+      </c>
+      <c r="F106" t="s">
+        <v>1831</v>
+      </c>
+      <c r="G106" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B107" t="s">
+        <v>90</v>
+      </c>
+      <c r="C107" t="s">
+        <v>72</v>
+      </c>
+      <c r="D107" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E107" t="b">
+        <v>0</v>
+      </c>
+      <c r="F107" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B108" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C108" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D108" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E108" t="b">
+        <v>0</v>
+      </c>
+      <c r="F108" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="A109" t="s">
+        <v>1793</v>
+      </c>
+      <c r="B109" t="s">
+        <v>200</v>
+      </c>
+      <c r="C109" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D109" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E109" t="b">
+        <v>1</v>
+      </c>
+      <c r="F109" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" t="s">
+        <v>1794</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1862</v>
+      </c>
+      <c r="C110" t="s">
+        <v>224</v>
+      </c>
+      <c r="D110" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E110" t="b">
+        <v>1</v>
+      </c>
+      <c r="F110" t="s">
+        <v>1832</v>
+      </c>
+      <c r="G110" t="s">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" t="s">
+        <v>1795</v>
+      </c>
+      <c r="B111" t="s">
+        <v>113</v>
+      </c>
+      <c r="C111" t="s">
+        <v>97</v>
+      </c>
+      <c r="D111" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E111" t="b">
+        <v>1</v>
+      </c>
+      <c r="F111" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B112" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C112" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D112" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E112" t="b">
+        <v>1</v>
+      </c>
+      <c r="F112" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" t="s">
+        <v>1797</v>
+      </c>
+      <c r="B113" t="s">
+        <v>151</v>
+      </c>
+      <c r="C113" t="s">
+        <v>138</v>
+      </c>
+      <c r="D113" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E113" t="b">
+        <v>1</v>
+      </c>
+      <c r="F113" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B114" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C114" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D114" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E114" t="b">
+        <v>0</v>
+      </c>
+      <c r="F114" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115" t="s">
+        <v>1799</v>
+      </c>
+      <c r="B115" t="s">
+        <v>563</v>
+      </c>
+      <c r="C115" t="s">
+        <v>568</v>
+      </c>
+      <c r="D115" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E115" t="b">
+        <v>1</v>
+      </c>
+      <c r="F115" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
+      <c r="A116" t="s">
+        <v>1800</v>
+      </c>
+      <c r="B116" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C116" t="s">
+        <v>1290</v>
+      </c>
+      <c r="D116" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E116" t="b">
+        <v>1</v>
+      </c>
+      <c r="F116" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
+      <c r="A117" t="s">
+        <v>1801</v>
+      </c>
+      <c r="B117" t="s">
+        <v>660</v>
+      </c>
+      <c r="C117" t="s">
+        <v>298</v>
+      </c>
+      <c r="D117" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E117" t="b">
+        <v>0</v>
+      </c>
+      <c r="F117" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
+      <c r="A118" t="s">
+        <v>1802</v>
+      </c>
+      <c r="B118" t="s">
+        <v>258</v>
+      </c>
+      <c r="C118" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D118" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E118" t="b">
+        <v>0</v>
+      </c>
+      <c r="F118" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
+      <c r="A119" t="s">
+        <v>1803</v>
+      </c>
+      <c r="B119" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C119" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D119" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E119" t="b">
+        <v>1</v>
+      </c>
+      <c r="F119" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
+      <c r="A120" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B120" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C120" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D120" t="s">
+        <v>1679</v>
+      </c>
+      <c r="E120" t="b">
+        <v>0</v>
+      </c>
+      <c r="F120" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="A121" t="s">
+        <v>1805</v>
+      </c>
+      <c r="B121" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C121" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D121" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E121" t="b">
+        <v>0</v>
+      </c>
+      <c r="F121" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
+      <c r="A122" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B122" t="s">
+        <v>85</v>
+      </c>
+      <c r="C122" t="s">
+        <v>67</v>
+      </c>
+      <c r="D122" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E122" t="b">
+        <v>0</v>
+      </c>
+      <c r="F122" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
+      <c r="A123" t="s">
+        <v>1807</v>
+      </c>
+      <c r="B123" t="s">
+        <v>89</v>
+      </c>
+      <c r="C123" t="s">
+        <v>71</v>
+      </c>
+      <c r="D123" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E123" t="b">
+        <v>1</v>
+      </c>
+      <c r="F123" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="A124" t="s">
+        <v>1808</v>
+      </c>
+      <c r="B124" t="s">
+        <v>1862</v>
+      </c>
+      <c r="C124" t="s">
+        <v>224</v>
+      </c>
+      <c r="D124" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E124" t="b">
+        <v>1</v>
+      </c>
+      <c r="F124" t="s">
+        <v>1833</v>
+      </c>
+      <c r="G124" t="s">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
+      <c r="A125" t="s">
+        <v>1809</v>
+      </c>
+      <c r="B125" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C125" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D125" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E125" t="b">
+        <v>0</v>
+      </c>
+      <c r="F125" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7">
+      <c r="A126" t="s">
+        <v>1810</v>
+      </c>
+      <c r="B126" t="s">
+        <v>87</v>
+      </c>
+      <c r="C126" t="s">
+        <v>69</v>
+      </c>
+      <c r="D126" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E126" t="b">
+        <v>1</v>
+      </c>
+      <c r="F126" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7">
+      <c r="A127" t="s">
+        <v>1811</v>
+      </c>
+      <c r="B127" t="s">
+        <v>596</v>
+      </c>
+      <c r="C127" t="s">
+        <v>232</v>
+      </c>
+      <c r="D127" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E127" t="b">
+        <v>1</v>
+      </c>
+      <c r="F127" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7">
+      <c r="A128" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B128" t="s">
+        <v>695</v>
+      </c>
+      <c r="C128" t="s">
+        <v>674</v>
+      </c>
+      <c r="D128" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E128" t="b">
+        <v>0</v>
+      </c>
+      <c r="F128" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05603EAD-B631-40FE-8A80-8AC165205E14}">
   <dimension ref="A1:J67"/>
   <sheetViews>

</xml_diff>

<commit_message>
Mapping OlvynSpells to potion images
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A58C2D8-9CCB-4806-B76D-5A03FEB115FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29ADF9FB-CEFF-43C5-858C-44DCF058DBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="10" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
   <sheets>
     <sheet name="Bullshit scroll price tinkering" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11125" uniqueCount="1874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11330" uniqueCount="1961">
   <si>
     <t>Caster Level</t>
   </si>
@@ -5662,6 +5662,267 @@
   </si>
   <si>
     <t>Protection From the Elements</t>
+  </si>
+  <si>
+    <t>potion-ai-120.png</t>
+  </si>
+  <si>
+    <t>potion-ai-121.png</t>
+  </si>
+  <si>
+    <t>potion-ai-122.png</t>
+  </si>
+  <si>
+    <t>potion-ai-123.png</t>
+  </si>
+  <si>
+    <t>potion-ai-124.png</t>
+  </si>
+  <si>
+    <t>potion-ai-125.png</t>
+  </si>
+  <si>
+    <t>potion-ai-126.png</t>
+  </si>
+  <si>
+    <t>potion-ai-127.png</t>
+  </si>
+  <si>
+    <t>potion-ai-128.png</t>
+  </si>
+  <si>
+    <t>potion-ai-129.png</t>
+  </si>
+  <si>
+    <t>potion-ai-130.png</t>
+  </si>
+  <si>
+    <t>potion-ai-131.png</t>
+  </si>
+  <si>
+    <t>potion-ai-132.png</t>
+  </si>
+  <si>
+    <t>potion-ai-133.png</t>
+  </si>
+  <si>
+    <t>potion-ai-133a.png</t>
+  </si>
+  <si>
+    <t>potion-ai-134.png</t>
+  </si>
+  <si>
+    <t>potion-ai-135.png</t>
+  </si>
+  <si>
+    <t>potion-ai-136.png</t>
+  </si>
+  <si>
+    <t>potion-ai-137.png</t>
+  </si>
+  <si>
+    <t>potion-ai-138.png</t>
+  </si>
+  <si>
+    <t>potion-ai-139.png</t>
+  </si>
+  <si>
+    <t>potion-ai-140.png</t>
+  </si>
+  <si>
+    <t>potion-ai-141.png</t>
+  </si>
+  <si>
+    <t>potion-ai-142.png</t>
+  </si>
+  <si>
+    <t>potion-ai-143.png</t>
+  </si>
+  <si>
+    <t>potion-ai-144.png</t>
+  </si>
+  <si>
+    <t>potion-ai-145.png</t>
+  </si>
+  <si>
+    <t>potion-ai-146.png</t>
+  </si>
+  <si>
+    <t>potion-ai-147.png</t>
+  </si>
+  <si>
+    <t>potion-ai-148.png</t>
+  </si>
+  <si>
+    <t>potion-ai-149.png</t>
+  </si>
+  <si>
+    <t>potion-ai-150.png</t>
+  </si>
+  <si>
+    <t>potion-ai-151.png</t>
+  </si>
+  <si>
+    <t>potion-ai-152.png</t>
+  </si>
+  <si>
+    <t>potion-ai-153.png</t>
+  </si>
+  <si>
+    <t>potion-ai-154.png</t>
+  </si>
+  <si>
+    <t>potion-ai-155.png</t>
+  </si>
+  <si>
+    <t>potion-ai-156.png</t>
+  </si>
+  <si>
+    <t>potion-ai-157.png</t>
+  </si>
+  <si>
+    <t>potion-ai-158.png</t>
+  </si>
+  <si>
+    <t>potion-ai-159.png</t>
+  </si>
+  <si>
+    <t>MEPR255;MEWI252</t>
+  </si>
+  <si>
+    <t>BZPN120I</t>
+  </si>
+  <si>
+    <t>BZPN130I</t>
+  </si>
+  <si>
+    <t>BZPN140I</t>
+  </si>
+  <si>
+    <t>BZPN150I</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>MEWI158</t>
+  </si>
+  <si>
+    <t>MEWI352;MEPR357</t>
+  </si>
+  <si>
+    <t>MEWI353</t>
+  </si>
+  <si>
+    <t>MEWI356</t>
+  </si>
+  <si>
+    <t>MEWI555</t>
+  </si>
+  <si>
+    <t>Ghostform</t>
+  </si>
+  <si>
+    <t>MEWI559</t>
+  </si>
+  <si>
+    <t>MEWI566</t>
+  </si>
+  <si>
+    <t>Omnipresence</t>
+  </si>
+  <si>
+    <t>MEWI855</t>
+  </si>
+  <si>
+    <t>SPWI857</t>
+  </si>
+  <si>
+    <t>MEWI951</t>
+  </si>
+  <si>
+    <t>MEWI953</t>
+  </si>
+  <si>
+    <t>MEWI960</t>
+  </si>
+  <si>
+    <t>MEPWI963</t>
+  </si>
+  <si>
+    <t>Camoflage</t>
+  </si>
+  <si>
+    <t>MEPR156</t>
+  </si>
+  <si>
+    <t>MEPR151</t>
+  </si>
+  <si>
+    <t>MEPR154</t>
+  </si>
+  <si>
+    <t>MEPR356</t>
+  </si>
+  <si>
+    <t>MEWI455</t>
+  </si>
+  <si>
+    <t>SPWI702;MEPR553</t>
+  </si>
+  <si>
+    <t>MEPR557</t>
+  </si>
+  <si>
+    <t>requires 6 potions :-/</t>
+  </si>
+  <si>
+    <t>Sphere of Protection from Fire</t>
+  </si>
+  <si>
+    <t>MESOS01</t>
+  </si>
+  <si>
+    <t>MEPR558</t>
+  </si>
+  <si>
+    <t>Sphere of Protection from Cold</t>
+  </si>
+  <si>
+    <t>MESOS02</t>
+  </si>
+  <si>
+    <t>Sphere of Protection from Electricity</t>
+  </si>
+  <si>
+    <t>MESOS03</t>
+  </si>
+  <si>
+    <t>Sphere of Protection from Acid</t>
+  </si>
+  <si>
+    <t>MESOS04</t>
+  </si>
+  <si>
+    <t>Sphere of Protection from Poison</t>
+  </si>
+  <si>
+    <t>MESOS05</t>
+  </si>
+  <si>
+    <t>Sphere of Protection from Petrification</t>
+  </si>
+  <si>
+    <t>MESOS06</t>
+  </si>
+  <si>
+    <t>MEPR653</t>
+  </si>
+  <si>
+    <t>MEPR656</t>
+  </si>
+  <si>
+    <t>MEPR754</t>
   </si>
 </sst>
 </file>
@@ -8599,11 +8860,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97994022-E0D3-4848-B3E3-1B87FDCE7E6E}">
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A100" sqref="A73:A100"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -9306,7 +9567,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>1271</v>
       </c>
@@ -9317,7 +9578,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>1583</v>
       </c>
@@ -9328,7 +9589,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>1199</v>
       </c>
@@ -9339,7 +9600,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>1105</v>
       </c>
@@ -9350,7 +9611,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
         <v>1108</v>
       </c>
@@ -9361,7 +9622,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>1155</v>
       </c>
@@ -9372,7 +9633,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
         <v>1686</v>
       </c>
@@ -9383,215 +9644,296 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>1584</v>
       </c>
       <c r="B73" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="74" spans="1:3">
+      <c r="D73" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>1585</v>
       </c>
       <c r="B74" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
+      <c r="D74" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>1586</v>
       </c>
       <c r="B75" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="76" spans="1:3">
+      <c r="D75" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>1587</v>
       </c>
       <c r="B76" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
+      <c r="D76" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
         <v>1588</v>
       </c>
       <c r="B77" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="78" spans="1:3">
+      <c r="D77" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
         <v>1589</v>
       </c>
       <c r="B78" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="79" spans="1:3">
+      <c r="D78" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
         <v>1590</v>
       </c>
       <c r="B79" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="80" spans="1:3">
+      <c r="D79" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
         <v>1591</v>
       </c>
       <c r="B80" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="81" spans="1:2">
+      <c r="D80" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
         <v>1592</v>
       </c>
       <c r="B81" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="82" spans="1:2">
+      <c r="D81" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>1593</v>
       </c>
       <c r="B82" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="83" spans="1:2">
+      <c r="D82" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>1594</v>
       </c>
       <c r="B83" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="84" spans="1:2">
+      <c r="D83" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" t="s">
         <v>1595</v>
       </c>
       <c r="B84" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="85" spans="1:2">
+      <c r="D84" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" t="s">
         <v>1596</v>
       </c>
       <c r="B85" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="86" spans="1:2">
+      <c r="D85" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
         <v>1597</v>
       </c>
       <c r="B86" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="87" spans="1:2">
+      <c r="D86" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
         <v>1598</v>
       </c>
       <c r="B87" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="88" spans="1:2">
+      <c r="D87" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
         <v>1599</v>
       </c>
       <c r="B88" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="89" spans="1:2">
+      <c r="D88" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
         <v>1600</v>
       </c>
       <c r="B89" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="90" spans="1:2">
+      <c r="D89" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>1601</v>
       </c>
       <c r="B90" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="91" spans="1:2">
+      <c r="D90" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>1602</v>
       </c>
       <c r="B91" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="92" spans="1:2">
+      <c r="D91" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>1603</v>
       </c>
       <c r="B92" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="93" spans="1:2">
+      <c r="D92" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
         <v>1604</v>
       </c>
       <c r="B93" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="94" spans="1:2">
+      <c r="D93" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>631</v>
       </c>
       <c r="B94" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="95" spans="1:2">
+      <c r="D94" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
         <v>1605</v>
       </c>
       <c r="B95" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="96" spans="1:2">
+      <c r="D95" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
         <v>1606</v>
       </c>
       <c r="B96" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="97" spans="1:2">
+      <c r="D96" t="s">
+        <v>1920</v>
+      </c>
+      <c r="E96" t="s">
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97" t="s">
         <v>1607</v>
       </c>
       <c r="B97" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="98" spans="1:2">
+      <c r="D97" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
         <v>1608</v>
       </c>
       <c r="B98" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="99" spans="1:2">
+      <c r="D98" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
         <v>1609</v>
       </c>
@@ -9599,7 +9941,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:4">
       <c r="A100" t="s">
         <v>1683</v>
       </c>
@@ -9614,18 +9956,18 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90FF5842-5F39-42CA-813E-70DCD245FAB4}">
-  <dimension ref="A1:G128"/>
+  <dimension ref="A1:G169"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B129" sqref="B129"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H163" sqref="H163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.1796875" bestFit="1" customWidth="1"/>
@@ -11192,7 +11534,7 @@
         <v>1873</v>
       </c>
       <c r="C78" t="s">
-        <v>271</v>
+        <v>1942</v>
       </c>
       <c r="D78" t="s">
         <v>1681</v>
@@ -12217,6 +12559,712 @@
       </c>
       <c r="F128" t="s">
         <v>1833</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7">
+      <c r="A129" t="s">
+        <v>1874</v>
+      </c>
+      <c r="B129" t="s">
+        <v>1593</v>
+      </c>
+      <c r="C129" t="s">
+        <v>1931</v>
+      </c>
+      <c r="D129" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E129" t="b">
+        <v>0</v>
+      </c>
+      <c r="F129" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7">
+      <c r="A130" t="s">
+        <v>1875</v>
+      </c>
+      <c r="B130" t="s">
+        <v>1601</v>
+      </c>
+      <c r="C130" t="s">
+        <v>1939</v>
+      </c>
+      <c r="D130" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E130" t="b">
+        <v>1</v>
+      </c>
+      <c r="F130" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7">
+      <c r="A131" t="s">
+        <v>1876</v>
+      </c>
+      <c r="B131" t="s">
+        <v>1609</v>
+      </c>
+      <c r="C131" t="s">
+        <v>1960</v>
+      </c>
+      <c r="D131" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E131" t="b">
+        <v>0</v>
+      </c>
+      <c r="F131" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7">
+      <c r="A132" t="s">
+        <v>1877</v>
+      </c>
+      <c r="B132" t="s">
+        <v>1599</v>
+      </c>
+      <c r="C132" t="s">
+        <v>1938</v>
+      </c>
+      <c r="D132" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E132" t="b">
+        <v>0</v>
+      </c>
+      <c r="F132" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7">
+      <c r="A133" t="s">
+        <v>1878</v>
+      </c>
+      <c r="B133" t="s">
+        <v>1605</v>
+      </c>
+      <c r="C133" t="s">
+        <v>1943</v>
+      </c>
+      <c r="D133" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E133" t="b">
+        <v>1</v>
+      </c>
+      <c r="F133" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7">
+      <c r="A134" t="s">
+        <v>1879</v>
+      </c>
+      <c r="B134" t="s">
+        <v>1591</v>
+      </c>
+      <c r="C134" t="s">
+        <v>1928</v>
+      </c>
+      <c r="D134" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E134" t="b">
+        <v>1</v>
+      </c>
+      <c r="F134" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7">
+      <c r="A135" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B135" t="s">
+        <v>1956</v>
+      </c>
+      <c r="C135" t="s">
+        <v>1947</v>
+      </c>
+      <c r="D135" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E135" t="b">
+        <v>1</v>
+      </c>
+      <c r="F135" t="s">
+        <v>1916</v>
+      </c>
+      <c r="G135" t="s">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7">
+      <c r="A136" t="s">
+        <v>1881</v>
+      </c>
+      <c r="B136" t="s">
+        <v>1604</v>
+      </c>
+      <c r="C136" t="s">
+        <v>1941</v>
+      </c>
+      <c r="D136" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E136" t="b">
+        <v>1</v>
+      </c>
+      <c r="F136" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7">
+      <c r="A137" t="s">
+        <v>1882</v>
+      </c>
+      <c r="B137" t="s">
+        <v>1926</v>
+      </c>
+      <c r="C137" t="s">
+        <v>1927</v>
+      </c>
+      <c r="D137" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E137" t="b">
+        <v>1</v>
+      </c>
+      <c r="F137" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7">
+      <c r="A138" t="s">
+        <v>1883</v>
+      </c>
+      <c r="B138" t="s">
+        <v>1594</v>
+      </c>
+      <c r="C138" t="s">
+        <v>1932</v>
+      </c>
+      <c r="D138" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E138" t="b">
+        <v>0</v>
+      </c>
+      <c r="F138" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7">
+      <c r="A139" t="s">
+        <v>1884</v>
+      </c>
+      <c r="B139" t="s">
+        <v>1929</v>
+      </c>
+      <c r="C139" t="s">
+        <v>1930</v>
+      </c>
+      <c r="D139" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E139" t="b">
+        <v>0</v>
+      </c>
+      <c r="F139" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7">
+      <c r="A140" t="s">
+        <v>1885</v>
+      </c>
+      <c r="F140" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7">
+      <c r="A141" t="s">
+        <v>1886</v>
+      </c>
+      <c r="B141" t="s">
+        <v>1945</v>
+      </c>
+      <c r="C141" t="s">
+        <v>1947</v>
+      </c>
+      <c r="D141" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E141" t="b">
+        <v>1</v>
+      </c>
+      <c r="F141" t="s">
+        <v>1917</v>
+      </c>
+      <c r="G141" t="s">
+        <v>1946</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7">
+      <c r="A142" t="s">
+        <v>1887</v>
+      </c>
+      <c r="F142" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7">
+      <c r="A143" t="s">
+        <v>1888</v>
+      </c>
+      <c r="B143" t="s">
+        <v>1589</v>
+      </c>
+      <c r="C143" t="s">
+        <v>1925</v>
+      </c>
+      <c r="D143" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E143" t="b">
+        <v>0</v>
+      </c>
+      <c r="F143" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7">
+      <c r="A144" t="s">
+        <v>1889</v>
+      </c>
+      <c r="B144" t="s">
+        <v>1936</v>
+      </c>
+      <c r="C144" t="s">
+        <v>1937</v>
+      </c>
+      <c r="D144" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E144" t="b">
+        <v>0</v>
+      </c>
+      <c r="F144" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7">
+      <c r="A145" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B145" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C145" t="s">
+        <v>1924</v>
+      </c>
+      <c r="D145" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E145" t="b">
+        <v>1</v>
+      </c>
+      <c r="F145" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7">
+      <c r="A146" t="s">
+        <v>1891</v>
+      </c>
+      <c r="F146" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7">
+      <c r="A147" t="s">
+        <v>1892</v>
+      </c>
+      <c r="B147" t="s">
+        <v>1600</v>
+      </c>
+      <c r="C147" t="s">
+        <v>1939</v>
+      </c>
+      <c r="D147" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E147" t="b">
+        <v>0</v>
+      </c>
+      <c r="F147" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7">
+      <c r="A148" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B148" t="s">
+        <v>1585</v>
+      </c>
+      <c r="C148" t="s">
+        <v>1915</v>
+      </c>
+      <c r="D148" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E148" t="b">
+        <v>0</v>
+      </c>
+      <c r="F148" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7">
+      <c r="A149" t="s">
+        <v>1894</v>
+      </c>
+      <c r="F149" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7">
+      <c r="A150" t="s">
+        <v>1895</v>
+      </c>
+      <c r="F150" t="s">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7">
+      <c r="A151" t="s">
+        <v>1896</v>
+      </c>
+      <c r="F151" t="s">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7">
+      <c r="A152" t="s">
+        <v>1897</v>
+      </c>
+      <c r="B152" t="s">
+        <v>1587</v>
+      </c>
+      <c r="C152" t="s">
+        <v>1923</v>
+      </c>
+      <c r="D152" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E152" t="b">
+        <v>1</v>
+      </c>
+      <c r="F152" t="s">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7">
+      <c r="A153" t="s">
+        <v>1898</v>
+      </c>
+      <c r="F153" t="s">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7">
+      <c r="A154" t="s">
+        <v>1899</v>
+      </c>
+      <c r="B154" t="s">
+        <v>1952</v>
+      </c>
+      <c r="C154" t="s">
+        <v>1947</v>
+      </c>
+      <c r="D154" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E154" t="b">
+        <v>1</v>
+      </c>
+      <c r="F154" t="s">
+        <v>1918</v>
+      </c>
+      <c r="G154" t="s">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7">
+      <c r="A155" t="s">
+        <v>1900</v>
+      </c>
+      <c r="B155" t="s">
+        <v>1597</v>
+      </c>
+      <c r="C155" t="s">
+        <v>1935</v>
+      </c>
+      <c r="D155" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E155" t="b">
+        <v>0</v>
+      </c>
+      <c r="F155" t="s">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7">
+      <c r="A156" t="s">
+        <v>1901</v>
+      </c>
+      <c r="F156" t="s">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7">
+      <c r="A157" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B157" t="s">
+        <v>1950</v>
+      </c>
+      <c r="C157" t="s">
+        <v>1947</v>
+      </c>
+      <c r="D157" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E157" t="b">
+        <v>1</v>
+      </c>
+      <c r="F157" t="s">
+        <v>1918</v>
+      </c>
+      <c r="G157" t="s">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7">
+      <c r="A158" t="s">
+        <v>1903</v>
+      </c>
+      <c r="B158" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C158" t="s">
+        <v>1922</v>
+      </c>
+      <c r="D158" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E158" t="b">
+        <v>1</v>
+      </c>
+      <c r="F158" t="s">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7">
+      <c r="A159" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B159" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C159" t="s">
+        <v>1959</v>
+      </c>
+      <c r="D159" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E159" t="b">
+        <v>0</v>
+      </c>
+      <c r="F159" t="s">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7">
+      <c r="A160" t="s">
+        <v>1905</v>
+      </c>
+      <c r="B160" t="s">
+        <v>1584</v>
+      </c>
+      <c r="C160" t="s">
+        <v>1921</v>
+      </c>
+      <c r="D160" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E160" t="b">
+        <v>0</v>
+      </c>
+      <c r="F160" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7">
+      <c r="A161" t="s">
+        <v>1906</v>
+      </c>
+      <c r="F161" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7">
+      <c r="A162" t="s">
+        <v>1907</v>
+      </c>
+      <c r="F162" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7">
+      <c r="A163" t="s">
+        <v>1908</v>
+      </c>
+      <c r="F163" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7">
+      <c r="A164" t="s">
+        <v>1909</v>
+      </c>
+      <c r="B164" t="s">
+        <v>1603</v>
+      </c>
+      <c r="C164" t="s">
+        <v>1940</v>
+      </c>
+      <c r="D164" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E164" t="b">
+        <v>0</v>
+      </c>
+      <c r="F164" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7">
+      <c r="A165" t="s">
+        <v>1910</v>
+      </c>
+      <c r="B165" t="s">
+        <v>1596</v>
+      </c>
+      <c r="C165" t="s">
+        <v>1934</v>
+      </c>
+      <c r="D165" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E165" t="b">
+        <v>1</v>
+      </c>
+      <c r="F165" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7">
+      <c r="A166" t="s">
+        <v>1911</v>
+      </c>
+      <c r="B166" t="s">
+        <v>1595</v>
+      </c>
+      <c r="C166" t="s">
+        <v>1933</v>
+      </c>
+      <c r="D166" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E166" t="b">
+        <v>0</v>
+      </c>
+      <c r="F166" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7">
+      <c r="A167" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B167" t="s">
+        <v>1948</v>
+      </c>
+      <c r="C167" t="s">
+        <v>1947</v>
+      </c>
+      <c r="D167" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E167" t="b">
+        <v>1</v>
+      </c>
+      <c r="F167" t="s">
+        <v>1919</v>
+      </c>
+      <c r="G167" t="s">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7">
+      <c r="A168" t="s">
+        <v>1913</v>
+      </c>
+      <c r="B168" t="s">
+        <v>1607</v>
+      </c>
+      <c r="C168" t="s">
+        <v>1958</v>
+      </c>
+      <c r="D168" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E168" t="b">
+        <v>0</v>
+      </c>
+      <c r="F168" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7">
+      <c r="A169" t="s">
+        <v>1914</v>
+      </c>
+      <c r="B169" t="s">
+        <v>1954</v>
+      </c>
+      <c r="C169" t="s">
+        <v>1947</v>
+      </c>
+      <c r="D169" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E169" t="b">
+        <v>1</v>
+      </c>
+      <c r="F169" t="s">
+        <v>1919</v>
+      </c>
+      <c r="G169" t="s">
+        <v>1955</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mapping icons to potions
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29ADF9FB-CEFF-43C5-858C-44DCF058DBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD86BE27-3A89-48FB-8121-52100ED9C169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="10" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
   <sheets>
     <sheet name="Bullshit scroll price tinkering" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11330" uniqueCount="1961">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11332" uniqueCount="1961">
   <si>
     <t>Caster Level</t>
   </si>
@@ -8862,9 +8862,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97994022-E0D3-4848-B3E3-1B87FDCE7E6E}">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D98" sqref="D98"/>
+      <selection pane="bottomLeft" activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -9940,6 +9940,9 @@
       <c r="B99" t="s">
         <v>1684</v>
       </c>
+      <c r="D99" t="s">
+        <v>1920</v>
+      </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
@@ -9947,6 +9950,9 @@
       </c>
       <c r="B100" t="s">
         <v>1684</v>
+      </c>
+      <c r="D100" t="s">
+        <v>1920</v>
       </c>
     </row>
   </sheetData>
@@ -9958,9 +9964,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90FF5842-5F39-42CA-813E-70DCD245FAB4}">
   <dimension ref="A1:G169"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H163" sqref="H163"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Adding newly rendered/colored icons
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97DD0CB-DBE4-4795-8D88-6D2711448967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373597EC-0B5B-44DE-B490-CC5E3521804D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11335" uniqueCount="1964">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11363" uniqueCount="1992">
   <si>
     <t>Caster Level</t>
   </si>
@@ -5932,6 +5932,90 @@
   </si>
   <si>
     <t>SPWI512; SPPR407</t>
+  </si>
+  <si>
+    <t>BAM</t>
+  </si>
+  <si>
+    <t>absolute-immunity.BAM</t>
+  </si>
+  <si>
+    <t>aid.BAM</t>
+  </si>
+  <si>
+    <t>armor.BAM</t>
+  </si>
+  <si>
+    <t>animal-rage.BAM</t>
+  </si>
+  <si>
+    <t>antiharm-shell.BAM</t>
+  </si>
+  <si>
+    <t>antimagic-shell.BAM</t>
+  </si>
+  <si>
+    <t>potion-ai-004e.png</t>
+  </si>
+  <si>
+    <t>potion-ai-004f.png</t>
+  </si>
+  <si>
+    <t>potion-ai-005a.png</t>
+  </si>
+  <si>
+    <t>potion-ai-005b.png</t>
+  </si>
+  <si>
+    <t>potion-ai-005c.png</t>
+  </si>
+  <si>
+    <t>potion-ai-005d.png</t>
+  </si>
+  <si>
+    <t>potion-ai-018a.png</t>
+  </si>
+  <si>
+    <t>potion-ai-008a.png</t>
+  </si>
+  <si>
+    <t>potion-ai-008b.png</t>
+  </si>
+  <si>
+    <t>potion-ai-008c.png</t>
+  </si>
+  <si>
+    <t>potion-ai-008d.png</t>
+  </si>
+  <si>
+    <t>potion-ai-012a.png</t>
+  </si>
+  <si>
+    <t>potion-ai-012b.png</t>
+  </si>
+  <si>
+    <t>potion-ai-019a.png</t>
+  </si>
+  <si>
+    <t>potion-ai-019b.png</t>
+  </si>
+  <si>
+    <t>potion-ai-025a.png</t>
+  </si>
+  <si>
+    <t>potion-ai-026a.png</t>
+  </si>
+  <si>
+    <t>potion-ai-026c.png</t>
+  </si>
+  <si>
+    <t>potion-ai-026b.png</t>
+  </si>
+  <si>
+    <t>potion-ai-040a.png</t>
+  </si>
+  <si>
+    <t>potion-ai-049a.png</t>
   </si>
 </sst>
 </file>
@@ -6018,7 +6102,7 @@
       <name val="Monospaced"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6054,6 +6138,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6103,7 +6193,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -6156,6 +6246,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent2" xfId="4" builtinId="33"/>
@@ -9971,11 +10062,11 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90FF5842-5F39-42CA-813E-70DCD245FAB4}">
-  <dimension ref="A1:L169"/>
+  <dimension ref="A1:L190"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C133" sqref="C133"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A191" sqref="A191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -9990,9 +10081,10 @@
     <col min="8" max="8" width="17.08984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.1796875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" s="23" t="s">
         <v>1814</v>
       </c>
@@ -10026,9 +10118,12 @@
       <c r="K1" s="23" t="s">
         <v>1957</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
+      <c r="L1" s="23" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="34" t="s">
         <v>1764</v>
       </c>
       <c r="B2">
@@ -10056,9 +10151,12 @@
       <c r="I2" t="s">
         <v>1829</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
+      <c r="L2" t="s">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="34" t="s">
         <v>1725</v>
       </c>
       <c r="B3">
@@ -10086,9 +10184,12 @@
       <c r="I3" t="s">
         <v>1824</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
+      <c r="L3" t="s">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="34" t="s">
         <v>1805</v>
       </c>
       <c r="B4">
@@ -10116,9 +10217,12 @@
       <c r="I4" t="s">
         <v>1833</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
+      <c r="L4" t="s">
+        <v>1968</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="34" t="s">
         <v>1910</v>
       </c>
       <c r="B5">
@@ -10146,9 +10250,12 @@
       <c r="I5" t="s">
         <v>1916</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
+      <c r="L5" t="s">
+        <v>1969</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="34" t="s">
         <v>1802</v>
       </c>
       <c r="B6">
@@ -10176,9 +10283,12 @@
       <c r="I6" t="s">
         <v>1832</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="s">
+      <c r="L6" t="s">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="34" t="s">
         <v>1705</v>
       </c>
       <c r="B7">
@@ -10206,8 +10316,11 @@
       <c r="I7" t="s">
         <v>1821</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>1732</v>
       </c>
@@ -10237,7 +10350,7 @@
         <v>1825</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>1908</v>
       </c>
@@ -10267,7 +10380,7 @@
         <v>1916</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>1784</v>
       </c>
@@ -10297,7 +10410,7 @@
         <v>1831</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>1715</v>
       </c>
@@ -10327,7 +10440,7 @@
         <v>1823</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>1813</v>
       </c>
@@ -10357,7 +10470,7 @@
         <v>1824</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>1690</v>
       </c>
@@ -10387,7 +10500,7 @@
         <v>1819</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>1733</v>
       </c>
@@ -10417,7 +10530,7 @@
         <v>1825</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>1740</v>
       </c>
@@ -10447,7 +10560,7 @@
         <v>1826</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>1886</v>
       </c>
@@ -14855,6 +14968,111 @@
       </c>
       <c r="I169" t="s">
         <v>1916</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9">
+      <c r="A170" t="s">
+        <v>1971</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9">
+      <c r="A171" t="s">
+        <v>1972</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9">
+      <c r="A172" t="s">
+        <v>1973</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9">
+      <c r="A173" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9">
+      <c r="A174" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9">
+      <c r="A175" t="s">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9">
+      <c r="A176" t="s">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" t="s">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" t="s">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" t="s">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" t="s">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1">
+      <c r="A181" t="s">
+        <v>1983</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" t="s">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" t="s">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" t="s">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1">
+      <c r="A185" t="s">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" t="s">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1">
+      <c r="A187" t="s">
+        <v>1989</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1">
+      <c r="A188" t="s">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1">
+      <c r="A189" t="s">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1">
+      <c r="A190" t="s">
+        <v>1991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working through the list of intended Potions
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373597EC-0B5B-44DE-B490-CC5E3521804D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA316EFD-AAA7-4F9B-9A62-B7A50A591BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11363" uniqueCount="1992">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11472" uniqueCount="2102">
   <si>
     <t>Caster Level</t>
   </si>
@@ -5838,9 +5838,6 @@
     <t>MEWI960</t>
   </si>
   <si>
-    <t>Camoflage</t>
-  </si>
-  <si>
     <t>MEPR156</t>
   </si>
   <si>
@@ -5946,6 +5943,18 @@
     <t>armor.BAM</t>
   </si>
   <si>
+    <t>barkskin.BAM</t>
+  </si>
+  <si>
+    <t>bless.BAM</t>
+  </si>
+  <si>
+    <t>blur.BAM</t>
+  </si>
+  <si>
+    <t>chant.BAM</t>
+  </si>
+  <si>
     <t>animal-rage.BAM</t>
   </si>
   <si>
@@ -5955,6 +5964,9 @@
     <t>antimagic-shell.BAM</t>
   </si>
   <si>
+    <t>attain-perfection.BAM</t>
+  </si>
+  <si>
     <t>potion-ai-004e.png</t>
   </si>
   <si>
@@ -6016,6 +6028,324 @@
   </si>
   <si>
     <t>potion-ai-049a.png</t>
+  </si>
+  <si>
+    <t>potion-ai-058a.png</t>
+  </si>
+  <si>
+    <t>armor-of-faith.BAM</t>
+  </si>
+  <si>
+    <t>aura-of-flaming-death.BAM</t>
+  </si>
+  <si>
+    <t>beast-claw.BAM</t>
+  </si>
+  <si>
+    <t>blood-rage.BAM</t>
+  </si>
+  <si>
+    <t>camoflauge.BAM</t>
+  </si>
+  <si>
+    <t>Camoflauge</t>
+  </si>
+  <si>
+    <t>cat's-grace.BAM</t>
+  </si>
+  <si>
+    <t>chain-lightning.BAM</t>
+  </si>
+  <si>
+    <t>champion's-strength.BAM</t>
+  </si>
+  <si>
+    <t>chaotic-commands.BAM</t>
+  </si>
+  <si>
+    <t>cloak-of-fear.BAM</t>
+  </si>
+  <si>
+    <t>cloud-of-pestilence.BAM</t>
+  </si>
+  <si>
+    <t>colossal-growth.BAM</t>
+  </si>
+  <si>
+    <t>cure-disease.BAM</t>
+  </si>
+  <si>
+    <t>cure-medium-wounds.BAM</t>
+  </si>
+  <si>
+    <t>cure-moderate-wounds.BAM</t>
+  </si>
+  <si>
+    <t>cure-serious-wounds.BAM</t>
+  </si>
+  <si>
+    <t>death-fog.BAM</t>
+  </si>
+  <si>
+    <t>death-ward.BAM</t>
+  </si>
+  <si>
+    <t>decastave.BAM</t>
+  </si>
+  <si>
+    <t>detect-invisibility.BAM</t>
+  </si>
+  <si>
+    <t>dispel-magic.BAM</t>
+  </si>
+  <si>
+    <t>displacement.BAM</t>
+  </si>
+  <si>
+    <t>draw-upon-holy-might.BAM</t>
+  </si>
+  <si>
+    <t>eclectic-recall.BAM</t>
+  </si>
+  <si>
+    <t>emotion-courage.BAM</t>
+  </si>
+  <si>
+    <t>emotion-hope.BAM</t>
+  </si>
+  <si>
+    <t>enchanted-weapon.BAM</t>
+  </si>
+  <si>
+    <t>entangle.BAM</t>
+  </si>
+  <si>
+    <t>entropy-shield.BAM</t>
+  </si>
+  <si>
+    <t>exaltation.BAM</t>
+  </si>
+  <si>
+    <t>expeditious-retreat.BAM</t>
+  </si>
+  <si>
+    <t>expose-to-the-elements.BAM</t>
+  </si>
+  <si>
+    <t>extend-vision.BAM</t>
+  </si>
+  <si>
+    <t>find-traps.BAM</t>
+  </si>
+  <si>
+    <t>fire-shield-red.BAM</t>
+  </si>
+  <si>
+    <t>fireball.BAM</t>
+  </si>
+  <si>
+    <t>fire-shield-blue.BAM</t>
+  </si>
+  <si>
+    <t>fly.BAM</t>
+  </si>
+  <si>
+    <t>free-action.BAM</t>
+  </si>
+  <si>
+    <t>friends.BAM</t>
+  </si>
+  <si>
+    <t>gedlee's-electric-barrier.BAM</t>
+  </si>
+  <si>
+    <t>ghost-armor.BAM</t>
+  </si>
+  <si>
+    <t>ghostform.BAM</t>
+  </si>
+  <si>
+    <t>ghostwalk.BAM</t>
+  </si>
+  <si>
+    <t>globe-of-invulnerability.BAM</t>
+  </si>
+  <si>
+    <t>grease.BAM</t>
+  </si>
+  <si>
+    <t>greater-malison.BAM</t>
+  </si>
+  <si>
+    <t>greater-restoration.BAM</t>
+  </si>
+  <si>
+    <t>greater-shield-of-lathander.BAM</t>
+  </si>
+  <si>
+    <t>heal.BAM</t>
+  </si>
+  <si>
+    <t>holy-power.BAM</t>
+  </si>
+  <si>
+    <t>impervious-sanctity-of-the-mind.BAM</t>
+  </si>
+  <si>
+    <t>improved-alacrity.BAM</t>
+  </si>
+  <si>
+    <t>improved-haste.BAM</t>
+  </si>
+  <si>
+    <t>improved-invisibility.BAM</t>
+  </si>
+  <si>
+    <t>improved-mantle.BAM</t>
+  </si>
+  <si>
+    <t>knock.BAM</t>
+  </si>
+  <si>
+    <t>legend-lore.BAM</t>
+  </si>
+  <si>
+    <t>lesser-restoration.BAM</t>
+  </si>
+  <si>
+    <t>luck.BAM</t>
+  </si>
+  <si>
+    <t>major-mirror-image.BAM</t>
+  </si>
+  <si>
+    <t>mantle.BAM</t>
+  </si>
+  <si>
+    <t>mental-agility.BAM</t>
+  </si>
+  <si>
+    <t>minor-globe-of-invulnerability.BAM</t>
+  </si>
+  <si>
+    <t>minor-spell-turning.BAM</t>
+  </si>
+  <si>
+    <t>mirror-image.BAM</t>
+  </si>
+  <si>
+    <t>mist-of-eldath.BAM</t>
+  </si>
+  <si>
+    <t>moonblade.BAM</t>
+  </si>
+  <si>
+    <t>nature's-beauty.BAM</t>
+  </si>
+  <si>
+    <t>negative-plane-protection.BAM</t>
+  </si>
+  <si>
+    <t>non-detection.BAM</t>
+  </si>
+  <si>
+    <t>omnipresence.BAM</t>
+  </si>
+  <si>
+    <t>otiluke's-resilient-sphere.BAM</t>
+  </si>
+  <si>
+    <t>perfect-invisibility.BAM</t>
+  </si>
+  <si>
+    <t>phantom-blade.BAM</t>
+  </si>
+  <si>
+    <t>piercing-shots.BAM</t>
+  </si>
+  <si>
+    <t>prayer.BAM</t>
+  </si>
+  <si>
+    <t>protection-from-acid.BAM</t>
+  </si>
+  <si>
+    <t>protection-from-cold.BAM</t>
+  </si>
+  <si>
+    <t>protection-from-electricity.BAM</t>
+  </si>
+  <si>
+    <t>protection-from-energy.BAM</t>
+  </si>
+  <si>
+    <t>protection-from-evil.BAM</t>
+  </si>
+  <si>
+    <t>protection-from-fire.BAM</t>
+  </si>
+  <si>
+    <t>protection-from-magic-energy.BAM</t>
+  </si>
+  <si>
+    <t>protection-from-magical-weapons.BAM</t>
+  </si>
+  <si>
+    <t>protection-from-non-silver-weapons.BAM</t>
+  </si>
+  <si>
+    <t>protection-from-normal-missiles.BAM</t>
+  </si>
+  <si>
+    <t>protection-from-normal-weapons.BAM</t>
+  </si>
+  <si>
+    <t>protection-from-petrification.BAM</t>
+  </si>
+  <si>
+    <t>protection-from-the-elements.BAM</t>
+  </si>
+  <si>
+    <t>recitation.BAM</t>
+  </si>
+  <si>
+    <t>reflect-attack.BAM</t>
+  </si>
+  <si>
+    <t>remove-curse.BAM</t>
+  </si>
+  <si>
+    <t>resist-fear.BAM</t>
+  </si>
+  <si>
+    <t>SPWI210;serveral others</t>
+  </si>
+  <si>
+    <t>resist-fire-and-cold.BAM</t>
+  </si>
+  <si>
+    <t>righteous-magic.BAM</t>
+  </si>
+  <si>
+    <t>righteous-wrath-of-the-faithful.BAM</t>
+  </si>
+  <si>
+    <t>sanctuary.BAM</t>
+  </si>
+  <si>
+    <t>searing-smite.BAM</t>
+  </si>
+  <si>
+    <t>shadow-door.BAM</t>
+  </si>
+  <si>
+    <t>shield.BAM</t>
+  </si>
+  <si>
+    <t>shield-of-lathander.BAM</t>
+  </si>
+  <si>
+    <t>sleep.BAM</t>
   </si>
 </sst>
 </file>
@@ -10008,7 +10338,7 @@
         <v>1917</v>
       </c>
       <c r="E96" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -10062,11 +10392,11 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90FF5842-5F39-42CA-813E-70DCD245FAB4}">
-  <dimension ref="A1:L190"/>
+  <dimension ref="A1:L191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A191" sqref="A191"/>
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L116" sqref="L116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -10074,14 +10404,14 @@
     <col min="1" max="1" width="16.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.08984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.1796875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -10098,10 +10428,10 @@
         <v>1817</v>
       </c>
       <c r="E1" s="23" t="s">
+        <v>1959</v>
+      </c>
+      <c r="F1" s="23" t="s">
         <v>1960</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>1961</v>
       </c>
       <c r="G1" s="23" t="s">
         <v>1676</v>
@@ -10113,13 +10443,13 @@
         <v>1818</v>
       </c>
       <c r="J1" s="23" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="K1" s="23" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="L1" s="23" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -10152,7 +10482,7 @@
         <v>1829</v>
       </c>
       <c r="L2" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -10185,7 +10515,7 @@
         <v>1824</v>
       </c>
       <c r="L3" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -10218,7 +10548,7 @@
         <v>1833</v>
       </c>
       <c r="L4" t="s">
-        <v>1968</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -10232,7 +10562,7 @@
         <v>1607</v>
       </c>
       <c r="D5" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="E5">
         <v>12</v>
@@ -10251,7 +10581,7 @@
         <v>1916</v>
       </c>
       <c r="L5" t="s">
-        <v>1969</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -10284,7 +10614,7 @@
         <v>1832</v>
       </c>
       <c r="L6" t="s">
-        <v>1970</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -10317,11 +10647,11 @@
         <v>1821</v>
       </c>
       <c r="L7" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" t="s">
+      <c r="A8" s="34" t="s">
         <v>1732</v>
       </c>
       <c r="B8">
@@ -10349,9 +10679,12 @@
       <c r="I8" t="s">
         <v>1825</v>
       </c>
+      <c r="L8" t="s">
+        <v>1997</v>
+      </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" t="s">
+      <c r="A9" s="34" t="s">
         <v>1908</v>
       </c>
       <c r="B9">
@@ -10379,12 +10712,15 @@
       <c r="I9" t="s">
         <v>1916</v>
       </c>
+      <c r="L9" t="s">
+        <v>1974</v>
+      </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" t="s">
+      <c r="A10" s="34" t="s">
         <v>1784</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>1399</v>
       </c>
       <c r="C10" t="s">
@@ -10409,9 +10745,12 @@
       <c r="I10" t="s">
         <v>1831</v>
       </c>
+      <c r="L10" t="s">
+        <v>1998</v>
+      </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" t="s">
+      <c r="A11" s="34" t="s">
         <v>1715</v>
       </c>
       <c r="B11">
@@ -10439,9 +10778,12 @@
       <c r="I11" t="s">
         <v>1823</v>
       </c>
+      <c r="L11" t="s">
+        <v>1967</v>
+      </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" t="s">
+      <c r="A12" s="34" t="s">
         <v>1813</v>
       </c>
       <c r="B12">
@@ -10469,9 +10811,12 @@
       <c r="I12" t="s">
         <v>1824</v>
       </c>
+      <c r="L12" t="s">
+        <v>1999</v>
+      </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" t="s">
+      <c r="A13" s="34" t="s">
         <v>1690</v>
       </c>
       <c r="B13">
@@ -10499,9 +10844,12 @@
       <c r="I13" t="s">
         <v>1819</v>
       </c>
+      <c r="L13" t="s">
+        <v>1968</v>
+      </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" t="s">
+      <c r="A14" s="34" t="s">
         <v>1733</v>
       </c>
       <c r="B14">
@@ -10529,9 +10877,12 @@
       <c r="I14" t="s">
         <v>1825</v>
       </c>
+      <c r="L14" t="s">
+        <v>2000</v>
+      </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" t="s">
+      <c r="A15" s="34" t="s">
         <v>1740</v>
       </c>
       <c r="B15">
@@ -10559,19 +10910,22 @@
       <c r="I15" t="s">
         <v>1826</v>
       </c>
+      <c r="L15" t="s">
+        <v>1969</v>
+      </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" t="s">
+      <c r="A16" s="34" t="s">
         <v>1886</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
+        <v>2002</v>
+      </c>
+      <c r="D16" t="s">
         <v>1932</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1933</v>
       </c>
       <c r="E16">
         <v>10</v>
@@ -10589,9 +10943,12 @@
       <c r="I16" t="s">
         <v>1914</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" t="s">
+      <c r="L16" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="34" t="s">
         <v>1793</v>
       </c>
       <c r="B17">
@@ -10619,9 +10976,12 @@
       <c r="I17" t="s">
         <v>1832</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" t="s">
+      <c r="L17" t="s">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="34" t="s">
         <v>1712</v>
       </c>
       <c r="B18">
@@ -10649,9 +11009,12 @@
       <c r="I18" t="s">
         <v>1822</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" t="s">
+      <c r="L18" t="s">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="34" t="s">
         <v>1745</v>
       </c>
       <c r="B19">
@@ -10679,9 +11042,12 @@
       <c r="I19" t="s">
         <v>1827</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" t="s">
+      <c r="L19" t="s">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="34" t="s">
         <v>1758</v>
       </c>
       <c r="B20">
@@ -10709,9 +11075,12 @@
       <c r="I20" t="s">
         <v>1828</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" t="s">
+      <c r="L20" t="s">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="34" t="s">
         <v>1729</v>
       </c>
       <c r="B21">
@@ -10739,9 +11108,12 @@
       <c r="I21" t="s">
         <v>1825</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" t="s">
+      <c r="L21" t="s">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="34" t="s">
         <v>1775</v>
       </c>
       <c r="B22">
@@ -10769,9 +11141,12 @@
       <c r="I22" t="s">
         <v>1830</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" t="s">
+      <c r="L22" t="s">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="34" t="s">
         <v>1707</v>
       </c>
       <c r="B23">
@@ -10799,19 +11174,22 @@
       <c r="I23" t="s">
         <v>1822</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" t="s">
+      <c r="L23" t="s">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="34" t="s">
         <v>1873</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>1399</v>
       </c>
       <c r="C24" t="s">
         <v>1609</v>
       </c>
       <c r="D24" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="E24">
         <v>16</v>
@@ -10829,9 +11207,12 @@
       <c r="I24" t="s">
         <v>1913</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" t="s">
+      <c r="L24" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="34" t="s">
         <v>1691</v>
       </c>
       <c r="B25">
@@ -10859,9 +11240,12 @@
       <c r="I25" t="s">
         <v>1819</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" t="s">
+      <c r="L25" t="s">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="34" t="s">
         <v>1777</v>
       </c>
       <c r="B26">
@@ -10889,9 +11273,12 @@
       <c r="I26" t="s">
         <v>1830</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" t="s">
+      <c r="L26" t="s">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="34" t="s">
         <v>1770</v>
       </c>
       <c r="B27">
@@ -10919,9 +11306,12 @@
       <c r="I27" t="s">
         <v>1829</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" t="s">
+      <c r="L27" t="s">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="34" t="s">
         <v>1735</v>
       </c>
       <c r="B28">
@@ -10949,9 +11339,12 @@
       <c r="I28" t="s">
         <v>1825</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" t="s">
+      <c r="L28" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="34" t="s">
         <v>1742</v>
       </c>
       <c r="B29">
@@ -10979,9 +11372,12 @@
       <c r="I29" t="s">
         <v>1826</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" t="s">
+      <c r="L29" t="s">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="34" t="s">
         <v>1744</v>
       </c>
       <c r="B30">
@@ -11009,9 +11405,12 @@
       <c r="I30" t="s">
         <v>1826</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" t="s">
+      <c r="L30" t="s">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="34" t="s">
         <v>1718</v>
       </c>
       <c r="B31">
@@ -11039,9 +11438,12 @@
       <c r="I31" t="s">
         <v>1823</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" t="s">
+      <c r="L31" t="s">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="34" t="s">
         <v>1761</v>
       </c>
       <c r="B32">
@@ -11069,9 +11471,12 @@
       <c r="I32" t="s">
         <v>1828</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" t="s">
+      <c r="L32" t="s">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="34" t="s">
         <v>1700</v>
       </c>
       <c r="B33">
@@ -11099,9 +11504,12 @@
       <c r="I33" t="s">
         <v>1820</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" t="s">
+      <c r="L33" t="s">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="34" t="s">
         <v>1894</v>
       </c>
       <c r="B34">
@@ -11129,9 +11537,12 @@
       <c r="I34" t="s">
         <v>1915</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" t="s">
+      <c r="L34" t="s">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="34" t="s">
         <v>1736</v>
       </c>
       <c r="B35">
@@ -11159,9 +11570,12 @@
       <c r="I35" t="s">
         <v>1826</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" t="s">
+      <c r="L35" t="s">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="34" t="s">
         <v>1907</v>
       </c>
       <c r="B36">
@@ -11189,9 +11603,12 @@
       <c r="I36" t="s">
         <v>1916</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" t="s">
+      <c r="L36" t="s">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="34" t="s">
         <v>1739</v>
       </c>
       <c r="B37">
@@ -11219,9 +11636,12 @@
       <c r="I37" t="s">
         <v>1826</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" t="s">
+      <c r="L37" t="s">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="34" t="s">
         <v>1748</v>
       </c>
       <c r="B38">
@@ -11249,9 +11669,12 @@
       <c r="I38" t="s">
         <v>1827</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" t="s">
+      <c r="L38" t="s">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="34" t="s">
         <v>1741</v>
       </c>
       <c r="B39">
@@ -11279,9 +11702,12 @@
       <c r="I39" t="s">
         <v>1826</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" t="s">
+      <c r="L39" t="s">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="34" t="s">
         <v>1711</v>
       </c>
       <c r="B40">
@@ -11309,9 +11735,12 @@
       <c r="I40" t="s">
         <v>1822</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" t="s">
+      <c r="L40" t="s">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="34" t="s">
         <v>1800</v>
       </c>
       <c r="B41">
@@ -11339,9 +11768,12 @@
       <c r="I41" t="s">
         <v>1832</v>
       </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" t="s">
+      <c r="L41" t="s">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="34" t="s">
         <v>1731</v>
       </c>
       <c r="B42">
@@ -11369,9 +11801,12 @@
       <c r="I42" t="s">
         <v>1825</v>
       </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" t="s">
+      <c r="L42" t="s">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="34" t="s">
         <v>1891</v>
       </c>
       <c r="B43">
@@ -11399,9 +11834,12 @@
       <c r="I43" t="s">
         <v>1914</v>
       </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" t="s">
+      <c r="L43" t="s">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="34" t="s">
         <v>1875</v>
       </c>
       <c r="B44">
@@ -11411,7 +11849,7 @@
         <v>1605</v>
       </c>
       <c r="D44" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="E44">
         <v>10</v>
@@ -11429,9 +11867,12 @@
       <c r="I44" t="s">
         <v>1913</v>
       </c>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" t="s">
+      <c r="L44" t="s">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="34" t="s">
         <v>1871</v>
       </c>
       <c r="B45">
@@ -11459,9 +11900,12 @@
       <c r="I45" t="s">
         <v>1913</v>
       </c>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" t="s">
+      <c r="L45" t="s">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="34" t="s">
         <v>1789</v>
       </c>
       <c r="B46">
@@ -11489,9 +11933,12 @@
       <c r="I46" t="s">
         <v>1831</v>
       </c>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" t="s">
+      <c r="L46" t="s">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="34" t="s">
         <v>1737</v>
       </c>
       <c r="B47">
@@ -11519,9 +11966,12 @@
       <c r="I47" t="s">
         <v>1826</v>
       </c>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" t="s">
+      <c r="L47" t="s">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="34" t="s">
         <v>1795</v>
       </c>
       <c r="B48">
@@ -11549,9 +11999,12 @@
       <c r="I48" t="s">
         <v>1832</v>
       </c>
-    </row>
-    <row r="49" spans="1:9">
-      <c r="A49" t="s">
+      <c r="L48" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" s="34" t="s">
         <v>1774</v>
       </c>
       <c r="B49">
@@ -11579,9 +12032,12 @@
       <c r="I49" t="s">
         <v>1830</v>
       </c>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" t="s">
+      <c r="L49" t="s">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" s="34" t="s">
         <v>1900</v>
       </c>
       <c r="B50">
@@ -11609,9 +12065,12 @@
       <c r="I50" t="s">
         <v>1915</v>
       </c>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" t="s">
+      <c r="L50" t="s">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" s="34" t="s">
         <v>1692</v>
       </c>
       <c r="B51">
@@ -11639,9 +12098,12 @@
       <c r="I51" t="s">
         <v>1819</v>
       </c>
-    </row>
-    <row r="52" spans="1:9">
-      <c r="A52" t="s">
+      <c r="L51" t="s">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" s="34" t="s">
         <v>1699</v>
       </c>
       <c r="B52">
@@ -11669,9 +12131,12 @@
       <c r="I52" t="s">
         <v>1820</v>
       </c>
-    </row>
-    <row r="53" spans="1:9">
-      <c r="A53" t="s">
+      <c r="L52" t="s">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" s="34" t="s">
         <v>1876</v>
       </c>
       <c r="B53">
@@ -11699,9 +12164,12 @@
       <c r="I53" t="s">
         <v>1913</v>
       </c>
-    </row>
-    <row r="54" spans="1:9">
-      <c r="A54" t="s">
+      <c r="L53" t="s">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" s="34" t="s">
         <v>1756</v>
       </c>
       <c r="B54">
@@ -11729,9 +12197,12 @@
       <c r="I54" t="s">
         <v>1828</v>
       </c>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="A55" t="s">
+      <c r="L54" t="s">
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" s="34" t="s">
         <v>1879</v>
       </c>
       <c r="B55">
@@ -11759,9 +12230,12 @@
       <c r="I55" t="s">
         <v>1913</v>
       </c>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="A56" t="s">
+      <c r="L55" t="s">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" s="34" t="s">
         <v>1890</v>
       </c>
       <c r="B56">
@@ -11789,9 +12263,12 @@
       <c r="I56" t="s">
         <v>1914</v>
       </c>
-    </row>
-    <row r="57" spans="1:9">
-      <c r="A57" t="s">
+      <c r="L56" t="s">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" s="34" t="s">
         <v>1694</v>
       </c>
       <c r="B57">
@@ -11819,9 +12296,12 @@
       <c r="I57" t="s">
         <v>1819</v>
       </c>
-    </row>
-    <row r="58" spans="1:9">
-      <c r="A58" t="s">
+      <c r="L57" t="s">
+        <v>2042</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" s="34" t="s">
         <v>1708</v>
       </c>
       <c r="B58">
@@ -11849,9 +12329,12 @@
       <c r="I58" t="s">
         <v>1822</v>
       </c>
-    </row>
-    <row r="59" spans="1:9">
-      <c r="A59" t="s">
+      <c r="L58" t="s">
+        <v>2043</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" s="34" t="s">
         <v>1797</v>
       </c>
       <c r="B59">
@@ -11879,9 +12362,12 @@
       <c r="I59" t="s">
         <v>1832</v>
       </c>
-    </row>
-    <row r="60" spans="1:9">
-      <c r="A60" t="s">
+      <c r="L59" t="s">
+        <v>2044</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" s="34" t="s">
         <v>1786</v>
       </c>
       <c r="B60">
@@ -11909,9 +12395,12 @@
       <c r="I60" t="s">
         <v>1831</v>
       </c>
-    </row>
-    <row r="61" spans="1:9">
-      <c r="A61" t="s">
+      <c r="L60" t="s">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" s="34" t="s">
         <v>1898</v>
       </c>
       <c r="B61">
@@ -11939,9 +12428,12 @@
       <c r="I61" t="s">
         <v>1915</v>
       </c>
-    </row>
-    <row r="62" spans="1:9">
-      <c r="A62" t="s">
+      <c r="L61" t="s">
+        <v>2046</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" s="34" t="s">
         <v>1804</v>
       </c>
       <c r="B62">
@@ -11969,9 +12461,12 @@
       <c r="I62" t="s">
         <v>1833</v>
       </c>
-    </row>
-    <row r="63" spans="1:9">
-      <c r="A63" t="s">
+      <c r="L62" t="s">
+        <v>2047</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" s="34" t="s">
         <v>1751</v>
       </c>
       <c r="B63">
@@ -11999,9 +12494,12 @@
       <c r="I63" t="s">
         <v>1827</v>
       </c>
-    </row>
-    <row r="64" spans="1:9">
-      <c r="A64" t="s">
+      <c r="L63" t="s">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" s="34" t="s">
         <v>1803</v>
       </c>
       <c r="B64">
@@ -12029,9 +12527,12 @@
       <c r="I64" t="s">
         <v>1833</v>
       </c>
-    </row>
-    <row r="65" spans="1:9">
-      <c r="A65" t="s">
+      <c r="L64" t="s">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" s="34" t="s">
         <v>1812</v>
       </c>
       <c r="B65">
@@ -12059,9 +12560,12 @@
       <c r="I65" t="s">
         <v>1833</v>
       </c>
-    </row>
-    <row r="66" spans="1:9">
-      <c r="A66" t="s">
+      <c r="L65" t="s">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" s="34" t="s">
         <v>1747</v>
       </c>
       <c r="B66">
@@ -12089,9 +12593,12 @@
       <c r="I66" t="s">
         <v>1827</v>
       </c>
-    </row>
-    <row r="67" spans="1:9">
-      <c r="A67" t="s">
+      <c r="L66" t="s">
+        <v>2051</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" s="34" t="s">
         <v>1782</v>
       </c>
       <c r="B67">
@@ -12119,9 +12626,12 @@
       <c r="I67" t="s">
         <v>1830</v>
       </c>
-    </row>
-    <row r="68" spans="1:9">
-      <c r="A68" t="s">
+      <c r="L67" t="s">
+        <v>2052</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68" s="34" t="s">
         <v>1801</v>
       </c>
       <c r="B68">
@@ -12149,9 +12659,12 @@
       <c r="I68" t="s">
         <v>1832</v>
       </c>
-    </row>
-    <row r="69" spans="1:9">
-      <c r="A69" t="s">
+      <c r="L68" t="s">
+        <v>2053</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" s="34" t="s">
         <v>1766</v>
       </c>
       <c r="B69">
@@ -12179,9 +12692,12 @@
       <c r="I69" t="s">
         <v>1829</v>
       </c>
-    </row>
-    <row r="70" spans="1:9">
-      <c r="A70" t="s">
+      <c r="L69" t="s">
+        <v>2054</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70" s="34" t="s">
         <v>1887</v>
       </c>
       <c r="B70">
@@ -12209,9 +12725,12 @@
       <c r="I70" t="s">
         <v>1914</v>
       </c>
-    </row>
-    <row r="71" spans="1:9">
-      <c r="A71" t="s">
+      <c r="L70" t="s">
+        <v>2055</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71" s="34" t="s">
         <v>1746</v>
       </c>
       <c r="B71">
@@ -12239,9 +12758,12 @@
       <c r="I71" t="s">
         <v>1827</v>
       </c>
-    </row>
-    <row r="72" spans="1:9">
-      <c r="A72" t="s">
+      <c r="L71" t="s">
+        <v>2056</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" s="34" t="s">
         <v>1780</v>
       </c>
       <c r="B72">
@@ -12269,9 +12791,12 @@
       <c r="I72" t="s">
         <v>1830</v>
       </c>
-    </row>
-    <row r="73" spans="1:9">
-      <c r="A73" t="s">
+      <c r="L72" t="s">
+        <v>2057</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="A73" s="34" t="s">
         <v>1885</v>
       </c>
       <c r="B73">
@@ -12299,9 +12824,12 @@
       <c r="I73" t="s">
         <v>1914</v>
       </c>
-    </row>
-    <row r="74" spans="1:9">
-      <c r="A74" t="s">
+      <c r="L73" t="s">
+        <v>2058</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="A74" s="34" t="s">
         <v>1723</v>
       </c>
       <c r="B74">
@@ -12329,9 +12857,12 @@
       <c r="I74" t="s">
         <v>1824</v>
       </c>
-    </row>
-    <row r="75" spans="1:9">
-      <c r="A75" t="s">
+      <c r="L74" t="s">
+        <v>2059</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="A75" s="34" t="s">
         <v>1897</v>
       </c>
       <c r="B75">
@@ -12341,7 +12872,7 @@
         <v>1597</v>
       </c>
       <c r="D75" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="E75">
         <v>20</v>
@@ -12359,9 +12890,12 @@
       <c r="I75" t="s">
         <v>1915</v>
       </c>
-    </row>
-    <row r="76" spans="1:9">
-      <c r="A76" t="s">
+      <c r="L75" t="s">
+        <v>2060</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
+      <c r="A76" s="34" t="s">
         <v>1765</v>
       </c>
       <c r="B76">
@@ -12389,9 +12923,12 @@
       <c r="I76" t="s">
         <v>1829</v>
       </c>
-    </row>
-    <row r="77" spans="1:9">
-      <c r="A77" t="s">
+      <c r="L76" t="s">
+        <v>2061</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
+      <c r="A77" s="34" t="s">
         <v>1759</v>
       </c>
       <c r="B77">
@@ -12419,9 +12956,12 @@
       <c r="I77" t="s">
         <v>1828</v>
       </c>
-    </row>
-    <row r="78" spans="1:9">
-      <c r="A78" t="s">
+      <c r="L77" t="s">
+        <v>2062</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
+      <c r="A78" s="34" t="s">
         <v>1810</v>
       </c>
       <c r="B78">
@@ -12449,9 +12989,12 @@
       <c r="I78" t="s">
         <v>1833</v>
       </c>
-    </row>
-    <row r="79" spans="1:9">
-      <c r="A79" t="s">
+      <c r="L78" t="s">
+        <v>2063</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
+      <c r="A79" s="34" t="s">
         <v>1792</v>
       </c>
       <c r="B79">
@@ -12479,9 +13022,12 @@
       <c r="I79" t="s">
         <v>1831</v>
       </c>
-    </row>
-    <row r="80" spans="1:9">
-      <c r="A80" t="s">
+      <c r="L79" t="s">
+        <v>2064</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
+      <c r="A80" s="34" t="s">
         <v>1757</v>
       </c>
       <c r="B80">
@@ -12509,9 +13055,12 @@
       <c r="I80" t="s">
         <v>1828</v>
       </c>
-    </row>
-    <row r="81" spans="1:9">
-      <c r="A81" t="s">
+      <c r="L80" t="s">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
+      <c r="A81" s="34" t="s">
         <v>1755</v>
       </c>
       <c r="B81">
@@ -12539,9 +13088,12 @@
       <c r="I81" t="s">
         <v>1828</v>
       </c>
-    </row>
-    <row r="82" spans="1:9">
-      <c r="A82" t="s">
+      <c r="L81" t="s">
+        <v>2066</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
+      <c r="A82" s="34" t="s">
         <v>1772</v>
       </c>
       <c r="B82">
@@ -12569,9 +13121,12 @@
       <c r="I82" t="s">
         <v>1829</v>
       </c>
-    </row>
-    <row r="83" spans="1:9">
-      <c r="A83" t="s">
+      <c r="L82" t="s">
+        <v>2067</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
+      <c r="A83" s="34" t="s">
         <v>1783</v>
       </c>
       <c r="B83">
@@ -12599,9 +13154,12 @@
       <c r="I83" t="s">
         <v>1831</v>
       </c>
-    </row>
-    <row r="84" spans="1:9">
-      <c r="A84" t="s">
+      <c r="L83" t="s">
+        <v>2068</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
+      <c r="A84" s="34" t="s">
         <v>1881</v>
       </c>
       <c r="B84">
@@ -12629,9 +13187,12 @@
       <c r="I84" t="s">
         <v>1914</v>
       </c>
-    </row>
-    <row r="85" spans="1:9">
-      <c r="A85" t="s">
+      <c r="L84" t="s">
+        <v>2069</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
+      <c r="A85" s="34" t="s">
         <v>1760</v>
       </c>
       <c r="B85">
@@ -12659,9 +13220,12 @@
       <c r="I85" t="s">
         <v>1828</v>
       </c>
-    </row>
-    <row r="86" spans="1:9">
-      <c r="A86" t="s">
+      <c r="L85" t="s">
+        <v>2070</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
+      <c r="A86" s="34" t="s">
         <v>1880</v>
       </c>
       <c r="B86">
@@ -12689,9 +13253,12 @@
       <c r="I86" t="s">
         <v>1913</v>
       </c>
-    </row>
-    <row r="87" spans="1:9">
-      <c r="A87" t="s">
+      <c r="L86" t="s">
+        <v>2071</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
+      <c r="A87" s="34" t="s">
         <v>1811</v>
       </c>
       <c r="B87">
@@ -12719,9 +13286,12 @@
       <c r="I87" t="s">
         <v>1833</v>
       </c>
-    </row>
-    <row r="88" spans="1:9">
-      <c r="A88" t="s">
+      <c r="L87" t="s">
+        <v>2072</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
+      <c r="A88" s="34" t="s">
         <v>1878</v>
       </c>
       <c r="B88">
@@ -12731,7 +13301,7 @@
         <v>1604</v>
       </c>
       <c r="D88" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="E88">
         <v>8</v>
@@ -12749,9 +13319,12 @@
       <c r="I88" t="s">
         <v>1913</v>
       </c>
-    </row>
-    <row r="89" spans="1:9">
-      <c r="A89" t="s">
+      <c r="L88" t="s">
+        <v>2073</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
+      <c r="A89" s="34" t="s">
         <v>1695</v>
       </c>
       <c r="B89">
@@ -12779,9 +13352,12 @@
       <c r="I89" t="s">
         <v>1820</v>
       </c>
-    </row>
-    <row r="90" spans="1:9">
-      <c r="A90" t="s">
+      <c r="L89" t="s">
+        <v>2074</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
+      <c r="A90" s="34" t="s">
         <v>1704</v>
       </c>
       <c r="B90">
@@ -12809,9 +13385,12 @@
       <c r="I90" t="s">
         <v>1821</v>
       </c>
-    </row>
-    <row r="91" spans="1:9">
-      <c r="A91" t="s">
+      <c r="L90" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
+      <c r="A91" s="34" t="s">
         <v>1799</v>
       </c>
       <c r="B91">
@@ -12839,9 +13418,12 @@
       <c r="I91" t="s">
         <v>1832</v>
       </c>
-    </row>
-    <row r="92" spans="1:9">
-      <c r="A92" t="s">
+      <c r="L91" t="s">
+        <v>2076</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
+      <c r="A92" s="34" t="s">
         <v>1701</v>
       </c>
       <c r="B92">
@@ -12851,7 +13433,7 @@
         <v>1864</v>
       </c>
       <c r="D92" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="E92">
         <v>9</v>
@@ -12869,9 +13451,12 @@
       <c r="I92" t="s">
         <v>1821</v>
       </c>
-    </row>
-    <row r="93" spans="1:9">
-      <c r="A93" t="s">
+      <c r="L92" t="s">
+        <v>2077</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
+      <c r="A93" s="34" t="s">
         <v>1696</v>
       </c>
       <c r="B93">
@@ -12899,9 +13484,12 @@
       <c r="I93" t="s">
         <v>1820</v>
       </c>
-    </row>
-    <row r="94" spans="1:9">
-      <c r="A94" t="s">
+      <c r="L93" t="s">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
+      <c r="A94" s="34" t="s">
         <v>1781</v>
       </c>
       <c r="B94">
@@ -12929,9 +13517,12 @@
       <c r="I94" t="s">
         <v>1830</v>
       </c>
-    </row>
-    <row r="95" spans="1:9">
-      <c r="A95" t="s">
+      <c r="L94" t="s">
+        <v>2079</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
+      <c r="A95" s="34" t="s">
         <v>1702</v>
       </c>
       <c r="B95">
@@ -12941,7 +13532,7 @@
         <v>1835</v>
       </c>
       <c r="D95" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="E95">
         <v>5</v>
@@ -12959,9 +13550,12 @@
       <c r="I95" t="s">
         <v>1821</v>
       </c>
-    </row>
-    <row r="96" spans="1:9">
-      <c r="A96" t="s">
+      <c r="L95" t="s">
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
+      <c r="A96" s="34" t="s">
         <v>1726</v>
       </c>
       <c r="B96">
@@ -12989,9 +13583,12 @@
       <c r="I96" t="s">
         <v>1824</v>
       </c>
-    </row>
-    <row r="97" spans="1:9">
-      <c r="A97" t="s">
+      <c r="L96" t="s">
+        <v>2081</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12">
+      <c r="A97" s="34" t="s">
         <v>1750</v>
       </c>
       <c r="B97">
@@ -13019,9 +13616,12 @@
       <c r="I97" t="s">
         <v>1827</v>
       </c>
-    </row>
-    <row r="98" spans="1:9">
-      <c r="A98" t="s">
+      <c r="L97" t="s">
+        <v>2082</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
+      <c r="A98" s="34" t="s">
         <v>1901</v>
       </c>
       <c r="B98">
@@ -13031,7 +13631,7 @@
         <v>1608</v>
       </c>
       <c r="D98" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="E98">
         <v>14</v>
@@ -13049,9 +13649,12 @@
       <c r="I98" t="s">
         <v>1915</v>
       </c>
-    </row>
-    <row r="99" spans="1:9">
-      <c r="A99" t="s">
+      <c r="L98" t="s">
+        <v>2083</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
+      <c r="A99" s="34" t="s">
         <v>1788</v>
       </c>
       <c r="B99">
@@ -13079,9 +13682,12 @@
       <c r="I99" t="s">
         <v>1831</v>
       </c>
-    </row>
-    <row r="100" spans="1:9">
-      <c r="A100" t="s">
+      <c r="L99" t="s">
+        <v>2084</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12">
+      <c r="A100" s="34" t="s">
         <v>1689</v>
       </c>
       <c r="B100">
@@ -13109,9 +13715,12 @@
       <c r="I100" t="s">
         <v>1819</v>
       </c>
-    </row>
-    <row r="101" spans="1:9">
-      <c r="A101" t="s">
+      <c r="L100" t="s">
+        <v>2085</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
+      <c r="A101" s="34" t="s">
         <v>1738</v>
       </c>
       <c r="B101">
@@ -13139,9 +13748,12 @@
       <c r="I101" t="s">
         <v>1826</v>
       </c>
-    </row>
-    <row r="102" spans="1:9">
-      <c r="A102" t="s">
+      <c r="L101" t="s">
+        <v>2086</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12">
+      <c r="A102" s="34" t="s">
         <v>1762</v>
       </c>
       <c r="B102">
@@ -13151,7 +13763,7 @@
         <v>1870</v>
       </c>
       <c r="D102" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="E102">
         <v>13</v>
@@ -13169,9 +13781,12 @@
       <c r="I102" t="s">
         <v>1828</v>
       </c>
-    </row>
-    <row r="103" spans="1:9">
-      <c r="A103" t="s">
+      <c r="L102" t="s">
+        <v>2087</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12">
+      <c r="A103" s="34" t="s">
         <v>1769</v>
       </c>
       <c r="B103">
@@ -13199,9 +13814,12 @@
       <c r="I103" t="s">
         <v>1829</v>
       </c>
-    </row>
-    <row r="104" spans="1:9">
-      <c r="A104" t="s">
+      <c r="L103" t="s">
+        <v>2088</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12">
+      <c r="A104" s="34" t="s">
         <v>1902</v>
       </c>
       <c r="B104">
@@ -13229,9 +13847,12 @@
       <c r="I104" t="s">
         <v>1916</v>
       </c>
-    </row>
-    <row r="105" spans="1:9">
-      <c r="A105" t="s">
+      <c r="L104" t="s">
+        <v>2089</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12">
+      <c r="A105" s="34" t="s">
         <v>1771</v>
       </c>
       <c r="B105">
@@ -13259,9 +13880,12 @@
       <c r="I105" t="s">
         <v>1829</v>
       </c>
-    </row>
-    <row r="106" spans="1:9">
-      <c r="A106" t="s">
+      <c r="L105" t="s">
+        <v>2090</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12">
+      <c r="A106" s="34" t="s">
         <v>1806</v>
       </c>
       <c r="B106">
@@ -13271,7 +13895,7 @@
         <v>85</v>
       </c>
       <c r="D106" t="s">
-        <v>67</v>
+        <v>2092</v>
       </c>
       <c r="E106">
         <v>4</v>
@@ -13289,9 +13913,12 @@
       <c r="I106" t="s">
         <v>1833</v>
       </c>
-    </row>
-    <row r="107" spans="1:9">
-      <c r="A107" t="s">
+      <c r="L106" t="s">
+        <v>2091</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12">
+      <c r="A107" s="34" t="s">
         <v>1697</v>
       </c>
       <c r="B107">
@@ -13319,9 +13946,12 @@
       <c r="I107" t="s">
         <v>1820</v>
       </c>
-    </row>
-    <row r="108" spans="1:9">
-      <c r="A108" t="s">
+      <c r="L107" t="s">
+        <v>2093</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12">
+      <c r="A108" s="34" t="s">
         <v>1796</v>
       </c>
       <c r="B108">
@@ -13349,9 +13979,12 @@
       <c r="I108" t="s">
         <v>1832</v>
       </c>
-    </row>
-    <row r="109" spans="1:9">
-      <c r="A109" t="s">
+      <c r="L108" t="s">
+        <v>2094</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12">
+      <c r="A109" s="34" t="s">
         <v>1809</v>
       </c>
       <c r="B109">
@@ -13379,9 +14012,12 @@
       <c r="I109" t="s">
         <v>1833</v>
       </c>
-    </row>
-    <row r="110" spans="1:9">
-      <c r="A110" t="s">
+      <c r="L109" t="s">
+        <v>2095</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12">
+      <c r="A110" s="34" t="s">
         <v>1703</v>
       </c>
       <c r="B110">
@@ -13409,9 +14045,12 @@
       <c r="I110" t="s">
         <v>1821</v>
       </c>
-    </row>
-    <row r="111" spans="1:9">
-      <c r="A111" t="s">
+      <c r="L110" t="s">
+        <v>2096</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12">
+      <c r="A111" s="34" t="s">
         <v>1872</v>
       </c>
       <c r="B111">
@@ -13421,7 +14060,7 @@
         <v>1601</v>
       </c>
       <c r="D111" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="E111">
         <v>4</v>
@@ -13439,9 +14078,12 @@
       <c r="I111" t="s">
         <v>1913</v>
       </c>
-    </row>
-    <row r="112" spans="1:9">
-      <c r="A112" t="s">
+      <c r="L111" t="s">
+        <v>2097</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12">
+      <c r="A112" s="34" t="s">
         <v>1688</v>
       </c>
       <c r="B112">
@@ -13469,9 +14111,12 @@
       <c r="I112" t="s">
         <v>1819</v>
       </c>
-    </row>
-    <row r="113" spans="1:11">
-      <c r="A113" t="s">
+      <c r="L112" t="s">
+        <v>2098</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12">
+      <c r="A113" s="34" t="s">
         <v>1763</v>
       </c>
       <c r="B113">
@@ -13499,9 +14144,12 @@
       <c r="I113" t="s">
         <v>1829</v>
       </c>
-    </row>
-    <row r="114" spans="1:11">
-      <c r="A114" t="s">
+      <c r="L113" t="s">
+        <v>2099</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12">
+      <c r="A114" s="34" t="s">
         <v>1717</v>
       </c>
       <c r="B114">
@@ -13532,9 +14180,12 @@
       <c r="K114" t="s">
         <v>1840</v>
       </c>
-    </row>
-    <row r="115" spans="1:11">
-      <c r="A115" t="s">
+      <c r="L114" t="s">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12">
+      <c r="A115" s="34" t="s">
         <v>1706</v>
       </c>
       <c r="B115">
@@ -13562,8 +14213,11 @@
       <c r="I115" t="s">
         <v>1822</v>
       </c>
-    </row>
-    <row r="116" spans="1:11">
+      <c r="L115" t="s">
+        <v>2101</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12">
       <c r="A116" t="s">
         <v>1874</v>
       </c>
@@ -13574,7 +14228,7 @@
         <v>1599</v>
       </c>
       <c r="D116" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="E116">
         <v>3</v>
@@ -13593,7 +14247,7 @@
         <v>1913</v>
       </c>
     </row>
-    <row r="117" spans="1:11">
+    <row r="117" spans="1:12">
       <c r="A117" t="s">
         <v>1714</v>
       </c>
@@ -13623,7 +14277,7 @@
         <v>1822</v>
       </c>
     </row>
-    <row r="118" spans="1:11">
+    <row r="118" spans="1:12">
       <c r="A118" t="s">
         <v>1768</v>
       </c>
@@ -13656,7 +14310,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="119" spans="1:11">
+    <row r="119" spans="1:12">
       <c r="A119" t="s">
         <v>1693</v>
       </c>
@@ -13689,7 +14343,7 @@
         <v>1848</v>
       </c>
     </row>
-    <row r="120" spans="1:11">
+    <row r="120" spans="1:12">
       <c r="A120" t="s">
         <v>1773</v>
       </c>
@@ -13722,7 +14376,7 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="121" spans="1:11">
+    <row r="121" spans="1:12">
       <c r="A121" t="s">
         <v>1790</v>
       </c>
@@ -13755,7 +14409,7 @@
         <v>1852</v>
       </c>
     </row>
-    <row r="122" spans="1:11">
+    <row r="122" spans="1:12">
       <c r="A122" t="s">
         <v>1720</v>
       </c>
@@ -13788,7 +14442,7 @@
         <v>1850</v>
       </c>
     </row>
-    <row r="123" spans="1:11">
+    <row r="123" spans="1:12">
       <c r="A123" t="s">
         <v>1787</v>
       </c>
@@ -13821,7 +14475,7 @@
         <v>1854</v>
       </c>
     </row>
-    <row r="124" spans="1:11">
+    <row r="124" spans="1:12">
       <c r="A124" t="s">
         <v>1730</v>
       </c>
@@ -13854,7 +14508,7 @@
         <v>1858</v>
       </c>
     </row>
-    <row r="125" spans="1:11">
+    <row r="125" spans="1:12">
       <c r="A125" t="s">
         <v>1754</v>
       </c>
@@ -13887,7 +14541,7 @@
         <v>1856</v>
       </c>
     </row>
-    <row r="126" spans="1:11">
+    <row r="126" spans="1:12">
       <c r="A126" t="s">
         <v>1794</v>
       </c>
@@ -13920,7 +14574,7 @@
         <v>1860</v>
       </c>
     </row>
-    <row r="127" spans="1:11">
+    <row r="127" spans="1:12">
       <c r="A127" t="s">
         <v>1808</v>
       </c>
@@ -13953,7 +14607,7 @@
         <v>1860</v>
       </c>
     </row>
-    <row r="128" spans="1:11">
+    <row r="128" spans="1:12">
       <c r="A128" t="s">
         <v>1779</v>
       </c>
@@ -14021,10 +14675,10 @@
         <v>5</v>
       </c>
       <c r="C130" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="D130" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="E130">
         <v>9</v>
@@ -14043,7 +14697,7 @@
         <v>1915</v>
       </c>
       <c r="J130" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="131" spans="1:10">
@@ -14054,10 +14708,10 @@
         <v>5</v>
       </c>
       <c r="C131" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="D131" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="E131">
         <v>9</v>
@@ -14076,7 +14730,7 @@
         <v>1916</v>
       </c>
       <c r="J131" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="132" spans="1:10">
@@ -14087,10 +14741,10 @@
         <v>5</v>
       </c>
       <c r="C132" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="D132" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="E132">
         <v>9</v>
@@ -14109,7 +14763,7 @@
         <v>1915</v>
       </c>
       <c r="J132" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="133" spans="1:10">
@@ -14120,10 +14774,10 @@
         <v>5</v>
       </c>
       <c r="C133" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="D133" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="E133">
         <v>9</v>
@@ -14142,7 +14796,7 @@
         <v>1914</v>
       </c>
       <c r="J133" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="134" spans="1:10">
@@ -14153,10 +14807,10 @@
         <v>5</v>
       </c>
       <c r="C134" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="D134" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="E134">
         <v>9</v>
@@ -14175,7 +14829,7 @@
         <v>1913</v>
       </c>
       <c r="J134" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="135" spans="1:10">
@@ -14186,10 +14840,10 @@
         <v>5</v>
       </c>
       <c r="C135" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="D135" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="E135">
         <v>9</v>
@@ -14208,7 +14862,7 @@
         <v>1916</v>
       </c>
       <c r="J135" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="136" spans="1:10">
@@ -14615,7 +15269,7 @@
         <v>1600</v>
       </c>
       <c r="D149" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="E149">
         <v>2</v>
@@ -14735,7 +15389,7 @@
         <v>1603</v>
       </c>
       <c r="D153" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="E153">
         <v>6</v>
@@ -14972,107 +15626,112 @@
     </row>
     <row r="170" spans="1:9">
       <c r="A170" t="s">
-        <v>1971</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="171" spans="1:9">
       <c r="A171" t="s">
-        <v>1972</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="172" spans="1:9">
       <c r="A172" t="s">
-        <v>1973</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="173" spans="1:9">
       <c r="A173" t="s">
-        <v>1974</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="174" spans="1:9">
       <c r="A174" t="s">
-        <v>1975</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="175" spans="1:9">
       <c r="A175" t="s">
-        <v>1976</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="176" spans="1:9">
       <c r="A176" t="s">
-        <v>1978</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>1979</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>1980</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>1981</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>1982</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>1983</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>1977</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>1984</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>1985</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>1986</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>1987</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>1989</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>1988</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>1990</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>1991</v>
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1">
+      <c r="A191" t="s">
+        <v>1996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish annotating BAM files and marking progress
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA316EFD-AAA7-4F9B-9A62-B7A50A591BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E1764B-114B-4202-B1E8-75FE2F610AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11472" uniqueCount="2102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11513" uniqueCount="2143">
   <si>
     <t>Caster Level</t>
   </si>
@@ -6346,6 +6346,129 @@
   </si>
   <si>
     <t>sleep.BAM</t>
+  </si>
+  <si>
+    <t>snake's-swiftness.BAM</t>
+  </si>
+  <si>
+    <t>snilloc's-snowball-swarm.BAM</t>
+  </si>
+  <si>
+    <t>spell-deflection.BAM</t>
+  </si>
+  <si>
+    <t>spell-immunity-abjuration.BAM</t>
+  </si>
+  <si>
+    <t>spell-immunity-alteration.BAM</t>
+  </si>
+  <si>
+    <t>spell-immunity-conjuration.BAM</t>
+  </si>
+  <si>
+    <t>spell-immunity-divination.BAM</t>
+  </si>
+  <si>
+    <t>spell-immunity-enchantment.BAM</t>
+  </si>
+  <si>
+    <t>spell-immunity-evocation.BAM</t>
+  </si>
+  <si>
+    <t>spell-immunity-illusion.BAM</t>
+  </si>
+  <si>
+    <t>spell-immunity-necromancy.BAM</t>
+  </si>
+  <si>
+    <t>spell-trap.BAM</t>
+  </si>
+  <si>
+    <t>spell-turning.BAM</t>
+  </si>
+  <si>
+    <t>sphere-of-protection-from-petrification.BAM</t>
+  </si>
+  <si>
+    <t>sphere-of-protection-from-acid.BAM</t>
+  </si>
+  <si>
+    <t>sphere-of-protection-from-cold.BAM</t>
+  </si>
+  <si>
+    <t>sphere-of-protection-from-poison.BAM</t>
+  </si>
+  <si>
+    <t>sphere-of-protection-from-electricity.BAM</t>
+  </si>
+  <si>
+    <t>sphere-of-protection-from-fire.BAM</t>
+  </si>
+  <si>
+    <t>spike-growth.BAM</t>
+  </si>
+  <si>
+    <t>spike-stones.BAM</t>
+  </si>
+  <si>
+    <t>spirit-armor.BAM</t>
+  </si>
+  <si>
+    <t>spirit-fire.BAM</t>
+  </si>
+  <si>
+    <t>spirit-ward.BAM</t>
+  </si>
+  <si>
+    <t>stinking-cloud.BAM</t>
+  </si>
+  <si>
+    <t>stoneskin.BAM</t>
+  </si>
+  <si>
+    <t>strength.BAM</t>
+  </si>
+  <si>
+    <t>strength-of-one.BAM</t>
+  </si>
+  <si>
+    <t>tenser's-transformation.BAM</t>
+  </si>
+  <si>
+    <t>trollish-fortitude.BAM</t>
+  </si>
+  <si>
+    <t>true-sight.BAM</t>
+  </si>
+  <si>
+    <t>true-strike.BAM</t>
+  </si>
+  <si>
+    <t>turning-weapon.BAM</t>
+  </si>
+  <si>
+    <t>unfailing-endurance.BAM</t>
+  </si>
+  <si>
+    <t>vocalize.BAM</t>
+  </si>
+  <si>
+    <t>web.BAM</t>
+  </si>
+  <si>
+    <t>wind-shots.BAM</t>
+  </si>
+  <si>
+    <t>wondrous-recall.BAM</t>
+  </si>
+  <si>
+    <t>wraithform.BAM</t>
+  </si>
+  <si>
+    <t>writhing-fog.BAM</t>
+  </si>
+  <si>
+    <t>zone-of-sweet-air.BAM</t>
   </si>
 </sst>
 </file>
@@ -6523,7 +6646,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -6577,6 +6700,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent2" xfId="4" builtinId="33"/>
@@ -10392,11 +10516,11 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90FF5842-5F39-42CA-813E-70DCD245FAB4}">
-  <dimension ref="A1:L191"/>
+  <dimension ref="A1:M191"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L116" sqref="L116"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L156" sqref="L156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -10411,7 +10535,7 @@
     <col min="8" max="8" width="17.08984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.1796875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="39.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -14218,7 +14342,7 @@
       </c>
     </row>
     <row r="116" spans="1:12">
-      <c r="A116" t="s">
+      <c r="A116" s="34" t="s">
         <v>1874</v>
       </c>
       <c r="B116">
@@ -14246,9 +14370,12 @@
       <c r="I116" t="s">
         <v>1913</v>
       </c>
+      <c r="L116" t="s">
+        <v>2102</v>
+      </c>
     </row>
     <row r="117" spans="1:12">
-      <c r="A117" t="s">
+      <c r="A117" s="34" t="s">
         <v>1714</v>
       </c>
       <c r="B117">
@@ -14276,9 +14403,12 @@
       <c r="I117" t="s">
         <v>1822</v>
       </c>
+      <c r="L117" t="s">
+        <v>2103</v>
+      </c>
     </row>
     <row r="118" spans="1:12">
-      <c r="A118" t="s">
+      <c r="A118" s="34" t="s">
         <v>1768</v>
       </c>
       <c r="B118">
@@ -14309,9 +14439,12 @@
       <c r="J118" t="s">
         <v>255</v>
       </c>
+      <c r="L118" t="s">
+        <v>2104</v>
+      </c>
     </row>
     <row r="119" spans="1:12">
-      <c r="A119" t="s">
+      <c r="A119" s="34" t="s">
         <v>1693</v>
       </c>
       <c r="B119">
@@ -14342,9 +14475,12 @@
       <c r="J119" t="s">
         <v>1848</v>
       </c>
+      <c r="L119" t="s">
+        <v>2105</v>
+      </c>
     </row>
     <row r="120" spans="1:12">
-      <c r="A120" t="s">
+      <c r="A120" s="34" t="s">
         <v>1773</v>
       </c>
       <c r="B120">
@@ -14375,9 +14511,12 @@
       <c r="J120" t="s">
         <v>1861</v>
       </c>
+      <c r="L120" t="s">
+        <v>2106</v>
+      </c>
     </row>
     <row r="121" spans="1:12">
-      <c r="A121" t="s">
+      <c r="A121" s="34" t="s">
         <v>1790</v>
       </c>
       <c r="B121">
@@ -14408,9 +14547,12 @@
       <c r="J121" t="s">
         <v>1852</v>
       </c>
+      <c r="L121" t="s">
+        <v>2107</v>
+      </c>
     </row>
     <row r="122" spans="1:12">
-      <c r="A122" t="s">
+      <c r="A122" s="34" t="s">
         <v>1720</v>
       </c>
       <c r="B122">
@@ -14441,9 +14583,12 @@
       <c r="J122" t="s">
         <v>1850</v>
       </c>
+      <c r="L122" t="s">
+        <v>2108</v>
+      </c>
     </row>
     <row r="123" spans="1:12">
-      <c r="A123" t="s">
+      <c r="A123" s="34" t="s">
         <v>1787</v>
       </c>
       <c r="B123">
@@ -14474,9 +14619,12 @@
       <c r="J123" t="s">
         <v>1854</v>
       </c>
+      <c r="L123" t="s">
+        <v>2109</v>
+      </c>
     </row>
     <row r="124" spans="1:12">
-      <c r="A124" t="s">
+      <c r="A124" s="34" t="s">
         <v>1730</v>
       </c>
       <c r="B124">
@@ -14507,9 +14655,12 @@
       <c r="J124" t="s">
         <v>1858</v>
       </c>
+      <c r="L124" t="s">
+        <v>2110</v>
+      </c>
     </row>
     <row r="125" spans="1:12">
-      <c r="A125" t="s">
+      <c r="A125" s="34" t="s">
         <v>1754</v>
       </c>
       <c r="B125">
@@ -14540,9 +14691,12 @@
       <c r="J125" t="s">
         <v>1856</v>
       </c>
+      <c r="L125" t="s">
+        <v>2111</v>
+      </c>
     </row>
     <row r="126" spans="1:12">
-      <c r="A126" t="s">
+      <c r="A126" s="34" t="s">
         <v>1794</v>
       </c>
       <c r="B126">
@@ -14573,89 +14727,95 @@
       <c r="J126" t="s">
         <v>1860</v>
       </c>
+      <c r="L126" t="s">
+        <v>2112</v>
+      </c>
     </row>
     <row r="127" spans="1:12">
-      <c r="A127" t="s">
-        <v>1808</v>
+      <c r="A127" s="34" t="s">
+        <v>1779</v>
       </c>
       <c r="B127">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C127" t="s">
-        <v>1859</v>
+        <v>679</v>
       </c>
       <c r="D127" t="s">
-        <v>224</v>
+        <v>514</v>
       </c>
       <c r="E127">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F127">
         <f>E127*2</f>
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="G127" t="s">
-        <v>1677</v>
+        <v>1681</v>
       </c>
       <c r="H127" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I127" t="s">
-        <v>1833</v>
-      </c>
-      <c r="J127" t="s">
-        <v>1860</v>
+        <v>1830</v>
+      </c>
+      <c r="L127" t="s">
+        <v>2113</v>
       </c>
     </row>
     <row r="128" spans="1:12">
-      <c r="A128" t="s">
-        <v>1779</v>
+      <c r="A128" s="34" t="s">
+        <v>1728</v>
       </c>
       <c r="B128">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C128" t="s">
-        <v>679</v>
+        <v>630</v>
       </c>
       <c r="D128" t="s">
-        <v>514</v>
+        <v>270</v>
       </c>
       <c r="E128">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F128">
         <f>E128*2</f>
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G128" t="s">
         <v>1681</v>
       </c>
       <c r="H128" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I128" t="s">
-        <v>1830</v>
-      </c>
-    </row>
-    <row r="129" spans="1:10">
-      <c r="A129" t="s">
-        <v>1728</v>
+        <v>1825</v>
+      </c>
+      <c r="L128" t="s">
+        <v>2114</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12">
+      <c r="A129" s="34" t="s">
+        <v>1896</v>
       </c>
       <c r="B129">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C129" t="s">
-        <v>630</v>
+        <v>1947</v>
       </c>
       <c r="D129" t="s">
-        <v>270</v>
+        <v>1942</v>
       </c>
       <c r="E129">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F129">
         <f>E129*2</f>
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="G129" t="s">
         <v>1681</v>
@@ -14664,18 +14824,24 @@
         <v>1</v>
       </c>
       <c r="I129" t="s">
-        <v>1825</v>
-      </c>
-    </row>
-    <row r="130" spans="1:10">
-      <c r="A130" t="s">
-        <v>1896</v>
+        <v>1915</v>
+      </c>
+      <c r="J129" t="s">
+        <v>1948</v>
+      </c>
+      <c r="L129" t="s">
+        <v>2116</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12">
+      <c r="A130" s="34" t="s">
+        <v>1909</v>
       </c>
       <c r="B130">
         <v>5</v>
       </c>
       <c r="C130" t="s">
-        <v>1947</v>
+        <v>1943</v>
       </c>
       <c r="D130" t="s">
         <v>1942</v>
@@ -14694,21 +14860,24 @@
         <v>1</v>
       </c>
       <c r="I130" t="s">
-        <v>1915</v>
+        <v>1916</v>
       </c>
       <c r="J130" t="s">
-        <v>1948</v>
-      </c>
-    </row>
-    <row r="131" spans="1:10">
-      <c r="A131" t="s">
-        <v>1909</v>
+        <v>1944</v>
+      </c>
+      <c r="L130" t="s">
+        <v>2117</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12">
+      <c r="A131" s="34" t="s">
+        <v>1899</v>
       </c>
       <c r="B131">
         <v>5</v>
       </c>
       <c r="C131" t="s">
-        <v>1943</v>
+        <v>1945</v>
       </c>
       <c r="D131" t="s">
         <v>1942</v>
@@ -14727,21 +14896,24 @@
         <v>1</v>
       </c>
       <c r="I131" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="J131" t="s">
-        <v>1944</v>
-      </c>
-    </row>
-    <row r="132" spans="1:10">
-      <c r="A132" t="s">
-        <v>1899</v>
+        <v>1946</v>
+      </c>
+      <c r="L131" t="s">
+        <v>2119</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12">
+      <c r="A132" s="34" t="s">
+        <v>1883</v>
       </c>
       <c r="B132">
         <v>5</v>
       </c>
       <c r="C132" t="s">
-        <v>1945</v>
+        <v>1940</v>
       </c>
       <c r="D132" t="s">
         <v>1942</v>
@@ -14760,21 +14932,24 @@
         <v>1</v>
       </c>
       <c r="I132" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="J132" t="s">
-        <v>1946</v>
-      </c>
-    </row>
-    <row r="133" spans="1:10">
-      <c r="A133" t="s">
-        <v>1883</v>
+        <v>1941</v>
+      </c>
+      <c r="L132" t="s">
+        <v>2120</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12">
+      <c r="A133" s="34" t="s">
+        <v>1980</v>
       </c>
       <c r="B133">
         <v>5</v>
       </c>
       <c r="C133" t="s">
-        <v>1940</v>
+        <v>1951</v>
       </c>
       <c r="D133" t="s">
         <v>1942</v>
@@ -14793,21 +14968,24 @@
         <v>1</v>
       </c>
       <c r="I133" t="s">
-        <v>1914</v>
+        <v>1820</v>
       </c>
       <c r="J133" t="s">
-        <v>1941</v>
-      </c>
-    </row>
-    <row r="134" spans="1:10">
-      <c r="A134" t="s">
-        <v>1877</v>
+        <v>1952</v>
+      </c>
+      <c r="L133" t="s">
+        <v>2115</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12">
+      <c r="A134" s="34" t="s">
+        <v>1911</v>
       </c>
       <c r="B134">
         <v>5</v>
       </c>
       <c r="C134" t="s">
-        <v>1951</v>
+        <v>1949</v>
       </c>
       <c r="D134" t="s">
         <v>1942</v>
@@ -14826,64 +15004,67 @@
         <v>1</v>
       </c>
       <c r="I134" t="s">
-        <v>1913</v>
+        <v>1916</v>
       </c>
       <c r="J134" t="s">
-        <v>1952</v>
-      </c>
-    </row>
-    <row r="135" spans="1:10">
-      <c r="A135" t="s">
-        <v>1911</v>
+        <v>1950</v>
+      </c>
+      <c r="L134" t="s">
+        <v>2118</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12">
+      <c r="A135" s="34" t="s">
+        <v>1749</v>
       </c>
       <c r="B135">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C135" t="s">
-        <v>1949</v>
+        <v>1056</v>
       </c>
       <c r="D135" t="s">
-        <v>1942</v>
+        <v>1408</v>
       </c>
       <c r="E135">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F135">
         <f>E135*2</f>
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G135" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="H135" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I135" t="s">
-        <v>1916</v>
-      </c>
-      <c r="J135" t="s">
-        <v>1950</v>
-      </c>
-    </row>
-    <row r="136" spans="1:10">
-      <c r="A136" t="s">
-        <v>1749</v>
+        <v>1827</v>
+      </c>
+      <c r="L135" t="s">
+        <v>2121</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12">
+      <c r="A136" s="34" t="s">
+        <v>1710</v>
       </c>
       <c r="B136">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C136" t="s">
-        <v>1056</v>
+        <v>1106</v>
       </c>
       <c r="D136" t="s">
         <v>1408</v>
       </c>
       <c r="E136">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F136">
         <f>E136*2</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G136" t="s">
         <v>1680</v>
@@ -14892,291 +15073,321 @@
         <v>0</v>
       </c>
       <c r="I136" t="s">
-        <v>1827</v>
-      </c>
-    </row>
-    <row r="137" spans="1:10">
-      <c r="A137" t="s">
-        <v>1710</v>
+        <v>1822</v>
+      </c>
+      <c r="L136" t="s">
+        <v>2122</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12">
+      <c r="A137" s="34" t="s">
+        <v>1767</v>
       </c>
       <c r="B137">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C137" t="s">
-        <v>1106</v>
+        <v>153</v>
       </c>
       <c r="D137" t="s">
-        <v>1408</v>
+        <v>140</v>
       </c>
       <c r="E137">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F137">
         <f>E137*2</f>
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G137" t="s">
-        <v>1680</v>
+        <v>1681</v>
       </c>
       <c r="H137" t="b">
         <v>0</v>
       </c>
       <c r="I137" t="s">
-        <v>1822</v>
-      </c>
-    </row>
-    <row r="138" spans="1:10">
-      <c r="A138" t="s">
-        <v>1767</v>
+        <v>1829</v>
+      </c>
+      <c r="L137" t="s">
+        <v>2123</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12">
+      <c r="A138" s="34" t="s">
+        <v>1713</v>
       </c>
       <c r="B138">
         <v>4</v>
       </c>
       <c r="C138" t="s">
-        <v>153</v>
+        <v>1252</v>
       </c>
       <c r="D138" t="s">
-        <v>140</v>
+        <v>1251</v>
       </c>
       <c r="E138">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F138">
         <f>E138*2</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G138" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="H138" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I138" t="s">
-        <v>1829</v>
-      </c>
-    </row>
-    <row r="139" spans="1:10">
-      <c r="A139" t="s">
-        <v>1713</v>
+        <v>1822</v>
+      </c>
+      <c r="L138" t="s">
+        <v>2124</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12">
+      <c r="A139" s="34" t="s">
+        <v>1716</v>
       </c>
       <c r="B139">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C139" t="s">
-        <v>1252</v>
+        <v>1246</v>
       </c>
       <c r="D139" t="s">
-        <v>1251</v>
+        <v>1245</v>
       </c>
       <c r="E139">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F139">
         <f>E139*2</f>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G139" t="s">
-        <v>1680</v>
+        <v>1681</v>
       </c>
       <c r="H139" t="b">
         <v>1</v>
       </c>
       <c r="I139" t="s">
-        <v>1822</v>
-      </c>
-    </row>
-    <row r="140" spans="1:10">
-      <c r="A140" t="s">
-        <v>1716</v>
+        <v>1823</v>
+      </c>
+      <c r="L139" t="s">
+        <v>2125</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12">
+      <c r="A140" s="34" t="s">
+        <v>1785</v>
       </c>
       <c r="B140">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C140" t="s">
-        <v>1246</v>
+        <v>88</v>
       </c>
       <c r="D140" t="s">
-        <v>1245</v>
+        <v>70</v>
       </c>
       <c r="E140">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F140">
         <f>E140*2</f>
+        <v>8</v>
+      </c>
+      <c r="G140" t="s">
+        <v>1680</v>
+      </c>
+      <c r="H140" t="b">
+        <v>0</v>
+      </c>
+      <c r="I140" t="s">
+        <v>1831</v>
+      </c>
+      <c r="L140" t="s">
+        <v>2126</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12">
+      <c r="A141" s="34" t="s">
+        <v>1734</v>
+      </c>
+      <c r="B141">
         <v>4</v>
       </c>
-      <c r="G140" t="s">
-        <v>1681</v>
-      </c>
-      <c r="H140" t="b">
-        <v>1</v>
-      </c>
-      <c r="I140" t="s">
-        <v>1823</v>
-      </c>
-    </row>
-    <row r="141" spans="1:10">
-      <c r="A141" t="s">
-        <v>1785</v>
-      </c>
-      <c r="B141">
-        <v>2</v>
-      </c>
       <c r="C141" t="s">
-        <v>88</v>
+        <v>1838</v>
       </c>
       <c r="D141" t="s">
-        <v>70</v>
+        <v>1839</v>
       </c>
       <c r="E141">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F141">
         <f>E141*2</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G141" t="s">
-        <v>1680</v>
+        <v>1681</v>
       </c>
       <c r="H141" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I141" t="s">
-        <v>1831</v>
-      </c>
-    </row>
-    <row r="142" spans="1:10">
-      <c r="A142" t="s">
-        <v>1734</v>
+        <v>1825</v>
+      </c>
+      <c r="L141" t="s">
+        <v>2127</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12">
+      <c r="A142" s="34" t="s">
+        <v>1807</v>
       </c>
       <c r="B142">
+        <v>2</v>
+      </c>
+      <c r="C142" t="s">
+        <v>89</v>
+      </c>
+      <c r="D142" t="s">
+        <v>71</v>
+      </c>
+      <c r="E142">
         <v>4</v>
-      </c>
-      <c r="C142" t="s">
-        <v>1838</v>
-      </c>
-      <c r="D142" t="s">
-        <v>1839</v>
-      </c>
-      <c r="E142">
-        <v>8</v>
       </c>
       <c r="F142">
         <f>E142*2</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G142" t="s">
-        <v>1681</v>
+        <v>1677</v>
       </c>
       <c r="H142" t="b">
         <v>1</v>
       </c>
       <c r="I142" t="s">
-        <v>1825</v>
-      </c>
-    </row>
-    <row r="143" spans="1:10">
-      <c r="A143" t="s">
-        <v>1807</v>
+        <v>1833</v>
+      </c>
+      <c r="L142" t="s">
+        <v>2128</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12">
+      <c r="A143" s="34" t="s">
+        <v>1778</v>
       </c>
       <c r="B143">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C143" t="s">
-        <v>89</v>
+        <v>990</v>
       </c>
       <c r="D143" t="s">
-        <v>71</v>
+        <v>1002</v>
       </c>
       <c r="E143">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F143">
         <f>E143*2</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G143" t="s">
         <v>1677</v>
       </c>
       <c r="H143" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I143" t="s">
-        <v>1833</v>
-      </c>
-    </row>
-    <row r="144" spans="1:10">
-      <c r="A144" t="s">
-        <v>1778</v>
+        <v>1830</v>
+      </c>
+      <c r="L143" t="s">
+        <v>2129</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12">
+      <c r="A144" s="34" t="s">
+        <v>1721</v>
       </c>
       <c r="B144">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C144" t="s">
-        <v>990</v>
+        <v>315</v>
       </c>
       <c r="D144" t="s">
-        <v>1002</v>
+        <v>186</v>
       </c>
       <c r="E144">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F144">
         <f>E144*2</f>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="G144" t="s">
         <v>1677</v>
       </c>
       <c r="H144" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I144" t="s">
-        <v>1830</v>
-      </c>
-    </row>
-    <row r="145" spans="1:12">
-      <c r="A145" t="s">
-        <v>1721</v>
+        <v>1823</v>
+      </c>
+      <c r="L144" t="s">
+        <v>2130</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13">
+      <c r="A145" s="34" t="s">
+        <v>1698</v>
       </c>
       <c r="B145">
         <v>6</v>
       </c>
       <c r="C145" t="s">
-        <v>315</v>
+        <v>269</v>
       </c>
       <c r="D145" t="s">
-        <v>186</v>
+        <v>1408</v>
       </c>
       <c r="E145">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F145">
         <f>E145*2</f>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G145" t="s">
         <v>1677</v>
       </c>
       <c r="H145" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I145" t="s">
-        <v>1823</v>
-      </c>
-    </row>
-    <row r="146" spans="1:12">
-      <c r="A146" t="s">
-        <v>1698</v>
+        <v>1820</v>
+      </c>
+      <c r="L145" t="s">
+        <v>2131</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13">
+      <c r="A146" s="34" t="s">
+        <v>1743</v>
       </c>
       <c r="B146">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C146" t="s">
-        <v>269</v>
+        <v>604</v>
       </c>
       <c r="D146" t="s">
-        <v>1408</v>
+        <v>1837</v>
       </c>
       <c r="E146">
         <v>10</v>
@@ -15192,28 +15403,31 @@
         <v>0</v>
       </c>
       <c r="I146" t="s">
-        <v>1820</v>
-      </c>
-    </row>
-    <row r="147" spans="1:12">
-      <c r="A147" t="s">
-        <v>1743</v>
+        <v>1826</v>
+      </c>
+      <c r="L146" t="s">
+        <v>2132</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13">
+      <c r="A147" s="34" t="s">
+        <v>1752</v>
       </c>
       <c r="B147">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C147" t="s">
-        <v>604</v>
+        <v>1683</v>
       </c>
       <c r="D147" t="s">
-        <v>1837</v>
+        <v>1842</v>
       </c>
       <c r="E147">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F147">
         <f>E147*2</f>
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="G147" t="s">
         <v>1677</v>
@@ -15222,21 +15436,27 @@
         <v>0</v>
       </c>
       <c r="I147" t="s">
-        <v>1826</v>
-      </c>
-    </row>
-    <row r="148" spans="1:12">
-      <c r="A148" t="s">
-        <v>1752</v>
+        <v>1827</v>
+      </c>
+      <c r="L147" t="s">
+        <v>2133</v>
+      </c>
+      <c r="M147" t="s">
+        <v>1843</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13">
+      <c r="A148" s="34" t="s">
+        <v>1889</v>
       </c>
       <c r="B148">
         <v>1</v>
       </c>
       <c r="C148" t="s">
-        <v>1683</v>
+        <v>1600</v>
       </c>
       <c r="D148" t="s">
-        <v>1842</v>
+        <v>1934</v>
       </c>
       <c r="E148">
         <v>2</v>
@@ -15252,84 +15472,90 @@
         <v>0</v>
       </c>
       <c r="I148" t="s">
-        <v>1827</v>
+        <v>1914</v>
       </c>
       <c r="L148" t="s">
-        <v>1843</v>
-      </c>
-    </row>
-    <row r="149" spans="1:12">
-      <c r="A149" t="s">
-        <v>1889</v>
+        <v>2134</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13">
+      <c r="A149" s="34" t="s">
+        <v>1687</v>
       </c>
       <c r="B149">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C149" t="s">
-        <v>1600</v>
+        <v>1084</v>
       </c>
       <c r="D149" t="s">
-        <v>1934</v>
+        <v>1408</v>
       </c>
       <c r="E149">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F149">
         <f>E149*2</f>
+        <v>16</v>
+      </c>
+      <c r="G149" t="s">
+        <v>1679</v>
+      </c>
+      <c r="H149" t="b">
+        <v>0</v>
+      </c>
+      <c r="I149" t="s">
+        <v>1819</v>
+      </c>
+      <c r="L149" t="s">
+        <v>2135</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13">
+      <c r="A150" s="34" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B150">
+        <v>2</v>
+      </c>
+      <c r="C150" t="s">
+        <v>93</v>
+      </c>
+      <c r="D150" t="s">
+        <v>76</v>
+      </c>
+      <c r="E150">
         <v>4</v>
-      </c>
-      <c r="G149" t="s">
-        <v>1677</v>
-      </c>
-      <c r="H149" t="b">
-        <v>0</v>
-      </c>
-      <c r="I149" t="s">
-        <v>1914</v>
-      </c>
-    </row>
-    <row r="150" spans="1:12">
-      <c r="A150" t="s">
-        <v>1687</v>
-      </c>
-      <c r="B150">
-        <v>4</v>
-      </c>
-      <c r="C150" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D150" t="s">
-        <v>1408</v>
-      </c>
-      <c r="E150">
-        <v>8</v>
       </c>
       <c r="F150">
         <f>E150*2</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G150" t="s">
-        <v>1679</v>
+        <v>1677</v>
       </c>
       <c r="H150" t="b">
         <v>0</v>
       </c>
       <c r="I150" t="s">
-        <v>1819</v>
-      </c>
-    </row>
-    <row r="151" spans="1:12">
-      <c r="A151" t="s">
-        <v>1719</v>
+        <v>1823</v>
+      </c>
+      <c r="L150" t="s">
+        <v>2136</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13">
+      <c r="A151" s="34" t="s">
+        <v>1791</v>
       </c>
       <c r="B151">
         <v>2</v>
       </c>
       <c r="C151" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D151" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E151">
         <v>4</v>
@@ -15339,64 +15565,70 @@
         <v>8</v>
       </c>
       <c r="G151" t="s">
-        <v>1677</v>
+        <v>1680</v>
       </c>
       <c r="H151" t="b">
         <v>0</v>
       </c>
       <c r="I151" t="s">
-        <v>1823</v>
-      </c>
-    </row>
-    <row r="152" spans="1:12">
-      <c r="A152" t="s">
-        <v>1791</v>
+        <v>1831</v>
+      </c>
+      <c r="L151" t="s">
+        <v>2137</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13">
+      <c r="A152" s="34" t="s">
+        <v>1906</v>
       </c>
       <c r="B152">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C152" t="s">
-        <v>90</v>
+        <v>1603</v>
       </c>
       <c r="D152" t="s">
-        <v>72</v>
+        <v>1935</v>
       </c>
       <c r="E152">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F152">
         <f>E152*2</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G152" t="s">
-        <v>1680</v>
+        <v>1677</v>
       </c>
       <c r="H152" t="b">
         <v>0</v>
       </c>
       <c r="I152" t="s">
-        <v>1831</v>
-      </c>
-    </row>
-    <row r="153" spans="1:12">
-      <c r="A153" t="s">
-        <v>1906</v>
+        <v>1916</v>
+      </c>
+      <c r="L152" t="s">
+        <v>2138</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13">
+      <c r="A153" s="34" t="s">
+        <v>1798</v>
       </c>
       <c r="B153">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C153" t="s">
-        <v>1603</v>
+        <v>1207</v>
       </c>
       <c r="D153" t="s">
-        <v>1935</v>
+        <v>1144</v>
       </c>
       <c r="E153">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F153">
         <f>E153*2</f>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="G153" t="s">
         <v>1677</v>
@@ -15405,51 +15637,57 @@
         <v>0</v>
       </c>
       <c r="I153" t="s">
-        <v>1916</v>
-      </c>
-    </row>
-    <row r="154" spans="1:12">
-      <c r="A154" t="s">
-        <v>1798</v>
+        <v>1832</v>
+      </c>
+      <c r="L153" t="s">
+        <v>2139</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13">
+      <c r="A154" s="34" t="s">
+        <v>1753</v>
       </c>
       <c r="B154">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C154" t="s">
-        <v>1207</v>
+        <v>1662</v>
       </c>
       <c r="D154" t="s">
-        <v>1144</v>
+        <v>108</v>
       </c>
       <c r="E154">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F154">
         <f>E154*2</f>
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="G154" t="s">
         <v>1677</v>
       </c>
       <c r="H154" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I154" t="s">
-        <v>1832</v>
-      </c>
-    </row>
-    <row r="155" spans="1:12">
-      <c r="A155" t="s">
-        <v>1753</v>
+        <v>1827</v>
+      </c>
+      <c r="L154" t="s">
+        <v>2140</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13">
+      <c r="A155" s="34" t="s">
+        <v>1709</v>
       </c>
       <c r="B155">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C155" t="s">
-        <v>1662</v>
+        <v>1248</v>
       </c>
       <c r="D155" t="s">
-        <v>108</v>
+        <v>1247</v>
       </c>
       <c r="E155">
         <v>5</v>
@@ -15459,34 +15697,37 @@
         <v>10</v>
       </c>
       <c r="G155" t="s">
-        <v>1677</v>
+        <v>1680</v>
       </c>
       <c r="H155" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I155" t="s">
-        <v>1827</v>
-      </c>
-    </row>
-    <row r="156" spans="1:12">
-      <c r="A156" t="s">
-        <v>1709</v>
+        <v>1822</v>
+      </c>
+      <c r="L155" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13">
+      <c r="A156" s="34" t="s">
+        <v>1727</v>
       </c>
       <c r="B156">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C156" t="s">
-        <v>1248</v>
+        <v>1191</v>
       </c>
       <c r="D156" t="s">
-        <v>1247</v>
+        <v>1067</v>
       </c>
       <c r="E156">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F156">
         <f>E156*2</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G156" t="s">
         <v>1680</v>
@@ -15495,249 +15736,242 @@
         <v>0</v>
       </c>
       <c r="I156" t="s">
-        <v>1822</v>
-      </c>
-    </row>
-    <row r="157" spans="1:12">
+        <v>1824</v>
+      </c>
+      <c r="L156" t="s">
+        <v>2142</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13">
       <c r="A157" t="s">
-        <v>1727</v>
-      </c>
-      <c r="B157">
-        <v>3</v>
-      </c>
-      <c r="C157" t="s">
-        <v>1191</v>
-      </c>
-      <c r="D157" t="s">
-        <v>1067</v>
-      </c>
-      <c r="E157">
-        <v>7</v>
-      </c>
-      <c r="F157">
-        <f>E157*2</f>
-        <v>14</v>
-      </c>
-      <c r="G157" t="s">
-        <v>1680</v>
-      </c>
-      <c r="H157" t="b">
-        <v>0</v>
-      </c>
-      <c r="I157" t="s">
-        <v>1824</v>
-      </c>
-    </row>
-    <row r="158" spans="1:12">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13">
       <c r="A158" t="s">
-        <v>1722</v>
-      </c>
-      <c r="I158" t="s">
-        <v>1824</v>
-      </c>
-    </row>
-    <row r="159" spans="1:12">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13">
       <c r="A159" t="s">
-        <v>1724</v>
-      </c>
-      <c r="I159" t="s">
-        <v>1824</v>
-      </c>
-    </row>
-    <row r="160" spans="1:12">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13">
       <c r="A160" t="s">
-        <v>1776</v>
-      </c>
-      <c r="I160" t="s">
-        <v>1830</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="161" spans="1:9">
       <c r="A161" t="s">
-        <v>1882</v>
-      </c>
-      <c r="I161" t="s">
-        <v>1914</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="162" spans="1:9">
       <c r="A162" t="s">
-        <v>1884</v>
-      </c>
-      <c r="I162" t="s">
-        <v>1914</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="163" spans="1:9">
       <c r="A163" t="s">
-        <v>1888</v>
-      </c>
-      <c r="I163" t="s">
-        <v>1914</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="164" spans="1:9">
       <c r="A164" t="s">
-        <v>1892</v>
-      </c>
-      <c r="I164" t="s">
-        <v>1915</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="165" spans="1:9">
       <c r="A165" t="s">
-        <v>1893</v>
-      </c>
-      <c r="I165" t="s">
-        <v>1915</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="166" spans="1:9">
       <c r="A166" t="s">
-        <v>1895</v>
-      </c>
-      <c r="I166" t="s">
-        <v>1915</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="167" spans="1:9">
       <c r="A167" t="s">
-        <v>1903</v>
-      </c>
-      <c r="I167" t="s">
-        <v>1916</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="168" spans="1:9">
       <c r="A168" t="s">
-        <v>1904</v>
-      </c>
-      <c r="I168" t="s">
-        <v>1916</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="169" spans="1:9">
       <c r="A169" t="s">
-        <v>1905</v>
-      </c>
-      <c r="I169" t="s">
-        <v>1916</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="170" spans="1:9">
       <c r="A170" t="s">
-        <v>1975</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="171" spans="1:9">
       <c r="A171" t="s">
-        <v>1976</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="172" spans="1:9">
       <c r="A172" t="s">
-        <v>1977</v>
+        <v>1722</v>
+      </c>
+      <c r="I172" t="s">
+        <v>1824</v>
       </c>
     </row>
     <row r="173" spans="1:9">
       <c r="A173" t="s">
-        <v>1978</v>
+        <v>1991</v>
+      </c>
+      <c r="I173" t="s">
+        <v>1824</v>
       </c>
     </row>
     <row r="174" spans="1:9">
       <c r="A174" t="s">
-        <v>1979</v>
+        <v>1993</v>
+      </c>
+      <c r="I174" t="s">
+        <v>1824</v>
       </c>
     </row>
     <row r="175" spans="1:9">
       <c r="A175" t="s">
-        <v>1980</v>
+        <v>1992</v>
+      </c>
+      <c r="I175" t="s">
+        <v>1824</v>
       </c>
     </row>
     <row r="176" spans="1:9">
       <c r="A176" t="s">
-        <v>1982</v>
-      </c>
-    </row>
-    <row r="177" spans="1:1">
+        <v>1724</v>
+      </c>
+      <c r="I176" t="s">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9">
       <c r="A177" t="s">
-        <v>1983</v>
-      </c>
-    </row>
-    <row r="178" spans="1:1">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9">
       <c r="A178" t="s">
-        <v>1984</v>
-      </c>
-    </row>
-    <row r="179" spans="1:1">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9">
       <c r="A179" t="s">
-        <v>1985</v>
-      </c>
-    </row>
-    <row r="180" spans="1:1">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9">
       <c r="A180" t="s">
-        <v>1986</v>
-      </c>
-    </row>
-    <row r="181" spans="1:1">
+        <v>1776</v>
+      </c>
+      <c r="I180" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9">
       <c r="A181" t="s">
-        <v>1987</v>
-      </c>
-    </row>
-    <row r="182" spans="1:1">
-      <c r="A182" t="s">
-        <v>1981</v>
-      </c>
-    </row>
-    <row r="183" spans="1:1">
+        <v>1808</v>
+      </c>
+      <c r="I181" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9">
+      <c r="A182" s="35" t="s">
+        <v>1877</v>
+      </c>
+      <c r="I182" t="s">
+        <v>1913</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9">
       <c r="A183" t="s">
-        <v>1988</v>
-      </c>
-    </row>
-    <row r="184" spans="1:1">
+        <v>1882</v>
+      </c>
+      <c r="I183" t="s">
+        <v>1914</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9">
       <c r="A184" t="s">
-        <v>1989</v>
-      </c>
-    </row>
-    <row r="185" spans="1:1">
+        <v>1884</v>
+      </c>
+      <c r="I184" t="s">
+        <v>1914</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9">
       <c r="A185" t="s">
-        <v>1990</v>
-      </c>
-    </row>
-    <row r="186" spans="1:1">
+        <v>1888</v>
+      </c>
+      <c r="I185" t="s">
+        <v>1914</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9">
       <c r="A186" t="s">
-        <v>1991</v>
-      </c>
-    </row>
-    <row r="187" spans="1:1">
+        <v>1892</v>
+      </c>
+      <c r="I186" t="s">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9">
       <c r="A187" t="s">
-        <v>1993</v>
-      </c>
-    </row>
-    <row r="188" spans="1:1">
+        <v>1893</v>
+      </c>
+      <c r="I187" t="s">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9">
       <c r="A188" t="s">
-        <v>1992</v>
-      </c>
-    </row>
-    <row r="189" spans="1:1">
+        <v>1895</v>
+      </c>
+      <c r="I188" t="s">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9">
       <c r="A189" t="s">
-        <v>1994</v>
-      </c>
-    </row>
-    <row r="190" spans="1:1">
+        <v>1903</v>
+      </c>
+      <c r="I189" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9">
       <c r="A190" t="s">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="191" spans="1:1">
+        <v>1904</v>
+      </c>
+      <c r="I190" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9">
       <c r="A191" t="s">
-        <v>1996</v>
+        <v>1905</v>
+      </c>
+      <c r="I191" t="s">
+        <v>1916</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L169">
-    <sortCondition ref="C2:C169"/>
-    <sortCondition ref="A2:A169"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M192">
+    <sortCondition ref="C2:C192"/>
+    <sortCondition ref="A2:A192"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Expose to the Elements
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA301F6-FAEB-4539-904E-38BD8713FE0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C07F4E-9236-4B7F-BCC1-1C207163D1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -10525,8 +10525,8 @@
   <dimension ref="A1:M191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L71" sqref="A71:L71"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L93" sqref="A93:L93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -13617,32 +13617,34 @@
       <c r="A93" s="34" t="s">
         <v>1875</v>
       </c>
-      <c r="B93">
+      <c r="B93" s="34">
         <v>5</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="34" t="s">
         <v>1605</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" s="34" t="s">
         <v>1937</v>
       </c>
-      <c r="E93">
+      <c r="E93" s="34">
         <v>10</v>
       </c>
-      <c r="F93">
+      <c r="F93" s="34">
         <f>E93*2</f>
         <v>20</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G93" s="34" t="s">
         <v>1680</v>
       </c>
-      <c r="H93" t="b">
-        <v>1</v>
-      </c>
-      <c r="I93" t="s">
+      <c r="H93" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I93" s="34" t="s">
         <v>1913</v>
       </c>
-      <c r="L93" t="s">
+      <c r="J93" s="34"/>
+      <c r="K93" s="34"/>
+      <c r="L93" s="34" t="s">
         <v>2028</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sphere of Security: Protection from Acid
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C07F4E-9236-4B7F-BCC1-1C207163D1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1845FB8C-8201-4E86-9578-6DA437FDB8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -5862,42 +5862,24 @@
     <t>Sphere of Protection from Fire</t>
   </si>
   <si>
-    <t>MESOS01</t>
-  </si>
-  <si>
     <t>MEPR558</t>
   </si>
   <si>
     <t>Sphere of Protection from Cold</t>
   </si>
   <si>
-    <t>MESOS02</t>
-  </si>
-  <si>
     <t>Sphere of Protection from Electricity</t>
   </si>
   <si>
-    <t>MESOS03</t>
-  </si>
-  <si>
     <t>Sphere of Protection from Acid</t>
   </si>
   <si>
-    <t>MESOS04</t>
-  </si>
-  <si>
     <t>Sphere of Protection from Poison</t>
   </si>
   <si>
-    <t>MESOS05</t>
-  </si>
-  <si>
     <t>Sphere of Protection from Petrification</t>
   </si>
   <si>
-    <t>MESOS06</t>
-  </si>
-  <si>
     <t>MEPR653</t>
   </si>
   <si>
@@ -6475,6 +6457,24 @@
   </si>
   <si>
     <t>MEPR455</t>
+  </si>
+  <si>
+    <t>MESOS04, etc.</t>
+  </si>
+  <si>
+    <t>MESOS02, etc.</t>
+  </si>
+  <si>
+    <t>MESOS03, etc.</t>
+  </si>
+  <si>
+    <t>MESOS01, etc.</t>
+  </si>
+  <si>
+    <t>MESOS06, etc.</t>
+  </si>
+  <si>
+    <t>MESOS05, etc.</t>
   </si>
 </sst>
 </file>
@@ -10525,8 +10525,8 @@
   <dimension ref="A1:M191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L93" sqref="A93:L93"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L94" sqref="A94:L94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -10540,7 +10540,7 @@
     <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.08984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.08984375" customWidth="1"/>
     <col min="12" max="12" width="39.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10558,10 +10558,10 @@
         <v>1817</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>1958</v>
+        <v>1952</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>1959</v>
+        <v>1953</v>
       </c>
       <c r="G1" s="23" t="s">
         <v>1676</v>
@@ -10573,13 +10573,13 @@
         <v>1818</v>
       </c>
       <c r="J1" s="23" t="s">
+        <v>1950</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>1949</v>
+      </c>
+      <c r="L1" s="23" t="s">
         <v>1956</v>
-      </c>
-      <c r="K1" s="23" t="s">
-        <v>1955</v>
-      </c>
-      <c r="L1" s="23" t="s">
-        <v>1962</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="34" customFormat="1">
@@ -10612,7 +10612,7 @@
         <v>1914</v>
       </c>
       <c r="L2" s="34" t="s">
-        <v>2027</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -10647,7 +10647,7 @@
       <c r="J3" s="34"/>
       <c r="K3" s="34"/>
       <c r="L3" s="34" t="s">
-        <v>2101</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -10661,7 +10661,7 @@
         <v>1601</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>2142</v>
+        <v>2136</v>
       </c>
       <c r="E4" s="34">
         <v>4</v>
@@ -10671,7 +10671,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>2143</v>
+        <v>2137</v>
       </c>
       <c r="H4" s="34" t="b">
         <v>1</v>
@@ -10682,7 +10682,7 @@
       <c r="J4" s="34"/>
       <c r="K4" s="34"/>
       <c r="L4" s="34" t="s">
-        <v>2096</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -10706,7 +10706,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="34" t="s">
-        <v>2143</v>
+        <v>2137</v>
       </c>
       <c r="H5" s="34" t="b">
         <v>0</v>
@@ -10717,7 +10717,7 @@
       <c r="J5" s="34"/>
       <c r="K5" s="34"/>
       <c r="L5" s="34" t="s">
-        <v>2133</v>
+        <v>2127</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -10728,7 +10728,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>2001</v>
+        <v>1995</v>
       </c>
       <c r="D6" s="34" t="s">
         <v>1932</v>
@@ -10752,7 +10752,7 @@
       <c r="J6" s="34"/>
       <c r="K6" s="34"/>
       <c r="L6" s="34" t="s">
-        <v>2000</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -10787,7 +10787,7 @@
       <c r="J7" s="34"/>
       <c r="K7" s="34"/>
       <c r="L7" s="34" t="s">
-        <v>2088</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -10820,7 +10820,7 @@
         <v>1819</v>
       </c>
       <c r="L8" t="s">
-        <v>1967</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -10853,7 +10853,7 @@
         <v>1822</v>
       </c>
       <c r="L9" t="s">
-        <v>2024</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -10886,7 +10886,7 @@
         <v>1821</v>
       </c>
       <c r="L10" t="s">
-        <v>2095</v>
+        <v>2089</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -10919,7 +10919,7 @@
         <v>1825</v>
       </c>
       <c r="L11" t="s">
-        <v>1996</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -10952,7 +10952,7 @@
         <v>1823</v>
       </c>
       <c r="L12" t="s">
-        <v>2124</v>
+        <v>2118</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -10985,7 +10985,7 @@
         <v>1822</v>
       </c>
       <c r="L13" t="s">
-        <v>2042</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -11018,7 +11018,7 @@
         <v>1821</v>
       </c>
       <c r="L14" t="s">
-        <v>1965</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -11051,7 +11051,7 @@
         <v>1820</v>
       </c>
       <c r="L15" t="s">
-        <v>2036</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -11084,7 +11084,7 @@
         <v>1826</v>
       </c>
       <c r="L16" t="s">
-        <v>2085</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -11117,7 +11117,7 @@
         <v>1827</v>
       </c>
       <c r="L17" t="s">
-        <v>2132</v>
+        <v>2126</v>
       </c>
       <c r="M17" t="s">
         <v>1843</v>
@@ -11153,7 +11153,7 @@
         <v>1830</v>
       </c>
       <c r="L18" t="s">
-        <v>2078</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -11186,7 +11186,7 @@
         <v>1829</v>
       </c>
       <c r="L19" t="s">
-        <v>2098</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -11219,7 +11219,7 @@
         <v>1822</v>
       </c>
       <c r="L20" t="s">
-        <v>2100</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -11252,7 +11252,7 @@
         <v>1824</v>
       </c>
       <c r="L21" t="s">
-        <v>1998</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -11285,7 +11285,7 @@
         <v>1832</v>
       </c>
       <c r="L22" t="s">
-        <v>2002</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -11318,7 +11318,7 @@
         <v>1829</v>
       </c>
       <c r="L23" t="s">
-        <v>2011</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -11351,7 +11351,7 @@
         <v>1823</v>
       </c>
       <c r="L24" t="s">
-        <v>2015</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -11384,7 +11384,7 @@
         <v>1822</v>
       </c>
       <c r="L25" t="s">
-        <v>2102</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -11419,7 +11419,7 @@
       <c r="J26" s="34"/>
       <c r="K26" s="34"/>
       <c r="L26" s="34" t="s">
-        <v>2040</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -11452,7 +11452,7 @@
         <v>1824</v>
       </c>
       <c r="L27" t="s">
-        <v>1964</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -11485,7 +11485,7 @@
         <v>1823</v>
       </c>
       <c r="L28" t="s">
-        <v>1966</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -11518,7 +11518,7 @@
         <v>1828</v>
       </c>
       <c r="L29" t="s">
-        <v>1969</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -11551,7 +11551,7 @@
         <v>1831</v>
       </c>
       <c r="L30" t="s">
-        <v>2030</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -11584,7 +11584,7 @@
         <v>1820</v>
       </c>
       <c r="L31" t="s">
-        <v>2092</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -11617,7 +11617,7 @@
         <v>1826</v>
       </c>
       <c r="L32" t="s">
-        <v>2019</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -11650,7 +11650,7 @@
         <v>1822</v>
       </c>
       <c r="L33" t="s">
-        <v>2140</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -11683,7 +11683,7 @@
         <v>1826</v>
       </c>
       <c r="L34" t="s">
-        <v>1968</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -11716,7 +11716,7 @@
         <v>1828</v>
       </c>
       <c r="L35" t="s">
-        <v>2016</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -11749,7 +11749,7 @@
         <v>1829</v>
       </c>
       <c r="L36" t="s">
-        <v>2053</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -11782,7 +11782,7 @@
         <v>1830</v>
       </c>
       <c r="L37" t="s">
-        <v>2056</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -11796,7 +11796,7 @@
         <v>85</v>
       </c>
       <c r="D38" t="s">
-        <v>2091</v>
+        <v>2085</v>
       </c>
       <c r="E38">
         <v>4</v>
@@ -11815,7 +11815,7 @@
         <v>1833</v>
       </c>
       <c r="L38" t="s">
-        <v>2090</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -11848,7 +11848,7 @@
         <v>1833</v>
       </c>
       <c r="L39" t="s">
-        <v>2062</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -11881,7 +11881,7 @@
         <v>1831</v>
       </c>
       <c r="L40" t="s">
-        <v>2125</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -11914,7 +11914,7 @@
         <v>1833</v>
       </c>
       <c r="L41" t="s">
-        <v>2127</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -11947,7 +11947,7 @@
         <v>1831</v>
       </c>
       <c r="L42" t="s">
-        <v>2136</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -11980,7 +11980,7 @@
         <v>1823</v>
       </c>
       <c r="L43" t="s">
-        <v>2135</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -12013,7 +12013,7 @@
         <v>1828</v>
       </c>
       <c r="L44" t="s">
-        <v>2064</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -12046,7 +12046,7 @@
         <v>1827</v>
       </c>
       <c r="L45" t="s">
-        <v>2120</v>
+        <v>2114</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -12070,7 +12070,7 @@
         <v>12</v>
       </c>
       <c r="G46" s="34" t="s">
-        <v>2143</v>
+        <v>2137</v>
       </c>
       <c r="H46" s="34" t="b">
         <v>0</v>
@@ -12081,7 +12081,7 @@
       <c r="J46" s="34"/>
       <c r="K46" s="34"/>
       <c r="L46" s="34" t="s">
-        <v>2137</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -12116,7 +12116,7 @@
       <c r="J47" s="34"/>
       <c r="K47" s="34"/>
       <c r="L47" s="34" t="s">
-        <v>2034</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -12151,7 +12151,7 @@
       <c r="J48" s="34"/>
       <c r="K48" s="34"/>
       <c r="L48" s="34" t="s">
-        <v>2018</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -12186,7 +12186,7 @@
       <c r="J49" s="34"/>
       <c r="K49" s="34"/>
       <c r="L49" s="34" t="s">
-        <v>2054</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -12219,7 +12219,7 @@
         <v>1820</v>
       </c>
       <c r="L50" t="s">
-        <v>2017</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -12233,7 +12233,7 @@
         <v>1835</v>
       </c>
       <c r="D51" t="s">
-        <v>1960</v>
+        <v>1954</v>
       </c>
       <c r="E51">
         <v>5</v>
@@ -12252,7 +12252,7 @@
         <v>1821</v>
       </c>
       <c r="L51" t="s">
-        <v>2079</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -12285,7 +12285,7 @@
         <v>1829</v>
       </c>
       <c r="L52" t="s">
-        <v>2089</v>
+        <v>2083</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -12318,7 +12318,7 @@
         <v>1830</v>
       </c>
       <c r="L53" t="s">
-        <v>2128</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -12351,7 +12351,7 @@
         <v>1830</v>
       </c>
       <c r="L54" t="s">
-        <v>2010</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -12384,7 +12384,7 @@
         <v>1819</v>
       </c>
       <c r="L55" t="s">
-        <v>2009</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -12417,7 +12417,7 @@
         <v>1824</v>
       </c>
       <c r="L56" t="s">
-        <v>2141</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -12450,7 +12450,7 @@
         <v>1820</v>
       </c>
       <c r="L57" t="s">
-        <v>2073</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -12483,7 +12483,7 @@
         <v>1825</v>
       </c>
       <c r="L58" t="s">
-        <v>2026</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -12516,7 +12516,7 @@
         <v>1832</v>
       </c>
       <c r="L59" t="s">
-        <v>2032</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -12549,7 +12549,7 @@
         <v>1831</v>
       </c>
       <c r="L60" t="s">
-        <v>2067</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -12582,7 +12582,7 @@
         <v>1831</v>
       </c>
       <c r="L61" t="s">
-        <v>2083</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -12615,7 +12615,7 @@
         <v>1827</v>
       </c>
       <c r="L62" t="s">
-        <v>2139</v>
+        <v>2133</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -12648,7 +12648,7 @@
         <v>1828</v>
       </c>
       <c r="L63" t="s">
-        <v>2038</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -12681,7 +12681,7 @@
         <v>1832</v>
       </c>
       <c r="L64" t="s">
-        <v>2075</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -12714,7 +12714,7 @@
         <v>1825</v>
       </c>
       <c r="L65" t="s">
-        <v>1999</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -12747,7 +12747,7 @@
         <v>1822</v>
       </c>
       <c r="L66" t="s">
-        <v>2007</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -12780,7 +12780,7 @@
         <v>1826</v>
       </c>
       <c r="L67" t="s">
-        <v>2021</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -12813,7 +12813,7 @@
         <v>1827</v>
       </c>
       <c r="L68" t="s">
-        <v>2022</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -12846,7 +12846,7 @@
         <v>1829</v>
       </c>
       <c r="L69" t="s">
-        <v>2087</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -12879,7 +12879,7 @@
         <v>1819</v>
       </c>
       <c r="L70" t="s">
-        <v>2134</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -12893,7 +12893,7 @@
         <v>1604</v>
       </c>
       <c r="D71" s="34" t="s">
-        <v>2144</v>
+        <v>2138</v>
       </c>
       <c r="E71" s="34">
         <v>8</v>
@@ -12903,7 +12903,7 @@
         <v>16</v>
       </c>
       <c r="G71" s="34" t="s">
-        <v>2143</v>
+        <v>2137</v>
       </c>
       <c r="H71" s="34" t="b">
         <v>1</v>
@@ -12914,7 +12914,7 @@
       <c r="J71" s="34"/>
       <c r="K71" s="34"/>
       <c r="L71" s="34" t="s">
-        <v>2072</v>
+        <v>2066</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -12947,7 +12947,7 @@
         <v>1825</v>
       </c>
       <c r="L72" t="s">
-        <v>2012</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="73" spans="1:12">
@@ -12980,7 +12980,7 @@
         <v>1819</v>
       </c>
       <c r="L73" t="s">
-        <v>2035</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="74" spans="1:12">
@@ -13013,7 +13013,7 @@
         <v>1826</v>
       </c>
       <c r="L74" t="s">
-        <v>2014</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="75" spans="1:12">
@@ -13046,7 +13046,7 @@
         <v>1827</v>
       </c>
       <c r="L75" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="76" spans="1:12">
@@ -13079,7 +13079,7 @@
         <v>1829</v>
       </c>
       <c r="L76" t="s">
-        <v>2066</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="77" spans="1:12">
@@ -13112,7 +13112,7 @@
         <v>1830</v>
       </c>
       <c r="L77" t="s">
-        <v>2006</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="78" spans="1:12">
@@ -13145,7 +13145,7 @@
         <v>1827</v>
       </c>
       <c r="L78" t="s">
-        <v>2055</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="79" spans="1:12">
@@ -13178,7 +13178,7 @@
         <v>1822</v>
       </c>
       <c r="L79" t="s">
-        <v>2123</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -13211,7 +13211,7 @@
         <v>1830</v>
       </c>
       <c r="L80" t="s">
-        <v>2033</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="81" spans="1:12">
@@ -13244,7 +13244,7 @@
         <v>1830</v>
       </c>
       <c r="L81" t="s">
-        <v>2051</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="82" spans="1:12">
@@ -13277,7 +13277,7 @@
         <v>1829</v>
       </c>
       <c r="L82" t="s">
-        <v>2060</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="83" spans="1:12">
@@ -13310,7 +13310,7 @@
         <v>1825</v>
       </c>
       <c r="L83" t="s">
-        <v>2126</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="84" spans="1:12">
@@ -13343,7 +13343,7 @@
         <v>1832</v>
       </c>
       <c r="L84" t="s">
-        <v>2043</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="85" spans="1:12">
@@ -13376,7 +13376,7 @@
         <v>1828</v>
       </c>
       <c r="L85" t="s">
-        <v>2069</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="86" spans="1:12">
@@ -13409,7 +13409,7 @@
         <v>1829</v>
       </c>
       <c r="L86" t="s">
-        <v>2122</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="87" spans="1:12">
@@ -13442,7 +13442,7 @@
         <v>1826</v>
       </c>
       <c r="L87" t="s">
-        <v>2023</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -13475,7 +13475,7 @@
         <v>1826</v>
       </c>
       <c r="L88" t="s">
-        <v>2031</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="89" spans="1:12">
@@ -13508,7 +13508,7 @@
         <v>1833</v>
       </c>
       <c r="L89" t="s">
-        <v>1970</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="90" spans="1:12">
@@ -13541,7 +13541,7 @@
         <v>1833</v>
       </c>
       <c r="L90" t="s">
-        <v>2094</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="91" spans="1:12">
@@ -13577,7 +13577,7 @@
         <v>1840</v>
       </c>
       <c r="L91" t="s">
-        <v>2099</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="92" spans="1:12">
@@ -13610,7 +13610,7 @@
         <v>1822</v>
       </c>
       <c r="L92" t="s">
-        <v>2121</v>
+        <v>2115</v>
       </c>
     </row>
     <row r="93" spans="1:12">
@@ -13645,43 +13645,44 @@
       <c r="J93" s="34"/>
       <c r="K93" s="34"/>
       <c r="L93" s="34" t="s">
-        <v>2028</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="94" spans="1:12">
       <c r="A94" s="34" t="s">
         <v>1896</v>
       </c>
-      <c r="B94">
+      <c r="B94" s="34">
         <v>5</v>
       </c>
-      <c r="C94" t="s">
-        <v>1946</v>
-      </c>
-      <c r="D94" t="s">
-        <v>1941</v>
-      </c>
-      <c r="E94">
+      <c r="C94" s="34" t="s">
+        <v>1943</v>
+      </c>
+      <c r="D94" s="34" t="s">
+        <v>1940</v>
+      </c>
+      <c r="E94" s="34">
         <v>9</v>
       </c>
-      <c r="F94">
+      <c r="F94" s="34">
         <f>E94*2</f>
         <v>18</v>
       </c>
-      <c r="G94" t="s">
+      <c r="G94" s="34" t="s">
         <v>1681</v>
       </c>
-      <c r="H94" t="b">
-        <v>1</v>
-      </c>
-      <c r="I94" t="s">
+      <c r="H94" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I94" s="34" t="s">
         <v>1915</v>
       </c>
-      <c r="J94" t="s">
-        <v>1947</v>
-      </c>
-      <c r="L94" t="s">
-        <v>2115</v>
+      <c r="J94" s="34" t="s">
+        <v>2139</v>
+      </c>
+      <c r="K94" s="34"/>
+      <c r="L94" s="34" t="s">
+        <v>2109</v>
       </c>
     </row>
     <row r="95" spans="1:12">
@@ -13692,10 +13693,10 @@
         <v>5</v>
       </c>
       <c r="C95" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="D95" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="E95">
         <v>9</v>
@@ -13714,10 +13715,10 @@
         <v>1916</v>
       </c>
       <c r="J95" t="s">
-        <v>1943</v>
+        <v>2140</v>
       </c>
       <c r="L95" t="s">
-        <v>2116</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="96" spans="1:12">
@@ -13728,10 +13729,10 @@
         <v>5</v>
       </c>
       <c r="C96" t="s">
-        <v>1944</v>
+        <v>1942</v>
       </c>
       <c r="D96" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="E96">
         <v>9</v>
@@ -13750,10 +13751,10 @@
         <v>1915</v>
       </c>
       <c r="J96" t="s">
-        <v>1945</v>
+        <v>2141</v>
       </c>
       <c r="L96" t="s">
-        <v>2118</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="97" spans="1:12">
@@ -13767,7 +13768,7 @@
         <v>1939</v>
       </c>
       <c r="D97" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="E97">
         <v>9</v>
@@ -13786,24 +13787,24 @@
         <v>1914</v>
       </c>
       <c r="J97" t="s">
-        <v>1940</v>
+        <v>2142</v>
       </c>
       <c r="L97" t="s">
-        <v>2119</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="34" t="s">
-        <v>1979</v>
+        <v>1973</v>
       </c>
       <c r="B98">
         <v>5</v>
       </c>
       <c r="C98" t="s">
-        <v>1950</v>
+        <v>1945</v>
       </c>
       <c r="D98" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="E98">
         <v>9</v>
@@ -13822,10 +13823,10 @@
         <v>1820</v>
       </c>
       <c r="J98" t="s">
-        <v>1951</v>
+        <v>2143</v>
       </c>
       <c r="L98" t="s">
-        <v>2114</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="99" spans="1:12">
@@ -13836,10 +13837,10 @@
         <v>5</v>
       </c>
       <c r="C99" t="s">
-        <v>1948</v>
+        <v>1944</v>
       </c>
       <c r="D99" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="E99">
         <v>9</v>
@@ -13858,10 +13859,10 @@
         <v>1916</v>
       </c>
       <c r="J99" t="s">
-        <v>1949</v>
+        <v>2144</v>
       </c>
       <c r="L99" t="s">
-        <v>2117</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="100" spans="1:12">
@@ -13894,7 +13895,7 @@
         <v>1914</v>
       </c>
       <c r="L100" t="s">
-        <v>2057</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="101" spans="1:12">
@@ -13927,7 +13928,7 @@
         <v>1913</v>
       </c>
       <c r="L101" t="s">
-        <v>2039</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="102" spans="1:12">
@@ -13960,7 +13961,7 @@
         <v>1913</v>
       </c>
       <c r="L102" t="s">
-        <v>2037</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="103" spans="1:12">
@@ -13993,7 +13994,7 @@
         <v>1826</v>
       </c>
       <c r="L103" t="s">
-        <v>2131</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="104" spans="1:12">
@@ -14026,7 +14027,7 @@
         <v>1827</v>
       </c>
       <c r="L104" t="s">
-        <v>2004</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="105" spans="1:12">
@@ -14059,7 +14060,7 @@
         <v>1825</v>
       </c>
       <c r="L105" t="s">
-        <v>2005</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="106" spans="1:12">
@@ -14092,7 +14093,7 @@
         <v>1832</v>
       </c>
       <c r="L106" t="s">
-        <v>2093</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="107" spans="1:12">
@@ -14125,7 +14126,7 @@
         <v>1819</v>
       </c>
       <c r="L107" t="s">
-        <v>2097</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="108" spans="1:12">
@@ -14161,7 +14162,7 @@
         <v>1848</v>
       </c>
       <c r="L108" t="s">
-        <v>2104</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="109" spans="1:12">
@@ -14197,7 +14198,7 @@
         <v>1861</v>
       </c>
       <c r="L109" t="s">
-        <v>2105</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="110" spans="1:12">
@@ -14233,7 +14234,7 @@
         <v>1852</v>
       </c>
       <c r="L110" t="s">
-        <v>2106</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="111" spans="1:12">
@@ -14269,7 +14270,7 @@
         <v>1850</v>
       </c>
       <c r="L111" t="s">
-        <v>2107</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="112" spans="1:12">
@@ -14305,7 +14306,7 @@
         <v>1854</v>
       </c>
       <c r="L112" t="s">
-        <v>2108</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="113" spans="1:12">
@@ -14341,7 +14342,7 @@
         <v>1858</v>
       </c>
       <c r="L113" t="s">
-        <v>2109</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="114" spans="1:12">
@@ -14377,7 +14378,7 @@
         <v>1856</v>
       </c>
       <c r="L114" t="s">
-        <v>2110</v>
+        <v>2104</v>
       </c>
     </row>
     <row r="115" spans="1:12">
@@ -14413,7 +14414,7 @@
         <v>1860</v>
       </c>
       <c r="L115" t="s">
-        <v>2111</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="116" spans="1:12">
@@ -14446,7 +14447,7 @@
         <v>1819</v>
       </c>
       <c r="L116" t="s">
-        <v>2084</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="117" spans="1:12">
@@ -14460,7 +14461,7 @@
         <v>1864</v>
       </c>
       <c r="D117" t="s">
-        <v>1961</v>
+        <v>1955</v>
       </c>
       <c r="E117">
         <v>9</v>
@@ -14479,7 +14480,7 @@
         <v>1821</v>
       </c>
       <c r="L117" t="s">
-        <v>2076</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="118" spans="1:12">
@@ -14512,7 +14513,7 @@
         <v>1821</v>
       </c>
       <c r="L118" t="s">
-        <v>2074</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="119" spans="1:12">
@@ -14545,7 +14546,7 @@
         <v>1833</v>
       </c>
       <c r="L119" t="s">
-        <v>2071</v>
+        <v>2065</v>
       </c>
     </row>
     <row r="120" spans="1:12">
@@ -14578,7 +14579,7 @@
         <v>1828</v>
       </c>
       <c r="L120" t="s">
-        <v>2061</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="121" spans="1:12">
@@ -14611,7 +14612,7 @@
         <v>1832</v>
       </c>
       <c r="L121" t="s">
-        <v>1972</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="122" spans="1:12">
@@ -14644,7 +14645,7 @@
         <v>1820</v>
       </c>
       <c r="L122" t="s">
-        <v>2130</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="123" spans="1:12">
@@ -14658,7 +14659,7 @@
         <v>1607</v>
       </c>
       <c r="D123" t="s">
-        <v>1952</v>
+        <v>1946</v>
       </c>
       <c r="E123">
         <v>12</v>
@@ -14677,7 +14678,7 @@
         <v>1916</v>
       </c>
       <c r="L123" t="s">
-        <v>1971</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="124" spans="1:12">
@@ -14691,7 +14692,7 @@
         <v>1608</v>
       </c>
       <c r="D124" t="s">
-        <v>1953</v>
+        <v>1947</v>
       </c>
       <c r="E124">
         <v>14</v>
@@ -14710,7 +14711,7 @@
         <v>1915</v>
       </c>
       <c r="L124" t="s">
-        <v>2082</v>
+        <v>2076</v>
       </c>
     </row>
     <row r="125" spans="1:12">
@@ -14743,7 +14744,7 @@
         <v>1833</v>
       </c>
       <c r="L125" t="s">
-        <v>2046</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="126" spans="1:12">
@@ -14776,7 +14777,7 @@
         <v>1832</v>
       </c>
       <c r="L126" t="s">
-        <v>2138</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="127" spans="1:12">
@@ -14809,7 +14810,7 @@
         <v>1832</v>
       </c>
       <c r="L127" t="s">
-        <v>2025</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="128" spans="1:12">
@@ -14845,7 +14846,7 @@
         <v>255</v>
       </c>
       <c r="L128" t="s">
-        <v>2103</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="129" spans="1:12">
@@ -14878,7 +14879,7 @@
         <v>1819</v>
       </c>
       <c r="L129" t="s">
-        <v>2041</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="130" spans="1:12">
@@ -14911,7 +14912,7 @@
         <v>1823</v>
       </c>
       <c r="L130" t="s">
-        <v>2129</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="131" spans="1:12">
@@ -14944,7 +14945,7 @@
         <v>1824</v>
       </c>
       <c r="L131" t="s">
-        <v>2080</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="132" spans="1:12">
@@ -14977,7 +14978,7 @@
         <v>1827</v>
       </c>
       <c r="L132" t="s">
-        <v>2081</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="133" spans="1:12">
@@ -15010,7 +15011,7 @@
         <v>1827</v>
       </c>
       <c r="L133" t="s">
-        <v>2050</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="134" spans="1:12">
@@ -15043,7 +15044,7 @@
         <v>1826</v>
       </c>
       <c r="L134" t="s">
-        <v>2013</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="135" spans="1:12">
@@ -15076,7 +15077,7 @@
         <v>1822</v>
       </c>
       <c r="L135" t="s">
-        <v>2003</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="136" spans="1:12">
@@ -15109,7 +15110,7 @@
         <v>1915</v>
       </c>
       <c r="L136" t="s">
-        <v>2045</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="137" spans="1:12">
@@ -15142,7 +15143,7 @@
         <v>1833</v>
       </c>
       <c r="L137" t="s">
-        <v>2048</v>
+        <v>2042</v>
       </c>
     </row>
     <row r="138" spans="1:12">
@@ -15175,7 +15176,7 @@
         <v>1831</v>
       </c>
       <c r="L138" t="s">
-        <v>2063</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="139" spans="1:12">
@@ -15208,7 +15209,7 @@
         <v>1828</v>
       </c>
       <c r="L139" t="s">
-        <v>2065</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="140" spans="1:12">
@@ -15241,7 +15242,7 @@
         <v>1831</v>
       </c>
       <c r="L140" t="s">
-        <v>2044</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="141" spans="1:12">
@@ -15274,7 +15275,7 @@
         <v>1825</v>
       </c>
       <c r="L141" t="s">
-        <v>2113</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="142" spans="1:12">
@@ -15307,7 +15308,7 @@
         <v>1828</v>
       </c>
       <c r="L142" t="s">
-        <v>2086</v>
+        <v>2080</v>
       </c>
     </row>
     <row r="143" spans="1:12">
@@ -15340,7 +15341,7 @@
         <v>1824</v>
       </c>
       <c r="L143" t="s">
-        <v>2058</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="144" spans="1:12">
@@ -15373,7 +15374,7 @@
         <v>1914</v>
       </c>
       <c r="L144" t="s">
-        <v>2068</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="145" spans="1:12">
@@ -15406,7 +15407,7 @@
         <v>1820</v>
       </c>
       <c r="L145" t="s">
-        <v>2077</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="146" spans="1:12">
@@ -15439,7 +15440,7 @@
         <v>1832</v>
       </c>
       <c r="L146" t="s">
-        <v>2052</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="147" spans="1:12">
@@ -15472,7 +15473,7 @@
         <v>1913</v>
       </c>
       <c r="L147" t="s">
-        <v>2029</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="148" spans="1:12">
@@ -15505,7 +15506,7 @@
         <v>1913</v>
       </c>
       <c r="L148" t="s">
-        <v>2070</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="149" spans="1:12">
@@ -15538,7 +15539,7 @@
         <v>1916</v>
       </c>
       <c r="L149" t="s">
-        <v>1973</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="150" spans="1:12">
@@ -15571,7 +15572,7 @@
         <v>1830</v>
       </c>
       <c r="L150" t="s">
-        <v>2112</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="151" spans="1:12">
@@ -15604,7 +15605,7 @@
         <v>1829</v>
       </c>
       <c r="L151" t="s">
-        <v>1963</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="152" spans="1:12">
@@ -15637,7 +15638,7 @@
         <v>1916</v>
       </c>
       <c r="L152" t="s">
-        <v>2020</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="153" spans="1:12">
@@ -15651,7 +15652,7 @@
         <v>1597</v>
       </c>
       <c r="D153" t="s">
-        <v>1957</v>
+        <v>1951</v>
       </c>
       <c r="E153">
         <v>20</v>
@@ -15670,7 +15671,7 @@
         <v>1915</v>
       </c>
       <c r="L153" t="s">
-        <v>2059</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="154" spans="1:12">
@@ -15703,7 +15704,7 @@
         <v>1833</v>
       </c>
       <c r="L154" t="s">
-        <v>2049</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="155" spans="1:12">
@@ -15717,7 +15718,7 @@
         <v>1609</v>
       </c>
       <c r="D155" t="s">
-        <v>1954</v>
+        <v>1948</v>
       </c>
       <c r="E155">
         <v>16</v>
@@ -15736,7 +15737,7 @@
         <v>1913</v>
       </c>
       <c r="L155" t="s">
-        <v>2008</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="156" spans="1:12">
@@ -15769,82 +15770,82 @@
         <v>1831</v>
       </c>
       <c r="L156" t="s">
-        <v>1997</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="157" spans="1:12">
       <c r="A157" t="s">
-        <v>1974</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="158" spans="1:12">
       <c r="A158" t="s">
-        <v>1975</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="159" spans="1:12">
       <c r="A159" t="s">
-        <v>1976</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="160" spans="1:12">
       <c r="A160" t="s">
-        <v>1977</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="161" spans="1:9">
       <c r="A161" t="s">
-        <v>1978</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="162" spans="1:9">
       <c r="A162" t="s">
-        <v>1981</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="163" spans="1:9">
       <c r="A163" t="s">
-        <v>1982</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="164" spans="1:9">
       <c r="A164" t="s">
-        <v>1983</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="165" spans="1:9">
       <c r="A165" t="s">
-        <v>1984</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="166" spans="1:9">
       <c r="A166" t="s">
-        <v>1985</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="167" spans="1:9">
       <c r="A167" t="s">
-        <v>1986</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="168" spans="1:9">
       <c r="A168" t="s">
-        <v>1980</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="169" spans="1:9">
       <c r="A169" t="s">
-        <v>1987</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="170" spans="1:9">
       <c r="A170" t="s">
-        <v>1988</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="171" spans="1:9">
       <c r="A171" t="s">
-        <v>1989</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="172" spans="1:9">
@@ -15857,7 +15858,7 @@
     </row>
     <row r="173" spans="1:9">
       <c r="A173" t="s">
-        <v>1990</v>
+        <v>1984</v>
       </c>
       <c r="I173" t="s">
         <v>1824</v>
@@ -15865,7 +15866,7 @@
     </row>
     <row r="174" spans="1:9">
       <c r="A174" t="s">
-        <v>1992</v>
+        <v>1986</v>
       </c>
       <c r="I174" t="s">
         <v>1824</v>
@@ -15873,7 +15874,7 @@
     </row>
     <row r="175" spans="1:9">
       <c r="A175" t="s">
-        <v>1991</v>
+        <v>1985</v>
       </c>
       <c r="I175" t="s">
         <v>1824</v>
@@ -15889,17 +15890,17 @@
     </row>
     <row r="177" spans="1:9">
       <c r="A177" t="s">
-        <v>1993</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="178" spans="1:9">
       <c r="A178" t="s">
-        <v>1994</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="179" spans="1:9">
       <c r="A179" t="s">
-        <v>1995</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="180" spans="1:9">

</xml_diff>

<commit_message>
Sphere of Security: Protection from Cold
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1845FB8C-8201-4E86-9578-6DA437FDB8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65B498C-6F05-4278-9A5C-803D123140C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -10526,7 +10526,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L94" sqref="A94:L94"/>
+      <selection pane="bottomLeft" activeCell="L95" sqref="B95:L95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -13689,35 +13689,36 @@
       <c r="A95" s="34" t="s">
         <v>1909</v>
       </c>
-      <c r="B95">
+      <c r="B95" s="34">
         <v>5</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="34" t="s">
         <v>1941</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" s="34" t="s">
         <v>1940</v>
       </c>
-      <c r="E95">
+      <c r="E95" s="34">
         <v>9</v>
       </c>
-      <c r="F95">
+      <c r="F95" s="34">
         <f>E95*2</f>
         <v>18</v>
       </c>
-      <c r="G95" t="s">
+      <c r="G95" s="34" t="s">
         <v>1681</v>
       </c>
-      <c r="H95" t="b">
-        <v>1</v>
-      </c>
-      <c r="I95" t="s">
+      <c r="H95" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I95" s="34" t="s">
         <v>1916</v>
       </c>
-      <c r="J95" t="s">
+      <c r="J95" s="34" t="s">
         <v>2140</v>
       </c>
-      <c r="L95" t="s">
+      <c r="K95" s="34"/>
+      <c r="L95" s="34" t="s">
         <v>2110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sphere of Security: Protection from Electricity
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65B498C-6F05-4278-9A5C-803D123140C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548574A0-C62B-464F-8DA5-C2F1B4CEDDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -10526,7 +10526,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L95" sqref="B95:L95"/>
+      <selection pane="bottomLeft" activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -13726,35 +13726,36 @@
       <c r="A96" s="34" t="s">
         <v>1899</v>
       </c>
-      <c r="B96">
+      <c r="B96" s="34">
         <v>5</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="34" t="s">
         <v>1942</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="34" t="s">
         <v>1940</v>
       </c>
-      <c r="E96">
+      <c r="E96" s="34">
         <v>9</v>
       </c>
-      <c r="F96">
+      <c r="F96" s="34">
         <f>E96*2</f>
         <v>18</v>
       </c>
-      <c r="G96" t="s">
+      <c r="G96" s="34" t="s">
         <v>1681</v>
       </c>
-      <c r="H96" t="b">
-        <v>1</v>
-      </c>
-      <c r="I96" t="s">
+      <c r="H96" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I96" s="34" t="s">
         <v>1915</v>
       </c>
-      <c r="J96" t="s">
+      <c r="J96" s="34" t="s">
         <v>2141</v>
       </c>
-      <c r="L96" t="s">
+      <c r="K96" s="34"/>
+      <c r="L96" s="34" t="s">
         <v>2112</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sphere of Security: Protection from Fire
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548574A0-C62B-464F-8DA5-C2F1B4CEDDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4B0DD9-BE0C-467E-A4E5-CF3EA5746FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -10526,7 +10526,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A96" sqref="A96"/>
+      <selection pane="bottomLeft" activeCell="B97" sqref="B97:L97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -13763,35 +13763,36 @@
       <c r="A97" s="34" t="s">
         <v>1883</v>
       </c>
-      <c r="B97">
+      <c r="B97" s="34">
         <v>5</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="34" t="s">
         <v>1939</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="34" t="s">
         <v>1940</v>
       </c>
-      <c r="E97">
+      <c r="E97" s="34">
         <v>9</v>
       </c>
-      <c r="F97">
+      <c r="F97" s="34">
         <f>E97*2</f>
         <v>18</v>
       </c>
-      <c r="G97" t="s">
+      <c r="G97" s="34" t="s">
         <v>1681</v>
       </c>
-      <c r="H97" t="b">
-        <v>1</v>
-      </c>
-      <c r="I97" t="s">
+      <c r="H97" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I97" s="34" t="s">
         <v>1914</v>
       </c>
-      <c r="J97" t="s">
+      <c r="J97" s="34" t="s">
         <v>2142</v>
       </c>
-      <c r="L97" t="s">
+      <c r="K97" s="34"/>
+      <c r="L97" s="34" t="s">
         <v>2113</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sphere of Security: Protection from Petrification
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4B0DD9-BE0C-467E-A4E5-CF3EA5746FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0042093-48D4-4A04-9CD4-538064460C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -10526,7 +10526,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B97" sqref="B97:L97"/>
+      <selection pane="bottomLeft" activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -13800,35 +13800,36 @@
       <c r="A98" s="34" t="s">
         <v>1973</v>
       </c>
-      <c r="B98">
+      <c r="B98" s="34">
         <v>5</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="34" t="s">
         <v>1945</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="34" t="s">
         <v>1940</v>
       </c>
-      <c r="E98">
+      <c r="E98" s="34">
         <v>9</v>
       </c>
-      <c r="F98">
+      <c r="F98" s="34">
         <f>E98*2</f>
         <v>18</v>
       </c>
-      <c r="G98" t="s">
+      <c r="G98" s="34" t="s">
         <v>1681</v>
       </c>
-      <c r="H98" t="b">
-        <v>1</v>
-      </c>
-      <c r="I98" t="s">
+      <c r="H98" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I98" s="34" t="s">
         <v>1820</v>
       </c>
-      <c r="J98" t="s">
+      <c r="J98" s="34" t="s">
         <v>2143</v>
       </c>
-      <c r="L98" t="s">
+      <c r="K98" s="34"/>
+      <c r="L98" s="34" t="s">
         <v>2108</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sphere of Security: Protection from Poison
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0042093-48D4-4A04-9CD4-538064460C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE328D0-1486-42CA-B179-A0C49AA32A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -10526,7 +10526,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C99" sqref="C99"/>
+      <selection pane="bottomLeft" activeCell="B99" sqref="B99:L99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -13837,35 +13837,36 @@
       <c r="A99" s="34" t="s">
         <v>1911</v>
       </c>
-      <c r="B99">
+      <c r="B99" s="34">
         <v>5</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="34" t="s">
         <v>1944</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" s="34" t="s">
         <v>1940</v>
       </c>
-      <c r="E99">
+      <c r="E99" s="34">
         <v>9</v>
       </c>
-      <c r="F99">
+      <c r="F99" s="34">
         <f>E99*2</f>
         <v>18</v>
       </c>
-      <c r="G99" t="s">
+      <c r="G99" s="34" t="s">
         <v>1681</v>
       </c>
-      <c r="H99" t="b">
-        <v>1</v>
-      </c>
-      <c r="I99" t="s">
+      <c r="H99" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I99" s="34" t="s">
         <v>1916</v>
       </c>
-      <c r="J99" t="s">
+      <c r="J99" s="34" t="s">
         <v>2144</v>
       </c>
-      <c r="L99" t="s">
+      <c r="K99" s="34"/>
+      <c r="L99" s="34" t="s">
         <v>2111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removing Major Mirror Image
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE328D0-1486-42CA-B179-A0C49AA32A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F634CB9-4744-4243-8D19-73A0C48F8F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11513" uniqueCount="2145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11509" uniqueCount="2143">
   <si>
     <t>Caster Level</t>
   </si>
@@ -5808,9 +5808,6 @@
     <t>MEWI356</t>
   </si>
   <si>
-    <t>MEWI555</t>
-  </si>
-  <si>
     <t>Ghostform</t>
   </si>
   <si>
@@ -6193,9 +6190,6 @@
   </si>
   <si>
     <t>luck.BAM</t>
-  </si>
-  <si>
-    <t>major-mirror-image.BAM</t>
   </si>
   <si>
     <t>mantle.BAM</t>
@@ -10468,7 +10462,7 @@
         <v>1917</v>
       </c>
       <c r="E96" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -10526,7 +10520,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B99" sqref="B99:L99"/>
+      <selection pane="bottomLeft" activeCell="L100" sqref="L100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -10558,10 +10552,10 @@
         <v>1817</v>
       </c>
       <c r="E1" s="23" t="s">
+        <v>1951</v>
+      </c>
+      <c r="F1" s="23" t="s">
         <v>1952</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>1953</v>
       </c>
       <c r="G1" s="23" t="s">
         <v>1676</v>
@@ -10573,13 +10567,13 @@
         <v>1818</v>
       </c>
       <c r="J1" s="23" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="K1" s="23" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="L1" s="23" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="34" customFormat="1">
@@ -10612,7 +10606,7 @@
         <v>1914</v>
       </c>
       <c r="L2" s="34" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -10626,7 +10620,7 @@
         <v>1599</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="E3" s="34">
         <v>3</v>
@@ -10647,7 +10641,7 @@
       <c r="J3" s="34"/>
       <c r="K3" s="34"/>
       <c r="L3" s="34" t="s">
-        <v>2095</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -10661,7 +10655,7 @@
         <v>1601</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>2136</v>
+        <v>2134</v>
       </c>
       <c r="E4" s="34">
         <v>4</v>
@@ -10671,7 +10665,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>2137</v>
+        <v>2135</v>
       </c>
       <c r="H4" s="34" t="b">
         <v>1</v>
@@ -10682,7 +10676,7 @@
       <c r="J4" s="34"/>
       <c r="K4" s="34"/>
       <c r="L4" s="34" t="s">
-        <v>2090</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -10696,7 +10690,7 @@
         <v>1600</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="E5" s="34">
         <v>2</v>
@@ -10706,7 +10700,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="34" t="s">
-        <v>2137</v>
+        <v>2135</v>
       </c>
       <c r="H5" s="34" t="b">
         <v>0</v>
@@ -10717,7 +10711,7 @@
       <c r="J5" s="34"/>
       <c r="K5" s="34"/>
       <c r="L5" s="34" t="s">
-        <v>2127</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -10728,10 +10722,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="E6" s="34">
         <v>10</v>
@@ -10752,7 +10746,7 @@
       <c r="J6" s="34"/>
       <c r="K6" s="34"/>
       <c r="L6" s="34" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -10787,7 +10781,7 @@
       <c r="J7" s="34"/>
       <c r="K7" s="34"/>
       <c r="L7" s="34" t="s">
-        <v>2082</v>
+        <v>2080</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -10820,7 +10814,7 @@
         <v>1819</v>
       </c>
       <c r="L8" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -10853,7 +10847,7 @@
         <v>1822</v>
       </c>
       <c r="L9" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -10886,7 +10880,7 @@
         <v>1821</v>
       </c>
       <c r="L10" t="s">
-        <v>2089</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -10919,7 +10913,7 @@
         <v>1825</v>
       </c>
       <c r="L11" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -10952,7 +10946,7 @@
         <v>1823</v>
       </c>
       <c r="L12" t="s">
-        <v>2118</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -10985,7 +10979,7 @@
         <v>1822</v>
       </c>
       <c r="L13" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -11018,7 +11012,7 @@
         <v>1821</v>
       </c>
       <c r="L14" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -11051,7 +11045,7 @@
         <v>1820</v>
       </c>
       <c r="L15" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -11084,7 +11078,7 @@
         <v>1826</v>
       </c>
       <c r="L16" t="s">
-        <v>2079</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -11117,7 +11111,7 @@
         <v>1827</v>
       </c>
       <c r="L17" t="s">
-        <v>2126</v>
+        <v>2124</v>
       </c>
       <c r="M17" t="s">
         <v>1843</v>
@@ -11153,7 +11147,7 @@
         <v>1830</v>
       </c>
       <c r="L18" t="s">
-        <v>2072</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -11186,7 +11180,7 @@
         <v>1829</v>
       </c>
       <c r="L19" t="s">
-        <v>2092</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -11219,7 +11213,7 @@
         <v>1822</v>
       </c>
       <c r="L20" t="s">
-        <v>2094</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -11252,7 +11246,7 @@
         <v>1824</v>
       </c>
       <c r="L21" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -11285,7 +11279,7 @@
         <v>1832</v>
       </c>
       <c r="L22" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -11318,7 +11312,7 @@
         <v>1829</v>
       </c>
       <c r="L23" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -11351,7 +11345,7 @@
         <v>1823</v>
       </c>
       <c r="L24" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -11384,7 +11378,7 @@
         <v>1822</v>
       </c>
       <c r="L25" t="s">
-        <v>2096</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -11419,7 +11413,7 @@
       <c r="J26" s="34"/>
       <c r="K26" s="34"/>
       <c r="L26" s="34" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -11452,7 +11446,7 @@
         <v>1824</v>
       </c>
       <c r="L27" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -11485,7 +11479,7 @@
         <v>1823</v>
       </c>
       <c r="L28" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -11518,7 +11512,7 @@
         <v>1828</v>
       </c>
       <c r="L29" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -11551,7 +11545,7 @@
         <v>1831</v>
       </c>
       <c r="L30" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -11584,7 +11578,7 @@
         <v>1820</v>
       </c>
       <c r="L31" t="s">
-        <v>2086</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -11617,7 +11611,7 @@
         <v>1826</v>
       </c>
       <c r="L32" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -11650,7 +11644,7 @@
         <v>1822</v>
       </c>
       <c r="L33" t="s">
-        <v>2134</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -11683,7 +11677,7 @@
         <v>1826</v>
       </c>
       <c r="L34" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -11716,7 +11710,7 @@
         <v>1828</v>
       </c>
       <c r="L35" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -11749,7 +11743,7 @@
         <v>1829</v>
       </c>
       <c r="L36" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -11782,7 +11776,7 @@
         <v>1830</v>
       </c>
       <c r="L37" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -11796,7 +11790,7 @@
         <v>85</v>
       </c>
       <c r="D38" t="s">
-        <v>2085</v>
+        <v>2083</v>
       </c>
       <c r="E38">
         <v>4</v>
@@ -11815,7 +11809,7 @@
         <v>1833</v>
       </c>
       <c r="L38" t="s">
-        <v>2084</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -11848,7 +11842,7 @@
         <v>1833</v>
       </c>
       <c r="L39" t="s">
-        <v>2056</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -11881,7 +11875,7 @@
         <v>1831</v>
       </c>
       <c r="L40" t="s">
-        <v>2119</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -11914,7 +11908,7 @@
         <v>1833</v>
       </c>
       <c r="L41" t="s">
-        <v>2121</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -11947,7 +11941,7 @@
         <v>1831</v>
       </c>
       <c r="L42" t="s">
-        <v>2130</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -11980,7 +11974,7 @@
         <v>1823</v>
       </c>
       <c r="L43" t="s">
-        <v>2129</v>
+        <v>2127</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -12013,7 +12007,7 @@
         <v>1828</v>
       </c>
       <c r="L44" t="s">
-        <v>2058</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -12046,7 +12040,7 @@
         <v>1827</v>
       </c>
       <c r="L45" t="s">
-        <v>2114</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -12060,7 +12054,7 @@
         <v>1603</v>
       </c>
       <c r="D46" s="34" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="E46" s="34">
         <v>6</v>
@@ -12070,7 +12064,7 @@
         <v>12</v>
       </c>
       <c r="G46" s="34" t="s">
-        <v>2137</v>
+        <v>2135</v>
       </c>
       <c r="H46" s="34" t="b">
         <v>0</v>
@@ -12081,7 +12075,7 @@
       <c r="J46" s="34"/>
       <c r="K46" s="34"/>
       <c r="L46" s="34" t="s">
-        <v>2131</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -12116,7 +12110,7 @@
       <c r="J47" s="34"/>
       <c r="K47" s="34"/>
       <c r="L47" s="34" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -12151,7 +12145,7 @@
       <c r="J48" s="34"/>
       <c r="K48" s="34"/>
       <c r="L48" s="34" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -12186,7 +12180,7 @@
       <c r="J49" s="34"/>
       <c r="K49" s="34"/>
       <c r="L49" s="34" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -12219,7 +12213,7 @@
         <v>1820</v>
       </c>
       <c r="L50" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -12233,7 +12227,7 @@
         <v>1835</v>
       </c>
       <c r="D51" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="E51">
         <v>5</v>
@@ -12252,7 +12246,7 @@
         <v>1821</v>
       </c>
       <c r="L51" t="s">
-        <v>2073</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -12285,7 +12279,7 @@
         <v>1829</v>
       </c>
       <c r="L52" t="s">
-        <v>2083</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -12318,7 +12312,7 @@
         <v>1830</v>
       </c>
       <c r="L53" t="s">
-        <v>2122</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -12351,7 +12345,7 @@
         <v>1830</v>
       </c>
       <c r="L54" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -12384,7 +12378,7 @@
         <v>1819</v>
       </c>
       <c r="L55" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -12417,7 +12411,7 @@
         <v>1824</v>
       </c>
       <c r="L56" t="s">
-        <v>2135</v>
+        <v>2133</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -12450,7 +12444,7 @@
         <v>1820</v>
       </c>
       <c r="L57" t="s">
-        <v>2067</v>
+        <v>2065</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -12483,7 +12477,7 @@
         <v>1825</v>
       </c>
       <c r="L58" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -12516,7 +12510,7 @@
         <v>1832</v>
       </c>
       <c r="L59" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -12549,7 +12543,7 @@
         <v>1831</v>
       </c>
       <c r="L60" t="s">
-        <v>2061</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -12582,7 +12576,7 @@
         <v>1831</v>
       </c>
       <c r="L61" t="s">
-        <v>2077</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -12615,7 +12609,7 @@
         <v>1827</v>
       </c>
       <c r="L62" t="s">
-        <v>2133</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -12648,7 +12642,7 @@
         <v>1828</v>
       </c>
       <c r="L63" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -12681,7 +12675,7 @@
         <v>1832</v>
       </c>
       <c r="L64" t="s">
-        <v>2069</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -12714,7 +12708,7 @@
         <v>1825</v>
       </c>
       <c r="L65" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -12747,7 +12741,7 @@
         <v>1822</v>
       </c>
       <c r="L66" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -12780,7 +12774,7 @@
         <v>1826</v>
       </c>
       <c r="L67" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -12813,7 +12807,7 @@
         <v>1827</v>
       </c>
       <c r="L68" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -12846,7 +12840,7 @@
         <v>1829</v>
       </c>
       <c r="L69" t="s">
-        <v>2081</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -12879,7 +12873,7 @@
         <v>1819</v>
       </c>
       <c r="L70" t="s">
-        <v>2128</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -12893,7 +12887,7 @@
         <v>1604</v>
       </c>
       <c r="D71" s="34" t="s">
-        <v>2138</v>
+        <v>2136</v>
       </c>
       <c r="E71" s="34">
         <v>8</v>
@@ -12903,7 +12897,7 @@
         <v>16</v>
       </c>
       <c r="G71" s="34" t="s">
-        <v>2137</v>
+        <v>2135</v>
       </c>
       <c r="H71" s="34" t="b">
         <v>1</v>
@@ -12914,7 +12908,7 @@
       <c r="J71" s="34"/>
       <c r="K71" s="34"/>
       <c r="L71" s="34" t="s">
-        <v>2066</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -12947,7 +12941,7 @@
         <v>1825</v>
       </c>
       <c r="L72" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="73" spans="1:12">
@@ -12980,7 +12974,7 @@
         <v>1819</v>
       </c>
       <c r="L73" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="74" spans="1:12">
@@ -13013,7 +13007,7 @@
         <v>1826</v>
       </c>
       <c r="L74" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="75" spans="1:12">
@@ -13046,7 +13040,7 @@
         <v>1827</v>
       </c>
       <c r="L75" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="76" spans="1:12">
@@ -13079,7 +13073,7 @@
         <v>1829</v>
       </c>
       <c r="L76" t="s">
-        <v>2060</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="77" spans="1:12">
@@ -13112,7 +13106,7 @@
         <v>1830</v>
       </c>
       <c r="L77" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="78" spans="1:12">
@@ -13145,7 +13139,7 @@
         <v>1827</v>
       </c>
       <c r="L78" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="79" spans="1:12">
@@ -13178,7 +13172,7 @@
         <v>1822</v>
       </c>
       <c r="L79" t="s">
-        <v>2117</v>
+        <v>2115</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -13211,7 +13205,7 @@
         <v>1830</v>
       </c>
       <c r="L80" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="81" spans="1:12">
@@ -13244,7 +13238,7 @@
         <v>1830</v>
       </c>
       <c r="L81" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="82" spans="1:12">
@@ -13277,7 +13271,7 @@
         <v>1829</v>
       </c>
       <c r="L82" t="s">
-        <v>2054</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="83" spans="1:12">
@@ -13310,7 +13304,7 @@
         <v>1825</v>
       </c>
       <c r="L83" t="s">
-        <v>2120</v>
+        <v>2118</v>
       </c>
     </row>
     <row r="84" spans="1:12">
@@ -13343,7 +13337,7 @@
         <v>1832</v>
       </c>
       <c r="L84" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="85" spans="1:12">
@@ -13376,7 +13370,7 @@
         <v>1828</v>
       </c>
       <c r="L85" t="s">
-        <v>2063</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="86" spans="1:12">
@@ -13409,7 +13403,7 @@
         <v>1829</v>
       </c>
       <c r="L86" t="s">
-        <v>2116</v>
+        <v>2114</v>
       </c>
     </row>
     <row r="87" spans="1:12">
@@ -13442,7 +13436,7 @@
         <v>1826</v>
       </c>
       <c r="L87" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -13475,7 +13469,7 @@
         <v>1826</v>
       </c>
       <c r="L88" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="89" spans="1:12">
@@ -13508,7 +13502,7 @@
         <v>1833</v>
       </c>
       <c r="L89" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="90" spans="1:12">
@@ -13541,7 +13535,7 @@
         <v>1833</v>
       </c>
       <c r="L90" t="s">
-        <v>2088</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="91" spans="1:12">
@@ -13577,7 +13571,7 @@
         <v>1840</v>
       </c>
       <c r="L91" t="s">
-        <v>2093</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="92" spans="1:12">
@@ -13610,7 +13604,7 @@
         <v>1822</v>
       </c>
       <c r="L92" t="s">
-        <v>2115</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="93" spans="1:12">
@@ -13624,7 +13618,7 @@
         <v>1605</v>
       </c>
       <c r="D93" s="34" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="E93" s="34">
         <v>10</v>
@@ -13645,7 +13639,7 @@
       <c r="J93" s="34"/>
       <c r="K93" s="34"/>
       <c r="L93" s="34" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="94" spans="1:12">
@@ -13656,10 +13650,10 @@
         <v>5</v>
       </c>
       <c r="C94" s="34" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="D94" s="34" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="E94" s="34">
         <v>9</v>
@@ -13678,11 +13672,11 @@
         <v>1915</v>
       </c>
       <c r="J94" s="34" t="s">
-        <v>2139</v>
+        <v>2137</v>
       </c>
       <c r="K94" s="34"/>
       <c r="L94" s="34" t="s">
-        <v>2109</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="95" spans="1:12">
@@ -13693,10 +13687,10 @@
         <v>5</v>
       </c>
       <c r="C95" s="34" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="D95" s="34" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="E95" s="34">
         <v>9</v>
@@ -13715,11 +13709,11 @@
         <v>1916</v>
       </c>
       <c r="J95" s="34" t="s">
-        <v>2140</v>
+        <v>2138</v>
       </c>
       <c r="K95" s="34"/>
       <c r="L95" s="34" t="s">
-        <v>2110</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="96" spans="1:12">
@@ -13730,10 +13724,10 @@
         <v>5</v>
       </c>
       <c r="C96" s="34" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="D96" s="34" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="E96" s="34">
         <v>9</v>
@@ -13752,11 +13746,11 @@
         <v>1915</v>
       </c>
       <c r="J96" s="34" t="s">
-        <v>2141</v>
+        <v>2139</v>
       </c>
       <c r="K96" s="34"/>
       <c r="L96" s="34" t="s">
-        <v>2112</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="97" spans="1:12">
@@ -13767,10 +13761,10 @@
         <v>5</v>
       </c>
       <c r="C97" s="34" t="s">
+        <v>1938</v>
+      </c>
+      <c r="D97" s="34" t="s">
         <v>1939</v>
-      </c>
-      <c r="D97" s="34" t="s">
-        <v>1940</v>
       </c>
       <c r="E97" s="34">
         <v>9</v>
@@ -13789,25 +13783,25 @@
         <v>1914</v>
       </c>
       <c r="J97" s="34" t="s">
-        <v>2142</v>
+        <v>2140</v>
       </c>
       <c r="K97" s="34"/>
       <c r="L97" s="34" t="s">
-        <v>2113</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="34" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="B98" s="34">
         <v>5</v>
       </c>
       <c r="C98" s="34" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="D98" s="34" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="E98" s="34">
         <v>9</v>
@@ -13826,11 +13820,11 @@
         <v>1820</v>
       </c>
       <c r="J98" s="34" t="s">
-        <v>2143</v>
+        <v>2141</v>
       </c>
       <c r="K98" s="34"/>
       <c r="L98" s="34" t="s">
-        <v>2108</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="99" spans="1:12">
@@ -13841,10 +13835,10 @@
         <v>5</v>
       </c>
       <c r="C99" s="34" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="D99" s="34" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="E99" s="34">
         <v>9</v>
@@ -13863,44 +13857,19 @@
         <v>1916</v>
       </c>
       <c r="J99" s="34" t="s">
-        <v>2144</v>
+        <v>2142</v>
       </c>
       <c r="K99" s="34"/>
       <c r="L99" s="34" t="s">
-        <v>2111</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="100" spans="1:12">
       <c r="A100" s="34" t="s">
         <v>1885</v>
       </c>
-      <c r="B100">
-        <v>5</v>
-      </c>
-      <c r="C100" t="s">
-        <v>1589</v>
-      </c>
-      <c r="D100" t="s">
-        <v>1922</v>
-      </c>
-      <c r="E100">
-        <v>11</v>
-      </c>
-      <c r="F100">
-        <f>E100*2</f>
-        <v>22</v>
-      </c>
-      <c r="G100" t="s">
-        <v>1681</v>
-      </c>
-      <c r="H100" t="b">
-        <v>0</v>
-      </c>
       <c r="I100" t="s">
         <v>1914</v>
-      </c>
-      <c r="L100" t="s">
-        <v>2051</v>
       </c>
     </row>
     <row r="101" spans="1:12">
@@ -13911,10 +13880,10 @@
         <v>5</v>
       </c>
       <c r="C101" t="s">
+        <v>1922</v>
+      </c>
+      <c r="D101" t="s">
         <v>1923</v>
-      </c>
-      <c r="D101" t="s">
-        <v>1924</v>
       </c>
       <c r="E101">
         <v>10</v>
@@ -13933,7 +13902,7 @@
         <v>1913</v>
       </c>
       <c r="L101" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="102" spans="1:12">
@@ -13947,7 +13916,7 @@
         <v>1591</v>
       </c>
       <c r="D102" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="E102">
         <v>9</v>
@@ -13966,7 +13935,7 @@
         <v>1913</v>
       </c>
       <c r="L102" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="103" spans="1:12">
@@ -13999,7 +13968,7 @@
         <v>1826</v>
       </c>
       <c r="L103" t="s">
-        <v>2125</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="104" spans="1:12">
@@ -14032,7 +14001,7 @@
         <v>1827</v>
       </c>
       <c r="L104" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="105" spans="1:12">
@@ -14065,7 +14034,7 @@
         <v>1825</v>
       </c>
       <c r="L105" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="106" spans="1:12">
@@ -14098,7 +14067,7 @@
         <v>1832</v>
       </c>
       <c r="L106" t="s">
-        <v>2087</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="107" spans="1:12">
@@ -14131,7 +14100,7 @@
         <v>1819</v>
       </c>
       <c r="L107" t="s">
-        <v>2091</v>
+        <v>2089</v>
       </c>
     </row>
     <row r="108" spans="1:12">
@@ -14167,7 +14136,7 @@
         <v>1848</v>
       </c>
       <c r="L108" t="s">
-        <v>2098</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="109" spans="1:12">
@@ -14203,7 +14172,7 @@
         <v>1861</v>
       </c>
       <c r="L109" t="s">
-        <v>2099</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="110" spans="1:12">
@@ -14239,7 +14208,7 @@
         <v>1852</v>
       </c>
       <c r="L110" t="s">
-        <v>2100</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="111" spans="1:12">
@@ -14275,7 +14244,7 @@
         <v>1850</v>
       </c>
       <c r="L111" t="s">
-        <v>2101</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="112" spans="1:12">
@@ -14311,7 +14280,7 @@
         <v>1854</v>
       </c>
       <c r="L112" t="s">
-        <v>2102</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="113" spans="1:12">
@@ -14347,7 +14316,7 @@
         <v>1858</v>
       </c>
       <c r="L113" t="s">
-        <v>2103</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="114" spans="1:12">
@@ -14383,7 +14352,7 @@
         <v>1856</v>
       </c>
       <c r="L114" t="s">
-        <v>2104</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="115" spans="1:12">
@@ -14419,7 +14388,7 @@
         <v>1860</v>
       </c>
       <c r="L115" t="s">
-        <v>2105</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="116" spans="1:12">
@@ -14452,7 +14421,7 @@
         <v>1819</v>
       </c>
       <c r="L116" t="s">
-        <v>2078</v>
+        <v>2076</v>
       </c>
     </row>
     <row r="117" spans="1:12">
@@ -14466,7 +14435,7 @@
         <v>1864</v>
       </c>
       <c r="D117" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="E117">
         <v>9</v>
@@ -14485,7 +14454,7 @@
         <v>1821</v>
       </c>
       <c r="L117" t="s">
-        <v>2070</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="118" spans="1:12">
@@ -14518,7 +14487,7 @@
         <v>1821</v>
       </c>
       <c r="L118" t="s">
-        <v>2068</v>
+        <v>2066</v>
       </c>
     </row>
     <row r="119" spans="1:12">
@@ -14551,7 +14520,7 @@
         <v>1833</v>
       </c>
       <c r="L119" t="s">
-        <v>2065</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="120" spans="1:12">
@@ -14584,7 +14553,7 @@
         <v>1828</v>
       </c>
       <c r="L120" t="s">
-        <v>2055</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="121" spans="1:12">
@@ -14617,7 +14586,7 @@
         <v>1832</v>
       </c>
       <c r="L121" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="122" spans="1:12">
@@ -14650,7 +14619,7 @@
         <v>1820</v>
       </c>
       <c r="L122" t="s">
-        <v>2124</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="123" spans="1:12">
@@ -14664,7 +14633,7 @@
         <v>1607</v>
       </c>
       <c r="D123" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="E123">
         <v>12</v>
@@ -14683,7 +14652,7 @@
         <v>1916</v>
       </c>
       <c r="L123" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="124" spans="1:12">
@@ -14697,7 +14666,7 @@
         <v>1608</v>
       </c>
       <c r="D124" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="E124">
         <v>14</v>
@@ -14716,7 +14685,7 @@
         <v>1915</v>
       </c>
       <c r="L124" t="s">
-        <v>2076</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="125" spans="1:12">
@@ -14749,7 +14718,7 @@
         <v>1833</v>
       </c>
       <c r="L125" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="126" spans="1:12">
@@ -14782,7 +14751,7 @@
         <v>1832</v>
       </c>
       <c r="L126" t="s">
-        <v>2132</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="127" spans="1:12">
@@ -14815,7 +14784,7 @@
         <v>1832</v>
       </c>
       <c r="L127" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="128" spans="1:12">
@@ -14851,7 +14820,7 @@
         <v>255</v>
       </c>
       <c r="L128" t="s">
-        <v>2097</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="129" spans="1:12">
@@ -14884,7 +14853,7 @@
         <v>1819</v>
       </c>
       <c r="L129" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="130" spans="1:12">
@@ -14917,7 +14886,7 @@
         <v>1823</v>
       </c>
       <c r="L130" t="s">
-        <v>2123</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="131" spans="1:12">
@@ -14950,7 +14919,7 @@
         <v>1824</v>
       </c>
       <c r="L131" t="s">
-        <v>2074</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="132" spans="1:12">
@@ -14983,7 +14952,7 @@
         <v>1827</v>
       </c>
       <c r="L132" t="s">
-        <v>2075</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="133" spans="1:12">
@@ -15016,7 +14985,7 @@
         <v>1827</v>
       </c>
       <c r="L133" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="134" spans="1:12">
@@ -15049,7 +15018,7 @@
         <v>1826</v>
       </c>
       <c r="L134" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="135" spans="1:12">
@@ -15082,7 +15051,7 @@
         <v>1822</v>
       </c>
       <c r="L135" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="136" spans="1:12">
@@ -15115,7 +15084,7 @@
         <v>1915</v>
       </c>
       <c r="L136" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="137" spans="1:12">
@@ -15148,7 +15117,7 @@
         <v>1833</v>
       </c>
       <c r="L137" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="138" spans="1:12">
@@ -15181,7 +15150,7 @@
         <v>1831</v>
       </c>
       <c r="L138" t="s">
-        <v>2057</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="139" spans="1:12">
@@ -15214,7 +15183,7 @@
         <v>1828</v>
       </c>
       <c r="L139" t="s">
-        <v>2059</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="140" spans="1:12">
@@ -15247,7 +15216,7 @@
         <v>1831</v>
       </c>
       <c r="L140" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="141" spans="1:12">
@@ -15280,7 +15249,7 @@
         <v>1825</v>
       </c>
       <c r="L141" t="s">
-        <v>2107</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="142" spans="1:12">
@@ -15294,7 +15263,7 @@
         <v>1870</v>
       </c>
       <c r="D142" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="E142">
         <v>13</v>
@@ -15313,7 +15282,7 @@
         <v>1828</v>
       </c>
       <c r="L142" t="s">
-        <v>2080</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="143" spans="1:12">
@@ -15346,7 +15315,7 @@
         <v>1824</v>
       </c>
       <c r="L143" t="s">
-        <v>2052</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="144" spans="1:12">
@@ -15357,10 +15326,10 @@
         <v>8</v>
       </c>
       <c r="C144" t="s">
+        <v>1925</v>
+      </c>
+      <c r="D144" t="s">
         <v>1926</v>
-      </c>
-      <c r="D144" t="s">
-        <v>1927</v>
       </c>
       <c r="E144">
         <v>16</v>
@@ -15379,7 +15348,7 @@
         <v>1914</v>
       </c>
       <c r="L144" t="s">
-        <v>2062</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="145" spans="1:12">
@@ -15412,7 +15381,7 @@
         <v>1820</v>
       </c>
       <c r="L145" t="s">
-        <v>2071</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="146" spans="1:12">
@@ -15445,7 +15414,7 @@
         <v>1832</v>
       </c>
       <c r="L146" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="147" spans="1:12">
@@ -15459,7 +15428,7 @@
         <v>1593</v>
       </c>
       <c r="D147" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="E147">
         <v>15</v>
@@ -15478,7 +15447,7 @@
         <v>1913</v>
       </c>
       <c r="L147" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="148" spans="1:12">
@@ -15492,7 +15461,7 @@
         <v>1594</v>
       </c>
       <c r="D148" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="E148">
         <v>18</v>
@@ -15511,7 +15480,7 @@
         <v>1913</v>
       </c>
       <c r="L148" t="s">
-        <v>2064</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="149" spans="1:12">
@@ -15525,7 +15494,7 @@
         <v>1595</v>
       </c>
       <c r="D149" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="E149">
         <v>18</v>
@@ -15544,7 +15513,7 @@
         <v>1916</v>
       </c>
       <c r="L149" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="150" spans="1:12">
@@ -15577,7 +15546,7 @@
         <v>1830</v>
       </c>
       <c r="L150" t="s">
-        <v>2106</v>
+        <v>2104</v>
       </c>
     </row>
     <row r="151" spans="1:12">
@@ -15610,7 +15579,7 @@
         <v>1829</v>
       </c>
       <c r="L151" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="152" spans="1:12">
@@ -15624,7 +15593,7 @@
         <v>1596</v>
       </c>
       <c r="D152" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="E152">
         <v>20</v>
@@ -15643,7 +15612,7 @@
         <v>1916</v>
       </c>
       <c r="L152" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="153" spans="1:12">
@@ -15657,7 +15626,7 @@
         <v>1597</v>
       </c>
       <c r="D153" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="E153">
         <v>20</v>
@@ -15676,7 +15645,7 @@
         <v>1915</v>
       </c>
       <c r="L153" t="s">
-        <v>2053</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="154" spans="1:12">
@@ -15709,7 +15678,7 @@
         <v>1833</v>
       </c>
       <c r="L154" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
     </row>
     <row r="155" spans="1:12">
@@ -15723,7 +15692,7 @@
         <v>1609</v>
       </c>
       <c r="D155" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="E155">
         <v>16</v>
@@ -15742,7 +15711,7 @@
         <v>1913</v>
       </c>
       <c r="L155" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="156" spans="1:12">
@@ -15775,82 +15744,82 @@
         <v>1831</v>
       </c>
       <c r="L156" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="157" spans="1:12">
       <c r="A157" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="158" spans="1:12">
       <c r="A158" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="159" spans="1:12">
       <c r="A159" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="160" spans="1:12">
       <c r="A160" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="161" spans="1:9">
       <c r="A161" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="162" spans="1:9">
       <c r="A162" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="163" spans="1:9">
       <c r="A163" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="164" spans="1:9">
       <c r="A164" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="165" spans="1:9">
       <c r="A165" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="166" spans="1:9">
       <c r="A166" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="167" spans="1:9">
       <c r="A167" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="168" spans="1:9">
       <c r="A168" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="169" spans="1:9">
       <c r="A169" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="170" spans="1:9">
       <c r="A170" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="171" spans="1:9">
       <c r="A171" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="172" spans="1:9">
@@ -15863,7 +15832,7 @@
     </row>
     <row r="173" spans="1:9">
       <c r="A173" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="I173" t="s">
         <v>1824</v>
@@ -15871,7 +15840,7 @@
     </row>
     <row r="174" spans="1:9">
       <c r="A174" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="I174" t="s">
         <v>1824</v>
@@ -15879,7 +15848,7 @@
     </row>
     <row r="175" spans="1:9">
       <c r="A175" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="I175" t="s">
         <v>1824</v>
@@ -15895,17 +15864,17 @@
     </row>
     <row r="177" spans="1:9">
       <c r="A177" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="178" spans="1:9">
       <c r="A178" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="179" spans="1:9">
       <c r="A179" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="180" spans="1:9">

</xml_diff>

<commit_message>
Protection From Non-Silver Weapons
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3B98FC-06CE-49D3-8190-2741F8435ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75951250-7D6A-4617-946E-9EFDFCD969DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11509" uniqueCount="2143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11505" uniqueCount="2140">
   <si>
     <t>Caster Level</t>
   </si>
@@ -5827,12 +5827,6 @@
     <t>MEWI566</t>
   </si>
   <si>
-    <t>Omnipresence</t>
-  </si>
-  <si>
-    <t>MEWI855</t>
-  </si>
-  <si>
     <t>SPWI857</t>
   </si>
   <si>
@@ -6230,9 +6224,6 @@
   </si>
   <si>
     <t>non-detection.BAM</t>
-  </si>
-  <si>
-    <t>omnipresence.BAM</t>
   </si>
   <si>
     <t>otiluke's-resilient-sphere.BAM</t>
@@ -10472,7 +10463,7 @@
         <v>1917</v>
       </c>
       <c r="E96" t="s">
-        <v>1937</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -10529,8 +10520,8 @@
   <dimension ref="A1:M191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D112" sqref="D112"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D134" sqref="D134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -10562,10 +10553,10 @@
         <v>1817</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>1951</v>
+        <v>1949</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>1952</v>
+        <v>1950</v>
       </c>
       <c r="G1" s="23" t="s">
         <v>1676</v>
@@ -10577,13 +10568,13 @@
         <v>1818</v>
       </c>
       <c r="J1" s="23" t="s">
-        <v>1949</v>
+        <v>1947</v>
       </c>
       <c r="K1" s="23" t="s">
-        <v>1948</v>
+        <v>1946</v>
       </c>
       <c r="L1" s="23" t="s">
-        <v>1955</v>
+        <v>1953</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="29" customFormat="1">
@@ -10616,7 +10607,7 @@
         <v>1914</v>
       </c>
       <c r="L2" s="29" t="s">
-        <v>2020</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -10630,7 +10621,7 @@
         <v>1599</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>1932</v>
+        <v>1930</v>
       </c>
       <c r="E3" s="29">
         <v>3</v>
@@ -10651,7 +10642,7 @@
       <c r="J3" s="29"/>
       <c r="K3" s="29"/>
       <c r="L3" s="29" t="s">
-        <v>2093</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -10665,7 +10656,7 @@
         <v>1600</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>1933</v>
+        <v>1931</v>
       </c>
       <c r="E4" s="29">
         <v>2</v>
@@ -10675,7 +10666,7 @@
         <v>4</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>2135</v>
+        <v>2132</v>
       </c>
       <c r="H4" s="29" t="b">
         <v>0</v>
@@ -10686,7 +10677,7 @@
       <c r="J4" s="29"/>
       <c r="K4" s="29"/>
       <c r="L4" s="29" t="s">
-        <v>2125</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -10697,10 +10688,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>1994</v>
+        <v>1992</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>1931</v>
+        <v>1929</v>
       </c>
       <c r="E5" s="29">
         <v>10</v>
@@ -10721,7 +10712,7 @@
       <c r="J5" s="29"/>
       <c r="K5" s="29"/>
       <c r="L5" s="29" t="s">
-        <v>1993</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -10735,7 +10726,7 @@
         <v>1601</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>2134</v>
+        <v>2131</v>
       </c>
       <c r="E6" s="29">
         <v>4</v>
@@ -10745,7 +10736,7 @@
         <v>8</v>
       </c>
       <c r="G6" s="29" t="s">
-        <v>2135</v>
+        <v>2132</v>
       </c>
       <c r="H6" s="29" t="b">
         <v>1</v>
@@ -10756,7 +10747,7 @@
       <c r="J6" s="29"/>
       <c r="K6" s="29"/>
       <c r="L6" s="29" t="s">
-        <v>2088</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -10791,7 +10782,7 @@
       <c r="J7" s="29"/>
       <c r="K7" s="29"/>
       <c r="L7" s="29" t="s">
-        <v>2080</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -10824,7 +10815,7 @@
         <v>1819</v>
       </c>
       <c r="L8" t="s">
-        <v>1960</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -10857,7 +10848,7 @@
         <v>1822</v>
       </c>
       <c r="L9" t="s">
-        <v>2017</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -10890,7 +10881,7 @@
         <v>1821</v>
       </c>
       <c r="L10" t="s">
-        <v>2087</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -10923,7 +10914,7 @@
         <v>1825</v>
       </c>
       <c r="L11" t="s">
-        <v>1989</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -10956,7 +10947,7 @@
         <v>1823</v>
       </c>
       <c r="L12" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -10989,7 +10980,7 @@
         <v>1822</v>
       </c>
       <c r="L13" t="s">
-        <v>2035</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -11022,7 +11013,7 @@
         <v>1821</v>
       </c>
       <c r="L14" t="s">
-        <v>1958</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -11055,7 +11046,7 @@
         <v>1820</v>
       </c>
       <c r="L15" t="s">
-        <v>2029</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -11088,7 +11079,7 @@
         <v>1826</v>
       </c>
       <c r="L16" t="s">
-        <v>2077</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -11121,7 +11112,7 @@
         <v>1827</v>
       </c>
       <c r="L17" t="s">
-        <v>2124</v>
+        <v>2121</v>
       </c>
       <c r="M17" t="s">
         <v>1843</v>
@@ -11157,7 +11148,7 @@
         <v>1830</v>
       </c>
       <c r="L18" t="s">
-        <v>2070</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -11190,7 +11181,7 @@
         <v>1829</v>
       </c>
       <c r="L19" t="s">
-        <v>2090</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -11223,7 +11214,7 @@
         <v>1822</v>
       </c>
       <c r="L20" t="s">
-        <v>2092</v>
+        <v>2089</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -11256,7 +11247,7 @@
         <v>1824</v>
       </c>
       <c r="L21" t="s">
-        <v>1991</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -11289,7 +11280,7 @@
         <v>1832</v>
       </c>
       <c r="L22" t="s">
-        <v>1995</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -11322,7 +11313,7 @@
         <v>1829</v>
       </c>
       <c r="L23" t="s">
-        <v>2004</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -11355,7 +11346,7 @@
         <v>1823</v>
       </c>
       <c r="L24" t="s">
-        <v>2008</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -11388,7 +11379,7 @@
         <v>1822</v>
       </c>
       <c r="L25" t="s">
-        <v>2094</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -11423,7 +11414,7 @@
       <c r="J26" s="29"/>
       <c r="K26" s="29"/>
       <c r="L26" s="29" t="s">
-        <v>2033</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -11456,7 +11447,7 @@
         <v>1824</v>
       </c>
       <c r="L27" t="s">
-        <v>1957</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -11489,7 +11480,7 @@
         <v>1823</v>
       </c>
       <c r="L28" t="s">
-        <v>1959</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -11522,7 +11513,7 @@
         <v>1828</v>
       </c>
       <c r="L29" t="s">
-        <v>1962</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -11555,7 +11546,7 @@
         <v>1831</v>
       </c>
       <c r="L30" t="s">
-        <v>2023</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -11588,7 +11579,7 @@
         <v>1820</v>
       </c>
       <c r="L31" t="s">
-        <v>2084</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -11621,7 +11612,7 @@
         <v>1826</v>
       </c>
       <c r="L32" t="s">
-        <v>2012</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -11654,7 +11645,7 @@
         <v>1822</v>
       </c>
       <c r="L33" t="s">
-        <v>2132</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -11687,7 +11678,7 @@
         <v>1826</v>
       </c>
       <c r="L34" t="s">
-        <v>1961</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -11720,7 +11711,7 @@
         <v>1828</v>
       </c>
       <c r="L35" t="s">
-        <v>2009</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -11753,7 +11744,7 @@
         <v>1829</v>
       </c>
       <c r="L36" t="s">
-        <v>2046</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -11786,7 +11777,7 @@
         <v>1830</v>
       </c>
       <c r="L37" t="s">
-        <v>2049</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -11800,7 +11791,7 @@
         <v>85</v>
       </c>
       <c r="D38" t="s">
-        <v>2083</v>
+        <v>2080</v>
       </c>
       <c r="E38">
         <v>4</v>
@@ -11819,7 +11810,7 @@
         <v>1833</v>
       </c>
       <c r="L38" t="s">
-        <v>2082</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -11852,7 +11843,7 @@
         <v>1833</v>
       </c>
       <c r="L39" t="s">
-        <v>2054</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -11885,7 +11876,7 @@
         <v>1831</v>
       </c>
       <c r="L40" t="s">
-        <v>2117</v>
+        <v>2114</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -11918,7 +11909,7 @@
         <v>1833</v>
       </c>
       <c r="L41" t="s">
-        <v>2119</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -11951,7 +11942,7 @@
         <v>1831</v>
       </c>
       <c r="L42" t="s">
-        <v>2128</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -11984,7 +11975,7 @@
         <v>1823</v>
       </c>
       <c r="L43" t="s">
-        <v>2127</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -12017,7 +12008,7 @@
         <v>1828</v>
       </c>
       <c r="L44" t="s">
-        <v>2056</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -12050,7 +12041,7 @@
         <v>1827</v>
       </c>
       <c r="L45" t="s">
-        <v>2112</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -12064,7 +12055,7 @@
         <v>1603</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>1934</v>
+        <v>1932</v>
       </c>
       <c r="E46" s="29">
         <v>6</v>
@@ -12074,7 +12065,7 @@
         <v>12</v>
       </c>
       <c r="G46" s="29" t="s">
-        <v>2135</v>
+        <v>2132</v>
       </c>
       <c r="H46" s="29" t="b">
         <v>0</v>
@@ -12085,7 +12076,7 @@
       <c r="J46" s="29"/>
       <c r="K46" s="29"/>
       <c r="L46" s="29" t="s">
-        <v>2129</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -12120,7 +12111,7 @@
       <c r="J47" s="29"/>
       <c r="K47" s="29"/>
       <c r="L47" s="29" t="s">
-        <v>2027</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -12155,7 +12146,7 @@
       <c r="J48" s="29"/>
       <c r="K48" s="29"/>
       <c r="L48" s="29" t="s">
-        <v>2011</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -12190,7 +12181,7 @@
       <c r="J49" s="29"/>
       <c r="K49" s="29"/>
       <c r="L49" s="29" t="s">
-        <v>2047</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -12223,7 +12214,7 @@
         <v>1820</v>
       </c>
       <c r="L50" t="s">
-        <v>2010</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -12237,7 +12228,7 @@
         <v>1835</v>
       </c>
       <c r="D51" t="s">
-        <v>1953</v>
+        <v>1951</v>
       </c>
       <c r="E51">
         <v>5</v>
@@ -12256,7 +12247,7 @@
         <v>1821</v>
       </c>
       <c r="L51" t="s">
-        <v>2071</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -12289,7 +12280,7 @@
         <v>1829</v>
       </c>
       <c r="L52" t="s">
-        <v>2081</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -12322,7 +12313,7 @@
         <v>1830</v>
       </c>
       <c r="L53" t="s">
-        <v>2120</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -12355,7 +12346,7 @@
         <v>1830</v>
       </c>
       <c r="L54" t="s">
-        <v>2003</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -12388,7 +12379,7 @@
         <v>1819</v>
       </c>
       <c r="L55" t="s">
-        <v>2002</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -12421,7 +12412,7 @@
         <v>1824</v>
       </c>
       <c r="L56" t="s">
-        <v>2133</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -12454,7 +12445,7 @@
         <v>1820</v>
       </c>
       <c r="L57" t="s">
-        <v>2065</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -12487,7 +12478,7 @@
         <v>1825</v>
       </c>
       <c r="L58" t="s">
-        <v>2019</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -12520,7 +12511,7 @@
         <v>1832</v>
       </c>
       <c r="L59" t="s">
-        <v>2025</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -12553,7 +12544,7 @@
         <v>1831</v>
       </c>
       <c r="L60" t="s">
-        <v>2059</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -12586,7 +12577,7 @@
         <v>1831</v>
       </c>
       <c r="L61" t="s">
-        <v>2075</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -12619,7 +12610,7 @@
         <v>1827</v>
       </c>
       <c r="L62" t="s">
-        <v>2131</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -12652,7 +12643,7 @@
         <v>1828</v>
       </c>
       <c r="L63" t="s">
-        <v>2031</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -12685,7 +12676,7 @@
         <v>1832</v>
       </c>
       <c r="L64" t="s">
-        <v>2067</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -12718,7 +12709,7 @@
         <v>1825</v>
       </c>
       <c r="L65" t="s">
-        <v>1992</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -12751,7 +12742,7 @@
         <v>1822</v>
       </c>
       <c r="L66" t="s">
-        <v>2000</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -12784,7 +12775,7 @@
         <v>1826</v>
       </c>
       <c r="L67" t="s">
-        <v>2014</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -12817,7 +12808,7 @@
         <v>1827</v>
       </c>
       <c r="L68" t="s">
-        <v>2015</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -12850,7 +12841,7 @@
         <v>1829</v>
       </c>
       <c r="L69" t="s">
-        <v>2079</v>
+        <v>2076</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -12883,7 +12874,7 @@
         <v>1819</v>
       </c>
       <c r="L70" t="s">
-        <v>2126</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -12897,7 +12888,7 @@
         <v>1604</v>
       </c>
       <c r="D71" s="29" t="s">
-        <v>2136</v>
+        <v>2133</v>
       </c>
       <c r="E71" s="29">
         <v>8</v>
@@ -12907,7 +12898,7 @@
         <v>16</v>
       </c>
       <c r="G71" s="29" t="s">
-        <v>2135</v>
+        <v>2132</v>
       </c>
       <c r="H71" s="29" t="b">
         <v>1</v>
@@ -12918,7 +12909,7 @@
       <c r="J71" s="29"/>
       <c r="K71" s="29"/>
       <c r="L71" s="29" t="s">
-        <v>2064</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -12951,7 +12942,7 @@
         <v>1825</v>
       </c>
       <c r="L72" t="s">
-        <v>2005</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="73" spans="1:12">
@@ -12984,7 +12975,7 @@
         <v>1819</v>
       </c>
       <c r="L73" t="s">
-        <v>2028</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="74" spans="1:12">
@@ -13017,7 +13008,7 @@
         <v>1826</v>
       </c>
       <c r="L74" t="s">
-        <v>2007</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="75" spans="1:12">
@@ -13050,7 +13041,7 @@
         <v>1827</v>
       </c>
       <c r="L75" t="s">
-        <v>2040</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="76" spans="1:12">
@@ -13083,7 +13074,7 @@
         <v>1829</v>
       </c>
       <c r="L76" t="s">
-        <v>2058</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="77" spans="1:12">
@@ -13116,7 +13107,7 @@
         <v>1830</v>
       </c>
       <c r="L77" t="s">
-        <v>1999</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="78" spans="1:12">
@@ -13149,7 +13140,7 @@
         <v>1827</v>
       </c>
       <c r="L78" t="s">
-        <v>2048</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="79" spans="1:12">
@@ -13182,7 +13173,7 @@
         <v>1822</v>
       </c>
       <c r="L79" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -13215,7 +13206,7 @@
         <v>1830</v>
       </c>
       <c r="L80" t="s">
-        <v>2026</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="81" spans="1:12">
@@ -13248,7 +13239,7 @@
         <v>1830</v>
       </c>
       <c r="L81" t="s">
-        <v>2044</v>
+        <v>2042</v>
       </c>
     </row>
     <row r="82" spans="1:12">
@@ -13281,7 +13272,7 @@
         <v>1829</v>
       </c>
       <c r="L82" t="s">
-        <v>2052</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="83" spans="1:12">
@@ -13314,7 +13305,7 @@
         <v>1825</v>
       </c>
       <c r="L83" t="s">
-        <v>2118</v>
+        <v>2115</v>
       </c>
     </row>
     <row r="84" spans="1:12">
@@ -13347,7 +13338,7 @@
         <v>1832</v>
       </c>
       <c r="L84" t="s">
-        <v>2036</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="85" spans="1:12">
@@ -13380,7 +13371,7 @@
         <v>1828</v>
       </c>
       <c r="L85" t="s">
-        <v>2061</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="86" spans="1:12">
@@ -13413,7 +13404,7 @@
         <v>1829</v>
       </c>
       <c r="L86" t="s">
-        <v>2114</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="87" spans="1:12">
@@ -13446,7 +13437,7 @@
         <v>1826</v>
       </c>
       <c r="L87" t="s">
-        <v>2016</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -13479,7 +13470,7 @@
         <v>1826</v>
       </c>
       <c r="L88" t="s">
-        <v>2024</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="89" spans="1:12">
@@ -13512,7 +13503,7 @@
         <v>1833</v>
       </c>
       <c r="L89" t="s">
-        <v>1963</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="90" spans="1:12">
@@ -13545,7 +13536,7 @@
         <v>1833</v>
       </c>
       <c r="L90" t="s">
-        <v>2086</v>
+        <v>2083</v>
       </c>
     </row>
     <row r="91" spans="1:12">
@@ -13581,7 +13572,7 @@
         <v>1840</v>
       </c>
       <c r="L91" t="s">
-        <v>2091</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="92" spans="1:12">
@@ -13614,7 +13605,7 @@
         <v>1822</v>
       </c>
       <c r="L92" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="93" spans="1:12">
@@ -13628,7 +13619,7 @@
         <v>1605</v>
       </c>
       <c r="D93" s="29" t="s">
-        <v>1936</v>
+        <v>1934</v>
       </c>
       <c r="E93" s="29">
         <v>10</v>
@@ -13649,7 +13640,7 @@
       <c r="J93" s="29"/>
       <c r="K93" s="29"/>
       <c r="L93" s="29" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="94" spans="1:12">
@@ -13660,10 +13651,10 @@
         <v>5</v>
       </c>
       <c r="C94" s="29" t="s">
-        <v>1942</v>
+        <v>1940</v>
       </c>
       <c r="D94" s="29" t="s">
-        <v>1939</v>
+        <v>1937</v>
       </c>
       <c r="E94" s="29">
         <v>9</v>
@@ -13682,11 +13673,11 @@
         <v>1915</v>
       </c>
       <c r="J94" s="29" t="s">
-        <v>2137</v>
+        <v>2134</v>
       </c>
       <c r="K94" s="29"/>
       <c r="L94" s="29" t="s">
-        <v>2107</v>
+        <v>2104</v>
       </c>
     </row>
     <row r="95" spans="1:12">
@@ -13697,10 +13688,10 @@
         <v>5</v>
       </c>
       <c r="C95" s="29" t="s">
-        <v>1940</v>
+        <v>1938</v>
       </c>
       <c r="D95" s="29" t="s">
-        <v>1939</v>
+        <v>1937</v>
       </c>
       <c r="E95" s="29">
         <v>9</v>
@@ -13719,11 +13710,11 @@
         <v>1916</v>
       </c>
       <c r="J95" s="29" t="s">
-        <v>2138</v>
+        <v>2135</v>
       </c>
       <c r="K95" s="29"/>
       <c r="L95" s="29" t="s">
-        <v>2108</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="96" spans="1:12">
@@ -13734,10 +13725,10 @@
         <v>5</v>
       </c>
       <c r="C96" s="29" t="s">
-        <v>1941</v>
+        <v>1939</v>
       </c>
       <c r="D96" s="29" t="s">
-        <v>1939</v>
+        <v>1937</v>
       </c>
       <c r="E96" s="29">
         <v>9</v>
@@ -13756,11 +13747,11 @@
         <v>1915</v>
       </c>
       <c r="J96" s="29" t="s">
-        <v>2139</v>
+        <v>2136</v>
       </c>
       <c r="K96" s="29"/>
       <c r="L96" s="29" t="s">
-        <v>2110</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="97" spans="1:12">
@@ -13771,10 +13762,10 @@
         <v>5</v>
       </c>
       <c r="C97" s="29" t="s">
-        <v>1938</v>
+        <v>1936</v>
       </c>
       <c r="D97" s="29" t="s">
-        <v>1939</v>
+        <v>1937</v>
       </c>
       <c r="E97" s="29">
         <v>9</v>
@@ -13793,25 +13784,25 @@
         <v>1914</v>
       </c>
       <c r="J97" s="29" t="s">
-        <v>2140</v>
+        <v>2137</v>
       </c>
       <c r="K97" s="29"/>
       <c r="L97" s="29" t="s">
-        <v>2111</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="29" t="s">
-        <v>1972</v>
+        <v>1970</v>
       </c>
       <c r="B98" s="29">
         <v>5</v>
       </c>
       <c r="C98" s="29" t="s">
-        <v>1944</v>
+        <v>1942</v>
       </c>
       <c r="D98" s="29" t="s">
-        <v>1939</v>
+        <v>1937</v>
       </c>
       <c r="E98" s="29">
         <v>9</v>
@@ -13830,11 +13821,11 @@
         <v>1820</v>
       </c>
       <c r="J98" s="29" t="s">
-        <v>2141</v>
+        <v>2138</v>
       </c>
       <c r="K98" s="29"/>
       <c r="L98" s="29" t="s">
-        <v>2106</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="99" spans="1:12">
@@ -13845,10 +13836,10 @@
         <v>5</v>
       </c>
       <c r="C99" s="29" t="s">
-        <v>1943</v>
+        <v>1941</v>
       </c>
       <c r="D99" s="29" t="s">
-        <v>1939</v>
+        <v>1937</v>
       </c>
       <c r="E99" s="29">
         <v>9</v>
@@ -13867,11 +13858,11 @@
         <v>1916</v>
       </c>
       <c r="J99" s="29" t="s">
-        <v>2142</v>
+        <v>2139</v>
       </c>
       <c r="K99" s="29"/>
       <c r="L99" s="29" t="s">
-        <v>2109</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="100" spans="1:12">
@@ -13906,7 +13897,7 @@
       <c r="J100" s="29"/>
       <c r="K100" s="29"/>
       <c r="L100" s="29" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="101" spans="1:12">
@@ -13941,7 +13932,7 @@
       <c r="J101" s="29"/>
       <c r="K101" s="29"/>
       <c r="L101" s="29" t="s">
-        <v>2030</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="102" spans="1:12">
@@ -13974,7 +13965,7 @@
         <v>1826</v>
       </c>
       <c r="L102" t="s">
-        <v>2123</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="103" spans="1:12">
@@ -14007,7 +13998,7 @@
         <v>1827</v>
       </c>
       <c r="L103" t="s">
-        <v>1997</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="104" spans="1:12">
@@ -14040,7 +14031,7 @@
         <v>1825</v>
       </c>
       <c r="L104" t="s">
-        <v>1998</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="105" spans="1:12">
@@ -14073,7 +14064,7 @@
         <v>1832</v>
       </c>
       <c r="L105" t="s">
-        <v>2085</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="106" spans="1:12">
@@ -14106,7 +14097,7 @@
         <v>1819</v>
       </c>
       <c r="L106" t="s">
-        <v>2089</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="107" spans="1:12">
@@ -14142,7 +14133,7 @@
         <v>1848</v>
       </c>
       <c r="L107" t="s">
-        <v>2096</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="108" spans="1:12">
@@ -14178,7 +14169,7 @@
         <v>1861</v>
       </c>
       <c r="L108" t="s">
-        <v>2097</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="109" spans="1:12">
@@ -14214,7 +14205,7 @@
         <v>1852</v>
       </c>
       <c r="L109" t="s">
-        <v>2098</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="110" spans="1:12">
@@ -14250,7 +14241,7 @@
         <v>1850</v>
       </c>
       <c r="L110" t="s">
-        <v>2099</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="111" spans="1:12">
@@ -14286,7 +14277,7 @@
         <v>1854</v>
       </c>
       <c r="L111" t="s">
-        <v>2100</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="112" spans="1:12">
@@ -14322,7 +14313,7 @@
         <v>1858</v>
       </c>
       <c r="L112" t="s">
-        <v>2101</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="113" spans="1:12">
@@ -14358,7 +14349,7 @@
         <v>1856</v>
       </c>
       <c r="L113" t="s">
-        <v>2102</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="114" spans="1:12">
@@ -14394,7 +14385,7 @@
         <v>1860</v>
       </c>
       <c r="L114" t="s">
-        <v>2103</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="115" spans="1:12">
@@ -14427,7 +14418,7 @@
         <v>1819</v>
       </c>
       <c r="L115" t="s">
-        <v>2076</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="116" spans="1:12">
@@ -14441,7 +14432,7 @@
         <v>1864</v>
       </c>
       <c r="D116" t="s">
-        <v>1954</v>
+        <v>1952</v>
       </c>
       <c r="E116">
         <v>9</v>
@@ -14460,7 +14451,7 @@
         <v>1821</v>
       </c>
       <c r="L116" t="s">
-        <v>2068</v>
+        <v>2065</v>
       </c>
     </row>
     <row r="117" spans="1:12">
@@ -14493,7 +14484,7 @@
         <v>1821</v>
       </c>
       <c r="L117" t="s">
-        <v>2066</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="118" spans="1:12">
@@ -14526,7 +14517,7 @@
         <v>1833</v>
       </c>
       <c r="L118" t="s">
-        <v>2063</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="119" spans="1:12">
@@ -14559,7 +14550,7 @@
         <v>1828</v>
       </c>
       <c r="L119" t="s">
-        <v>2053</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="120" spans="1:12">
@@ -14592,7 +14583,7 @@
         <v>1832</v>
       </c>
       <c r="L120" t="s">
-        <v>1965</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="121" spans="1:12">
@@ -14625,7 +14616,7 @@
         <v>1820</v>
       </c>
       <c r="L121" t="s">
-        <v>2122</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="122" spans="1:12">
@@ -14639,7 +14630,7 @@
         <v>1607</v>
       </c>
       <c r="D122" s="29" t="s">
-        <v>1945</v>
+        <v>1943</v>
       </c>
       <c r="E122" s="29">
         <v>12</v>
@@ -14660,40 +14651,42 @@
       <c r="J122" s="29"/>
       <c r="K122" s="29"/>
       <c r="L122" s="29" t="s">
-        <v>1964</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="123" spans="1:12">
       <c r="A123" s="29" t="s">
         <v>1901</v>
       </c>
-      <c r="B123">
+      <c r="B123" s="29">
         <v>6</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C123" s="29" t="s">
         <v>1608</v>
       </c>
-      <c r="D123" t="s">
-        <v>1946</v>
-      </c>
-      <c r="E123">
+      <c r="D123" s="29" t="s">
+        <v>1944</v>
+      </c>
+      <c r="E123" s="29">
         <v>14</v>
       </c>
-      <c r="F123">
+      <c r="F123" s="29">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="G123" t="s">
+      <c r="G123" s="29" t="s">
         <v>1681</v>
       </c>
-      <c r="H123" t="b">
-        <v>0</v>
-      </c>
-      <c r="I123" t="s">
+      <c r="H123" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="I123" s="29" t="s">
         <v>1915</v>
       </c>
-      <c r="L123" t="s">
-        <v>2074</v>
+      <c r="J123" s="29"/>
+      <c r="K123" s="29"/>
+      <c r="L123" s="29" t="s">
+        <v>2071</v>
       </c>
     </row>
     <row r="124" spans="1:12">
@@ -14726,7 +14719,7 @@
         <v>1833</v>
       </c>
       <c r="L124" t="s">
-        <v>2039</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="125" spans="1:12">
@@ -14759,7 +14752,7 @@
         <v>1832</v>
       </c>
       <c r="L125" t="s">
-        <v>2130</v>
+        <v>2127</v>
       </c>
     </row>
     <row r="126" spans="1:12">
@@ -14792,7 +14785,7 @@
         <v>1832</v>
       </c>
       <c r="L126" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="127" spans="1:12">
@@ -14828,7 +14821,7 @@
         <v>255</v>
       </c>
       <c r="L127" t="s">
-        <v>2095</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="128" spans="1:12">
@@ -14861,7 +14854,7 @@
         <v>1819</v>
       </c>
       <c r="L128" t="s">
-        <v>2034</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="129" spans="1:12">
@@ -14894,7 +14887,7 @@
         <v>1823</v>
       </c>
       <c r="L129" t="s">
-        <v>2121</v>
+        <v>2118</v>
       </c>
     </row>
     <row r="130" spans="1:12">
@@ -14927,7 +14920,7 @@
         <v>1824</v>
       </c>
       <c r="L130" t="s">
-        <v>2072</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="131" spans="1:12">
@@ -14960,7 +14953,7 @@
         <v>1827</v>
       </c>
       <c r="L131" t="s">
-        <v>2073</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="132" spans="1:12">
@@ -14993,7 +14986,7 @@
         <v>1827</v>
       </c>
       <c r="L132" t="s">
-        <v>2043</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="133" spans="1:12">
@@ -15026,7 +15019,7 @@
         <v>1826</v>
       </c>
       <c r="L133" t="s">
-        <v>2006</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="134" spans="1:12">
@@ -15059,7 +15052,7 @@
         <v>1822</v>
       </c>
       <c r="L134" t="s">
-        <v>1996</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="135" spans="1:12">
@@ -15092,7 +15085,7 @@
         <v>1915</v>
       </c>
       <c r="L135" t="s">
-        <v>2038</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="136" spans="1:12">
@@ -15125,7 +15118,7 @@
         <v>1833</v>
       </c>
       <c r="L136" t="s">
-        <v>2041</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="137" spans="1:12">
@@ -15158,7 +15151,7 @@
         <v>1831</v>
       </c>
       <c r="L137" t="s">
-        <v>2055</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="138" spans="1:12">
@@ -15191,7 +15184,7 @@
         <v>1828</v>
       </c>
       <c r="L138" t="s">
-        <v>2057</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="139" spans="1:12">
@@ -15224,7 +15217,7 @@
         <v>1831</v>
       </c>
       <c r="L139" t="s">
-        <v>2037</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="140" spans="1:12">
@@ -15257,7 +15250,7 @@
         <v>1825</v>
       </c>
       <c r="L140" t="s">
-        <v>2105</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="141" spans="1:12">
@@ -15271,7 +15264,7 @@
         <v>1870</v>
       </c>
       <c r="D141" t="s">
-        <v>1935</v>
+        <v>1933</v>
       </c>
       <c r="E141">
         <v>13</v>
@@ -15290,7 +15283,7 @@
         <v>1828</v>
       </c>
       <c r="L141" t="s">
-        <v>2078</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="142" spans="1:12">
@@ -15323,40 +15316,15 @@
         <v>1824</v>
       </c>
       <c r="L142" t="s">
-        <v>2050</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="143" spans="1:12">
       <c r="A143" s="29" t="s">
         <v>1881</v>
       </c>
-      <c r="B143">
-        <v>8</v>
-      </c>
-      <c r="C143" t="s">
-        <v>1925</v>
-      </c>
-      <c r="D143" t="s">
-        <v>1926</v>
-      </c>
-      <c r="E143">
-        <v>16</v>
-      </c>
-      <c r="F143">
-        <f t="shared" si="4"/>
-        <v>32</v>
-      </c>
-      <c r="G143" t="s">
-        <v>1677</v>
-      </c>
-      <c r="H143" t="b">
-        <v>0</v>
-      </c>
       <c r="I143" t="s">
         <v>1914</v>
-      </c>
-      <c r="L143" t="s">
-        <v>2060</v>
       </c>
     </row>
     <row r="144" spans="1:12">
@@ -15389,7 +15357,7 @@
         <v>1820</v>
       </c>
       <c r="L144" t="s">
-        <v>2069</v>
+        <v>2066</v>
       </c>
     </row>
     <row r="145" spans="1:12">
@@ -15422,7 +15390,7 @@
         <v>1832</v>
       </c>
       <c r="L145" t="s">
-        <v>2045</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="146" spans="1:12">
@@ -15436,7 +15404,7 @@
         <v>1593</v>
       </c>
       <c r="D146" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
       <c r="E146">
         <v>15</v>
@@ -15455,7 +15423,7 @@
         <v>1913</v>
       </c>
       <c r="L146" t="s">
-        <v>2022</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="147" spans="1:12">
@@ -15469,7 +15437,7 @@
         <v>1594</v>
       </c>
       <c r="D147" t="s">
-        <v>1928</v>
+        <v>1926</v>
       </c>
       <c r="E147">
         <v>18</v>
@@ -15488,7 +15456,7 @@
         <v>1913</v>
       </c>
       <c r="L147" t="s">
-        <v>2062</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="148" spans="1:12">
@@ -15502,7 +15470,7 @@
         <v>1595</v>
       </c>
       <c r="D148" t="s">
-        <v>1929</v>
+        <v>1927</v>
       </c>
       <c r="E148">
         <v>18</v>
@@ -15521,7 +15489,7 @@
         <v>1916</v>
       </c>
       <c r="L148" t="s">
-        <v>1966</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="149" spans="1:12">
@@ -15554,7 +15522,7 @@
         <v>1830</v>
       </c>
       <c r="L149" t="s">
-        <v>2104</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="150" spans="1:12">
@@ -15587,7 +15555,7 @@
         <v>1829</v>
       </c>
       <c r="L150" t="s">
-        <v>1956</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="151" spans="1:12">
@@ -15601,7 +15569,7 @@
         <v>1596</v>
       </c>
       <c r="D151" t="s">
-        <v>1930</v>
+        <v>1928</v>
       </c>
       <c r="E151">
         <v>20</v>
@@ -15620,7 +15588,7 @@
         <v>1916</v>
       </c>
       <c r="L151" t="s">
-        <v>2013</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="152" spans="1:12">
@@ -15634,7 +15602,7 @@
         <v>1597</v>
       </c>
       <c r="D152" t="s">
-        <v>1950</v>
+        <v>1948</v>
       </c>
       <c r="E152">
         <v>20</v>
@@ -15653,7 +15621,7 @@
         <v>1915</v>
       </c>
       <c r="L152" t="s">
-        <v>2051</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="153" spans="1:12">
@@ -15686,7 +15654,7 @@
         <v>1833</v>
       </c>
       <c r="L153" t="s">
-        <v>2042</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="154" spans="1:12">
@@ -15700,7 +15668,7 @@
         <v>1609</v>
       </c>
       <c r="D154" t="s">
-        <v>1947</v>
+        <v>1945</v>
       </c>
       <c r="E154">
         <v>16</v>
@@ -15719,7 +15687,7 @@
         <v>1913</v>
       </c>
       <c r="L154" t="s">
-        <v>2001</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="155" spans="1:12">
@@ -15752,7 +15720,7 @@
         <v>1831</v>
       </c>
       <c r="L155" t="s">
-        <v>1990</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="156" spans="1:12">
@@ -15765,77 +15733,77 @@
     </row>
     <row r="157" spans="1:12">
       <c r="A157" t="s">
-        <v>1967</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="158" spans="1:12">
       <c r="A158" t="s">
-        <v>1968</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="159" spans="1:12">
       <c r="A159" t="s">
-        <v>1969</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="160" spans="1:12">
       <c r="A160" t="s">
-        <v>1970</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="161" spans="1:9">
       <c r="A161" t="s">
-        <v>1971</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="162" spans="1:9">
       <c r="A162" t="s">
-        <v>1974</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="163" spans="1:9">
       <c r="A163" t="s">
-        <v>1975</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="164" spans="1:9">
       <c r="A164" t="s">
-        <v>1976</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="165" spans="1:9">
       <c r="A165" t="s">
-        <v>1977</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="166" spans="1:9">
       <c r="A166" t="s">
-        <v>1978</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="167" spans="1:9">
       <c r="A167" t="s">
-        <v>1979</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="168" spans="1:9">
       <c r="A168" t="s">
-        <v>1973</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="169" spans="1:9">
       <c r="A169" t="s">
-        <v>1980</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="170" spans="1:9">
       <c r="A170" t="s">
-        <v>1981</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="171" spans="1:9">
       <c r="A171" t="s">
-        <v>1982</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="172" spans="1:9">
@@ -15848,7 +15816,7 @@
     </row>
     <row r="173" spans="1:9">
       <c r="A173" t="s">
-        <v>1983</v>
+        <v>1981</v>
       </c>
       <c r="I173" t="s">
         <v>1824</v>
@@ -15856,7 +15824,7 @@
     </row>
     <row r="174" spans="1:9">
       <c r="A174" t="s">
-        <v>1985</v>
+        <v>1983</v>
       </c>
       <c r="I174" t="s">
         <v>1824</v>
@@ -15864,7 +15832,7 @@
     </row>
     <row r="175" spans="1:9">
       <c r="A175" t="s">
-        <v>1984</v>
+        <v>1982</v>
       </c>
       <c r="I175" t="s">
         <v>1824</v>
@@ -15880,17 +15848,17 @@
     </row>
     <row r="177" spans="1:9">
       <c r="A177" t="s">
-        <v>1986</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="178" spans="1:9">
       <c r="A178" t="s">
-        <v>1987</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="179" spans="1:9">
       <c r="A179" t="s">
-        <v>1988</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="180" spans="1:9">

</xml_diff>

<commit_message>
Accidentally had "I" postfix rather than "D" for description BAMs
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E64C42A-022A-4BD6-97EE-6AFC1BCCF247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD739B33-AB63-4E10-A0DB-72F81FD86635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -5509,51 +5509,6 @@
     <t>Descrption BAM</t>
   </si>
   <si>
-    <t>BZPN001I</t>
-  </si>
-  <si>
-    <t>BZPN005I</t>
-  </si>
-  <si>
-    <t>BZPN008I</t>
-  </si>
-  <si>
-    <t>BZPN013I</t>
-  </si>
-  <si>
-    <t>BZPN019I</t>
-  </si>
-  <si>
-    <t>BZPN026I</t>
-  </si>
-  <si>
-    <t>BZPN032I</t>
-  </si>
-  <si>
-    <t>BZPN040I</t>
-  </si>
-  <si>
-    <t>BZPN049I</t>
-  </si>
-  <si>
-    <t>BZPN058I</t>
-  </si>
-  <si>
-    <t>BZPN070I</t>
-  </si>
-  <si>
-    <t>BZPN080I</t>
-  </si>
-  <si>
-    <t>BZPN090I</t>
-  </si>
-  <si>
-    <t>BZPN100I</t>
-  </si>
-  <si>
-    <t>BZPN110I</t>
-  </si>
-  <si>
     <t>SPPR303;SPWI326</t>
   </si>
   <si>
@@ -5791,18 +5746,6 @@
     <t>MEPR255;MEWI252</t>
   </si>
   <si>
-    <t>BZPN120I</t>
-  </si>
-  <si>
-    <t>BZPN130I</t>
-  </si>
-  <si>
-    <t>BZPN140I</t>
-  </si>
-  <si>
-    <t>BZPN150I</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -6470,6 +6413,63 @@
   </si>
   <si>
     <t>MESOS05, etc.</t>
+  </si>
+  <si>
+    <t>BZPN130D</t>
+  </si>
+  <si>
+    <t>BZPN120D</t>
+  </si>
+  <si>
+    <t>BZPN150D</t>
+  </si>
+  <si>
+    <t>BZPN040D</t>
+  </si>
+  <si>
+    <t>BZPN080D</t>
+  </si>
+  <si>
+    <t>BZPN070D</t>
+  </si>
+  <si>
+    <t>BZPN100D</t>
+  </si>
+  <si>
+    <t>BZPN090D</t>
+  </si>
+  <si>
+    <t>BZPN110D</t>
+  </si>
+  <si>
+    <t>BZPN140D</t>
+  </si>
+  <si>
+    <t>BZPN008D</t>
+  </si>
+  <si>
+    <t>BZPN058D</t>
+  </si>
+  <si>
+    <t>BZPN001D</t>
+  </si>
+  <si>
+    <t>BZPN013D</t>
+  </si>
+  <si>
+    <t>BZPN005D</t>
+  </si>
+  <si>
+    <t>BZPN019D</t>
+  </si>
+  <si>
+    <t>BZPN049D</t>
+  </si>
+  <si>
+    <t>BZPN032D</t>
+  </si>
+  <si>
+    <t>BZPN026D</t>
   </si>
 </sst>
 </file>
@@ -10210,7 +10210,7 @@
         <v>1684</v>
       </c>
       <c r="D73" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -10221,7 +10221,7 @@
         <v>1684</v>
       </c>
       <c r="D74" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -10232,7 +10232,7 @@
         <v>1684</v>
       </c>
       <c r="D75" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -10243,7 +10243,7 @@
         <v>1684</v>
       </c>
       <c r="D76" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -10254,7 +10254,7 @@
         <v>1684</v>
       </c>
       <c r="D77" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -10265,7 +10265,7 @@
         <v>1684</v>
       </c>
       <c r="D78" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -10276,7 +10276,7 @@
         <v>1684</v>
       </c>
       <c r="D79" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -10287,7 +10287,7 @@
         <v>1684</v>
       </c>
       <c r="D80" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -10298,7 +10298,7 @@
         <v>1684</v>
       </c>
       <c r="D81" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -10309,7 +10309,7 @@
         <v>1684</v>
       </c>
       <c r="D82" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -10320,7 +10320,7 @@
         <v>1684</v>
       </c>
       <c r="D83" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -10331,7 +10331,7 @@
         <v>1684</v>
       </c>
       <c r="D84" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -10342,7 +10342,7 @@
         <v>1684</v>
       </c>
       <c r="D85" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -10353,7 +10353,7 @@
         <v>1684</v>
       </c>
       <c r="D86" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -10364,7 +10364,7 @@
         <v>1684</v>
       </c>
       <c r="D87" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -10375,7 +10375,7 @@
         <v>1684</v>
       </c>
       <c r="D88" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -10386,7 +10386,7 @@
         <v>1684</v>
       </c>
       <c r="D89" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -10397,7 +10397,7 @@
         <v>1684</v>
       </c>
       <c r="D90" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -10408,7 +10408,7 @@
         <v>1684</v>
       </c>
       <c r="D91" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -10419,7 +10419,7 @@
         <v>1684</v>
       </c>
       <c r="D92" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -10430,7 +10430,7 @@
         <v>1684</v>
       </c>
       <c r="D93" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -10441,7 +10441,7 @@
         <v>1684</v>
       </c>
       <c r="D94" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -10452,7 +10452,7 @@
         <v>1684</v>
       </c>
       <c r="D95" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -10463,10 +10463,10 @@
         <v>1684</v>
       </c>
       <c r="D96" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
       <c r="E96" t="s">
-        <v>1935</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -10477,7 +10477,7 @@
         <v>1684</v>
       </c>
       <c r="D97" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -10488,7 +10488,7 @@
         <v>1684</v>
       </c>
       <c r="D98" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -10499,7 +10499,7 @@
         <v>1684</v>
       </c>
       <c r="D99" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -10510,7 +10510,7 @@
         <v>1684</v>
       </c>
       <c r="D100" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
     </row>
   </sheetData>
@@ -10523,8 +10523,8 @@
   <dimension ref="A1:M191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L44" sqref="A44:L44"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -10556,10 +10556,10 @@
         <v>1817</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>1949</v>
+        <v>1930</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>1950</v>
+        <v>1931</v>
       </c>
       <c r="G1" s="23" t="s">
         <v>1676</v>
@@ -10571,18 +10571,18 @@
         <v>1818</v>
       </c>
       <c r="J1" s="23" t="s">
-        <v>1947</v>
+        <v>1928</v>
       </c>
       <c r="K1" s="23" t="s">
-        <v>1946</v>
+        <v>1927</v>
       </c>
       <c r="L1" s="23" t="s">
-        <v>1953</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="29" customFormat="1">
       <c r="A2" s="29" t="s">
-        <v>1891</v>
+        <v>1876</v>
       </c>
       <c r="B2" s="29">
         <v>1</v>
@@ -10607,15 +10607,15 @@
         <v>0</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>1914</v>
+        <v>2121</v>
       </c>
       <c r="L2" s="29" t="s">
-        <v>2018</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="29" t="s">
-        <v>1874</v>
+        <v>1859</v>
       </c>
       <c r="B3" s="29">
         <v>1</v>
@@ -10624,7 +10624,7 @@
         <v>1599</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>1930</v>
+        <v>1911</v>
       </c>
       <c r="E3" s="29">
         <v>3</v>
@@ -10640,17 +10640,17 @@
         <v>0</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>1913</v>
+        <v>2122</v>
       </c>
       <c r="J3" s="29"/>
       <c r="K3" s="29"/>
       <c r="L3" s="29" t="s">
-        <v>2090</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="29" t="s">
-        <v>1889</v>
+        <v>1874</v>
       </c>
       <c r="B4" s="29">
         <v>1</v>
@@ -10659,7 +10659,7 @@
         <v>1600</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>1931</v>
+        <v>1912</v>
       </c>
       <c r="E4" s="29">
         <v>2</v>
@@ -10669,32 +10669,32 @@
         <v>4</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>2132</v>
+        <v>2113</v>
       </c>
       <c r="H4" s="29" t="b">
         <v>0</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>1914</v>
+        <v>2121</v>
       </c>
       <c r="J4" s="29"/>
       <c r="K4" s="29"/>
       <c r="L4" s="29" t="s">
-        <v>2122</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="29" t="s">
-        <v>1886</v>
+        <v>1871</v>
       </c>
       <c r="B5" s="29">
         <v>1</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>1992</v>
+        <v>1973</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>1929</v>
+        <v>1910</v>
       </c>
       <c r="E5" s="29">
         <v>10</v>
@@ -10710,17 +10710,17 @@
         <v>0</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>1914</v>
+        <v>2121</v>
       </c>
       <c r="J5" s="29"/>
       <c r="K5" s="29"/>
       <c r="L5" s="29" t="s">
-        <v>1991</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="29" t="s">
-        <v>1872</v>
+        <v>1857</v>
       </c>
       <c r="B6" s="29">
         <v>1</v>
@@ -10729,7 +10729,7 @@
         <v>1601</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>2131</v>
+        <v>2112</v>
       </c>
       <c r="E6" s="29">
         <v>4</v>
@@ -10739,23 +10739,23 @@
         <v>8</v>
       </c>
       <c r="G6" s="29" t="s">
-        <v>2132</v>
+        <v>2113</v>
       </c>
       <c r="H6" s="29" t="b">
         <v>1</v>
       </c>
       <c r="I6" s="29" t="s">
-        <v>1913</v>
+        <v>2122</v>
       </c>
       <c r="J6" s="29"/>
       <c r="K6" s="29"/>
       <c r="L6" s="29" t="s">
-        <v>2085</v>
+        <v>2066</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="29" t="s">
-        <v>1902</v>
+        <v>1887</v>
       </c>
       <c r="B7" s="29">
         <v>1</v>
@@ -10764,7 +10764,7 @@
         <v>1584</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>1918</v>
+        <v>1899</v>
       </c>
       <c r="E7" s="29">
         <v>4</v>
@@ -10780,12 +10780,12 @@
         <v>0</v>
       </c>
       <c r="I7" s="29" t="s">
-        <v>1916</v>
+        <v>2123</v>
       </c>
       <c r="J7" s="29"/>
       <c r="K7" s="29"/>
       <c r="L7" s="29" t="s">
-        <v>2077</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -10815,10 +10815,10 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>1819</v>
+        <v>2133</v>
       </c>
       <c r="L8" t="s">
-        <v>1958</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -10848,10 +10848,10 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>1822</v>
+        <v>2134</v>
       </c>
       <c r="L9" t="s">
-        <v>2015</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -10881,10 +10881,10 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>1821</v>
+        <v>2131</v>
       </c>
       <c r="L10" t="s">
-        <v>2084</v>
+        <v>2065</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -10914,10 +10914,10 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>1825</v>
+        <v>2138</v>
       </c>
       <c r="L11" t="s">
-        <v>1987</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -10947,10 +10947,10 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>1823</v>
+        <v>2136</v>
       </c>
       <c r="L12" t="s">
-        <v>2113</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -10980,10 +10980,10 @@
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>1822</v>
+        <v>2134</v>
       </c>
       <c r="L13" t="s">
-        <v>2033</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -11013,10 +11013,10 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>1821</v>
+        <v>2131</v>
       </c>
       <c r="L14" t="s">
-        <v>1956</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -11046,10 +11046,10 @@
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>1820</v>
+        <v>2135</v>
       </c>
       <c r="L15" t="s">
-        <v>2027</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -11060,7 +11060,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>1841</v>
+        <v>1826</v>
       </c>
       <c r="D16" t="s">
         <v>26</v>
@@ -11079,10 +11079,10 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>1826</v>
+        <v>2124</v>
       </c>
       <c r="L16" t="s">
-        <v>2074</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -11096,7 +11096,7 @@
         <v>1683</v>
       </c>
       <c r="D17" t="s">
-        <v>1842</v>
+        <v>1827</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -11112,13 +11112,13 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>1827</v>
+        <v>2137</v>
       </c>
       <c r="L17" t="s">
-        <v>2121</v>
+        <v>2102</v>
       </c>
       <c r="M17" t="s">
-        <v>1843</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -11148,10 +11148,10 @@
         <v>1</v>
       </c>
       <c r="I18" t="s">
-        <v>1830</v>
+        <v>2125</v>
       </c>
       <c r="L18" t="s">
-        <v>2067</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -11181,10 +11181,10 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>1829</v>
+        <v>2126</v>
       </c>
       <c r="L19" t="s">
-        <v>2087</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -11208,16 +11208,16 @@
         <v>4</v>
       </c>
       <c r="G20" t="s">
-        <v>1844</v>
+        <v>1829</v>
       </c>
       <c r="H20" t="b">
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>1822</v>
+        <v>2134</v>
       </c>
       <c r="L20" t="s">
-        <v>2089</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -11247,12 +11247,12 @@
         <v>0</v>
       </c>
       <c r="I21" s="29" t="s">
-        <v>1824</v>
+        <v>2139</v>
       </c>
       <c r="J21" s="29"/>
       <c r="K21" s="29"/>
       <c r="L21" s="29" t="s">
-        <v>1989</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -11282,12 +11282,12 @@
         <v>1</v>
       </c>
       <c r="I22" s="29" t="s">
-        <v>1832</v>
+        <v>2127</v>
       </c>
       <c r="J22" s="29"/>
       <c r="K22" s="29"/>
       <c r="L22" s="29" t="s">
-        <v>1993</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -11317,12 +11317,12 @@
         <v>0</v>
       </c>
       <c r="I23" s="29" t="s">
-        <v>1829</v>
+        <v>2126</v>
       </c>
       <c r="J23" s="29"/>
       <c r="K23" s="29"/>
       <c r="L23" s="29" t="s">
-        <v>2002</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -11352,12 +11352,12 @@
         <v>1</v>
       </c>
       <c r="I24" s="29" t="s">
-        <v>1823</v>
+        <v>2136</v>
       </c>
       <c r="J24" s="29"/>
       <c r="K24" s="29"/>
       <c r="L24" s="29" t="s">
-        <v>2006</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -11387,17 +11387,17 @@
         <v>1</v>
       </c>
       <c r="I25" s="29" t="s">
-        <v>1822</v>
+        <v>2134</v>
       </c>
       <c r="J25" s="29"/>
       <c r="K25" s="29"/>
       <c r="L25" s="29" t="s">
-        <v>2091</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="29" t="s">
-        <v>1890</v>
+        <v>1875</v>
       </c>
       <c r="B26" s="29">
         <v>2</v>
@@ -11406,7 +11406,7 @@
         <v>1585</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>1912</v>
+        <v>1897</v>
       </c>
       <c r="E26" s="29">
         <v>3</v>
@@ -11422,12 +11422,12 @@
         <v>0</v>
       </c>
       <c r="I26" s="29" t="s">
-        <v>1914</v>
+        <v>2121</v>
       </c>
       <c r="J26" s="29"/>
       <c r="K26" s="29"/>
       <c r="L26" s="29" t="s">
-        <v>2031</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -11457,10 +11457,10 @@
         <v>1</v>
       </c>
       <c r="I27" t="s">
-        <v>1824</v>
+        <v>2139</v>
       </c>
       <c r="L27" t="s">
-        <v>1955</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -11490,10 +11490,10 @@
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>1823</v>
+        <v>2136</v>
       </c>
       <c r="L28" t="s">
-        <v>1957</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -11523,10 +11523,10 @@
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>1828</v>
+        <v>2132</v>
       </c>
       <c r="L29" t="s">
-        <v>1960</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -11556,10 +11556,10 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>1831</v>
+        <v>2128</v>
       </c>
       <c r="L30" t="s">
-        <v>2021</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -11589,10 +11589,10 @@
         <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>1820</v>
+        <v>2135</v>
       </c>
       <c r="L31" t="s">
-        <v>2081</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -11622,10 +11622,10 @@
         <v>1</v>
       </c>
       <c r="I32" t="s">
-        <v>1826</v>
+        <v>2124</v>
       </c>
       <c r="L32" t="s">
-        <v>2010</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -11655,10 +11655,10 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>1822</v>
+        <v>2134</v>
       </c>
       <c r="L33" t="s">
-        <v>2129</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -11688,10 +11688,10 @@
         <v>1</v>
       </c>
       <c r="I34" t="s">
-        <v>1826</v>
+        <v>2124</v>
       </c>
       <c r="L34" t="s">
-        <v>1959</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -11721,10 +11721,10 @@
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>1828</v>
+        <v>2132</v>
       </c>
       <c r="L35" t="s">
-        <v>2007</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -11754,10 +11754,10 @@
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>1829</v>
+        <v>2126</v>
       </c>
       <c r="L36" t="s">
-        <v>2044</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -11787,10 +11787,10 @@
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>1830</v>
+        <v>2125</v>
       </c>
       <c r="L37" t="s">
-        <v>2047</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -11804,7 +11804,7 @@
         <v>85</v>
       </c>
       <c r="D38" t="s">
-        <v>2080</v>
+        <v>2061</v>
       </c>
       <c r="E38">
         <v>4</v>
@@ -11820,10 +11820,10 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>1833</v>
+        <v>2129</v>
       </c>
       <c r="L38" t="s">
-        <v>2079</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -11853,10 +11853,10 @@
         <v>1</v>
       </c>
       <c r="I39" t="s">
-        <v>1833</v>
+        <v>2129</v>
       </c>
       <c r="L39" t="s">
-        <v>2052</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -11886,10 +11886,10 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>1831</v>
+        <v>2128</v>
       </c>
       <c r="L40" t="s">
-        <v>2114</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -11919,10 +11919,10 @@
         <v>1</v>
       </c>
       <c r="I41" t="s">
-        <v>1833</v>
+        <v>2129</v>
       </c>
       <c r="L41" t="s">
-        <v>2116</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -11952,10 +11952,10 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>1831</v>
+        <v>2128</v>
       </c>
       <c r="L42" t="s">
-        <v>2125</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -11985,10 +11985,10 @@
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>1823</v>
+        <v>2136</v>
       </c>
       <c r="L43" t="s">
-        <v>2124</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -12018,12 +12018,12 @@
         <v>0</v>
       </c>
       <c r="I44" s="29" t="s">
-        <v>1828</v>
+        <v>2132</v>
       </c>
       <c r="J44" s="29"/>
       <c r="K44" s="29"/>
       <c r="L44" s="29" t="s">
-        <v>2054</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -12053,15 +12053,15 @@
         <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>1827</v>
+        <v>2137</v>
       </c>
       <c r="L45" t="s">
-        <v>2109</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="29" t="s">
-        <v>1906</v>
+        <v>1891</v>
       </c>
       <c r="B46" s="29">
         <v>3</v>
@@ -12070,7 +12070,7 @@
         <v>1603</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>1932</v>
+        <v>1913</v>
       </c>
       <c r="E46" s="29">
         <v>6</v>
@@ -12080,23 +12080,23 @@
         <v>12</v>
       </c>
       <c r="G46" s="29" t="s">
-        <v>2132</v>
+        <v>2113</v>
       </c>
       <c r="H46" s="29" t="b">
         <v>0</v>
       </c>
       <c r="I46" s="29" t="s">
-        <v>1916</v>
+        <v>2123</v>
       </c>
       <c r="J46" s="29"/>
       <c r="K46" s="29"/>
       <c r="L46" s="29" t="s">
-        <v>2126</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="29" t="s">
-        <v>1900</v>
+        <v>1885</v>
       </c>
       <c r="B47" s="29">
         <v>3</v>
@@ -12105,7 +12105,7 @@
         <v>1586</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>1919</v>
+        <v>1900</v>
       </c>
       <c r="E47" s="29">
         <v>6</v>
@@ -12121,17 +12121,17 @@
         <v>1</v>
       </c>
       <c r="I47" s="29" t="s">
-        <v>1915</v>
+        <v>2130</v>
       </c>
       <c r="J47" s="29"/>
       <c r="K47" s="29"/>
       <c r="L47" s="29" t="s">
-        <v>2025</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="29" t="s">
-        <v>1894</v>
+        <v>1879</v>
       </c>
       <c r="B48" s="29">
         <v>3</v>
@@ -12140,7 +12140,7 @@
         <v>1587</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>1920</v>
+        <v>1901</v>
       </c>
       <c r="E48" s="29">
         <v>5</v>
@@ -12156,17 +12156,17 @@
         <v>1</v>
       </c>
       <c r="I48" s="29" t="s">
-        <v>1915</v>
+        <v>2130</v>
       </c>
       <c r="J48" s="29"/>
       <c r="K48" s="29"/>
       <c r="L48" s="29" t="s">
-        <v>2009</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="29" t="s">
-        <v>1887</v>
+        <v>1872</v>
       </c>
       <c r="B49" s="29">
         <v>3</v>
@@ -12175,7 +12175,7 @@
         <v>1588</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>1921</v>
+        <v>1902</v>
       </c>
       <c r="E49" s="29">
         <v>5</v>
@@ -12191,12 +12191,12 @@
         <v>1</v>
       </c>
       <c r="I49" s="29" t="s">
-        <v>1914</v>
+        <v>2121</v>
       </c>
       <c r="J49" s="29"/>
       <c r="K49" s="29"/>
       <c r="L49" s="29" t="s">
-        <v>2045</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -12210,7 +12210,7 @@
         <v>112</v>
       </c>
       <c r="D50" t="s">
-        <v>1834</v>
+        <v>1819</v>
       </c>
       <c r="E50">
         <v>7</v>
@@ -12226,10 +12226,10 @@
         <v>0</v>
       </c>
       <c r="I50" t="s">
-        <v>1820</v>
+        <v>2135</v>
       </c>
       <c r="L50" t="s">
-        <v>2008</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -12240,10 +12240,10 @@
         <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>1835</v>
+        <v>1820</v>
       </c>
       <c r="D51" t="s">
-        <v>1951</v>
+        <v>1932</v>
       </c>
       <c r="E51">
         <v>5</v>
@@ -12259,10 +12259,10 @@
         <v>1</v>
       </c>
       <c r="I51" t="s">
-        <v>1821</v>
+        <v>2131</v>
       </c>
       <c r="L51" t="s">
-        <v>2068</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -12276,7 +12276,7 @@
         <v>149</v>
       </c>
       <c r="D52" t="s">
-        <v>1836</v>
+        <v>1821</v>
       </c>
       <c r="E52">
         <v>5</v>
@@ -12292,10 +12292,10 @@
         <v>0</v>
       </c>
       <c r="I52" t="s">
-        <v>1829</v>
+        <v>2126</v>
       </c>
       <c r="L52" t="s">
-        <v>2078</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -12325,10 +12325,10 @@
         <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>1830</v>
+        <v>2125</v>
       </c>
       <c r="L53" t="s">
-        <v>2117</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -12358,10 +12358,10 @@
         <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>1830</v>
+        <v>2125</v>
       </c>
       <c r="L54" t="s">
-        <v>2001</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -12391,10 +12391,10 @@
         <v>0</v>
       </c>
       <c r="I55" t="s">
-        <v>1819</v>
+        <v>2133</v>
       </c>
       <c r="L55" t="s">
-        <v>2000</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -12424,10 +12424,10 @@
         <v>0</v>
       </c>
       <c r="I56" t="s">
-        <v>1824</v>
+        <v>2139</v>
       </c>
       <c r="L56" t="s">
-        <v>2130</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -12457,10 +12457,10 @@
         <v>0</v>
       </c>
       <c r="I57" t="s">
-        <v>1820</v>
+        <v>2135</v>
       </c>
       <c r="L57" t="s">
-        <v>2062</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -12490,10 +12490,10 @@
         <v>1</v>
       </c>
       <c r="I58" t="s">
-        <v>1825</v>
+        <v>2138</v>
       </c>
       <c r="L58" t="s">
-        <v>2017</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -12523,10 +12523,10 @@
         <v>1</v>
       </c>
       <c r="I59" t="s">
-        <v>1832</v>
+        <v>2127</v>
       </c>
       <c r="L59" t="s">
-        <v>2023</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -12556,10 +12556,10 @@
         <v>0</v>
       </c>
       <c r="I60" t="s">
-        <v>1831</v>
+        <v>2128</v>
       </c>
       <c r="L60" t="s">
-        <v>2057</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -12570,7 +12570,7 @@
         <v>3</v>
       </c>
       <c r="C61" t="s">
-        <v>1845</v>
+        <v>1830</v>
       </c>
       <c r="D61" t="s">
         <v>104</v>
@@ -12589,10 +12589,10 @@
         <v>0</v>
       </c>
       <c r="I61" t="s">
-        <v>1831</v>
+        <v>2128</v>
       </c>
       <c r="L61" t="s">
-        <v>2072</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -12622,10 +12622,10 @@
         <v>1</v>
       </c>
       <c r="I62" t="s">
-        <v>1827</v>
+        <v>2137</v>
       </c>
       <c r="L62" t="s">
-        <v>2128</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -12655,10 +12655,10 @@
         <v>0</v>
       </c>
       <c r="I63" t="s">
-        <v>1828</v>
+        <v>2132</v>
       </c>
       <c r="L63" t="s">
-        <v>2029</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -12688,10 +12688,10 @@
         <v>1</v>
       </c>
       <c r="I64" t="s">
-        <v>1832</v>
+        <v>2127</v>
       </c>
       <c r="L64" t="s">
-        <v>2064</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -12721,10 +12721,10 @@
         <v>0</v>
       </c>
       <c r="I65" t="s">
-        <v>1825</v>
+        <v>2138</v>
       </c>
       <c r="L65" t="s">
-        <v>1990</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -12754,10 +12754,10 @@
         <v>0</v>
       </c>
       <c r="I66" t="s">
-        <v>1822</v>
+        <v>2134</v>
       </c>
       <c r="L66" t="s">
-        <v>1998</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -12787,10 +12787,10 @@
         <v>0</v>
       </c>
       <c r="I67" t="s">
-        <v>1826</v>
+        <v>2124</v>
       </c>
       <c r="L67" t="s">
-        <v>2012</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -12820,10 +12820,10 @@
         <v>0</v>
       </c>
       <c r="I68" t="s">
-        <v>1827</v>
+        <v>2137</v>
       </c>
       <c r="L68" t="s">
-        <v>2013</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -12853,10 +12853,10 @@
         <v>0</v>
       </c>
       <c r="I69" t="s">
-        <v>1829</v>
+        <v>2126</v>
       </c>
       <c r="L69" t="s">
-        <v>2076</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -12886,15 +12886,15 @@
         <v>0</v>
       </c>
       <c r="I70" t="s">
-        <v>1819</v>
+        <v>2133</v>
       </c>
       <c r="L70" t="s">
-        <v>2123</v>
+        <v>2104</v>
       </c>
     </row>
     <row r="71" spans="1:12">
       <c r="A71" s="29" t="s">
-        <v>1878</v>
+        <v>1863</v>
       </c>
       <c r="B71" s="29">
         <v>4</v>
@@ -12903,7 +12903,7 @@
         <v>1604</v>
       </c>
       <c r="D71" s="29" t="s">
-        <v>2133</v>
+        <v>2114</v>
       </c>
       <c r="E71" s="29">
         <v>8</v>
@@ -12913,18 +12913,18 @@
         <v>16</v>
       </c>
       <c r="G71" s="29" t="s">
-        <v>2132</v>
+        <v>2113</v>
       </c>
       <c r="H71" s="29" t="b">
         <v>1</v>
       </c>
       <c r="I71" s="29" t="s">
-        <v>1913</v>
+        <v>2122</v>
       </c>
       <c r="J71" s="29"/>
       <c r="K71" s="29"/>
       <c r="L71" s="29" t="s">
-        <v>2061</v>
+        <v>2042</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -12954,10 +12954,10 @@
         <v>0</v>
       </c>
       <c r="I72" t="s">
-        <v>1825</v>
+        <v>2138</v>
       </c>
       <c r="L72" t="s">
-        <v>2003</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="73" spans="1:12">
@@ -12987,10 +12987,10 @@
         <v>1</v>
       </c>
       <c r="I73" t="s">
-        <v>1819</v>
+        <v>2133</v>
       </c>
       <c r="L73" t="s">
-        <v>2026</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="74" spans="1:12">
@@ -13020,10 +13020,10 @@
         <v>1</v>
       </c>
       <c r="I74" t="s">
-        <v>1826</v>
+        <v>2124</v>
       </c>
       <c r="L74" t="s">
-        <v>2005</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="75" spans="1:12">
@@ -13053,10 +13053,10 @@
         <v>1</v>
       </c>
       <c r="I75" t="s">
-        <v>1827</v>
+        <v>2137</v>
       </c>
       <c r="L75" t="s">
-        <v>2038</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="76" spans="1:12">
@@ -13086,10 +13086,10 @@
         <v>0</v>
       </c>
       <c r="I76" t="s">
-        <v>1829</v>
+        <v>2126</v>
       </c>
       <c r="L76" t="s">
-        <v>2056</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="77" spans="1:12">
@@ -13119,10 +13119,10 @@
         <v>0</v>
       </c>
       <c r="I77" t="s">
-        <v>1830</v>
+        <v>2125</v>
       </c>
       <c r="L77" t="s">
-        <v>1997</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="78" spans="1:12">
@@ -13152,10 +13152,10 @@
         <v>0</v>
       </c>
       <c r="I78" t="s">
-        <v>1827</v>
+        <v>2137</v>
       </c>
       <c r="L78" t="s">
-        <v>2046</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="79" spans="1:12">
@@ -13185,10 +13185,10 @@
         <v>1</v>
       </c>
       <c r="I79" t="s">
-        <v>1822</v>
+        <v>2134</v>
       </c>
       <c r="L79" t="s">
-        <v>2112</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -13199,7 +13199,7 @@
         <v>4</v>
       </c>
       <c r="C80" t="s">
-        <v>1846</v>
+        <v>1831</v>
       </c>
       <c r="D80" t="s">
         <v>129</v>
@@ -13218,10 +13218,10 @@
         <v>1</v>
       </c>
       <c r="I80" t="s">
-        <v>1830</v>
+        <v>2125</v>
       </c>
       <c r="L80" t="s">
-        <v>2024</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="81" spans="1:12">
@@ -13251,10 +13251,10 @@
         <v>1</v>
       </c>
       <c r="I81" t="s">
-        <v>1830</v>
+        <v>2125</v>
       </c>
       <c r="L81" t="s">
-        <v>2042</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="82" spans="1:12">
@@ -13284,10 +13284,10 @@
         <v>1</v>
       </c>
       <c r="I82" t="s">
-        <v>1829</v>
+        <v>2126</v>
       </c>
       <c r="L82" t="s">
-        <v>2050</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="83" spans="1:12">
@@ -13298,10 +13298,10 @@
         <v>4</v>
       </c>
       <c r="C83" t="s">
-        <v>1838</v>
+        <v>1823</v>
       </c>
       <c r="D83" t="s">
-        <v>1839</v>
+        <v>1824</v>
       </c>
       <c r="E83">
         <v>8</v>
@@ -13317,10 +13317,10 @@
         <v>1</v>
       </c>
       <c r="I83" t="s">
-        <v>1825</v>
+        <v>2138</v>
       </c>
       <c r="L83" t="s">
-        <v>2115</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="84" spans="1:12">
@@ -13350,10 +13350,10 @@
         <v>1</v>
       </c>
       <c r="I84" t="s">
-        <v>1832</v>
+        <v>2127</v>
       </c>
       <c r="L84" t="s">
-        <v>2034</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="85" spans="1:12">
@@ -13383,10 +13383,10 @@
         <v>0</v>
       </c>
       <c r="I85" t="s">
-        <v>1828</v>
+        <v>2132</v>
       </c>
       <c r="L85" t="s">
-        <v>2058</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="86" spans="1:12">
@@ -13416,10 +13416,10 @@
         <v>0</v>
       </c>
       <c r="I86" t="s">
-        <v>1829</v>
+        <v>2126</v>
       </c>
       <c r="L86" t="s">
-        <v>2111</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="87" spans="1:12">
@@ -13449,10 +13449,10 @@
         <v>1</v>
       </c>
       <c r="I87" t="s">
-        <v>1826</v>
+        <v>2124</v>
       </c>
       <c r="L87" t="s">
-        <v>2014</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -13482,10 +13482,10 @@
         <v>1</v>
       </c>
       <c r="I88" t="s">
-        <v>1826</v>
+        <v>2124</v>
       </c>
       <c r="L88" t="s">
-        <v>2022</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="89" spans="1:12">
@@ -13515,10 +13515,10 @@
         <v>0</v>
       </c>
       <c r="I89" t="s">
-        <v>1833</v>
+        <v>2129</v>
       </c>
       <c r="L89" t="s">
-        <v>1961</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="90" spans="1:12">
@@ -13548,10 +13548,10 @@
         <v>0</v>
       </c>
       <c r="I90" t="s">
-        <v>1833</v>
+        <v>2129</v>
       </c>
       <c r="L90" t="s">
-        <v>2083</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="91" spans="1:12">
@@ -13581,13 +13581,13 @@
         <v>0</v>
       </c>
       <c r="I91" t="s">
-        <v>1823</v>
+        <v>2136</v>
       </c>
       <c r="K91" t="s">
-        <v>1840</v>
+        <v>1825</v>
       </c>
       <c r="L91" t="s">
-        <v>2088</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="92" spans="1:12">
@@ -13617,15 +13617,15 @@
         <v>0</v>
       </c>
       <c r="I92" t="s">
-        <v>1822</v>
+        <v>2134</v>
       </c>
       <c r="L92" t="s">
-        <v>2110</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="93" spans="1:12">
       <c r="A93" s="29" t="s">
-        <v>1875</v>
+        <v>1860</v>
       </c>
       <c r="B93" s="29">
         <v>5</v>
@@ -13634,7 +13634,7 @@
         <v>1605</v>
       </c>
       <c r="D93" s="29" t="s">
-        <v>1934</v>
+        <v>1915</v>
       </c>
       <c r="E93" s="29">
         <v>10</v>
@@ -13650,26 +13650,26 @@
         <v>1</v>
       </c>
       <c r="I93" s="29" t="s">
-        <v>1913</v>
+        <v>2122</v>
       </c>
       <c r="J93" s="29"/>
       <c r="K93" s="29"/>
       <c r="L93" s="29" t="s">
-        <v>2019</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="94" spans="1:12">
       <c r="A94" s="29" t="s">
-        <v>1896</v>
+        <v>1881</v>
       </c>
       <c r="B94" s="29">
         <v>5</v>
       </c>
       <c r="C94" s="29" t="s">
-        <v>1940</v>
+        <v>1921</v>
       </c>
       <c r="D94" s="29" t="s">
-        <v>1937</v>
+        <v>1918</v>
       </c>
       <c r="E94" s="29">
         <v>9</v>
@@ -13685,28 +13685,28 @@
         <v>1</v>
       </c>
       <c r="I94" s="29" t="s">
-        <v>1915</v>
+        <v>2130</v>
       </c>
       <c r="J94" s="29" t="s">
-        <v>2134</v>
+        <v>2115</v>
       </c>
       <c r="K94" s="29"/>
       <c r="L94" s="29" t="s">
-        <v>2104</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="95" spans="1:12">
       <c r="A95" s="29" t="s">
-        <v>1909</v>
+        <v>1894</v>
       </c>
       <c r="B95" s="29">
         <v>5</v>
       </c>
       <c r="C95" s="29" t="s">
-        <v>1938</v>
+        <v>1919</v>
       </c>
       <c r="D95" s="29" t="s">
-        <v>1937</v>
+        <v>1918</v>
       </c>
       <c r="E95" s="29">
         <v>9</v>
@@ -13722,28 +13722,28 @@
         <v>1</v>
       </c>
       <c r="I95" s="29" t="s">
-        <v>1916</v>
+        <v>2123</v>
       </c>
       <c r="J95" s="29" t="s">
-        <v>2135</v>
+        <v>2116</v>
       </c>
       <c r="K95" s="29"/>
       <c r="L95" s="29" t="s">
-        <v>2105</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="96" spans="1:12">
       <c r="A96" s="29" t="s">
-        <v>1899</v>
+        <v>1884</v>
       </c>
       <c r="B96" s="29">
         <v>5</v>
       </c>
       <c r="C96" s="29" t="s">
-        <v>1939</v>
+        <v>1920</v>
       </c>
       <c r="D96" s="29" t="s">
-        <v>1937</v>
+        <v>1918</v>
       </c>
       <c r="E96" s="29">
         <v>9</v>
@@ -13759,28 +13759,28 @@
         <v>1</v>
       </c>
       <c r="I96" s="29" t="s">
-        <v>1915</v>
+        <v>2130</v>
       </c>
       <c r="J96" s="29" t="s">
-        <v>2136</v>
+        <v>2117</v>
       </c>
       <c r="K96" s="29"/>
       <c r="L96" s="29" t="s">
-        <v>2107</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="97" spans="1:12">
       <c r="A97" s="29" t="s">
-        <v>1883</v>
+        <v>1868</v>
       </c>
       <c r="B97" s="29">
         <v>5</v>
       </c>
       <c r="C97" s="29" t="s">
-        <v>1936</v>
+        <v>1917</v>
       </c>
       <c r="D97" s="29" t="s">
-        <v>1937</v>
+        <v>1918</v>
       </c>
       <c r="E97" s="29">
         <v>9</v>
@@ -13796,28 +13796,28 @@
         <v>1</v>
       </c>
       <c r="I97" s="29" t="s">
-        <v>1914</v>
+        <v>2121</v>
       </c>
       <c r="J97" s="29" t="s">
-        <v>2137</v>
+        <v>2118</v>
       </c>
       <c r="K97" s="29"/>
       <c r="L97" s="29" t="s">
-        <v>2108</v>
+        <v>2089</v>
       </c>
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="29" t="s">
-        <v>1970</v>
+        <v>1951</v>
       </c>
       <c r="B98" s="29">
         <v>5</v>
       </c>
       <c r="C98" s="29" t="s">
-        <v>1942</v>
+        <v>1923</v>
       </c>
       <c r="D98" s="29" t="s">
-        <v>1937</v>
+        <v>1918</v>
       </c>
       <c r="E98" s="29">
         <v>9</v>
@@ -13833,28 +13833,28 @@
         <v>1</v>
       </c>
       <c r="I98" s="29" t="s">
-        <v>1820</v>
+        <v>2135</v>
       </c>
       <c r="J98" s="29" t="s">
-        <v>2138</v>
+        <v>2119</v>
       </c>
       <c r="K98" s="29"/>
       <c r="L98" s="29" t="s">
-        <v>2103</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="99" spans="1:12">
       <c r="A99" s="29" t="s">
-        <v>1911</v>
+        <v>1896</v>
       </c>
       <c r="B99" s="29">
         <v>5</v>
       </c>
       <c r="C99" s="29" t="s">
-        <v>1941</v>
+        <v>1922</v>
       </c>
       <c r="D99" s="29" t="s">
-        <v>1937</v>
+        <v>1918</v>
       </c>
       <c r="E99" s="29">
         <v>9</v>
@@ -13870,28 +13870,28 @@
         <v>1</v>
       </c>
       <c r="I99" s="29" t="s">
-        <v>1916</v>
+        <v>2123</v>
       </c>
       <c r="J99" s="29" t="s">
-        <v>2139</v>
+        <v>2120</v>
       </c>
       <c r="K99" s="29"/>
       <c r="L99" s="29" t="s">
-        <v>2106</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="100" spans="1:12">
       <c r="A100" s="29" t="s">
-        <v>1879</v>
+        <v>1864</v>
       </c>
       <c r="B100" s="29">
         <v>5</v>
       </c>
       <c r="C100" s="29" t="s">
-        <v>1922</v>
+        <v>1903</v>
       </c>
       <c r="D100" s="29" t="s">
-        <v>1923</v>
+        <v>1904</v>
       </c>
       <c r="E100" s="29">
         <v>10</v>
@@ -13907,17 +13907,17 @@
         <v>1</v>
       </c>
       <c r="I100" s="29" t="s">
-        <v>1913</v>
+        <v>2122</v>
       </c>
       <c r="J100" s="29"/>
       <c r="K100" s="29"/>
       <c r="L100" s="29" t="s">
-        <v>2030</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="101" spans="1:12">
       <c r="A101" s="29" t="s">
-        <v>1876</v>
+        <v>1861</v>
       </c>
       <c r="B101" s="29">
         <v>5</v>
@@ -13926,7 +13926,7 @@
         <v>1591</v>
       </c>
       <c r="D101" s="29" t="s">
-        <v>1924</v>
+        <v>1905</v>
       </c>
       <c r="E101" s="29">
         <v>9</v>
@@ -13942,12 +13942,12 @@
         <v>1</v>
       </c>
       <c r="I101" s="29" t="s">
-        <v>1913</v>
+        <v>2122</v>
       </c>
       <c r="J101" s="29"/>
       <c r="K101" s="29"/>
       <c r="L101" s="29" t="s">
-        <v>2028</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="102" spans="1:12">
@@ -13961,7 +13961,7 @@
         <v>604</v>
       </c>
       <c r="D102" t="s">
-        <v>1837</v>
+        <v>1822</v>
       </c>
       <c r="E102">
         <v>10</v>
@@ -13977,10 +13977,10 @@
         <v>0</v>
       </c>
       <c r="I102" t="s">
-        <v>1826</v>
+        <v>2124</v>
       </c>
       <c r="L102" t="s">
-        <v>2120</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="103" spans="1:12">
@@ -14010,10 +14010,10 @@
         <v>1</v>
       </c>
       <c r="I103" t="s">
-        <v>1827</v>
+        <v>2137</v>
       </c>
       <c r="L103" t="s">
-        <v>1995</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="104" spans="1:12">
@@ -14043,10 +14043,10 @@
         <v>1</v>
       </c>
       <c r="I104" t="s">
-        <v>1825</v>
+        <v>2138</v>
       </c>
       <c r="L104" t="s">
-        <v>1996</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="105" spans="1:12">
@@ -14076,10 +14076,10 @@
         <v>1</v>
       </c>
       <c r="I105" t="s">
-        <v>1832</v>
+        <v>2127</v>
       </c>
       <c r="L105" t="s">
-        <v>2082</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="106" spans="1:12">
@@ -14109,10 +14109,10 @@
         <v>1</v>
       </c>
       <c r="I106" t="s">
-        <v>1819</v>
+        <v>2133</v>
       </c>
       <c r="L106" t="s">
-        <v>2086</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="107" spans="1:12">
@@ -14123,7 +14123,7 @@
         <v>5</v>
       </c>
       <c r="C107" t="s">
-        <v>1847</v>
+        <v>1832</v>
       </c>
       <c r="D107" t="s">
         <v>224</v>
@@ -14142,13 +14142,13 @@
         <v>1</v>
       </c>
       <c r="I107" t="s">
-        <v>1819</v>
+        <v>2133</v>
       </c>
       <c r="J107" t="s">
-        <v>1848</v>
+        <v>1833</v>
       </c>
       <c r="L107" t="s">
-        <v>2093</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="108" spans="1:12">
@@ -14159,7 +14159,7 @@
         <v>5</v>
       </c>
       <c r="C108" t="s">
-        <v>1862</v>
+        <v>1847</v>
       </c>
       <c r="D108" t="s">
         <v>224</v>
@@ -14178,13 +14178,13 @@
         <v>1</v>
       </c>
       <c r="I108" t="s">
-        <v>1830</v>
+        <v>2125</v>
       </c>
       <c r="J108" t="s">
-        <v>1861</v>
+        <v>1846</v>
       </c>
       <c r="L108" t="s">
-        <v>2094</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="109" spans="1:12">
@@ -14195,7 +14195,7 @@
         <v>5</v>
       </c>
       <c r="C109" t="s">
-        <v>1851</v>
+        <v>1836</v>
       </c>
       <c r="D109" t="s">
         <v>224</v>
@@ -14214,13 +14214,13 @@
         <v>1</v>
       </c>
       <c r="I109" t="s">
-        <v>1831</v>
+        <v>2128</v>
       </c>
       <c r="J109" t="s">
-        <v>1852</v>
+        <v>1837</v>
       </c>
       <c r="L109" t="s">
-        <v>2095</v>
+        <v>2076</v>
       </c>
     </row>
     <row r="110" spans="1:12">
@@ -14231,7 +14231,7 @@
         <v>5</v>
       </c>
       <c r="C110" t="s">
-        <v>1849</v>
+        <v>1834</v>
       </c>
       <c r="D110" t="s">
         <v>224</v>
@@ -14250,13 +14250,13 @@
         <v>1</v>
       </c>
       <c r="I110" t="s">
-        <v>1823</v>
+        <v>2136</v>
       </c>
       <c r="J110" t="s">
-        <v>1850</v>
+        <v>1835</v>
       </c>
       <c r="L110" t="s">
-        <v>2096</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="111" spans="1:12">
@@ -14267,7 +14267,7 @@
         <v>5</v>
       </c>
       <c r="C111" t="s">
-        <v>1853</v>
+        <v>1838</v>
       </c>
       <c r="D111" t="s">
         <v>224</v>
@@ -14286,13 +14286,13 @@
         <v>1</v>
       </c>
       <c r="I111" t="s">
-        <v>1831</v>
+        <v>2128</v>
       </c>
       <c r="J111" t="s">
-        <v>1854</v>
+        <v>1839</v>
       </c>
       <c r="L111" t="s">
-        <v>2097</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="112" spans="1:12">
@@ -14303,7 +14303,7 @@
         <v>5</v>
       </c>
       <c r="C112" t="s">
-        <v>1857</v>
+        <v>1842</v>
       </c>
       <c r="D112" t="s">
         <v>224</v>
@@ -14322,13 +14322,13 @@
         <v>1</v>
       </c>
       <c r="I112" t="s">
-        <v>1825</v>
+        <v>2138</v>
       </c>
       <c r="J112" t="s">
-        <v>1858</v>
+        <v>1843</v>
       </c>
       <c r="L112" t="s">
-        <v>2098</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="113" spans="1:12">
@@ -14339,7 +14339,7 @@
         <v>5</v>
       </c>
       <c r="C113" t="s">
-        <v>1855</v>
+        <v>1840</v>
       </c>
       <c r="D113" t="s">
         <v>224</v>
@@ -14358,13 +14358,13 @@
         <v>1</v>
       </c>
       <c r="I113" t="s">
-        <v>1828</v>
+        <v>2132</v>
       </c>
       <c r="J113" t="s">
-        <v>1856</v>
+        <v>1841</v>
       </c>
       <c r="L113" t="s">
-        <v>2099</v>
+        <v>2080</v>
       </c>
     </row>
     <row r="114" spans="1:12">
@@ -14375,7 +14375,7 @@
         <v>5</v>
       </c>
       <c r="C114" t="s">
-        <v>1859</v>
+        <v>1844</v>
       </c>
       <c r="D114" t="s">
         <v>224</v>
@@ -14394,13 +14394,13 @@
         <v>1</v>
       </c>
       <c r="I114" t="s">
-        <v>1832</v>
+        <v>2127</v>
       </c>
       <c r="J114" t="s">
-        <v>1860</v>
+        <v>1845</v>
       </c>
       <c r="L114" t="s">
-        <v>2100</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="115" spans="1:12">
@@ -14411,7 +14411,7 @@
         <v>5</v>
       </c>
       <c r="C115" t="s">
-        <v>1863</v>
+        <v>1848</v>
       </c>
       <c r="D115" t="s">
         <v>225</v>
@@ -14430,10 +14430,10 @@
         <v>1</v>
       </c>
       <c r="I115" t="s">
-        <v>1819</v>
+        <v>2133</v>
       </c>
       <c r="L115" t="s">
-        <v>2073</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="116" spans="1:12">
@@ -14444,10 +14444,10 @@
         <v>5</v>
       </c>
       <c r="C116" t="s">
-        <v>1864</v>
+        <v>1849</v>
       </c>
       <c r="D116" t="s">
-        <v>1952</v>
+        <v>1933</v>
       </c>
       <c r="E116">
         <v>9</v>
@@ -14463,10 +14463,10 @@
         <v>1</v>
       </c>
       <c r="I116" t="s">
-        <v>1821</v>
+        <v>2131</v>
       </c>
       <c r="L116" t="s">
-        <v>2065</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="117" spans="1:12">
@@ -14477,7 +14477,7 @@
         <v>5</v>
       </c>
       <c r="C117" t="s">
-        <v>1865</v>
+        <v>1850</v>
       </c>
       <c r="D117" t="s">
         <v>231</v>
@@ -14496,10 +14496,10 @@
         <v>1</v>
       </c>
       <c r="I117" t="s">
-        <v>1821</v>
+        <v>2131</v>
       </c>
       <c r="L117" t="s">
-        <v>2063</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="118" spans="1:12">
@@ -14529,10 +14529,10 @@
         <v>1</v>
       </c>
       <c r="I118" t="s">
-        <v>1833</v>
+        <v>2129</v>
       </c>
       <c r="L118" t="s">
-        <v>2060</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="119" spans="1:12">
@@ -14562,10 +14562,10 @@
         <v>1</v>
       </c>
       <c r="I119" t="s">
-        <v>1828</v>
+        <v>2132</v>
       </c>
       <c r="L119" t="s">
-        <v>2051</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="120" spans="1:12">
@@ -14595,10 +14595,10 @@
         <v>0</v>
       </c>
       <c r="I120" t="s">
-        <v>1832</v>
+        <v>2127</v>
       </c>
       <c r="L120" t="s">
-        <v>1963</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="121" spans="1:12">
@@ -14628,15 +14628,15 @@
         <v>0</v>
       </c>
       <c r="I121" t="s">
-        <v>1820</v>
+        <v>2135</v>
       </c>
       <c r="L121" t="s">
-        <v>2119</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="122" spans="1:12">
       <c r="A122" s="29" t="s">
-        <v>1910</v>
+        <v>1895</v>
       </c>
       <c r="B122" s="29">
         <v>6</v>
@@ -14645,7 +14645,7 @@
         <v>1607</v>
       </c>
       <c r="D122" s="29" t="s">
-        <v>1943</v>
+        <v>1924</v>
       </c>
       <c r="E122" s="29">
         <v>12</v>
@@ -14661,17 +14661,17 @@
         <v>0</v>
       </c>
       <c r="I122" s="29" t="s">
-        <v>1916</v>
+        <v>2123</v>
       </c>
       <c r="J122" s="29"/>
       <c r="K122" s="29"/>
       <c r="L122" s="29" t="s">
-        <v>1962</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="123" spans="1:12">
       <c r="A123" s="29" t="s">
-        <v>1901</v>
+        <v>1886</v>
       </c>
       <c r="B123" s="29">
         <v>6</v>
@@ -14680,7 +14680,7 @@
         <v>1608</v>
       </c>
       <c r="D123" s="29" t="s">
-        <v>1944</v>
+        <v>1925</v>
       </c>
       <c r="E123" s="29">
         <v>14</v>
@@ -14696,12 +14696,12 @@
         <v>0</v>
       </c>
       <c r="I123" s="29" t="s">
-        <v>1915</v>
+        <v>2130</v>
       </c>
       <c r="J123" s="29"/>
       <c r="K123" s="29"/>
       <c r="L123" s="29" t="s">
-        <v>2071</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="124" spans="1:12">
@@ -14731,10 +14731,10 @@
         <v>0</v>
       </c>
       <c r="I124" t="s">
-        <v>1833</v>
+        <v>2129</v>
       </c>
       <c r="L124" t="s">
-        <v>2037</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="125" spans="1:12">
@@ -14764,10 +14764,10 @@
         <v>0</v>
       </c>
       <c r="I125" t="s">
-        <v>1832</v>
+        <v>2127</v>
       </c>
       <c r="L125" t="s">
-        <v>2127</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="126" spans="1:12">
@@ -14797,10 +14797,10 @@
         <v>1</v>
       </c>
       <c r="I126" t="s">
-        <v>1832</v>
+        <v>2127</v>
       </c>
       <c r="L126" t="s">
-        <v>2016</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="127" spans="1:12">
@@ -14811,10 +14811,10 @@
         <v>6</v>
       </c>
       <c r="C127" t="s">
-        <v>1869</v>
+        <v>1854</v>
       </c>
       <c r="D127" t="s">
-        <v>1868</v>
+        <v>1853</v>
       </c>
       <c r="E127">
         <v>12</v>
@@ -14830,13 +14830,13 @@
         <v>1</v>
       </c>
       <c r="I127" t="s">
-        <v>1829</v>
+        <v>2126</v>
       </c>
       <c r="J127" t="s">
         <v>255</v>
       </c>
       <c r="L127" t="s">
-        <v>2092</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="128" spans="1:12">
@@ -14866,10 +14866,10 @@
         <v>1</v>
       </c>
       <c r="I128" t="s">
-        <v>1819</v>
+        <v>2133</v>
       </c>
       <c r="L128" t="s">
-        <v>2032</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="129" spans="1:12">
@@ -14899,10 +14899,10 @@
         <v>1</v>
       </c>
       <c r="I129" t="s">
-        <v>1823</v>
+        <v>2136</v>
       </c>
       <c r="L129" t="s">
-        <v>2118</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="130" spans="1:12">
@@ -14913,7 +14913,7 @@
         <v>6</v>
       </c>
       <c r="C130" t="s">
-        <v>1866</v>
+        <v>1851</v>
       </c>
       <c r="D130" t="s">
         <v>243</v>
@@ -14932,10 +14932,10 @@
         <v>1</v>
       </c>
       <c r="I130" t="s">
-        <v>1824</v>
+        <v>2139</v>
       </c>
       <c r="L130" t="s">
-        <v>2069</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="131" spans="1:12">
@@ -14946,7 +14946,7 @@
         <v>6</v>
       </c>
       <c r="C131" t="s">
-        <v>1867</v>
+        <v>1852</v>
       </c>
       <c r="D131" t="s">
         <v>248</v>
@@ -14965,10 +14965,10 @@
         <v>0</v>
       </c>
       <c r="I131" t="s">
-        <v>1827</v>
+        <v>2137</v>
       </c>
       <c r="L131" t="s">
-        <v>2070</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="132" spans="1:12">
@@ -14998,10 +14998,10 @@
         <v>1</v>
       </c>
       <c r="I132" t="s">
-        <v>1827</v>
+        <v>2137</v>
       </c>
       <c r="L132" t="s">
-        <v>2041</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="133" spans="1:12">
@@ -15031,10 +15031,10 @@
         <v>0</v>
       </c>
       <c r="I133" t="s">
-        <v>1826</v>
+        <v>2124</v>
       </c>
       <c r="L133" t="s">
-        <v>2004</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="134" spans="1:12">
@@ -15064,15 +15064,15 @@
         <v>1</v>
       </c>
       <c r="I134" t="s">
-        <v>1822</v>
+        <v>2134</v>
       </c>
       <c r="L134" t="s">
-        <v>1994</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="135" spans="1:12">
       <c r="A135" s="29" t="s">
-        <v>1898</v>
+        <v>1883</v>
       </c>
       <c r="B135">
         <v>7</v>
@@ -15097,10 +15097,10 @@
         <v>0</v>
       </c>
       <c r="I135" t="s">
-        <v>1915</v>
+        <v>2130</v>
       </c>
       <c r="L135" t="s">
-        <v>2036</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="136" spans="1:12">
@@ -15130,10 +15130,10 @@
         <v>1</v>
       </c>
       <c r="I136" t="s">
-        <v>1833</v>
+        <v>2129</v>
       </c>
       <c r="L136" t="s">
-        <v>2039</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="137" spans="1:12">
@@ -15163,10 +15163,10 @@
         <v>0</v>
       </c>
       <c r="I137" t="s">
-        <v>1831</v>
+        <v>2128</v>
       </c>
       <c r="L137" t="s">
-        <v>2053</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="138" spans="1:12">
@@ -15196,10 +15196,10 @@
         <v>0</v>
       </c>
       <c r="I138" t="s">
-        <v>1828</v>
+        <v>2132</v>
       </c>
       <c r="L138" t="s">
-        <v>2055</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="139" spans="1:12">
@@ -15229,10 +15229,10 @@
         <v>0</v>
       </c>
       <c r="I139" t="s">
-        <v>1831</v>
+        <v>2128</v>
       </c>
       <c r="L139" t="s">
-        <v>2035</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="140" spans="1:12">
@@ -15262,10 +15262,10 @@
         <v>1</v>
       </c>
       <c r="I140" t="s">
-        <v>1825</v>
+        <v>2138</v>
       </c>
       <c r="L140" t="s">
-        <v>2102</v>
+        <v>2083</v>
       </c>
     </row>
     <row r="141" spans="1:12">
@@ -15276,10 +15276,10 @@
         <v>7</v>
       </c>
       <c r="C141" t="s">
-        <v>1870</v>
+        <v>1855</v>
       </c>
       <c r="D141" t="s">
-        <v>1933</v>
+        <v>1914</v>
       </c>
       <c r="E141">
         <v>13</v>
@@ -15295,10 +15295,10 @@
         <v>1</v>
       </c>
       <c r="I141" t="s">
-        <v>1828</v>
+        <v>2132</v>
       </c>
       <c r="L141" t="s">
-        <v>2075</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="142" spans="1:12">
@@ -15328,10 +15328,10 @@
         <v>0</v>
       </c>
       <c r="I142" t="s">
-        <v>1824</v>
+        <v>2139</v>
       </c>
       <c r="L142" t="s">
-        <v>2048</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="143" spans="1:12">
@@ -15361,10 +15361,10 @@
         <v>1</v>
       </c>
       <c r="I143" t="s">
-        <v>1820</v>
+        <v>2135</v>
       </c>
       <c r="L143" t="s">
-        <v>2066</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="144" spans="1:12">
@@ -15394,15 +15394,15 @@
         <v>0</v>
       </c>
       <c r="I144" t="s">
-        <v>1832</v>
+        <v>2127</v>
       </c>
       <c r="L144" t="s">
-        <v>2043</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="145" spans="1:12">
       <c r="A145" s="29" t="s">
-        <v>1871</v>
+        <v>1856</v>
       </c>
       <c r="B145">
         <v>8</v>
@@ -15411,7 +15411,7 @@
         <v>1593</v>
       </c>
       <c r="D145" t="s">
-        <v>1925</v>
+        <v>1906</v>
       </c>
       <c r="E145">
         <v>15</v>
@@ -15427,15 +15427,15 @@
         <v>0</v>
       </c>
       <c r="I145" t="s">
-        <v>1913</v>
+        <v>2122</v>
       </c>
       <c r="L145" t="s">
-        <v>2020</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="146" spans="1:12">
       <c r="A146" s="29" t="s">
-        <v>1880</v>
+        <v>1865</v>
       </c>
       <c r="B146" s="29">
         <v>9</v>
@@ -15444,7 +15444,7 @@
         <v>1594</v>
       </c>
       <c r="D146" s="29" t="s">
-        <v>1926</v>
+        <v>1907</v>
       </c>
       <c r="E146" s="29">
         <v>18</v>
@@ -15460,17 +15460,17 @@
         <v>0</v>
       </c>
       <c r="I146" s="29" t="s">
-        <v>1913</v>
+        <v>2122</v>
       </c>
       <c r="J146" s="29"/>
       <c r="K146" s="29"/>
       <c r="L146" s="29" t="s">
-        <v>2059</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="147" spans="1:12">
       <c r="A147" s="29" t="s">
-        <v>1908</v>
+        <v>1893</v>
       </c>
       <c r="B147" s="29">
         <v>9</v>
@@ -15479,7 +15479,7 @@
         <v>1595</v>
       </c>
       <c r="D147" s="29" t="s">
-        <v>1927</v>
+        <v>1908</v>
       </c>
       <c r="E147" s="29">
         <v>18</v>
@@ -15495,12 +15495,12 @@
         <v>0</v>
       </c>
       <c r="I147" s="29" t="s">
-        <v>1916</v>
+        <v>2123</v>
       </c>
       <c r="J147" s="29"/>
       <c r="K147" s="29"/>
       <c r="L147" s="29" t="s">
-        <v>1964</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="148" spans="1:12">
@@ -15530,10 +15530,10 @@
         <v>0</v>
       </c>
       <c r="I148" t="s">
-        <v>1830</v>
+        <v>2125</v>
       </c>
       <c r="L148" t="s">
-        <v>2101</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="149" spans="1:12">
@@ -15563,15 +15563,15 @@
         <v>0</v>
       </c>
       <c r="I149" t="s">
-        <v>1829</v>
+        <v>2126</v>
       </c>
       <c r="L149" t="s">
-        <v>1954</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="150" spans="1:12">
       <c r="A150" s="29" t="s">
-        <v>1907</v>
+        <v>1892</v>
       </c>
       <c r="B150" s="29">
         <v>10</v>
@@ -15580,7 +15580,7 @@
         <v>1596</v>
       </c>
       <c r="D150" s="29" t="s">
-        <v>1928</v>
+        <v>1909</v>
       </c>
       <c r="E150" s="29">
         <v>20</v>
@@ -15596,17 +15596,17 @@
         <v>1</v>
       </c>
       <c r="I150" s="29" t="s">
-        <v>1916</v>
+        <v>2123</v>
       </c>
       <c r="J150" s="29"/>
       <c r="K150" s="29"/>
       <c r="L150" s="29" t="s">
-        <v>2011</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="151" spans="1:12">
       <c r="A151" s="29" t="s">
-        <v>1897</v>
+        <v>1882</v>
       </c>
       <c r="B151" s="29">
         <v>10</v>
@@ -15615,7 +15615,7 @@
         <v>1597</v>
       </c>
       <c r="D151" s="29" t="s">
-        <v>1948</v>
+        <v>1929</v>
       </c>
       <c r="E151" s="29">
         <v>20</v>
@@ -15631,12 +15631,12 @@
         <v>0</v>
       </c>
       <c r="I151" s="29" t="s">
-        <v>1915</v>
+        <v>2130</v>
       </c>
       <c r="J151" s="29"/>
       <c r="K151" s="29"/>
       <c r="L151" s="29" t="s">
-        <v>2049</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="152" spans="1:12">
@@ -15666,15 +15666,15 @@
         <v>0</v>
       </c>
       <c r="I152" t="s">
-        <v>1833</v>
+        <v>2129</v>
       </c>
       <c r="L152" t="s">
-        <v>2040</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="153" spans="1:12">
       <c r="A153" s="29" t="s">
-        <v>1873</v>
+        <v>1858</v>
       </c>
       <c r="B153" s="36" t="s">
         <v>1399</v>
@@ -15683,7 +15683,7 @@
         <v>1609</v>
       </c>
       <c r="D153" s="29" t="s">
-        <v>1945</v>
+        <v>1926</v>
       </c>
       <c r="E153" s="29">
         <v>20</v>
@@ -15699,12 +15699,12 @@
         <v>0</v>
       </c>
       <c r="I153" s="29" t="s">
-        <v>1913</v>
+        <v>2122</v>
       </c>
       <c r="J153" s="29"/>
       <c r="K153" s="29"/>
       <c r="L153" s="29" t="s">
-        <v>1999</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="154" spans="1:12">
@@ -15734,101 +15734,101 @@
         <v>1</v>
       </c>
       <c r="I154" t="s">
-        <v>1831</v>
+        <v>2128</v>
       </c>
       <c r="L154" t="s">
-        <v>1988</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="155" spans="1:12">
       <c r="A155" s="29" t="s">
-        <v>1881</v>
+        <v>1866</v>
       </c>
       <c r="I155" t="s">
-        <v>1914</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="156" spans="1:12">
       <c r="A156" s="29" t="s">
-        <v>1885</v>
+        <v>1870</v>
       </c>
       <c r="I156" t="s">
-        <v>1914</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="157" spans="1:12">
       <c r="A157" t="s">
-        <v>1965</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="158" spans="1:12">
       <c r="A158" t="s">
-        <v>1966</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="159" spans="1:12">
       <c r="A159" t="s">
-        <v>1967</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="160" spans="1:12">
       <c r="A160" t="s">
-        <v>1968</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="161" spans="1:9">
       <c r="A161" t="s">
-        <v>1969</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="162" spans="1:9">
       <c r="A162" t="s">
-        <v>1972</v>
+        <v>1953</v>
       </c>
     </row>
     <row r="163" spans="1:9">
       <c r="A163" t="s">
-        <v>1973</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="164" spans="1:9">
       <c r="A164" t="s">
-        <v>1974</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="165" spans="1:9">
       <c r="A165" t="s">
-        <v>1975</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="166" spans="1:9">
       <c r="A166" t="s">
-        <v>1976</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="167" spans="1:9">
       <c r="A167" t="s">
-        <v>1977</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="168" spans="1:9">
       <c r="A168" t="s">
-        <v>1971</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="169" spans="1:9">
       <c r="A169" t="s">
-        <v>1978</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="170" spans="1:9">
       <c r="A170" t="s">
-        <v>1979</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="171" spans="1:9">
       <c r="A171" t="s">
-        <v>1980</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="172" spans="1:9">
@@ -15836,31 +15836,31 @@
         <v>1722</v>
       </c>
       <c r="I172" t="s">
-        <v>1824</v>
+        <v>2139</v>
       </c>
     </row>
     <row r="173" spans="1:9">
       <c r="A173" t="s">
-        <v>1981</v>
+        <v>1962</v>
       </c>
       <c r="I173" t="s">
-        <v>1824</v>
+        <v>2139</v>
       </c>
     </row>
     <row r="174" spans="1:9">
       <c r="A174" t="s">
-        <v>1983</v>
+        <v>1964</v>
       </c>
       <c r="I174" t="s">
-        <v>1824</v>
+        <v>2139</v>
       </c>
     </row>
     <row r="175" spans="1:9">
       <c r="A175" t="s">
-        <v>1982</v>
+        <v>1963</v>
       </c>
       <c r="I175" t="s">
-        <v>1824</v>
+        <v>2139</v>
       </c>
     </row>
     <row r="176" spans="1:9">
@@ -15868,22 +15868,22 @@
         <v>1724</v>
       </c>
       <c r="I176" t="s">
-        <v>1824</v>
+        <v>2139</v>
       </c>
     </row>
     <row r="177" spans="1:9">
       <c r="A177" t="s">
-        <v>1984</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="178" spans="1:9">
       <c r="A178" t="s">
-        <v>1985</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="179" spans="1:9">
       <c r="A179" t="s">
-        <v>1986</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="180" spans="1:9">
@@ -15891,7 +15891,7 @@
         <v>1776</v>
       </c>
       <c r="I180" t="s">
-        <v>1830</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="181" spans="1:9">
@@ -15899,87 +15899,87 @@
         <v>1808</v>
       </c>
       <c r="I181" t="s">
-        <v>1833</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="182" spans="1:9">
       <c r="A182" s="30" t="s">
-        <v>1877</v>
+        <v>1862</v>
       </c>
       <c r="I182" t="s">
-        <v>1913</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="183" spans="1:9">
       <c r="A183" t="s">
-        <v>1882</v>
+        <v>1867</v>
       </c>
       <c r="I183" t="s">
-        <v>1914</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="184" spans="1:9">
       <c r="A184" t="s">
-        <v>1884</v>
+        <v>1869</v>
       </c>
       <c r="I184" t="s">
-        <v>1914</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="185" spans="1:9">
       <c r="A185" t="s">
-        <v>1888</v>
+        <v>1873</v>
       </c>
       <c r="I185" t="s">
-        <v>1914</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="186" spans="1:9">
       <c r="A186" t="s">
-        <v>1892</v>
+        <v>1877</v>
       </c>
       <c r="I186" t="s">
-        <v>1915</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="187" spans="1:9">
       <c r="A187" t="s">
-        <v>1893</v>
+        <v>1878</v>
       </c>
       <c r="I187" t="s">
-        <v>1915</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="188" spans="1:9">
       <c r="A188" t="s">
-        <v>1895</v>
+        <v>1880</v>
       </c>
       <c r="I188" t="s">
-        <v>1915</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="189" spans="1:9">
       <c r="A189" t="s">
-        <v>1903</v>
+        <v>1888</v>
       </c>
       <c r="I189" t="s">
-        <v>1916</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="190" spans="1:9">
       <c r="A190" t="s">
-        <v>1904</v>
+        <v>1889</v>
       </c>
       <c r="I190" t="s">
-        <v>1916</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="191" spans="1:9">
       <c r="A191" t="s">
-        <v>1905</v>
+        <v>1890</v>
       </c>
       <c r="I191" t="s">
-        <v>1916</v>
+        <v>2123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Righteous Wrath of the Faithful
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65FDBBA-CA9E-4C2D-A498-22E6061E759D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1773B8-280B-4B81-BDC5-4ED26B15C251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -10524,7 +10524,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G90" sqref="G90"/>
+      <selection pane="bottomLeft" activeCell="L90" sqref="A90:L90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -13541,32 +13541,34 @@
       <c r="A90" s="29" t="s">
         <v>1809</v>
       </c>
-      <c r="B90">
+      <c r="B90" s="29">
         <v>5</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="29" t="s">
         <v>1105</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90" s="29" t="s">
         <v>1408</v>
       </c>
-      <c r="E90">
+      <c r="E90" s="29">
         <v>9</v>
       </c>
-      <c r="F90">
+      <c r="F90" s="29">
         <f>E90*2</f>
         <v>18</v>
       </c>
       <c r="G90" s="29" t="s">
         <v>2113</v>
       </c>
-      <c r="H90" t="b">
-        <v>0</v>
-      </c>
-      <c r="I90" t="s">
+      <c r="H90" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="I90" s="29" t="s">
         <v>2129</v>
       </c>
-      <c r="L90" t="s">
+      <c r="J90" s="29"/>
+      <c r="K90" s="29"/>
+      <c r="L90" s="29" t="s">
         <v>2064</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Impervious Sanctity of Mind
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF62139-7AC5-473F-A6DB-E9F08CA14BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3F4638-9337-46CD-8061-B0DB645D4249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -10523,8 +10523,8 @@
   <dimension ref="A1:M191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C126" sqref="C126"/>
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L136" sqref="A136:L136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -15132,32 +15132,34 @@
       <c r="A136" s="29" t="s">
         <v>1803</v>
       </c>
-      <c r="B136">
+      <c r="B136" s="29">
         <v>7</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C136" s="29" t="s">
         <v>1155</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D136" s="29" t="s">
         <v>1408</v>
       </c>
-      <c r="E136">
+      <c r="E136" s="29">
         <v>10</v>
       </c>
-      <c r="F136">
+      <c r="F136" s="29">
         <f>E136*2</f>
         <v>20</v>
       </c>
-      <c r="G136" t="s">
+      <c r="G136" s="29" t="s">
         <v>1681</v>
       </c>
-      <c r="H136" t="b">
-        <v>1</v>
-      </c>
-      <c r="I136" t="s">
+      <c r="H136" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I136" s="29" t="s">
         <v>2129</v>
       </c>
-      <c r="L136" t="s">
+      <c r="J136" s="29"/>
+      <c r="K136" s="29"/>
+      <c r="L136" s="29" t="s">
         <v>2020</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Greater Shield of Lathander
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3F4638-9337-46CD-8061-B0DB645D4249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A828709D-EFF8-45D6-B573-C541CB00F637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -10523,8 +10523,8 @@
   <dimension ref="A1:M191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L136" sqref="A136:L136"/>
+      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I157" sqref="I157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -15099,32 +15099,34 @@
       <c r="A135" s="29" t="s">
         <v>1883</v>
       </c>
-      <c r="B135">
+      <c r="B135" s="29">
         <v>7</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C135" s="29" t="s">
         <v>1157</v>
       </c>
-      <c r="D135" t="s">
+      <c r="D135" s="29" t="s">
         <v>1408</v>
       </c>
-      <c r="E135">
+      <c r="E135" s="29">
         <v>14</v>
       </c>
-      <c r="F135">
+      <c r="F135" s="29">
         <f>E135*2</f>
         <v>28</v>
       </c>
-      <c r="G135" t="s">
+      <c r="G135" s="29" t="s">
         <v>1681</v>
       </c>
-      <c r="H135" t="b">
-        <v>0</v>
-      </c>
-      <c r="I135" t="s">
+      <c r="H135" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="I135" s="29" t="s">
         <v>2130</v>
       </c>
-      <c r="L135" t="s">
+      <c r="J135" s="29"/>
+      <c r="K135" s="29"/>
+      <c r="L135" s="29" t="s">
         <v>2017</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Populate missing Description icons
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A828709D-EFF8-45D6-B573-C541CB00F637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEF2670-910C-4C67-9E55-17AE3569B3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11505" uniqueCount="2140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11523" uniqueCount="2140">
   <si>
     <t>Caster Level</t>
   </si>
@@ -10523,8 +10523,8 @@
   <dimension ref="A1:M191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I157" sqref="I157"/>
+      <pane ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I180" sqref="I180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -15789,76 +15789,121 @@
       <c r="A157" t="s">
         <v>1946</v>
       </c>
+      <c r="I157" t="s">
+        <v>2133</v>
+      </c>
     </row>
     <row r="158" spans="1:12">
       <c r="A158" t="s">
         <v>1947</v>
       </c>
+      <c r="I158" t="s">
+        <v>2133</v>
+      </c>
     </row>
     <row r="159" spans="1:12">
       <c r="A159" t="s">
         <v>1948</v>
       </c>
+      <c r="I159" t="s">
+        <v>2135</v>
+      </c>
     </row>
     <row r="160" spans="1:12">
       <c r="A160" t="s">
         <v>1949</v>
       </c>
+      <c r="I160" t="s">
+        <v>2135</v>
+      </c>
     </row>
     <row r="161" spans="1:9">
       <c r="A161" t="s">
         <v>1950</v>
       </c>
+      <c r="I161" t="s">
+        <v>2135</v>
+      </c>
     </row>
     <row r="162" spans="1:9">
       <c r="A162" t="s">
         <v>1953</v>
       </c>
+      <c r="I162" t="s">
+        <v>2131</v>
+      </c>
     </row>
     <row r="163" spans="1:9">
       <c r="A163" t="s">
         <v>1954</v>
       </c>
+      <c r="I163" t="s">
+        <v>2131</v>
+      </c>
     </row>
     <row r="164" spans="1:9">
       <c r="A164" t="s">
         <v>1955</v>
       </c>
+      <c r="I164" t="s">
+        <v>2131</v>
+      </c>
     </row>
     <row r="165" spans="1:9">
       <c r="A165" t="s">
         <v>1956</v>
       </c>
+      <c r="I165" t="s">
+        <v>2131</v>
+      </c>
     </row>
     <row r="166" spans="1:9">
       <c r="A166" t="s">
         <v>1957</v>
       </c>
+      <c r="I166" t="s">
+        <v>2131</v>
+      </c>
     </row>
     <row r="167" spans="1:9">
       <c r="A167" t="s">
         <v>1958</v>
       </c>
+      <c r="I167" t="s">
+        <v>2131</v>
+      </c>
     </row>
     <row r="168" spans="1:9">
       <c r="A168" t="s">
         <v>1952</v>
       </c>
+      <c r="I168" t="s">
+        <v>2134</v>
+      </c>
     </row>
     <row r="169" spans="1:9">
       <c r="A169" t="s">
         <v>1959</v>
       </c>
+      <c r="I169" t="s">
+        <v>2136</v>
+      </c>
     </row>
     <row r="170" spans="1:9">
       <c r="A170" t="s">
         <v>1960</v>
       </c>
+      <c r="I170" t="s">
+        <v>2136</v>
+      </c>
     </row>
     <row r="171" spans="1:9">
       <c r="A171" t="s">
         <v>1961</v>
       </c>
+      <c r="I171" t="s">
+        <v>2136</v>
+      </c>
     </row>
     <row r="172" spans="1:9">
       <c r="A172" t="s">
@@ -15904,15 +15949,24 @@
       <c r="A177" t="s">
         <v>1965</v>
       </c>
+      <c r="I177" t="s">
+        <v>2124</v>
+      </c>
     </row>
     <row r="178" spans="1:9">
       <c r="A178" t="s">
         <v>1966</v>
       </c>
+      <c r="I178" t="s">
+        <v>2137</v>
+      </c>
     </row>
     <row r="179" spans="1:9">
       <c r="A179" t="s">
         <v>1967</v>
+      </c>
+      <c r="I179" t="s">
+        <v>2132</v>
       </c>
     </row>
     <row r="180" spans="1:9">

</xml_diff>

<commit_message>
Resist Fire and Cold
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE54416-6A55-4F7E-9EA5-4193F936AB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225E6370-0D09-4DF6-977E-4FC683CA9251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -10524,7 +10524,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -11602,32 +11602,34 @@
       <c r="A31" s="29" t="s">
         <v>1697</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="29">
         <v>2</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="29" t="s">
         <v>1267</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="29" t="s">
         <v>977</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="29">
         <v>5</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="29">
         <f>E31*2</f>
         <v>10</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="29" t="s">
         <v>1681</v>
       </c>
-      <c r="H31" t="b">
-        <v>1</v>
-      </c>
-      <c r="I31" t="s">
+      <c r="H31" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" s="29" t="s">
         <v>2135</v>
       </c>
-      <c r="L31" t="s">
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="29" t="s">
         <v>2062</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Draw Upon Holy Might
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225E6370-0D09-4DF6-977E-4FC683CA9251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAE43A3-7118-43DD-85F7-90F88D8ED75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -10524,7 +10524,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+      <selection pane="bottomLeft" activeCell="L32" sqref="A32:L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -11637,32 +11637,34 @@
       <c r="A32" s="29" t="s">
         <v>1736</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="29">
         <v>2</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="29" t="s">
         <v>968</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="29" t="s">
         <v>982</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="29">
         <v>5</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="29">
         <f>E32*2</f>
         <v>10</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="29" t="s">
         <v>1677</v>
       </c>
-      <c r="H32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I32" t="s">
+      <c r="H32" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="29" t="s">
         <v>2124</v>
       </c>
-      <c r="L32" t="s">
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+      <c r="L32" s="29" t="s">
         <v>1991</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Zone of Sweet Air
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EA4478-0793-47E2-B150-BE8A5B7B8F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07DB429-8718-4157-B2A0-E851AE330587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -10524,7 +10524,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B55" sqref="B55:L55"/>
+      <selection pane="bottomLeft" activeCell="L56" sqref="B56:L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -12477,32 +12477,34 @@
       <c r="A56" s="29" t="s">
         <v>1727</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="29">
         <v>3</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="29" t="s">
         <v>1191</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="29" t="s">
         <v>1067</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="29">
         <v>7</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="29">
         <f>E56*2</f>
         <v>14</v>
       </c>
-      <c r="G56" t="s">
-        <v>1680</v>
-      </c>
-      <c r="H56" t="b">
-        <v>0</v>
-      </c>
-      <c r="I56" t="s">
+      <c r="G56" s="29" t="s">
+        <v>1679</v>
+      </c>
+      <c r="H56" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="I56" s="29" t="s">
         <v>2139</v>
       </c>
-      <c r="L56" t="s">
+      <c r="J56" s="29"/>
+      <c r="K56" s="29"/>
+      <c r="L56" s="29" t="s">
         <v>2111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Protection From Normal Missiles
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F30ABD-8584-4740-88DB-99678C186223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA19B904-1A73-4168-9A49-A38D582F07FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -10521,7 +10521,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B59" sqref="B59:L59"/>
+      <selection pane="bottomLeft" activeCell="B60" sqref="B60:L60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -12614,32 +12614,34 @@
       <c r="A60" s="29" t="s">
         <v>1788</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="29">
         <v>3</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="29" t="s">
         <v>1830</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="E60">
+      <c r="E60" s="29">
         <v>6</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="29">
         <f>E60*2</f>
         <v>12</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G60" s="29" t="s">
         <v>1681</v>
       </c>
-      <c r="H60" t="b">
-        <v>0</v>
-      </c>
-      <c r="I60" t="s">
+      <c r="H60" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="I60" s="29" t="s">
         <v>2127</v>
       </c>
-      <c r="L60" t="s">
+      <c r="J60" s="29"/>
+      <c r="K60" s="29"/>
+      <c r="L60" s="29" t="s">
         <v>2052</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor Globe of Invulnerability
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC506D42-5804-4E65-A4A5-4FEBC9B717EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0252A56-68F8-4875-8B22-BFB27002F5A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -10521,7 +10521,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L80" sqref="B80:L80"/>
+      <selection pane="bottomLeft" activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -13349,32 +13349,34 @@
       <c r="A81" s="29" t="s">
         <v>1765</v>
       </c>
-      <c r="B81">
+      <c r="B81" s="29">
         <v>4</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="E81">
+      <c r="E81" s="29">
         <v>8</v>
       </c>
-      <c r="F81">
+      <c r="F81" s="29">
         <f>E81*2</f>
         <v>16</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G81" s="29" t="s">
         <v>1681</v>
       </c>
-      <c r="H81" t="b">
-        <v>1</v>
-      </c>
-      <c r="I81" t="s">
+      <c r="H81" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I81" s="29" t="s">
         <v>2125</v>
       </c>
-      <c r="L81" t="s">
+      <c r="J81" s="29"/>
+      <c r="K81" s="29"/>
+      <c r="L81" s="29" t="s">
         <v>2031</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Protection From Normal Weapons
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46578051-1A56-4E31-9C1C-40DB50A3A7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF465625-F843-4CE6-A749-8CC761E49758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -10521,7 +10521,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L113" sqref="B113:L113"/>
+      <selection pane="bottomLeft" activeCell="B114" sqref="B114:L114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -14220,7 +14220,7 @@
         <v>18</v>
       </c>
       <c r="G105" s="29" t="s">
-        <v>1677</v>
+        <v>1681</v>
       </c>
       <c r="H105" s="29" t="b">
         <v>1</v>
@@ -14255,7 +14255,7 @@
         <v>20</v>
       </c>
       <c r="G106" s="29" t="s">
-        <v>1677</v>
+        <v>1681</v>
       </c>
       <c r="H106" s="29" t="b">
         <v>1</v>
@@ -14292,7 +14292,7 @@
         <v>20</v>
       </c>
       <c r="G107" s="29" t="s">
-        <v>1677</v>
+        <v>1681</v>
       </c>
       <c r="H107" s="29" t="b">
         <v>1</v>
@@ -14329,7 +14329,7 @@
         <v>20</v>
       </c>
       <c r="G108" s="29" t="s">
-        <v>1677</v>
+        <v>1681</v>
       </c>
       <c r="H108" s="29" t="b">
         <v>1</v>
@@ -14366,7 +14366,7 @@
         <v>20</v>
       </c>
       <c r="G109" s="29" t="s">
-        <v>1677</v>
+        <v>1681</v>
       </c>
       <c r="H109" s="29" t="b">
         <v>1</v>
@@ -14403,7 +14403,7 @@
         <v>20</v>
       </c>
       <c r="G110" s="29" t="s">
-        <v>1677</v>
+        <v>1681</v>
       </c>
       <c r="H110" s="29" t="b">
         <v>1</v>
@@ -14440,7 +14440,7 @@
         <v>20</v>
       </c>
       <c r="G111" s="29" t="s">
-        <v>1677</v>
+        <v>1681</v>
       </c>
       <c r="H111" s="29" t="b">
         <v>1</v>
@@ -14477,7 +14477,7 @@
         <v>20</v>
       </c>
       <c r="G112" s="29" t="s">
-        <v>1677</v>
+        <v>1681</v>
       </c>
       <c r="H112" s="29" t="b">
         <v>1</v>
@@ -14514,7 +14514,7 @@
         <v>20</v>
       </c>
       <c r="G113" s="29" t="s">
-        <v>1677</v>
+        <v>1681</v>
       </c>
       <c r="H113" s="29" t="b">
         <v>1</v>
@@ -14534,32 +14534,34 @@
       <c r="A114" s="29" t="s">
         <v>1689</v>
       </c>
-      <c r="B114">
+      <c r="B114" s="29">
         <v>5</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C114" s="29" t="s">
         <v>1848</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D114" s="29" t="s">
         <v>225</v>
       </c>
-      <c r="E114">
+      <c r="E114" s="29">
         <v>10</v>
       </c>
-      <c r="F114">
+      <c r="F114" s="29">
         <f>E114*2</f>
         <v>20</v>
       </c>
-      <c r="G114" t="s">
+      <c r="G114" s="29" t="s">
         <v>1681</v>
       </c>
-      <c r="H114" t="b">
-        <v>1</v>
-      </c>
-      <c r="I114" t="s">
+      <c r="H114" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I114" s="29" t="s">
         <v>2132</v>
       </c>
-      <c r="L114" t="s">
+      <c r="J114" s="29"/>
+      <c r="K114" s="29"/>
+      <c r="L114" s="29" t="s">
         <v>2053</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Protection From Magic Energy
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9107408-A30B-44AD-ACDC-F30FB80E4A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1C8D2A-2B7F-4364-B9BF-E7AD8F7F59F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -10521,7 +10521,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G127" sqref="G127"/>
+      <selection pane="bottomLeft" activeCell="B128" sqref="B128:L128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -15024,32 +15024,34 @@
       <c r="A128" s="29" t="s">
         <v>1726</v>
       </c>
-      <c r="B128">
+      <c r="B128" s="29">
         <v>6</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C128" s="29" t="s">
         <v>1851</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D128" s="29" t="s">
         <v>243</v>
       </c>
-      <c r="E128">
-        <v>12</v>
-      </c>
-      <c r="F128">
+      <c r="E128" s="29">
+        <v>13</v>
+      </c>
+      <c r="F128" s="29">
         <f>E128*2</f>
-        <v>24</v>
-      </c>
-      <c r="G128" t="s">
+        <v>26</v>
+      </c>
+      <c r="G128" s="29" t="s">
         <v>1681</v>
       </c>
-      <c r="H128" t="b">
-        <v>1</v>
-      </c>
-      <c r="I128" t="s">
+      <c r="H128" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I128" s="29" t="s">
         <v>2137</v>
       </c>
-      <c r="L128" t="s">
+      <c r="J128" s="29"/>
+      <c r="K128" s="29"/>
+      <c r="L128" s="29" t="s">
         <v>2048</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Protection From Magical Weapons
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1C8D2A-2B7F-4364-B9BF-E7AD8F7F59F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31E3EE1-11D1-4743-A43E-7327DBF8BB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -10520,8 +10520,8 @@
   <dimension ref="A1:M191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B128" sqref="B128:L128"/>
+      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B129" sqref="B129:L129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -15059,32 +15059,34 @@
       <c r="A129" s="29" t="s">
         <v>1750</v>
       </c>
-      <c r="B129">
+      <c r="B129" s="29">
         <v>6</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C129" s="29" t="s">
         <v>1852</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D129" s="29" t="s">
         <v>248</v>
       </c>
-      <c r="E129">
+      <c r="E129" s="29">
         <v>12</v>
       </c>
-      <c r="F129">
+      <c r="F129" s="29">
         <f>E129*2</f>
         <v>24</v>
       </c>
-      <c r="G129" t="s">
+      <c r="G129" s="29" t="s">
         <v>1681</v>
       </c>
-      <c r="H129" t="b">
-        <v>0</v>
-      </c>
-      <c r="I129" t="s">
+      <c r="H129" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="I129" s="29" t="s">
         <v>2135</v>
       </c>
-      <c r="L129" t="s">
+      <c r="J129" s="29"/>
+      <c r="K129" s="29"/>
+      <c r="L129" s="29" t="s">
         <v>2049</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Protection From The Elements
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0B75BE-3E4D-44A2-8411-908B3101013C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA71272A-BFB6-4E63-9107-086D4693110A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -10521,7 +10521,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B139" sqref="B139:L139"/>
+      <selection pane="bottomLeft" activeCell="L140" sqref="B140:L140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -15446,32 +15446,34 @@
       <c r="A140" s="29" t="s">
         <v>1762</v>
       </c>
-      <c r="B140">
+      <c r="B140" s="29">
         <v>7</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C140" s="29" t="s">
         <v>1854</v>
       </c>
-      <c r="D140" t="s">
+      <c r="D140" s="29" t="s">
         <v>1913</v>
       </c>
-      <c r="E140">
+      <c r="E140" s="29">
         <v>13</v>
       </c>
-      <c r="F140">
+      <c r="F140" s="29">
         <f>E140*2</f>
         <v>26</v>
       </c>
-      <c r="G140" t="s">
+      <c r="G140" s="29" t="s">
         <v>1681</v>
       </c>
-      <c r="H140" t="b">
-        <v>1</v>
-      </c>
-      <c r="I140" t="s">
+      <c r="H140" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I140" s="29" t="s">
         <v>2130</v>
       </c>
-      <c r="L140" t="s">
+      <c r="J140" s="29"/>
+      <c r="K140" s="29"/>
+      <c r="L140" s="29" t="s">
         <v>2054</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Aura of Flaming Death
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B22C55-E144-441F-B592-84F08A18B322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2C0DF3-E27A-42D8-A7E1-70D0C40170F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -10521,7 +10521,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L151" sqref="B151:L151"/>
+      <selection pane="bottomLeft" activeCell="E154" sqref="E154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -15911,11 +15911,11 @@
         <v>1232</v>
       </c>
       <c r="E153">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F153">
         <f>E153*2</f>
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G153" t="s">
         <v>1681</v>

</xml_diff>

<commit_message>
Moving assets that have been allocated to spells
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2C0DF3-E27A-42D8-A7E1-70D0C40170F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18B34FA-27F3-4C52-8F5E-67C4C8C5E4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -10520,8 +10520,8 @@
   <dimension ref="A1:M191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E154" sqref="E154"/>
+      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A154" sqref="A154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -11247,48 +11247,48 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="29" t="s">
-        <v>1813</v>
+        <v>1714</v>
       </c>
       <c r="B21" s="29">
         <v>2</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>1045</v>
+        <v>197</v>
       </c>
       <c r="D21" s="29" t="s">
         <v>1408</v>
       </c>
       <c r="E21" s="29">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" s="29">
         <f>E21*2</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G21" s="29" t="s">
-        <v>1677</v>
+        <v>1680</v>
       </c>
       <c r="H21" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="29" t="s">
-        <v>2136</v>
+        <v>2131</v>
       </c>
       <c r="J21" s="29"/>
       <c r="K21" s="29"/>
       <c r="L21" s="29" t="s">
-        <v>1968</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="29" t="s">
-        <v>1793</v>
+        <v>1718</v>
       </c>
       <c r="B22" s="29">
         <v>2</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D22" s="29" t="s">
         <v>1408</v>
@@ -11307,12 +11307,12 @@
         <v>1</v>
       </c>
       <c r="I22" s="29" t="s">
-        <v>2124</v>
+        <v>2133</v>
       </c>
       <c r="J22" s="29"/>
       <c r="K22" s="29"/>
       <c r="L22" s="29" t="s">
-        <v>1972</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -11352,13 +11352,13 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="29" t="s">
-        <v>1718</v>
+        <v>1793</v>
       </c>
       <c r="B24" s="29">
         <v>2</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D24" s="29" t="s">
         <v>1408</v>
@@ -11377,47 +11377,47 @@
         <v>1</v>
       </c>
       <c r="I24" s="29" t="s">
-        <v>2133</v>
+        <v>2124</v>
       </c>
       <c r="J24" s="29"/>
       <c r="K24" s="29"/>
       <c r="L24" s="29" t="s">
-        <v>1985</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="29" t="s">
-        <v>1714</v>
+        <v>1813</v>
       </c>
       <c r="B25" s="29">
         <v>2</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>197</v>
+        <v>1045</v>
       </c>
       <c r="D25" s="29" t="s">
         <v>1408</v>
       </c>
       <c r="E25" s="29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F25" s="29">
         <f>E25*2</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G25" s="29" t="s">
-        <v>1680</v>
+        <v>1677</v>
       </c>
       <c r="H25" s="29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" s="29" t="s">
-        <v>2131</v>
+        <v>2136</v>
       </c>
       <c r="J25" s="29"/>
       <c r="K25" s="29"/>
       <c r="L25" s="29" t="s">
-        <v>2069</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -12052,37 +12052,37 @@
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="29" t="s">
-        <v>1757</v>
+        <v>1731</v>
       </c>
       <c r="B44" s="29">
         <v>3</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D44" s="29" t="s">
         <v>1408</v>
       </c>
       <c r="E44" s="29">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F44" s="29">
         <f>E44*2</f>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G44" s="29" t="s">
-        <v>1677</v>
+        <v>1681</v>
       </c>
       <c r="H44" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44" s="29" t="s">
-        <v>2129</v>
+        <v>2135</v>
       </c>
       <c r="J44" s="29"/>
       <c r="K44" s="29"/>
       <c r="L44" s="29" t="s">
-        <v>2033</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -12122,37 +12122,37 @@
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="29" t="s">
-        <v>1731</v>
+        <v>1757</v>
       </c>
       <c r="B46" s="29">
         <v>3</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="D46" s="29" t="s">
         <v>1408</v>
       </c>
       <c r="E46" s="29">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F46" s="29">
         <f>E46*2</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G46" s="29" t="s">
-        <v>1681</v>
+        <v>1677</v>
       </c>
       <c r="H46" s="29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I46" s="29" t="s">
-        <v>2135</v>
+        <v>2129</v>
       </c>
       <c r="J46" s="29"/>
       <c r="K46" s="29"/>
       <c r="L46" s="29" t="s">
-        <v>1996</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -12752,13 +12752,13 @@
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="29" t="s">
-        <v>1733</v>
+        <v>1687</v>
       </c>
       <c r="B64" s="29">
         <v>4</v>
       </c>
       <c r="C64" s="29" t="s">
-        <v>1080</v>
+        <v>1084</v>
       </c>
       <c r="D64" s="29" t="s">
         <v>1408</v>
@@ -12771,18 +12771,18 @@
         <v>16</v>
       </c>
       <c r="G64" s="29" t="s">
-        <v>2110</v>
+        <v>1679</v>
       </c>
       <c r="H64" s="29" t="b">
         <v>0</v>
       </c>
       <c r="I64" s="29" t="s">
-        <v>2135</v>
+        <v>2130</v>
       </c>
       <c r="J64" s="29"/>
       <c r="K64" s="29"/>
       <c r="L64" s="29" t="s">
-        <v>1969</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -12822,13 +12822,13 @@
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="29" t="s">
-        <v>1739</v>
+        <v>1733</v>
       </c>
       <c r="B66" s="29">
         <v>4</v>
       </c>
       <c r="C66" s="29" t="s">
-        <v>216</v>
+        <v>1080</v>
       </c>
       <c r="D66" s="29" t="s">
         <v>1408</v>
@@ -12841,29 +12841,29 @@
         <v>16</v>
       </c>
       <c r="G66" s="29" t="s">
-        <v>1677</v>
+        <v>2110</v>
       </c>
       <c r="H66" s="29" t="b">
         <v>0</v>
       </c>
       <c r="I66" s="29" t="s">
-        <v>2121</v>
+        <v>2135</v>
       </c>
       <c r="J66" s="29"/>
       <c r="K66" s="29"/>
       <c r="L66" s="29" t="s">
-        <v>1991</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="29" t="s">
-        <v>1748</v>
+        <v>1739</v>
       </c>
       <c r="B67" s="29">
         <v>4</v>
       </c>
       <c r="C67" s="29" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D67" s="29" t="s">
         <v>1408</v>
@@ -12882,23 +12882,23 @@
         <v>0</v>
       </c>
       <c r="I67" s="29" t="s">
-        <v>2134</v>
+        <v>2121</v>
       </c>
       <c r="J67" s="29"/>
       <c r="K67" s="29"/>
       <c r="L67" s="29" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="68" spans="1:12">
       <c r="A68" s="29" t="s">
-        <v>1769</v>
+        <v>1748</v>
       </c>
       <c r="B68" s="29">
         <v>4</v>
       </c>
       <c r="C68" s="29" t="s">
-        <v>1079</v>
+        <v>218</v>
       </c>
       <c r="D68" s="29" t="s">
         <v>1408</v>
@@ -12911,29 +12911,29 @@
         <v>16</v>
       </c>
       <c r="G68" s="29" t="s">
-        <v>2110</v>
+        <v>1677</v>
       </c>
       <c r="H68" s="29" t="b">
         <v>0</v>
       </c>
       <c r="I68" s="29" t="s">
-        <v>2123</v>
+        <v>2134</v>
       </c>
       <c r="J68" s="29"/>
       <c r="K68" s="29"/>
       <c r="L68" s="29" t="s">
-        <v>2054</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="29" t="s">
-        <v>1687</v>
+        <v>1769</v>
       </c>
       <c r="B69" s="29">
         <v>4</v>
       </c>
       <c r="C69" s="29" t="s">
-        <v>1084</v>
+        <v>1079</v>
       </c>
       <c r="D69" s="29" t="s">
         <v>1408</v>
@@ -12946,18 +12946,18 @@
         <v>16</v>
       </c>
       <c r="G69" s="29" t="s">
-        <v>1679</v>
+        <v>2110</v>
       </c>
       <c r="H69" s="29" t="b">
         <v>0</v>
       </c>
       <c r="I69" s="29" t="s">
-        <v>2130</v>
+        <v>2123</v>
       </c>
       <c r="J69" s="29"/>
       <c r="K69" s="29"/>
       <c r="L69" s="29" t="s">
-        <v>2101</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -13592,48 +13592,48 @@
     </row>
     <row r="88" spans="1:12">
       <c r="A88" s="29" t="s">
-        <v>1805</v>
+        <v>1710</v>
       </c>
       <c r="B88" s="29">
         <v>5</v>
       </c>
       <c r="C88" s="29" t="s">
-        <v>1111</v>
+        <v>1106</v>
       </c>
       <c r="D88" s="29" t="s">
         <v>1408</v>
       </c>
       <c r="E88" s="29">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F88" s="29">
         <f>E88*2</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G88" s="29" t="s">
-        <v>2110</v>
+        <v>1680</v>
       </c>
       <c r="H88" s="29" t="b">
         <v>0</v>
       </c>
       <c r="I88" s="29" t="s">
-        <v>2126</v>
+        <v>2131</v>
       </c>
       <c r="J88" s="29"/>
       <c r="K88" s="29"/>
       <c r="L88" s="29" t="s">
-        <v>1940</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="89" spans="1:12">
       <c r="A89" s="29" t="s">
-        <v>1809</v>
+        <v>1717</v>
       </c>
       <c r="B89" s="29">
         <v>5</v>
       </c>
       <c r="C89" s="29" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="D89" s="29" t="s">
         <v>1408</v>
@@ -13646,29 +13646,31 @@
         <v>18</v>
       </c>
       <c r="G89" s="29" t="s">
-        <v>2110</v>
+        <v>1681</v>
       </c>
       <c r="H89" s="29" t="b">
         <v>0</v>
       </c>
       <c r="I89" s="29" t="s">
-        <v>2126</v>
+        <v>2133</v>
       </c>
       <c r="J89" s="29"/>
-      <c r="K89" s="29"/>
+      <c r="K89" s="29" t="s">
+        <v>1825</v>
+      </c>
       <c r="L89" s="29" t="s">
-        <v>2061</v>
+        <v>2066</v>
       </c>
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="29" t="s">
-        <v>1717</v>
+        <v>1805</v>
       </c>
       <c r="B90" s="29">
         <v>5</v>
       </c>
       <c r="C90" s="29" t="s">
-        <v>1108</v>
+        <v>1111</v>
       </c>
       <c r="D90" s="29" t="s">
         <v>1408</v>
@@ -13681,55 +13683,53 @@
         <v>18</v>
       </c>
       <c r="G90" s="29" t="s">
-        <v>1681</v>
+        <v>2110</v>
       </c>
       <c r="H90" s="29" t="b">
         <v>0</v>
       </c>
       <c r="I90" s="29" t="s">
-        <v>2133</v>
+        <v>2126</v>
       </c>
       <c r="J90" s="29"/>
-      <c r="K90" s="29" t="s">
-        <v>1825</v>
-      </c>
+      <c r="K90" s="29"/>
       <c r="L90" s="29" t="s">
-        <v>2066</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="91" spans="1:12">
       <c r="A91" s="29" t="s">
-        <v>1710</v>
+        <v>1809</v>
       </c>
       <c r="B91" s="29">
         <v>5</v>
       </c>
       <c r="C91" s="29" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="D91" s="29" t="s">
         <v>1408</v>
       </c>
       <c r="E91" s="29">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" s="29">
         <f>E91*2</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G91" s="29" t="s">
-        <v>1680</v>
+        <v>2110</v>
       </c>
       <c r="H91" s="29" t="b">
         <v>0</v>
       </c>
       <c r="I91" s="29" t="s">
-        <v>2131</v>
+        <v>2126</v>
       </c>
       <c r="J91" s="29"/>
       <c r="K91" s="29"/>
       <c r="L91" s="29" t="s">
-        <v>2088</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="92" spans="1:12">
@@ -13769,13 +13769,13 @@
     </row>
     <row r="93" spans="1:12">
       <c r="A93" s="29" t="s">
-        <v>1880</v>
+        <v>1949</v>
       </c>
       <c r="B93" s="29">
         <v>5</v>
       </c>
       <c r="C93" s="29" t="s">
-        <v>1919</v>
+        <v>1921</v>
       </c>
       <c r="D93" s="29" t="s">
         <v>1916</v>
@@ -13794,25 +13794,25 @@
         <v>1</v>
       </c>
       <c r="I93" s="29" t="s">
-        <v>2127</v>
+        <v>2132</v>
       </c>
       <c r="J93" s="29" t="s">
-        <v>2112</v>
+        <v>2116</v>
       </c>
       <c r="K93" s="29"/>
       <c r="L93" s="29" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="94" spans="1:12">
       <c r="A94" s="29" t="s">
-        <v>1893</v>
+        <v>1867</v>
       </c>
       <c r="B94" s="29">
         <v>5</v>
       </c>
       <c r="C94" s="29" t="s">
-        <v>1917</v>
+        <v>1915</v>
       </c>
       <c r="D94" s="29" t="s">
         <v>1916</v>
@@ -13831,25 +13831,25 @@
         <v>1</v>
       </c>
       <c r="I94" s="29" t="s">
-        <v>2120</v>
+        <v>2118</v>
       </c>
       <c r="J94" s="29" t="s">
-        <v>2113</v>
+        <v>2115</v>
       </c>
       <c r="K94" s="29"/>
       <c r="L94" s="29" t="s">
-        <v>2083</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="95" spans="1:12">
       <c r="A95" s="29" t="s">
-        <v>1883</v>
+        <v>1880</v>
       </c>
       <c r="B95" s="29">
         <v>5</v>
       </c>
       <c r="C95" s="29" t="s">
-        <v>1918</v>
+        <v>1919</v>
       </c>
       <c r="D95" s="29" t="s">
         <v>1916</v>
@@ -13871,22 +13871,22 @@
         <v>2127</v>
       </c>
       <c r="J95" s="29" t="s">
-        <v>2114</v>
+        <v>2112</v>
       </c>
       <c r="K95" s="29"/>
       <c r="L95" s="29" t="s">
-        <v>2085</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="96" spans="1:12">
       <c r="A96" s="29" t="s">
-        <v>1867</v>
+        <v>1883</v>
       </c>
       <c r="B96" s="29">
         <v>5</v>
       </c>
       <c r="C96" s="29" t="s">
-        <v>1915</v>
+        <v>1918</v>
       </c>
       <c r="D96" s="29" t="s">
         <v>1916</v>
@@ -13905,25 +13905,25 @@
         <v>1</v>
       </c>
       <c r="I96" s="29" t="s">
-        <v>2118</v>
+        <v>2127</v>
       </c>
       <c r="J96" s="29" t="s">
-        <v>2115</v>
+        <v>2114</v>
       </c>
       <c r="K96" s="29"/>
       <c r="L96" s="29" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="97" spans="1:12">
       <c r="A97" s="29" t="s">
-        <v>1949</v>
+        <v>1893</v>
       </c>
       <c r="B97" s="29">
         <v>5</v>
       </c>
       <c r="C97" s="29" t="s">
-        <v>1921</v>
+        <v>1917</v>
       </c>
       <c r="D97" s="29" t="s">
         <v>1916</v>
@@ -13942,14 +13942,14 @@
         <v>1</v>
       </c>
       <c r="I97" s="29" t="s">
-        <v>2132</v>
+        <v>2120</v>
       </c>
       <c r="J97" s="29" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
       <c r="K97" s="29"/>
       <c r="L97" s="29" t="s">
-        <v>2081</v>
+        <v>2083</v>
       </c>
     </row>
     <row r="98" spans="1:12">
@@ -14273,13 +14273,13 @@
     </row>
     <row r="107" spans="1:12">
       <c r="A107" s="29" t="s">
-        <v>1773</v>
+        <v>1720</v>
       </c>
       <c r="B107" s="29">
         <v>5</v>
       </c>
       <c r="C107" s="29" t="s">
-        <v>1847</v>
+        <v>1834</v>
       </c>
       <c r="D107" s="29" t="s">
         <v>224</v>
@@ -14298,25 +14298,25 @@
         <v>1</v>
       </c>
       <c r="I107" s="29" t="s">
-        <v>2122</v>
+        <v>2133</v>
       </c>
       <c r="J107" s="29" t="s">
-        <v>1846</v>
+        <v>1835</v>
       </c>
       <c r="K107" s="29"/>
       <c r="L107" s="29" t="s">
-        <v>2072</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="108" spans="1:12">
       <c r="A108" s="29" t="s">
-        <v>1790</v>
+        <v>1730</v>
       </c>
       <c r="B108" s="29">
         <v>5</v>
       </c>
       <c r="C108" s="29" t="s">
-        <v>1836</v>
+        <v>1842</v>
       </c>
       <c r="D108" s="29" t="s">
         <v>224</v>
@@ -14335,25 +14335,25 @@
         <v>1</v>
       </c>
       <c r="I108" s="29" t="s">
-        <v>2125</v>
+        <v>2135</v>
       </c>
       <c r="J108" s="29" t="s">
-        <v>1837</v>
+        <v>1843</v>
       </c>
       <c r="K108" s="29"/>
       <c r="L108" s="29" t="s">
-        <v>2073</v>
+        <v>2076</v>
       </c>
     </row>
     <row r="109" spans="1:12">
       <c r="A109" s="29" t="s">
-        <v>1720</v>
+        <v>1754</v>
       </c>
       <c r="B109" s="29">
         <v>5</v>
       </c>
       <c r="C109" s="29" t="s">
-        <v>1834</v>
+        <v>1840</v>
       </c>
       <c r="D109" s="29" t="s">
         <v>224</v>
@@ -14372,25 +14372,25 @@
         <v>1</v>
       </c>
       <c r="I109" s="29" t="s">
-        <v>2133</v>
+        <v>2129</v>
       </c>
       <c r="J109" s="29" t="s">
-        <v>1835</v>
+        <v>1841</v>
       </c>
       <c r="K109" s="29"/>
       <c r="L109" s="29" t="s">
-        <v>2074</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="110" spans="1:12">
       <c r="A110" s="29" t="s">
-        <v>1787</v>
+        <v>1773</v>
       </c>
       <c r="B110" s="29">
         <v>5</v>
       </c>
       <c r="C110" s="29" t="s">
-        <v>1838</v>
+        <v>1847</v>
       </c>
       <c r="D110" s="29" t="s">
         <v>224</v>
@@ -14409,25 +14409,25 @@
         <v>1</v>
       </c>
       <c r="I110" s="29" t="s">
-        <v>2125</v>
+        <v>2122</v>
       </c>
       <c r="J110" s="29" t="s">
-        <v>1839</v>
+        <v>1846</v>
       </c>
       <c r="K110" s="29"/>
       <c r="L110" s="29" t="s">
-        <v>2075</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="111" spans="1:12">
       <c r="A111" s="29" t="s">
-        <v>1730</v>
+        <v>1787</v>
       </c>
       <c r="B111" s="29">
         <v>5</v>
       </c>
       <c r="C111" s="29" t="s">
-        <v>1842</v>
+        <v>1838</v>
       </c>
       <c r="D111" s="29" t="s">
         <v>224</v>
@@ -14446,25 +14446,25 @@
         <v>1</v>
       </c>
       <c r="I111" s="29" t="s">
-        <v>2135</v>
+        <v>2125</v>
       </c>
       <c r="J111" s="29" t="s">
-        <v>1843</v>
+        <v>1839</v>
       </c>
       <c r="K111" s="29"/>
       <c r="L111" s="29" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="112" spans="1:12">
       <c r="A112" s="29" t="s">
-        <v>1754</v>
+        <v>1790</v>
       </c>
       <c r="B112" s="29">
         <v>5</v>
       </c>
       <c r="C112" s="29" t="s">
-        <v>1840</v>
+        <v>1836</v>
       </c>
       <c r="D112" s="29" t="s">
         <v>224</v>
@@ -14483,14 +14483,14 @@
         <v>1</v>
       </c>
       <c r="I112" s="29" t="s">
-        <v>2129</v>
+        <v>2125</v>
       </c>
       <c r="J112" s="29" t="s">
-        <v>1841</v>
+        <v>1837</v>
       </c>
       <c r="K112" s="29"/>
       <c r="L112" s="29" t="s">
-        <v>2077</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="113" spans="1:12">
@@ -14707,72 +14707,72 @@
     </row>
     <row r="119" spans="1:12">
       <c r="A119" s="29" t="s">
-        <v>1802</v>
+        <v>1698</v>
       </c>
       <c r="B119" s="29">
         <v>6</v>
       </c>
       <c r="C119" s="29" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
       <c r="D119" s="29" t="s">
         <v>1408</v>
       </c>
       <c r="E119" s="29">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F119" s="29">
         <f>E119*2</f>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G119" s="29" t="s">
-        <v>1681</v>
+        <v>1677</v>
       </c>
       <c r="H119" s="29" t="b">
         <v>0</v>
       </c>
       <c r="I119" s="29" t="s">
-        <v>2124</v>
+        <v>2132</v>
       </c>
       <c r="J119" s="29"/>
       <c r="K119" s="29"/>
       <c r="L119" s="29" t="s">
-        <v>1942</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="120" spans="1:12">
       <c r="A120" s="29" t="s">
-        <v>1698</v>
+        <v>1802</v>
       </c>
       <c r="B120" s="29">
         <v>6</v>
       </c>
       <c r="C120" s="29" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="D120" s="29" t="s">
         <v>1408</v>
       </c>
       <c r="E120" s="29">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F120" s="29">
         <f>E120*2</f>
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G120" s="29" t="s">
-        <v>1677</v>
+        <v>1681</v>
       </c>
       <c r="H120" s="29" t="b">
         <v>0</v>
       </c>
       <c r="I120" s="29" t="s">
-        <v>2132</v>
+        <v>2124</v>
       </c>
       <c r="J120" s="29"/>
       <c r="K120" s="29"/>
       <c r="L120" s="29" t="s">
-        <v>2097</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="121" spans="1:12">
@@ -15234,37 +15234,37 @@
     </row>
     <row r="134" spans="1:12">
       <c r="A134" s="29" t="s">
-        <v>1882</v>
+        <v>1792</v>
       </c>
       <c r="B134" s="29">
         <v>7</v>
       </c>
       <c r="C134" s="29" t="s">
-        <v>1157</v>
+        <v>1159</v>
       </c>
       <c r="D134" s="29" t="s">
         <v>1408</v>
       </c>
       <c r="E134" s="29">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F134" s="29">
         <f>E134*2</f>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G134" s="29" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="H134" s="29" t="b">
         <v>0</v>
       </c>
       <c r="I134" s="29" t="s">
-        <v>2127</v>
+        <v>2125</v>
       </c>
       <c r="J134" s="29"/>
       <c r="K134" s="29"/>
       <c r="L134" s="29" t="s">
-        <v>2015</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="135" spans="1:12">
@@ -15304,37 +15304,37 @@
     </row>
     <row r="136" spans="1:12">
       <c r="A136" s="29" t="s">
-        <v>1792</v>
+        <v>1882</v>
       </c>
       <c r="B136" s="29">
         <v>7</v>
       </c>
       <c r="C136" s="29" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D136" s="29" t="s">
         <v>1408</v>
       </c>
       <c r="E136" s="29">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F136" s="29">
         <f>E136*2</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G136" s="29" t="s">
-        <v>1680</v>
+        <v>1681</v>
       </c>
       <c r="H136" s="29" t="b">
         <v>0</v>
       </c>
       <c r="I136" s="29" t="s">
-        <v>2125</v>
+        <v>2127</v>
       </c>
       <c r="J136" s="29"/>
       <c r="K136" s="29"/>
       <c r="L136" s="29" t="s">
-        <v>2032</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="137" spans="1:12">
@@ -15901,79 +15901,81 @@
       <c r="A153" s="29" t="s">
         <v>1784</v>
       </c>
-      <c r="B153" s="1" t="s">
+      <c r="B153" s="36" t="s">
         <v>1399</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C153" s="29" t="s">
         <v>1223</v>
       </c>
-      <c r="D153" t="s">
+      <c r="D153" s="29" t="s">
         <v>1232</v>
       </c>
-      <c r="E153">
+      <c r="E153" s="29">
         <v>18</v>
       </c>
-      <c r="F153">
+      <c r="F153" s="29">
         <f>E153*2</f>
         <v>36</v>
       </c>
-      <c r="G153" t="s">
+      <c r="G153" s="29" t="s">
         <v>1681</v>
       </c>
-      <c r="H153" t="b">
-        <v>1</v>
-      </c>
-      <c r="I153" t="s">
+      <c r="H153" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I153" s="29" t="s">
         <v>2125</v>
       </c>
-      <c r="L153" t="s">
+      <c r="J153" s="29"/>
+      <c r="K153" s="29"/>
+      <c r="L153" s="29" t="s">
         <v>1967</v>
       </c>
     </row>
     <row r="154" spans="1:12">
-      <c r="A154" s="29" t="s">
-        <v>1695</v>
-      </c>
-      <c r="D154" s="30"/>
+      <c r="A154" t="s">
+        <v>1944</v>
+      </c>
       <c r="I154" t="s">
-        <v>2132</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="155" spans="1:12">
-      <c r="A155" s="30" t="s">
-        <v>1865</v>
+      <c r="A155" t="s">
+        <v>1945</v>
       </c>
       <c r="I155" t="s">
-        <v>2118</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="156" spans="1:12">
       <c r="A156" s="30" t="s">
-        <v>1869</v>
-      </c>
+        <v>1695</v>
+      </c>
+      <c r="D156" s="30"/>
       <c r="I156" t="s">
-        <v>2118</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="157" spans="1:12">
       <c r="A157" t="s">
-        <v>1944</v>
+        <v>1946</v>
       </c>
       <c r="I157" t="s">
-        <v>2130</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="158" spans="1:12">
       <c r="A158" t="s">
-        <v>1945</v>
+        <v>1947</v>
       </c>
       <c r="I158" t="s">
-        <v>2130</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="159" spans="1:12">
       <c r="A159" t="s">
-        <v>1946</v>
+        <v>1948</v>
       </c>
       <c r="I159" t="s">
         <v>2132</v>
@@ -15981,23 +15983,23 @@
     </row>
     <row r="160" spans="1:12">
       <c r="A160" t="s">
-        <v>1947</v>
+        <v>1951</v>
       </c>
       <c r="I160" t="s">
-        <v>2132</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="161" spans="1:9">
       <c r="A161" t="s">
-        <v>1948</v>
+        <v>1952</v>
       </c>
       <c r="I161" t="s">
-        <v>2132</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="162" spans="1:9">
       <c r="A162" t="s">
-        <v>1951</v>
+        <v>1953</v>
       </c>
       <c r="I162" t="s">
         <v>2128</v>
@@ -16005,7 +16007,7 @@
     </row>
     <row r="163" spans="1:9">
       <c r="A163" t="s">
-        <v>1952</v>
+        <v>1954</v>
       </c>
       <c r="I163" t="s">
         <v>2128</v>
@@ -16013,7 +16015,7 @@
     </row>
     <row r="164" spans="1:9">
       <c r="A164" t="s">
-        <v>1953</v>
+        <v>1955</v>
       </c>
       <c r="I164" t="s">
         <v>2128</v>
@@ -16021,7 +16023,7 @@
     </row>
     <row r="165" spans="1:9">
       <c r="A165" t="s">
-        <v>1954</v>
+        <v>1956</v>
       </c>
       <c r="I165" t="s">
         <v>2128</v>
@@ -16029,31 +16031,31 @@
     </row>
     <row r="166" spans="1:9">
       <c r="A166" t="s">
-        <v>1955</v>
+        <v>1950</v>
       </c>
       <c r="I166" t="s">
-        <v>2128</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="167" spans="1:9">
       <c r="A167" t="s">
-        <v>1956</v>
+        <v>1957</v>
       </c>
       <c r="I167" t="s">
-        <v>2128</v>
+        <v>2133</v>
       </c>
     </row>
     <row r="168" spans="1:9">
       <c r="A168" t="s">
-        <v>1950</v>
+        <v>1958</v>
       </c>
       <c r="I168" t="s">
-        <v>2131</v>
+        <v>2133</v>
       </c>
     </row>
     <row r="169" spans="1:9">
       <c r="A169" t="s">
-        <v>1957</v>
+        <v>1959</v>
       </c>
       <c r="I169" t="s">
         <v>2133</v>
@@ -16061,23 +16063,23 @@
     </row>
     <row r="170" spans="1:9">
       <c r="A170" t="s">
-        <v>1958</v>
+        <v>1722</v>
       </c>
       <c r="I170" t="s">
-        <v>2133</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="171" spans="1:9">
       <c r="A171" t="s">
-        <v>1959</v>
+        <v>1960</v>
       </c>
       <c r="I171" t="s">
-        <v>2133</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="172" spans="1:9">
       <c r="A172" t="s">
-        <v>1722</v>
+        <v>1962</v>
       </c>
       <c r="I172" t="s">
         <v>2136</v>
@@ -16085,7 +16087,7 @@
     </row>
     <row r="173" spans="1:9">
       <c r="A173" t="s">
-        <v>1960</v>
+        <v>1961</v>
       </c>
       <c r="I173" t="s">
         <v>2136</v>
@@ -16093,7 +16095,7 @@
     </row>
     <row r="174" spans="1:9">
       <c r="A174" t="s">
-        <v>1962</v>
+        <v>1724</v>
       </c>
       <c r="I174" t="s">
         <v>2136</v>
@@ -16101,79 +16103,79 @@
     </row>
     <row r="175" spans="1:9">
       <c r="A175" t="s">
-        <v>1961</v>
+        <v>1963</v>
       </c>
       <c r="I175" t="s">
-        <v>2136</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="176" spans="1:9">
       <c r="A176" t="s">
-        <v>1724</v>
+        <v>1964</v>
       </c>
       <c r="I176" t="s">
-        <v>2136</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="177" spans="1:9">
       <c r="A177" t="s">
-        <v>1963</v>
+        <v>1965</v>
       </c>
       <c r="I177" t="s">
-        <v>2121</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="178" spans="1:9">
       <c r="A178" t="s">
-        <v>1964</v>
+        <v>1776</v>
       </c>
       <c r="I178" t="s">
-        <v>2134</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="179" spans="1:9">
       <c r="A179" t="s">
-        <v>1965</v>
+        <v>1808</v>
       </c>
       <c r="I179" t="s">
-        <v>2129</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="180" spans="1:9">
-      <c r="A180" t="s">
-        <v>1776</v>
+      <c r="A180" s="30" t="s">
+        <v>1861</v>
       </c>
       <c r="I180" t="s">
-        <v>2122</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="181" spans="1:9">
-      <c r="A181" t="s">
-        <v>1808</v>
+      <c r="A181" s="30" t="s">
+        <v>1865</v>
       </c>
       <c r="I181" t="s">
-        <v>2126</v>
+        <v>2118</v>
       </c>
     </row>
     <row r="182" spans="1:9">
-      <c r="A182" s="30" t="s">
-        <v>1861</v>
+      <c r="A182" t="s">
+        <v>1866</v>
       </c>
       <c r="I182" t="s">
-        <v>2119</v>
+        <v>2118</v>
       </c>
     </row>
     <row r="183" spans="1:9">
       <c r="A183" t="s">
-        <v>1866</v>
+        <v>1868</v>
       </c>
       <c r="I183" t="s">
         <v>2118</v>
       </c>
     </row>
     <row r="184" spans="1:9">
-      <c r="A184" t="s">
-        <v>1868</v>
+      <c r="A184" s="30" t="s">
+        <v>1869</v>
       </c>
       <c r="I184" t="s">
         <v>2118</v>
@@ -16239,6 +16241,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M191">
     <sortCondition ref="B2:B191"/>
     <sortCondition ref="D2:D191"/>
+    <sortCondition ref="A2:A191"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixing Searing Smit's magnitude being erroneous
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18B34FA-27F3-4C52-8F5E-67C4C8C5E4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510D09F9-40D6-406E-8D3F-40CFF8D338A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -35,22 +35,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11519" uniqueCount="2139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11520" uniqueCount="2140">
   <si>
     <t>Caster Level</t>
   </si>
@@ -6467,6 +6457,9 @@
   </si>
   <si>
     <t>MEWI857</t>
+  </si>
+  <si>
+    <t>Broken?</t>
   </si>
 </sst>
 </file>
@@ -6683,7 +6676,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6700,7 +6695,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -10519,9 +10514,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90FF5842-5F39-42CA-813E-70DCD245FAB4}">
   <dimension ref="A1:M191"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A154" sqref="A154"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -10577,7 +10572,7 @@
         <v>1932</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="30" customFormat="1">
+    <row r="2" spans="1:12">
       <c r="A2" s="29" t="s">
         <v>1875</v>
       </c>
@@ -10594,7 +10589,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="29">
-        <f>E2*2</f>
+        <f t="shared" ref="F2:F33" si="0">E2*2</f>
         <v>4</v>
       </c>
       <c r="G2" s="29" t="s">
@@ -10629,7 +10624,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="29">
-        <f>E3*2</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G3" s="29" t="s">
@@ -10664,7 +10659,7 @@
         <v>2</v>
       </c>
       <c r="F4" s="29">
-        <f>E4*2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G4" s="29" t="s">
@@ -10699,7 +10694,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="29">
-        <f>E5*2</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="G5" s="29" t="s">
@@ -10734,14 +10729,14 @@
         <v>4</v>
       </c>
       <c r="F6" s="29">
-        <f>E6*2</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G6" s="29" t="s">
         <v>2110</v>
       </c>
-      <c r="H6" s="29" t="b">
-        <v>1</v>
+      <c r="H6" s="36" t="s">
+        <v>2139</v>
       </c>
       <c r="I6" s="29" t="s">
         <v>2119</v>
@@ -10769,7 +10764,7 @@
         <v>4</v>
       </c>
       <c r="F7" s="29">
-        <f>E7*2</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G7" s="29" t="s">
@@ -10804,7 +10799,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="29">
-        <f>E8*2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G8" s="29" t="s">
@@ -10839,7 +10834,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="29">
-        <f>E9*2</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G9" s="29" t="s">
@@ -10874,7 +10869,7 @@
         <v>4</v>
       </c>
       <c r="F10" s="29">
-        <f>E10*2</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G10" s="29" t="s">
@@ -10909,7 +10904,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="29">
-        <f>E11*2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G11" s="29" t="s">
@@ -10944,7 +10939,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="29">
-        <f>E12*2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G12" s="29" t="s">
@@ -10979,7 +10974,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="29">
-        <f>E13*2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G13" s="29" t="s">
@@ -11014,7 +11009,7 @@
         <v>2</v>
       </c>
       <c r="F14" s="29">
-        <f>E14*2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G14" s="29" t="s">
@@ -11049,7 +11044,7 @@
         <v>2</v>
       </c>
       <c r="F15" s="29">
-        <f>E15*2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G15" s="29" t="s">
@@ -11084,7 +11079,7 @@
         <v>2</v>
       </c>
       <c r="F16" s="29">
-        <f>E16*2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G16" s="29" t="s">
@@ -11119,7 +11114,7 @@
         <v>2</v>
       </c>
       <c r="F17" s="29">
-        <f>E17*2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G17" s="29" t="s">
@@ -11157,7 +11152,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="29">
-        <f>E18*2</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G18" s="29" t="s">
@@ -11192,7 +11187,7 @@
         <v>2</v>
       </c>
       <c r="F19" s="29">
-        <f>E19*2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G19" s="29" t="s">
@@ -11227,7 +11222,7 @@
         <v>2</v>
       </c>
       <c r="F20" s="29">
-        <f>E20*2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G20" s="29" t="s">
@@ -11262,7 +11257,7 @@
         <v>4</v>
       </c>
       <c r="F21" s="29">
-        <f>E21*2</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G21" s="29" t="s">
@@ -11297,7 +11292,7 @@
         <v>4</v>
       </c>
       <c r="F22" s="29">
-        <f>E22*2</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G22" s="29" t="s">
@@ -11332,7 +11327,7 @@
         <v>3</v>
       </c>
       <c r="F23" s="29">
-        <f>E23*2</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G23" s="29" t="s">
@@ -11367,7 +11362,7 @@
         <v>4</v>
       </c>
       <c r="F24" s="29">
-        <f>E24*2</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G24" s="29" t="s">
@@ -11402,7 +11397,7 @@
         <v>5</v>
       </c>
       <c r="F25" s="29">
-        <f>E25*2</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G25" s="29" t="s">
@@ -11437,7 +11432,7 @@
         <v>3</v>
       </c>
       <c r="F26" s="29">
-        <f>E26*2</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G26" s="29" t="s">
@@ -11472,7 +11467,7 @@
         <v>4</v>
       </c>
       <c r="F27" s="29">
-        <f>E27*2</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G27" s="29" t="s">
@@ -11507,7 +11502,7 @@
         <v>4</v>
       </c>
       <c r="F28" s="29">
-        <f>E28*2</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G28" s="29" t="s">
@@ -11542,7 +11537,7 @@
         <v>5</v>
       </c>
       <c r="F29" s="29">
-        <f>E29*2</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G29" s="29" t="s">
@@ -11577,7 +11572,7 @@
         <v>4</v>
       </c>
       <c r="F30" s="29">
-        <f>E30*2</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G30" s="29" t="s">
@@ -11612,7 +11607,7 @@
         <v>5</v>
       </c>
       <c r="F31" s="29">
-        <f>E31*2</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G31" s="29" t="s">
@@ -11647,7 +11642,7 @@
         <v>5</v>
       </c>
       <c r="F32" s="29">
-        <f>E32*2</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G32" s="29" t="s">
@@ -11682,7 +11677,7 @@
         <v>5</v>
       </c>
       <c r="F33" s="29">
-        <f>E33*2</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G33" s="29" t="s">
@@ -11717,7 +11712,7 @@
         <v>4</v>
       </c>
       <c r="F34" s="29">
-        <f>E34*2</f>
+        <f t="shared" ref="F34:F65" si="1">E34*2</f>
         <v>8</v>
       </c>
       <c r="G34" s="29" t="s">
@@ -11752,7 +11747,7 @@
         <v>3</v>
       </c>
       <c r="F35" s="29">
-        <f>E35*2</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="G35" s="29" t="s">
@@ -11787,7 +11782,7 @@
         <v>4</v>
       </c>
       <c r="F36" s="29">
-        <f>E36*2</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G36" s="29" t="s">
@@ -11822,7 +11817,7 @@
         <v>4</v>
       </c>
       <c r="F37" s="29">
-        <f>E37*2</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G37" s="29" t="s">
@@ -11857,7 +11852,7 @@
         <v>4</v>
       </c>
       <c r="F38" s="29">
-        <f>E38*2</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G38" s="29" t="s">
@@ -11892,7 +11887,7 @@
         <v>4</v>
       </c>
       <c r="F39" s="29">
-        <f>E39*2</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G39" s="29" t="s">
@@ -11927,7 +11922,7 @@
         <v>4</v>
       </c>
       <c r="F40" s="29">
-        <f>E40*2</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G40" s="29" t="s">
@@ -11962,7 +11957,7 @@
         <v>4</v>
       </c>
       <c r="F41" s="29">
-        <f>E41*2</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G41" s="29" t="s">
@@ -11997,7 +11992,7 @@
         <v>4</v>
       </c>
       <c r="F42" s="29">
-        <f>E42*2</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G42" s="29" t="s">
@@ -12032,7 +12027,7 @@
         <v>4</v>
       </c>
       <c r="F43" s="29">
-        <f>E43*2</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G43" s="29" t="s">
@@ -12067,7 +12062,7 @@
         <v>5</v>
       </c>
       <c r="F44" s="29">
-        <f>E44*2</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="G44" s="29" t="s">
@@ -12102,7 +12097,7 @@
         <v>6</v>
       </c>
       <c r="F45" s="29">
-        <f>E45*2</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="G45" s="29" t="s">
@@ -12137,7 +12132,7 @@
         <v>7</v>
       </c>
       <c r="F46" s="29">
-        <f>E46*2</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="G46" s="29" t="s">
@@ -12172,7 +12167,7 @@
         <v>6</v>
       </c>
       <c r="F47" s="29">
-        <f>E47*2</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="G47" s="29" t="s">
@@ -12207,7 +12202,7 @@
         <v>6</v>
       </c>
       <c r="F48" s="29">
-        <f>E48*2</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="G48" s="29" t="s">
@@ -12242,7 +12237,7 @@
         <v>5</v>
       </c>
       <c r="F49" s="29">
-        <f>E49*2</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="G49" s="29" t="s">
@@ -12277,7 +12272,7 @@
         <v>5</v>
       </c>
       <c r="F50" s="29">
-        <f>E50*2</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="G50" s="29" t="s">
@@ -12312,7 +12307,7 @@
         <v>7</v>
       </c>
       <c r="F51" s="29">
-        <f>E51*2</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="G51" s="29" t="s">
@@ -12347,7 +12342,7 @@
         <v>5</v>
       </c>
       <c r="F52" s="29">
-        <f>E52*2</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="G52" s="29" t="s">
@@ -12382,7 +12377,7 @@
         <v>5</v>
       </c>
       <c r="F53" s="29">
-        <f>E53*2</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="G53" s="29" t="s">
@@ -12417,7 +12412,7 @@
         <v>6</v>
       </c>
       <c r="F54" s="29">
-        <f>E54*2</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="G54" s="29" t="s">
@@ -12452,7 +12447,7 @@
         <v>5</v>
       </c>
       <c r="F55" s="29">
-        <f>E55*2</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="G55" s="29" t="s">
@@ -12487,7 +12482,7 @@
         <v>6</v>
       </c>
       <c r="F56" s="29">
-        <f>E56*2</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="G56" s="29" t="s">
@@ -12522,7 +12517,7 @@
         <v>7</v>
       </c>
       <c r="F57" s="29">
-        <f>E57*2</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="G57" s="29" t="s">
@@ -12557,7 +12552,7 @@
         <v>6</v>
       </c>
       <c r="F58" s="29">
-        <f>E58*2</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="G58" s="29" t="s">
@@ -12592,7 +12587,7 @@
         <v>5</v>
       </c>
       <c r="F59" s="29">
-        <f>E59*2</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="G59" s="29" t="s">
@@ -12627,7 +12622,7 @@
         <v>6</v>
       </c>
       <c r="F60" s="29">
-        <f>E60*2</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="G60" s="29" t="s">
@@ -12662,7 +12657,7 @@
         <v>7</v>
       </c>
       <c r="F61" s="29">
-        <f>E61*2</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="G61" s="29" t="s">
@@ -12697,7 +12692,7 @@
         <v>5</v>
       </c>
       <c r="F62" s="29">
-        <f>E62*2</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="G62" s="29" t="s">
@@ -12732,7 +12727,7 @@
         <v>5</v>
       </c>
       <c r="F63" s="29">
-        <f>E63*2</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="G63" s="29" t="s">
@@ -12767,7 +12762,7 @@
         <v>8</v>
       </c>
       <c r="F64" s="29">
-        <f>E64*2</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="G64" s="29" t="s">
@@ -12802,7 +12797,7 @@
         <v>8</v>
       </c>
       <c r="F65" s="29">
-        <f>E65*2</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="G65" s="29" t="s">
@@ -12837,7 +12832,7 @@
         <v>8</v>
       </c>
       <c r="F66" s="29">
-        <f>E66*2</f>
+        <f t="shared" ref="F66:F97" si="2">E66*2</f>
         <v>16</v>
       </c>
       <c r="G66" s="29" t="s">
@@ -12872,7 +12867,7 @@
         <v>8</v>
       </c>
       <c r="F67" s="29">
-        <f>E67*2</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G67" s="29" t="s">
@@ -12907,7 +12902,7 @@
         <v>8</v>
       </c>
       <c r="F68" s="29">
-        <f>E68*2</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G68" s="29" t="s">
@@ -12942,7 +12937,7 @@
         <v>8</v>
       </c>
       <c r="F69" s="29">
-        <f>E69*2</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G69" s="29" t="s">
@@ -12977,7 +12972,7 @@
         <v>8</v>
       </c>
       <c r="F70" s="29">
-        <f>E70*2</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G70" s="29" t="s">
@@ -13012,7 +13007,7 @@
         <v>7</v>
       </c>
       <c r="F71" s="29">
-        <f>E71*2</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="G71" s="29" t="s">
@@ -13047,7 +13042,7 @@
         <v>8</v>
       </c>
       <c r="F72" s="29">
-        <f>E72*2</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G72" s="29" t="s">
@@ -13082,7 +13077,7 @@
         <v>7</v>
       </c>
       <c r="F73" s="29">
-        <f>E73*2</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="G73" s="29" t="s">
@@ -13117,7 +13112,7 @@
         <v>8</v>
       </c>
       <c r="F74" s="29">
-        <f>E74*2</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G74" s="29" t="s">
@@ -13152,7 +13147,7 @@
         <v>7</v>
       </c>
       <c r="F75" s="29">
-        <f>E75*2</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="G75" s="29" t="s">
@@ -13187,7 +13182,7 @@
         <v>8</v>
       </c>
       <c r="F76" s="29">
-        <f>E76*2</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G76" s="29" t="s">
@@ -13222,7 +13217,7 @@
         <v>7</v>
       </c>
       <c r="F77" s="29">
-        <f>E77*2</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="G77" s="29" t="s">
@@ -13257,7 +13252,7 @@
         <v>8</v>
       </c>
       <c r="F78" s="29">
-        <f>E78*2</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G78" s="29" t="s">
@@ -13292,7 +13287,7 @@
         <v>7</v>
       </c>
       <c r="F79" s="29">
-        <f>E79*2</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="G79" s="29" t="s">
@@ -13327,7 +13322,7 @@
         <v>8</v>
       </c>
       <c r="F80" s="29">
-        <f>E80*2</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G80" s="29" t="s">
@@ -13362,7 +13357,7 @@
         <v>8</v>
       </c>
       <c r="F81" s="29">
-        <f>E81*2</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G81" s="29" t="s">
@@ -13397,7 +13392,7 @@
         <v>8</v>
       </c>
       <c r="F82" s="29">
-        <f>E82*2</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G82" s="29" t="s">
@@ -13432,7 +13427,7 @@
         <v>8</v>
       </c>
       <c r="F83" s="29">
-        <f>E83*2</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G83" s="29" t="s">
@@ -13467,7 +13462,7 @@
         <v>8</v>
       </c>
       <c r="F84" s="29">
-        <f>E84*2</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G84" s="29" t="s">
@@ -13502,7 +13497,7 @@
         <v>7</v>
       </c>
       <c r="F85" s="29">
-        <f>E85*2</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="G85" s="29" t="s">
@@ -13537,7 +13532,7 @@
         <v>8</v>
       </c>
       <c r="F86" s="29">
-        <f>E86*2</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G86" s="29" t="s">
@@ -13572,7 +13567,7 @@
         <v>8</v>
       </c>
       <c r="F87" s="29">
-        <f>E87*2</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G87" s="29" t="s">
@@ -13607,7 +13602,7 @@
         <v>10</v>
       </c>
       <c r="F88" s="29">
-        <f>E88*2</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="G88" s="29" t="s">
@@ -13642,7 +13637,7 @@
         <v>9</v>
       </c>
       <c r="F89" s="29">
-        <f>E89*2</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G89" s="29" t="s">
@@ -13679,7 +13674,7 @@
         <v>9</v>
       </c>
       <c r="F90" s="29">
-        <f>E90*2</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G90" s="29" t="s">
@@ -13714,7 +13709,7 @@
         <v>9</v>
       </c>
       <c r="F91" s="29">
-        <f>E91*2</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G91" s="29" t="s">
@@ -13749,7 +13744,7 @@
         <v>10</v>
       </c>
       <c r="F92" s="29">
-        <f>E92*2</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="G92" s="29" t="s">
@@ -13784,7 +13779,7 @@
         <v>9</v>
       </c>
       <c r="F93" s="29">
-        <f>E93*2</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G93" s="29" t="s">
@@ -13821,7 +13816,7 @@
         <v>9</v>
       </c>
       <c r="F94" s="29">
-        <f>E94*2</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G94" s="29" t="s">
@@ -13858,7 +13853,7 @@
         <v>9</v>
       </c>
       <c r="F95" s="29">
-        <f>E95*2</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G95" s="29" t="s">
@@ -13895,7 +13890,7 @@
         <v>9</v>
       </c>
       <c r="F96" s="29">
-        <f>E96*2</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G96" s="29" t="s">
@@ -13932,7 +13927,7 @@
         <v>9</v>
       </c>
       <c r="F97" s="29">
-        <f>E97*2</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G97" s="29" t="s">
@@ -13969,7 +13964,7 @@
         <v>9</v>
       </c>
       <c r="F98" s="29">
-        <f>E98*2</f>
+        <f t="shared" ref="F98:F129" si="3">E98*2</f>
         <v>18</v>
       </c>
       <c r="G98" s="29" t="s">
@@ -14006,7 +14001,7 @@
         <v>10</v>
       </c>
       <c r="F99" s="29">
-        <f>E99*2</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="G99" s="29" t="s">
@@ -14041,7 +14036,7 @@
         <v>9</v>
       </c>
       <c r="F100" s="29">
-        <f>E100*2</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G100" s="29" t="s">
@@ -14076,7 +14071,7 @@
         <v>10</v>
       </c>
       <c r="F101" s="29">
-        <f>E101*2</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="G101" s="29" t="s">
@@ -14111,7 +14106,7 @@
         <v>14</v>
       </c>
       <c r="F102" s="29">
-        <f>E102*2</f>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="G102" s="29" t="s">
@@ -14146,7 +14141,7 @@
         <v>9</v>
       </c>
       <c r="F103" s="29">
-        <f>E103*2</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G103" s="29" t="s">
@@ -14181,7 +14176,7 @@
         <v>10</v>
       </c>
       <c r="F104" s="29">
-        <f>E104*2</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="G104" s="29" t="s">
@@ -14216,7 +14211,7 @@
         <v>9</v>
       </c>
       <c r="F105" s="29">
-        <f>E105*2</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G105" s="29" t="s">
@@ -14251,7 +14246,7 @@
         <v>10</v>
       </c>
       <c r="F106" s="29">
-        <f>E106*2</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="G106" s="29" t="s">
@@ -14288,7 +14283,7 @@
         <v>10</v>
       </c>
       <c r="F107" s="29">
-        <f>E107*2</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="G107" s="29" t="s">
@@ -14325,7 +14320,7 @@
         <v>10</v>
       </c>
       <c r="F108" s="29">
-        <f>E108*2</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="G108" s="29" t="s">
@@ -14362,7 +14357,7 @@
         <v>10</v>
       </c>
       <c r="F109" s="29">
-        <f>E109*2</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="G109" s="29" t="s">
@@ -14399,7 +14394,7 @@
         <v>10</v>
       </c>
       <c r="F110" s="29">
-        <f>E110*2</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="G110" s="29" t="s">
@@ -14436,7 +14431,7 @@
         <v>10</v>
       </c>
       <c r="F111" s="29">
-        <f>E111*2</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="G111" s="29" t="s">
@@ -14473,7 +14468,7 @@
         <v>10</v>
       </c>
       <c r="F112" s="29">
-        <f>E112*2</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="G112" s="29" t="s">
@@ -14510,7 +14505,7 @@
         <v>10</v>
       </c>
       <c r="F113" s="29">
-        <f>E113*2</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="G113" s="29" t="s">
@@ -14547,7 +14542,7 @@
         <v>10</v>
       </c>
       <c r="F114" s="29">
-        <f>E114*2</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="G114" s="29" t="s">
@@ -14582,7 +14577,7 @@
         <v>9</v>
       </c>
       <c r="F115" s="29">
-        <f>E115*2</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G115" s="29" t="s">
@@ -14617,7 +14612,7 @@
         <v>9</v>
       </c>
       <c r="F116" s="29">
-        <f>E116*2</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G116" s="29" t="s">
@@ -14652,7 +14647,7 @@
         <v>10</v>
       </c>
       <c r="F117" s="29">
-        <f>E117*2</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="G117" s="29" t="s">
@@ -14687,7 +14682,7 @@
         <v>10</v>
       </c>
       <c r="F118" s="29">
-        <f>E118*2</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="G118" s="29" t="s">
@@ -14722,7 +14717,7 @@
         <v>10</v>
       </c>
       <c r="F119" s="29">
-        <f>E119*2</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="G119" s="29" t="s">
@@ -14757,7 +14752,7 @@
         <v>12</v>
       </c>
       <c r="F120" s="29">
-        <f>E120*2</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="G120" s="29" t="s">
@@ -14792,7 +14787,7 @@
         <v>12</v>
       </c>
       <c r="F121" s="29">
-        <f>E121*2</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="G121" s="29" t="s">
@@ -14827,7 +14822,7 @@
         <v>14</v>
       </c>
       <c r="F122" s="29">
-        <f>E122*2</f>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="G122" s="29" t="s">
@@ -14862,7 +14857,7 @@
         <v>12</v>
       </c>
       <c r="F123" s="29">
-        <f>E123*2</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="G123" s="29" t="s">
@@ -14897,7 +14892,7 @@
         <v>12</v>
       </c>
       <c r="F124" s="29">
-        <f>E124*2</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="G124" s="29" t="s">
@@ -14932,7 +14927,7 @@
         <v>12</v>
       </c>
       <c r="F125" s="29">
-        <f>E125*2</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="G125" s="29" t="s">
@@ -14967,7 +14962,7 @@
         <v>12</v>
       </c>
       <c r="F126" s="29">
-        <f>E126*2</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="G126" s="29" t="s">
@@ -15002,7 +14997,7 @@
         <v>16</v>
       </c>
       <c r="F127" s="29">
-        <f>E127*2</f>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="G127" s="29" t="s">
@@ -15037,7 +15032,7 @@
         <v>13</v>
       </c>
       <c r="F128" s="29">
-        <f>E128*2</f>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="G128" s="29" t="s">
@@ -15072,7 +15067,7 @@
         <v>12</v>
       </c>
       <c r="F129" s="29">
-        <f>E129*2</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="G129" s="29" t="s">
@@ -15107,7 +15102,7 @@
         <v>12</v>
       </c>
       <c r="F130" s="29">
-        <f>E130*2</f>
+        <f t="shared" ref="F130:F161" si="4">E130*2</f>
         <v>24</v>
       </c>
       <c r="G130" s="29" t="s">
@@ -15142,7 +15137,7 @@
         <v>12</v>
       </c>
       <c r="F131" s="29">
-        <f>E131*2</f>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="G131" s="29" t="s">
@@ -15177,7 +15172,7 @@
         <v>12</v>
       </c>
       <c r="F132" s="29">
-        <f>E132*2</f>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="G132" s="29" t="s">
@@ -15212,7 +15207,7 @@
         <v>13</v>
       </c>
       <c r="F133" s="29">
-        <f>E133*2</f>
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
       <c r="G133" s="29" t="s">
@@ -15249,7 +15244,7 @@
         <v>13</v>
       </c>
       <c r="F134" s="29">
-        <f>E134*2</f>
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
       <c r="G134" s="29" t="s">
@@ -15284,7 +15279,7 @@
         <v>10</v>
       </c>
       <c r="F135" s="29">
-        <f>E135*2</f>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="G135" s="29" t="s">
@@ -15319,7 +15314,7 @@
         <v>14</v>
       </c>
       <c r="F136" s="29">
-        <f>E136*2</f>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="G136" s="29" t="s">
@@ -15354,7 +15349,7 @@
         <v>14</v>
       </c>
       <c r="F137" s="29">
-        <f>E137*2</f>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="G137" s="29" t="s">
@@ -15389,7 +15384,7 @@
         <v>14</v>
       </c>
       <c r="F138" s="29">
-        <f>E138*2</f>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="G138" s="29" t="s">
@@ -15424,7 +15419,7 @@
         <v>14</v>
       </c>
       <c r="F139" s="29">
-        <f>E139*2</f>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="G139" s="29" t="s">
@@ -15459,7 +15454,7 @@
         <v>13</v>
       </c>
       <c r="F140" s="29">
-        <f>E140*2</f>
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
       <c r="G140" s="29" t="s">
@@ -15494,7 +15489,7 @@
         <v>14</v>
       </c>
       <c r="F141" s="29">
-        <f>E141*2</f>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="G141" s="29" t="s">
@@ -15529,7 +15524,7 @@
         <v>15</v>
       </c>
       <c r="F142" s="29">
-        <f>E142*2</f>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="G142" s="29" t="s">
@@ -15564,7 +15559,7 @@
         <v>15</v>
       </c>
       <c r="F143" s="29">
-        <f>E143*2</f>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="G143" s="29" t="s">
@@ -15599,7 +15594,7 @@
         <v>16</v>
       </c>
       <c r="F144" s="29">
-        <f>E144*2</f>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="G144" s="29" t="s">
@@ -15634,7 +15629,7 @@
         <v>18</v>
       </c>
       <c r="F145" s="29">
-        <f>E145*2</f>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="G145" s="29" t="s">
@@ -15669,7 +15664,7 @@
         <v>18</v>
       </c>
       <c r="F146" s="29">
-        <f>E146*2</f>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="G146" s="29" t="s">
@@ -15704,7 +15699,7 @@
         <v>18</v>
       </c>
       <c r="F147" s="29">
-        <f>E147*2</f>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="G147" s="29" t="s">
@@ -15739,7 +15734,7 @@
         <v>20</v>
       </c>
       <c r="F148" s="29">
-        <f>E148*2</f>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="G148" s="29" t="s">
@@ -15774,7 +15769,7 @@
         <v>20</v>
       </c>
       <c r="F149" s="29">
-        <f>E149*2</f>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="G149" s="29" t="s">
@@ -15809,7 +15804,7 @@
         <v>20</v>
       </c>
       <c r="F150" s="29">
-        <f>E150*2</f>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="G150" s="29" t="s">
@@ -15844,7 +15839,7 @@
         <v>20</v>
       </c>
       <c r="F151" s="29">
-        <f>E151*2</f>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="G151" s="29" t="s">
@@ -15866,7 +15861,7 @@
       <c r="A152" s="29" t="s">
         <v>1857</v>
       </c>
-      <c r="B152" s="36" t="s">
+      <c r="B152" s="30" t="s">
         <v>1399</v>
       </c>
       <c r="C152" s="29" t="s">
@@ -15879,7 +15874,7 @@
         <v>20</v>
       </c>
       <c r="F152" s="29">
-        <f>E152*2</f>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="G152" s="29" t="s">
@@ -15901,7 +15896,7 @@
       <c r="A153" s="29" t="s">
         <v>1784</v>
       </c>
-      <c r="B153" s="36" t="s">
+      <c r="B153" s="30" t="s">
         <v>1399</v>
       </c>
       <c r="C153" s="29" t="s">
@@ -15914,7 +15909,7 @@
         <v>18</v>
       </c>
       <c r="F153" s="29">
-        <f>E153*2</f>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="G153" s="29" t="s">
@@ -15949,10 +15944,9 @@
       </c>
     </row>
     <row r="156" spans="1:12">
-      <c r="A156" s="30" t="s">
+      <c r="A156" t="s">
         <v>1695</v>
       </c>
-      <c r="D156" s="30"/>
       <c r="I156" t="s">
         <v>2132</v>
       </c>
@@ -16142,7 +16136,7 @@
       </c>
     </row>
     <row r="180" spans="1:9">
-      <c r="A180" s="30" t="s">
+      <c r="A180" t="s">
         <v>1861</v>
       </c>
       <c r="I180" t="s">
@@ -16150,7 +16144,7 @@
       </c>
     </row>
     <row r="181" spans="1:9">
-      <c r="A181" s="30" t="s">
+      <c r="A181" t="s">
         <v>1865</v>
       </c>
       <c r="I181" t="s">
@@ -16174,7 +16168,7 @@
       </c>
     </row>
     <row r="184" spans="1:9">
-      <c r="A184" s="30" t="s">
+      <c r="A184" t="s">
         <v>1869</v>
       </c>
       <c r="I184" t="s">

</xml_diff>

<commit_message>
Making an arcane version of Wondrous Recall potion
</commit_message>
<xml_diff>
--- a/.research/research.xlsx
+++ b/.research/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Game Mods\Baldur's Gate\Caster Crafting\.research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510D09F9-40D6-406E-8D3F-40CFF8D338A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F5A057-E20A-4CCC-A770-ED4498A33D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="7" activeTab="11" xr2:uid="{73FDBA9F-2EEA-4C02-A136-1EA93E7B6B65}"/>
   </bookViews>
@@ -27,6 +27,9 @@
     <sheet name="Mapping Potions" sheetId="13" r:id="rId12"/>
     <sheet name="Potions (IWD2)" sheetId="9" r:id="rId13"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Mapping Potions'!$A$1:$M$191</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId14"/>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11520" uniqueCount="2140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11524" uniqueCount="2141">
   <si>
     <t>Caster Level</t>
   </si>
@@ -6460,6 +6463,9 @@
   </si>
   <si>
     <t>Broken?</t>
+  </si>
+  <si>
+    <t>wondrous-recall-arcane.BAM</t>
   </si>
 </sst>
 </file>
@@ -6679,6 +6685,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6692,9 +6701,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -8269,13 +8275,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>1404</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" s="23"/>
@@ -10515,8 +10521,8 @@
   <dimension ref="A1:M191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C125" sqref="C125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -10589,7 +10595,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="29">
-        <f t="shared" ref="F2:F33" si="0">E2*2</f>
+        <f>E2*2</f>
         <v>4</v>
       </c>
       <c r="G2" s="29" t="s">
@@ -10624,7 +10630,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="29">
-        <f t="shared" si="0"/>
+        <f>E3*2</f>
         <v>6</v>
       </c>
       <c r="G3" s="29" t="s">
@@ -10659,7 +10665,7 @@
         <v>2</v>
       </c>
       <c r="F4" s="29">
-        <f t="shared" si="0"/>
+        <f>E4*2</f>
         <v>4</v>
       </c>
       <c r="G4" s="29" t="s">
@@ -10694,7 +10700,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="29">
-        <f t="shared" si="0"/>
+        <f>E5*2</f>
         <v>20</v>
       </c>
       <c r="G5" s="29" t="s">
@@ -10729,13 +10735,13 @@
         <v>4</v>
       </c>
       <c r="F6" s="29">
-        <f t="shared" si="0"/>
+        <f>E6*2</f>
         <v>8</v>
       </c>
       <c r="G6" s="29" t="s">
         <v>2110</v>
       </c>
-      <c r="H6" s="36" t="s">
+      <c r="H6" s="31" t="s">
         <v>2139</v>
       </c>
       <c r="I6" s="29" t="s">
@@ -10764,7 +10770,7 @@
         <v>4</v>
       </c>
       <c r="F7" s="29">
-        <f t="shared" si="0"/>
+        <f>E7*2</f>
         <v>8</v>
       </c>
       <c r="G7" s="29" t="s">
@@ -10799,7 +10805,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="29">
-        <f t="shared" si="0"/>
+        <f>E8*2</f>
         <v>4</v>
       </c>
       <c r="G8" s="29" t="s">
@@ -10834,7 +10840,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="29">
-        <f t="shared" si="0"/>
+        <f>E9*2</f>
         <v>6</v>
       </c>
       <c r="G9" s="29" t="s">
@@ -10869,7 +10875,7 @@
         <v>4</v>
       </c>
       <c r="F10" s="29">
-        <f t="shared" si="0"/>
+        <f>E10*2</f>
         <v>8</v>
       </c>
       <c r="G10" s="29" t="s">
@@ -10904,7 +10910,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="29">
-        <f t="shared" si="0"/>
+        <f>E11*2</f>
         <v>4</v>
       </c>
       <c r="G11" s="29" t="s">
@@ -10939,7 +10945,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="29">
-        <f t="shared" si="0"/>
+        <f>E12*2</f>
         <v>4</v>
       </c>
       <c r="G12" s="29" t="s">
@@ -10974,7 +10980,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="29">
-        <f t="shared" si="0"/>
+        <f>E13*2</f>
         <v>4</v>
       </c>
       <c r="G13" s="29" t="s">
@@ -11009,7 +11015,7 @@
         <v>2</v>
       </c>
       <c r="F14" s="29">
-        <f t="shared" si="0"/>
+        <f>E14*2</f>
         <v>4</v>
       </c>
       <c r="G14" s="29" t="s">
@@ -11044,7 +11050,7 @@
         <v>2</v>
       </c>
       <c r="F15" s="29">
-        <f t="shared" si="0"/>
+        <f>E15*2</f>
         <v>4</v>
       </c>
       <c r="G15" s="29" t="s">
@@ -11079,7 +11085,7 @@
         <v>2</v>
       </c>
       <c r="F16" s="29">
-        <f t="shared" si="0"/>
+        <f>E16*2</f>
         <v>4</v>
       </c>
       <c r="G16" s="29" t="s">
@@ -11114,7 +11120,7 @@
         <v>2</v>
       </c>
       <c r="F17" s="29">
-        <f t="shared" si="0"/>
+        <f>E17*2</f>
         <v>4</v>
       </c>
       <c r="G17" s="29" t="s">
@@ -11152,7 +11158,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="29">
-        <f t="shared" si="0"/>
+        <f>E18*2</f>
         <v>2</v>
       </c>
       <c r="G18" s="29" t="s">
@@ -11187,7 +11193,7 @@
         <v>2</v>
       </c>
       <c r="F19" s="29">
-        <f t="shared" si="0"/>
+        <f>E19*2</f>
         <v>4</v>
       </c>
       <c r="G19" s="29" t="s">
@@ -11222,7 +11228,7 @@
         <v>2</v>
       </c>
       <c r="F20" s="29">
-        <f t="shared" si="0"/>
+        <f>E20*2</f>
         <v>4</v>
       </c>
       <c r="G20" s="29" t="s">
@@ -11257,7 +11263,7 @@
         <v>4</v>
       </c>
       <c r="F21" s="29">
-        <f t="shared" si="0"/>
+        <f>E21*2</f>
         <v>8</v>
       </c>
       <c r="G21" s="29" t="s">
@@ -11292,7 +11298,7 @@
         <v>4</v>
       </c>
       <c r="F22" s="29">
-        <f t="shared" si="0"/>
+        <f>E22*2</f>
         <v>8</v>
       </c>
       <c r="G22" s="29" t="s">
@@ -11327,7 +11333,7 @@
         <v>3</v>
       </c>
       <c r="F23" s="29">
-        <f t="shared" si="0"/>
+        <f>E23*2</f>
         <v>6</v>
       </c>
       <c r="G23" s="29" t="s">
@@ -11362,7 +11368,7 @@
         <v>4</v>
       </c>
       <c r="F24" s="29">
-        <f t="shared" si="0"/>
+        <f>E24*2</f>
         <v>8</v>
       </c>
       <c r="G24" s="29" t="s">
@@ -11397,7 +11403,7 @@
         <v>5</v>
       </c>
       <c r="F25" s="29">
-        <f t="shared" si="0"/>
+        <f>E25*2</f>
         <v>10</v>
       </c>
       <c r="G25" s="29" t="s">
@@ -11432,7 +11438,7 @@
         <v>3</v>
       </c>
       <c r="F26" s="29">
-        <f t="shared" si="0"/>
+        <f>E26*2</f>
         <v>6</v>
       </c>
       <c r="G26" s="29" t="s">
@@ -11467,7 +11473,7 @@
         <v>4</v>
       </c>
       <c r="F27" s="29">
-        <f t="shared" si="0"/>
+        <f>E27*2</f>
         <v>8</v>
       </c>
       <c r="G27" s="29" t="s">
@@ -11502,7 +11508,7 @@
         <v>4</v>
       </c>
       <c r="F28" s="29">
-        <f t="shared" si="0"/>
+        <f>E28*2</f>
         <v>8</v>
       </c>
       <c r="G28" s="29" t="s">
@@ -11537,7 +11543,7 @@
         <v>5</v>
       </c>
       <c r="F29" s="29">
-        <f t="shared" si="0"/>
+        <f>E29*2</f>
         <v>10</v>
       </c>
       <c r="G29" s="29" t="s">
@@ -11572,7 +11578,7 @@
         <v>4</v>
       </c>
       <c r="F30" s="29">
-        <f t="shared" si="0"/>
+        <f>E30*2</f>
         <v>8</v>
       </c>
       <c r="G30" s="29" t="s">
@@ -11607,7 +11613,7 @@
         <v>5</v>
       </c>
       <c r="F31" s="29">
-        <f t="shared" si="0"/>
+        <f>E31*2</f>
         <v>10</v>
       </c>
       <c r="G31" s="29" t="s">
@@ -11642,7 +11648,7 @@
         <v>5</v>
       </c>
       <c r="F32" s="29">
-        <f t="shared" si="0"/>
+        <f>E32*2</f>
         <v>10</v>
       </c>
       <c r="G32" s="29" t="s">
@@ -11677,7 +11683,7 @@
         <v>5</v>
       </c>
       <c r="F33" s="29">
-        <f t="shared" si="0"/>
+        <f>E33*2</f>
         <v>10</v>
       </c>
       <c r="G33" s="29" t="s">
@@ -11712,7 +11718,7 @@
         <v>4</v>
       </c>
       <c r="F34" s="29">
-        <f t="shared" ref="F34:F65" si="1">E34*2</f>
+        <f>E34*2</f>
         <v>8</v>
       </c>
       <c r="G34" s="29" t="s">
@@ -11747,7 +11753,7 @@
         <v>3</v>
       </c>
       <c r="F35" s="29">
-        <f t="shared" si="1"/>
+        <f>E35*2</f>
         <v>6</v>
       </c>
       <c r="G35" s="29" t="s">
@@ -11782,7 +11788,7 @@
         <v>4</v>
       </c>
       <c r="F36" s="29">
-        <f t="shared" si="1"/>
+        <f>E36*2</f>
         <v>8</v>
       </c>
       <c r="G36" s="29" t="s">
@@ -11817,7 +11823,7 @@
         <v>4</v>
       </c>
       <c r="F37" s="29">
-        <f t="shared" si="1"/>
+        <f>E37*2</f>
         <v>8</v>
       </c>
       <c r="G37" s="29" t="s">
@@ -11852,7 +11858,7 @@
         <v>4</v>
       </c>
       <c r="F38" s="29">
-        <f t="shared" si="1"/>
+        <f>E38*2</f>
         <v>8</v>
       </c>
       <c r="G38" s="29" t="s">
@@ -11887,7 +11893,7 @@
         <v>4</v>
       </c>
       <c r="F39" s="29">
-        <f t="shared" si="1"/>
+        <f>E39*2</f>
         <v>8</v>
       </c>
       <c r="G39" s="29" t="s">
@@ -11922,7 +11928,7 @@
         <v>4</v>
       </c>
       <c r="F40" s="29">
-        <f t="shared" si="1"/>
+        <f>E40*2</f>
         <v>8</v>
       </c>
       <c r="G40" s="29" t="s">
@@ -11957,7 +11963,7 @@
         <v>4</v>
       </c>
       <c r="F41" s="29">
-        <f t="shared" si="1"/>
+        <f>E41*2</f>
         <v>8</v>
       </c>
       <c r="G41" s="29" t="s">
@@ -11992,7 +11998,7 @@
         <v>4</v>
       </c>
       <c r="F42" s="29">
-        <f t="shared" si="1"/>
+        <f>E42*2</f>
         <v>8</v>
       </c>
       <c r="G42" s="29" t="s">
@@ -12027,7 +12033,7 @@
         <v>4</v>
       </c>
       <c r="F43" s="29">
-        <f t="shared" si="1"/>
+        <f>E43*2</f>
         <v>8</v>
       </c>
       <c r="G43" s="29" t="s">
@@ -12062,7 +12068,7 @@
         <v>5</v>
       </c>
       <c r="F44" s="29">
-        <f t="shared" si="1"/>
+        <f>E44*2</f>
         <v>10</v>
       </c>
       <c r="G44" s="29" t="s">
@@ -12097,7 +12103,7 @@
         <v>6</v>
       </c>
       <c r="F45" s="29">
-        <f t="shared" si="1"/>
+        <f>E45*2</f>
         <v>12</v>
       </c>
       <c r="G45" s="29" t="s">
@@ -12132,7 +12138,7 @@
         <v>7</v>
       </c>
       <c r="F46" s="29">
-        <f t="shared" si="1"/>
+        <f>E46*2</f>
         <v>14</v>
       </c>
       <c r="G46" s="29" t="s">
@@ -12167,7 +12173,7 @@
         <v>6</v>
       </c>
       <c r="F47" s="29">
-        <f t="shared" si="1"/>
+        <f>E47*2</f>
         <v>12</v>
       </c>
       <c r="G47" s="29" t="s">
@@ -12202,7 +12208,7 @@
         <v>6</v>
       </c>
       <c r="F48" s="29">
-        <f t="shared" si="1"/>
+        <f>E48*2</f>
         <v>12</v>
       </c>
       <c r="G48" s="29" t="s">
@@ -12237,7 +12243,7 @@
         <v>5</v>
       </c>
       <c r="F49" s="29">
-        <f t="shared" si="1"/>
+        <f>E49*2</f>
         <v>10</v>
       </c>
       <c r="G49" s="29" t="s">
@@ -12272,7 +12278,7 @@
         <v>5</v>
       </c>
       <c r="F50" s="29">
-        <f t="shared" si="1"/>
+        <f>E50*2</f>
         <v>10</v>
       </c>
       <c r="G50" s="29" t="s">
@@ -12307,7 +12313,7 @@
         <v>7</v>
       </c>
       <c r="F51" s="29">
-        <f t="shared" si="1"/>
+        <f>E51*2</f>
         <v>14</v>
       </c>
       <c r="G51" s="29" t="s">
@@ -12342,7 +12348,7 @@
         <v>5</v>
       </c>
       <c r="F52" s="29">
-        <f t="shared" si="1"/>
+        <f>E52*2</f>
         <v>10</v>
       </c>
       <c r="G52" s="29" t="s">
@@ -12377,7 +12383,7 @@
         <v>5</v>
       </c>
       <c r="F53" s="29">
-        <f t="shared" si="1"/>
+        <f>E53*2</f>
         <v>10</v>
       </c>
       <c r="G53" s="29" t="s">
@@ -12412,7 +12418,7 @@
         <v>6</v>
       </c>
       <c r="F54" s="29">
-        <f t="shared" si="1"/>
+        <f>E54*2</f>
         <v>12</v>
       </c>
       <c r="G54" s="29" t="s">
@@ -12447,7 +12453,7 @@
         <v>5</v>
       </c>
       <c r="F55" s="29">
-        <f t="shared" si="1"/>
+        <f>E55*2</f>
         <v>10</v>
       </c>
       <c r="G55" s="29" t="s">
@@ -12482,7 +12488,7 @@
         <v>6</v>
       </c>
       <c r="F56" s="29">
-        <f t="shared" si="1"/>
+        <f>E56*2</f>
         <v>12</v>
       </c>
       <c r="G56" s="29" t="s">
@@ -12517,7 +12523,7 @@
         <v>7</v>
       </c>
       <c r="F57" s="29">
-        <f t="shared" si="1"/>
+        <f>E57*2</f>
         <v>14</v>
       </c>
       <c r="G57" s="29" t="s">
@@ -12552,7 +12558,7 @@
         <v>6</v>
       </c>
       <c r="F58" s="29">
-        <f t="shared" si="1"/>
+        <f>E58*2</f>
         <v>12</v>
       </c>
       <c r="G58" s="29" t="s">
@@ -12587,7 +12593,7 @@
         <v>5</v>
       </c>
       <c r="F59" s="29">
-        <f t="shared" si="1"/>
+        <f>E59*2</f>
         <v>10</v>
       </c>
       <c r="G59" s="29" t="s">
@@ -12622,7 +12628,7 @@
         <v>6</v>
       </c>
       <c r="F60" s="29">
-        <f t="shared" si="1"/>
+        <f>E60*2</f>
         <v>12</v>
       </c>
       <c r="G60" s="29" t="s">
@@ -12657,7 +12663,7 @@
         <v>7</v>
       </c>
       <c r="F61" s="29">
-        <f t="shared" si="1"/>
+        <f>E61*2</f>
         <v>14</v>
       </c>
       <c r="G61" s="29" t="s">
@@ -12692,7 +12698,7 @@
         <v>5</v>
       </c>
       <c r="F62" s="29">
-        <f t="shared" si="1"/>
+        <f>E62*2</f>
         <v>10</v>
       </c>
       <c r="G62" s="29" t="s">
@@ -12727,7 +12733,7 @@
         <v>5</v>
       </c>
       <c r="F63" s="29">
-        <f t="shared" si="1"/>
+        <f>E63*2</f>
         <v>10</v>
       </c>
       <c r="G63" s="29" t="s">
@@ -12762,7 +12768,7 @@
         <v>8</v>
       </c>
       <c r="F64" s="29">
-        <f t="shared" si="1"/>
+        <f>E64*2</f>
         <v>16</v>
       </c>
       <c r="G64" s="29" t="s">
@@ -12797,7 +12803,7 @@
         <v>8</v>
       </c>
       <c r="F65" s="29">
-        <f t="shared" si="1"/>
+        <f>E65*2</f>
         <v>16</v>
       </c>
       <c r="G65" s="29" t="s">
@@ -12832,7 +12838,7 @@
         <v>8</v>
       </c>
       <c r="F66" s="29">
-        <f t="shared" ref="F66:F97" si="2">E66*2</f>
+        <f>E66*2</f>
         <v>16</v>
       </c>
       <c r="G66" s="29" t="s">
@@ -12867,7 +12873,7 @@
         <v>8</v>
       </c>
       <c r="F67" s="29">
-        <f t="shared" si="2"/>
+        <f>E67*2</f>
         <v>16</v>
       </c>
       <c r="G67" s="29" t="s">
@@ -12902,7 +12908,7 @@
         <v>8</v>
       </c>
       <c r="F68" s="29">
-        <f t="shared" si="2"/>
+        <f>E68*2</f>
         <v>16</v>
       </c>
       <c r="G68" s="29" t="s">
@@ -12937,7 +12943,7 @@
         <v>8</v>
       </c>
       <c r="F69" s="29">
-        <f t="shared" si="2"/>
+        <f>E69*2</f>
         <v>16</v>
       </c>
       <c r="G69" s="29" t="s">
@@ -12972,7 +12978,7 @@
         <v>8</v>
       </c>
       <c r="F70" s="29">
-        <f t="shared" si="2"/>
+        <f>E70*2</f>
         <v>16</v>
       </c>
       <c r="G70" s="29" t="s">
@@ -13007,7 +13013,7 @@
         <v>7</v>
       </c>
       <c r="F71" s="29">
-        <f t="shared" si="2"/>
+        <f>E71*2</f>
         <v>14</v>
       </c>
       <c r="G71" s="29" t="s">
@@ -13042,7 +13048,7 @@
         <v>8</v>
       </c>
       <c r="F72" s="29">
-        <f t="shared" si="2"/>
+        <f>E72*2</f>
         <v>16</v>
       </c>
       <c r="G72" s="29" t="s">
@@ -13077,7 +13083,7 @@
         <v>7</v>
       </c>
       <c r="F73" s="29">
-        <f t="shared" si="2"/>
+        <f>E73*2</f>
         <v>14</v>
       </c>
       <c r="G73" s="29" t="s">
@@ -13112,7 +13118,7 @@
         <v>8</v>
       </c>
       <c r="F74" s="29">
-        <f t="shared" si="2"/>
+        <f>E74*2</f>
         <v>16</v>
       </c>
       <c r="G74" s="29" t="s">
@@ -13147,7 +13153,7 @@
         <v>7</v>
       </c>
       <c r="F75" s="29">
-        <f t="shared" si="2"/>
+        <f>E75*2</f>
         <v>14</v>
       </c>
       <c r="G75" s="29" t="s">
@@ -13182,7 +13188,7 @@
         <v>8</v>
       </c>
       <c r="F76" s="29">
-        <f t="shared" si="2"/>
+        <f>E76*2</f>
         <v>16</v>
       </c>
       <c r="G76" s="29" t="s">
@@ -13217,7 +13223,7 @@
         <v>7</v>
       </c>
       <c r="F77" s="29">
-        <f t="shared" si="2"/>
+        <f>E77*2</f>
         <v>14</v>
       </c>
       <c r="G77" s="29" t="s">
@@ -13252,7 +13258,7 @@
         <v>8</v>
       </c>
       <c r="F78" s="29">
-        <f t="shared" si="2"/>
+        <f>E78*2</f>
         <v>16</v>
       </c>
       <c r="G78" s="29" t="s">
@@ -13287,7 +13293,7 @@
         <v>7</v>
       </c>
       <c r="F79" s="29">
-        <f t="shared" si="2"/>
+        <f>E79*2</f>
         <v>14</v>
       </c>
       <c r="G79" s="29" t="s">
@@ -13322,7 +13328,7 @@
         <v>8</v>
       </c>
       <c r="F80" s="29">
-        <f t="shared" si="2"/>
+        <f>E80*2</f>
         <v>16</v>
       </c>
       <c r="G80" s="29" t="s">
@@ -13357,7 +13363,7 @@
         <v>8</v>
       </c>
       <c r="F81" s="29">
-        <f t="shared" si="2"/>
+        <f>E81*2</f>
         <v>16</v>
       </c>
       <c r="G81" s="29" t="s">
@@ -13392,7 +13398,7 @@
         <v>8</v>
       </c>
       <c r="F82" s="29">
-        <f t="shared" si="2"/>
+        <f>E82*2</f>
         <v>16</v>
       </c>
       <c r="G82" s="29" t="s">
@@ -13427,7 +13433,7 @@
         <v>8</v>
       </c>
       <c r="F83" s="29">
-        <f t="shared" si="2"/>
+        <f>E83*2</f>
         <v>16</v>
       </c>
       <c r="G83" s="29" t="s">
@@ -13462,7 +13468,7 @@
         <v>8</v>
       </c>
       <c r="F84" s="29">
-        <f t="shared" si="2"/>
+        <f>E84*2</f>
         <v>16</v>
       </c>
       <c r="G84" s="29" t="s">
@@ -13497,7 +13503,7 @@
         <v>7</v>
       </c>
       <c r="F85" s="29">
-        <f t="shared" si="2"/>
+        <f>E85*2</f>
         <v>14</v>
       </c>
       <c r="G85" s="29" t="s">
@@ -13532,7 +13538,7 @@
         <v>8</v>
       </c>
       <c r="F86" s="29">
-        <f t="shared" si="2"/>
+        <f>E86*2</f>
         <v>16</v>
       </c>
       <c r="G86" s="29" t="s">
@@ -13567,7 +13573,7 @@
         <v>8</v>
       </c>
       <c r="F87" s="29">
-        <f t="shared" si="2"/>
+        <f>E87*2</f>
         <v>16</v>
       </c>
       <c r="G87" s="29" t="s">
@@ -13602,7 +13608,7 @@
         <v>10</v>
       </c>
       <c r="F88" s="29">
-        <f t="shared" si="2"/>
+        <f>E88*2</f>
         <v>20</v>
       </c>
       <c r="G88" s="29" t="s">
@@ -13637,7 +13643,7 @@
         <v>9</v>
       </c>
       <c r="F89" s="29">
-        <f t="shared" si="2"/>
+        <f>E89*2</f>
         <v>18</v>
       </c>
       <c r="G89" s="29" t="s">
@@ -13674,7 +13680,7 @@
         <v>9</v>
       </c>
       <c r="F90" s="29">
-        <f t="shared" si="2"/>
+        <f>E90*2</f>
         <v>18</v>
       </c>
       <c r="G90" s="29" t="s">
@@ -13709,7 +13715,7 @@
         <v>9</v>
       </c>
       <c r="F91" s="29">
-        <f t="shared" si="2"/>
+        <f>E91*2</f>
         <v>18</v>
       </c>
       <c r="G91" s="29" t="s">
@@ -13744,7 +13750,7 @@
         <v>10</v>
       </c>
       <c r="F92" s="29">
-        <f t="shared" si="2"/>
+        <f>E92*2</f>
         <v>20</v>
       </c>
       <c r="G92" s="29" t="s">
@@ -13779,7 +13785,7 @@
         <v>9</v>
       </c>
       <c r="F93" s="29">
-        <f t="shared" si="2"/>
+        <f>E93*2</f>
         <v>18</v>
       </c>
       <c r="G93" s="29" t="s">
@@ -13816,7 +13822,7 @@
         <v>9</v>
       </c>
       <c r="F94" s="29">
-        <f t="shared" si="2"/>
+        <f>E94*2</f>
         <v>18</v>
       </c>
       <c r="G94" s="29" t="s">
@@ -13853,7 +13859,7 @@
         <v>9</v>
       </c>
       <c r="F95" s="29">
-        <f t="shared" si="2"/>
+        <f>E95*2</f>
         <v>18</v>
       </c>
       <c r="G95" s="29" t="s">
@@ -13890,7 +13896,7 @@
         <v>9</v>
       </c>
       <c r="F96" s="29">
-        <f t="shared" si="2"/>
+        <f>E96*2</f>
         <v>18</v>
       </c>
       <c r="G96" s="29" t="s">
@@ -13927,7 +13933,7 @@
         <v>9</v>
       </c>
       <c r="F97" s="29">
-        <f t="shared" si="2"/>
+        <f>E97*2</f>
         <v>18</v>
       </c>
       <c r="G97" s="29" t="s">
@@ -13964,7 +13970,7 @@
         <v>9</v>
       </c>
       <c r="F98" s="29">
-        <f t="shared" ref="F98:F129" si="3">E98*2</f>
+        <f>E98*2</f>
         <v>18</v>
       </c>
       <c r="G98" s="29" t="s">
@@ -14001,7 +14007,7 @@
         <v>10</v>
       </c>
       <c r="F99" s="29">
-        <f t="shared" si="3"/>
+        <f>E99*2</f>
         <v>20</v>
       </c>
       <c r="G99" s="29" t="s">
@@ -14036,7 +14042,7 @@
         <v>9</v>
       </c>
       <c r="F100" s="29">
-        <f t="shared" si="3"/>
+        <f>E100*2</f>
         <v>18</v>
       </c>
       <c r="G100" s="29" t="s">
@@ -14071,7 +14077,7 @@
         <v>10</v>
       </c>
       <c r="F101" s="29">
-        <f t="shared" si="3"/>
+        <f>E101*2</f>
         <v>20</v>
       </c>
       <c r="G101" s="29" t="s">
@@ -14106,7 +14112,7 @@
         <v>14</v>
       </c>
       <c r="F102" s="29">
-        <f t="shared" si="3"/>
+        <f>E102*2</f>
         <v>28</v>
       </c>
       <c r="G102" s="29" t="s">
@@ -14141,7 +14147,7 @@
         <v>9</v>
       </c>
       <c r="F103" s="29">
-        <f t="shared" si="3"/>
+        <f>E103*2</f>
         <v>18</v>
       </c>
       <c r="G103" s="29" t="s">
@@ -14176,7 +14182,7 @@
         <v>10</v>
       </c>
       <c r="F104" s="29">
-        <f t="shared" si="3"/>
+        <f>E104*2</f>
         <v>20</v>
       </c>
       <c r="G104" s="29" t="s">
@@ -14211,7 +14217,7 @@
         <v>9</v>
       </c>
       <c r="F105" s="29">
-        <f t="shared" si="3"/>
+        <f>E105*2</f>
         <v>18</v>
       </c>
       <c r="G105" s="29" t="s">
@@ -14246,7 +14252,7 @@
         <v>10</v>
       </c>
       <c r="F106" s="29">
-        <f t="shared" si="3"/>
+        <f>E106*2</f>
         <v>20</v>
       </c>
       <c r="G106" s="29" t="s">
@@ -14283,7 +14289,7 @@
         <v>10</v>
       </c>
       <c r="F107" s="29">
-        <f t="shared" si="3"/>
+        <f>E107*2</f>
         <v>20</v>
       </c>
       <c r="G107" s="29" t="s">
@@ -14320,7 +14326,7 @@
         <v>10</v>
       </c>
       <c r="F108" s="29">
-        <f t="shared" si="3"/>
+        <f>E108*2</f>
         <v>20</v>
       </c>
       <c r="G108" s="29" t="s">
@@ -14357,7 +14363,7 @@
         <v>10</v>
       </c>
       <c r="F109" s="29">
-        <f t="shared" si="3"/>
+        <f>E109*2</f>
         <v>20</v>
       </c>
       <c r="G109" s="29" t="s">
@@ -14394,7 +14400,7 @@
         <v>10</v>
       </c>
       <c r="F110" s="29">
-        <f t="shared" si="3"/>
+        <f>E110*2</f>
         <v>20</v>
       </c>
       <c r="G110" s="29" t="s">
@@ -14431,7 +14437,7 @@
         <v>10</v>
       </c>
       <c r="F111" s="29">
-        <f t="shared" si="3"/>
+        <f>E111*2</f>
         <v>20</v>
       </c>
       <c r="G111" s="29" t="s">
@@ -14468,7 +14474,7 @@
         <v>10</v>
       </c>
       <c r="F112" s="29">
-        <f t="shared" si="3"/>
+        <f>E112*2</f>
         <v>20</v>
       </c>
       <c r="G112" s="29" t="s">
@@ -14505,7 +14511,7 @@
         <v>10</v>
       </c>
       <c r="F113" s="29">
-        <f t="shared" si="3"/>
+        <f>E113*2</f>
         <v>20</v>
       </c>
       <c r="G113" s="29" t="s">
@@ -14542,7 +14548,7 @@
         <v>10</v>
       </c>
       <c r="F114" s="29">
-        <f t="shared" si="3"/>
+        <f>E114*2</f>
         <v>20</v>
       </c>
       <c r="G114" s="29" t="s">
@@ -14577,7 +14583,7 @@
         <v>9</v>
       </c>
       <c r="F115" s="29">
-        <f t="shared" si="3"/>
+        <f>E115*2</f>
         <v>18</v>
       </c>
       <c r="G115" s="29" t="s">
@@ -14612,7 +14618,7 @@
         <v>9</v>
       </c>
       <c r="F116" s="29">
-        <f t="shared" si="3"/>
+        <f>E116*2</f>
         <v>18</v>
       </c>
       <c r="G116" s="29" t="s">
@@ -14647,7 +14653,7 @@
         <v>10</v>
       </c>
       <c r="F117" s="29">
-        <f t="shared" si="3"/>
+        <f>E117*2</f>
         <v>20</v>
       </c>
       <c r="G117" s="29" t="s">
@@ -14682,7 +14688,7 @@
         <v>10</v>
       </c>
       <c r="F118" s="29">
-        <f t="shared" si="3"/>
+        <f>E118*2</f>
         <v>20</v>
       </c>
       <c r="G118" s="29" t="s">
@@ -14717,7 +14723,7 @@
         <v>10</v>
       </c>
       <c r="F119" s="29">
-        <f t="shared" si="3"/>
+        <f>E119*2</f>
         <v>20</v>
       </c>
       <c r="G119" s="29" t="s">
@@ -14752,7 +14758,7 @@
         <v>12</v>
       </c>
       <c r="F120" s="29">
-        <f t="shared" si="3"/>
+        <f>E120*2</f>
         <v>24</v>
       </c>
       <c r="G120" s="29" t="s">
@@ -14787,7 +14793,7 @@
         <v>12</v>
       </c>
       <c r="F121" s="29">
-        <f t="shared" si="3"/>
+        <f>E121*2</f>
         <v>24</v>
       </c>
       <c r="G121" s="29" t="s">
@@ -14822,7 +14828,7 @@
         <v>14</v>
       </c>
       <c r="F122" s="29">
-        <f t="shared" si="3"/>
+        <f>E122*2</f>
         <v>28</v>
       </c>
       <c r="G122" s="29" t="s">
@@ -14857,7 +14863,7 @@
         <v>12</v>
       </c>
       <c r="F123" s="29">
-        <f t="shared" si="3"/>
+        <f>E123*2</f>
         <v>24</v>
       </c>
       <c r="G123" s="29" t="s">
@@ -14892,7 +14898,7 @@
         <v>12</v>
       </c>
       <c r="F124" s="29">
-        <f t="shared" si="3"/>
+        <f>E124*2</f>
         <v>24</v>
       </c>
       <c r="G124" s="29" t="s">
@@ -14912,57 +14918,57 @@
     </row>
     <row r="125" spans="1:12">
       <c r="A125" s="29" t="s">
-        <v>1800</v>
+        <v>1868</v>
       </c>
       <c r="B125" s="29">
         <v>6</v>
       </c>
       <c r="C125" s="29" t="s">
-        <v>1130</v>
+        <v>1207</v>
       </c>
       <c r="D125" s="29" t="s">
-        <v>1290</v>
+        <v>1144</v>
       </c>
       <c r="E125" s="29">
         <v>12</v>
       </c>
       <c r="F125" s="29">
-        <f t="shared" si="3"/>
+        <f>E125*2</f>
         <v>24</v>
       </c>
       <c r="G125" s="29" t="s">
-        <v>1681</v>
+        <v>1677</v>
       </c>
       <c r="H125" s="29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I125" s="29" t="s">
-        <v>2124</v>
+        <v>2118</v>
       </c>
       <c r="J125" s="29"/>
       <c r="K125" s="29"/>
       <c r="L125" s="29" t="s">
-        <v>1995</v>
+        <v>2140</v>
       </c>
     </row>
     <row r="126" spans="1:12">
       <c r="A126" s="29" t="s">
-        <v>1694</v>
+        <v>1800</v>
       </c>
       <c r="B126" s="29">
         <v>6</v>
       </c>
       <c r="C126" s="29" t="s">
-        <v>190</v>
+        <v>1130</v>
       </c>
       <c r="D126" s="29" t="s">
-        <v>185</v>
+        <v>1290</v>
       </c>
       <c r="E126" s="29">
         <v>12</v>
       </c>
       <c r="F126" s="29">
-        <f t="shared" si="3"/>
+        <f>E126*2</f>
         <v>24</v>
       </c>
       <c r="G126" s="29" t="s">
@@ -14972,144 +14978,144 @@
         <v>1</v>
       </c>
       <c r="I126" s="29" t="s">
-        <v>2130</v>
+        <v>2124</v>
       </c>
       <c r="J126" s="29"/>
       <c r="K126" s="29"/>
       <c r="L126" s="29" t="s">
-        <v>2011</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="127" spans="1:12">
       <c r="A127" s="29" t="s">
-        <v>1721</v>
+        <v>1694</v>
       </c>
       <c r="B127" s="29">
         <v>6</v>
       </c>
       <c r="C127" s="29" t="s">
-        <v>315</v>
+        <v>190</v>
       </c>
       <c r="D127" s="29" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E127" s="29">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F127" s="29">
-        <f t="shared" si="3"/>
-        <v>32</v>
+        <f>E127*2</f>
+        <v>24</v>
       </c>
       <c r="G127" s="29" t="s">
-        <v>2110</v>
+        <v>1681</v>
       </c>
       <c r="H127" s="29" t="b">
         <v>1</v>
       </c>
       <c r="I127" s="29" t="s">
-        <v>2133</v>
+        <v>2130</v>
       </c>
       <c r="J127" s="29"/>
       <c r="K127" s="29"/>
       <c r="L127" s="29" t="s">
-        <v>2096</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="128" spans="1:12">
       <c r="A128" s="29" t="s">
-        <v>1726</v>
+        <v>1721</v>
       </c>
       <c r="B128" s="29">
         <v>6</v>
       </c>
       <c r="C128" s="29" t="s">
-        <v>1851</v>
+        <v>315</v>
       </c>
       <c r="D128" s="29" t="s">
-        <v>243</v>
+        <v>186</v>
       </c>
       <c r="E128" s="29">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F128" s="29">
-        <f t="shared" si="3"/>
-        <v>26</v>
+        <f>E128*2</f>
+        <v>32</v>
       </c>
       <c r="G128" s="29" t="s">
-        <v>1681</v>
+        <v>2110</v>
       </c>
       <c r="H128" s="29" t="b">
         <v>1</v>
       </c>
       <c r="I128" s="29" t="s">
-        <v>2136</v>
+        <v>2133</v>
       </c>
       <c r="J128" s="29"/>
       <c r="K128" s="29"/>
       <c r="L128" s="29" t="s">
-        <v>2047</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="129" spans="1:12">
       <c r="A129" s="29" t="s">
-        <v>1750</v>
+        <v>1726</v>
       </c>
       <c r="B129" s="29">
         <v>6</v>
       </c>
       <c r="C129" s="29" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="D129" s="29" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="E129" s="29">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F129" s="29">
-        <f t="shared" si="3"/>
-        <v>24</v>
+        <f>E129*2</f>
+        <v>26</v>
       </c>
       <c r="G129" s="29" t="s">
         <v>1681</v>
       </c>
       <c r="H129" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I129" s="29" t="s">
-        <v>2134</v>
+        <v>2136</v>
       </c>
       <c r="J129" s="29"/>
       <c r="K129" s="29"/>
       <c r="L129" s="29" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="130" spans="1:12">
       <c r="A130" s="29" t="s">
-        <v>1747</v>
+        <v>1750</v>
       </c>
       <c r="B130" s="29">
         <v>6</v>
       </c>
       <c r="C130" s="29" t="s">
-        <v>606</v>
+        <v>1852</v>
       </c>
       <c r="D130" s="29" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E130" s="29">
         <v>12</v>
       </c>
       <c r="F130" s="29">
-        <f t="shared" ref="F130:F161" si="4">E130*2</f>
+        <f>E130*2</f>
         <v>24</v>
       </c>
       <c r="G130" s="29" t="s">
-        <v>2110</v>
+        <v>1681</v>
       </c>
       <c r="H130" s="29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I130" s="29" t="s">
         <v>2134</v>
@@ -15117,345 +15123,345 @@
       <c r="J130" s="29"/>
       <c r="K130" s="29"/>
       <c r="L130" s="29" t="s">
-        <v>2020</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="131" spans="1:12">
       <c r="A131" s="29" t="s">
-        <v>1742</v>
+        <v>1747</v>
       </c>
       <c r="B131" s="29">
         <v>6</v>
       </c>
       <c r="C131" s="29" t="s">
-        <v>260</v>
+        <v>606</v>
       </c>
       <c r="D131" s="29" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E131" s="29">
         <v>12</v>
       </c>
       <c r="F131" s="29">
-        <f t="shared" si="4"/>
+        <f>E131*2</f>
         <v>24</v>
       </c>
       <c r="G131" s="29" t="s">
-        <v>1680</v>
+        <v>2110</v>
       </c>
       <c r="H131" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I131" s="29" t="s">
-        <v>2121</v>
+        <v>2134</v>
       </c>
       <c r="J131" s="29"/>
       <c r="K131" s="29"/>
       <c r="L131" s="29" t="s">
-        <v>1983</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="132" spans="1:12">
       <c r="A132" s="29" t="s">
-        <v>1712</v>
+        <v>1742</v>
       </c>
       <c r="B132" s="29">
         <v>6</v>
       </c>
       <c r="C132" s="29" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D132" s="29" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E132" s="29">
         <v>12</v>
       </c>
       <c r="F132" s="29">
-        <f t="shared" si="4"/>
+        <f>E132*2</f>
         <v>24</v>
       </c>
       <c r="G132" s="29" t="s">
         <v>1680</v>
       </c>
       <c r="H132" s="29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I132" s="29" t="s">
-        <v>2131</v>
+        <v>2121</v>
       </c>
       <c r="J132" s="29"/>
       <c r="K132" s="29"/>
       <c r="L132" s="29" t="s">
-        <v>1973</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="133" spans="1:12">
       <c r="A133" s="29" t="s">
-        <v>1768</v>
+        <v>1712</v>
       </c>
       <c r="B133" s="29">
         <v>6</v>
       </c>
       <c r="C133" s="29" t="s">
-        <v>1853</v>
+        <v>259</v>
       </c>
       <c r="D133" s="29" t="s">
-        <v>2137</v>
+        <v>252</v>
       </c>
       <c r="E133" s="29">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F133" s="29">
-        <f t="shared" si="4"/>
-        <v>26</v>
+        <f>E133*2</f>
+        <v>24</v>
       </c>
       <c r="G133" s="29" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="H133" s="29" t="b">
         <v>1</v>
       </c>
       <c r="I133" s="29" t="s">
-        <v>2123</v>
-      </c>
-      <c r="J133" s="29" t="s">
-        <v>255</v>
-      </c>
+        <v>2131</v>
+      </c>
+      <c r="J133" s="29"/>
       <c r="K133" s="29"/>
       <c r="L133" s="29" t="s">
-        <v>2070</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="134" spans="1:12">
       <c r="A134" s="29" t="s">
-        <v>1792</v>
+        <v>1768</v>
       </c>
       <c r="B134" s="29">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C134" s="29" t="s">
-        <v>1159</v>
+        <v>1853</v>
       </c>
       <c r="D134" s="29" t="s">
-        <v>1408</v>
+        <v>2137</v>
       </c>
       <c r="E134" s="29">
         <v>13</v>
       </c>
       <c r="F134" s="29">
-        <f t="shared" si="4"/>
+        <f>E134*2</f>
         <v>26</v>
       </c>
       <c r="G134" s="29" t="s">
-        <v>1680</v>
+        <v>1681</v>
       </c>
       <c r="H134" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I134" s="29" t="s">
-        <v>2125</v>
-      </c>
-      <c r="J134" s="29"/>
+        <v>2123</v>
+      </c>
+      <c r="J134" s="29" t="s">
+        <v>255</v>
+      </c>
       <c r="K134" s="29"/>
       <c r="L134" s="29" t="s">
-        <v>2032</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="135" spans="1:12">
       <c r="A135" s="29" t="s">
-        <v>1803</v>
+        <v>1792</v>
       </c>
       <c r="B135" s="29">
         <v>7</v>
       </c>
       <c r="C135" s="29" t="s">
-        <v>1155</v>
+        <v>1159</v>
       </c>
       <c r="D135" s="29" t="s">
         <v>1408</v>
       </c>
       <c r="E135" s="29">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F135" s="29">
-        <f t="shared" si="4"/>
-        <v>20</v>
+        <f>E135*2</f>
+        <v>26</v>
       </c>
       <c r="G135" s="29" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="H135" s="29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I135" s="29" t="s">
-        <v>2126</v>
+        <v>2125</v>
       </c>
       <c r="J135" s="29"/>
       <c r="K135" s="29"/>
       <c r="L135" s="29" t="s">
-        <v>2018</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="136" spans="1:12">
       <c r="A136" s="29" t="s">
-        <v>1882</v>
+        <v>1803</v>
       </c>
       <c r="B136" s="29">
         <v>7</v>
       </c>
       <c r="C136" s="29" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="D136" s="29" t="s">
         <v>1408</v>
       </c>
       <c r="E136" s="29">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F136" s="29">
-        <f t="shared" si="4"/>
-        <v>28</v>
+        <f>E136*2</f>
+        <v>20</v>
       </c>
       <c r="G136" s="29" t="s">
         <v>1681</v>
       </c>
       <c r="H136" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I136" s="29" t="s">
-        <v>2127</v>
+        <v>2126</v>
       </c>
       <c r="J136" s="29"/>
       <c r="K136" s="29"/>
       <c r="L136" s="29" t="s">
-        <v>2015</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="137" spans="1:12">
       <c r="A137" s="29" t="s">
-        <v>1755</v>
+        <v>1882</v>
       </c>
       <c r="B137" s="29">
         <v>7</v>
       </c>
       <c r="C137" s="29" t="s">
-        <v>1212</v>
+        <v>1157</v>
       </c>
       <c r="D137" s="29" t="s">
-        <v>1164</v>
+        <v>1408</v>
       </c>
       <c r="E137" s="29">
         <v>14</v>
       </c>
       <c r="F137" s="29">
-        <f t="shared" si="4"/>
+        <f>E137*2</f>
         <v>28</v>
       </c>
       <c r="G137" s="29" t="s">
-        <v>1677</v>
+        <v>1681</v>
       </c>
       <c r="H137" s="29" t="b">
         <v>0</v>
       </c>
       <c r="I137" s="29" t="s">
-        <v>2129</v>
+        <v>2127</v>
       </c>
       <c r="J137" s="29"/>
       <c r="K137" s="29"/>
       <c r="L137" s="29" t="s">
-        <v>2034</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="138" spans="1:12">
       <c r="A138" s="29" t="s">
-        <v>1786</v>
+        <v>1755</v>
       </c>
       <c r="B138" s="29">
         <v>7</v>
       </c>
       <c r="C138" s="29" t="s">
-        <v>9</v>
+        <v>1212</v>
       </c>
       <c r="D138" s="29" t="s">
-        <v>1173</v>
+        <v>1164</v>
       </c>
       <c r="E138" s="29">
         <v>14</v>
       </c>
       <c r="F138" s="29">
-        <f t="shared" si="4"/>
+        <f>E138*2</f>
         <v>28</v>
       </c>
       <c r="G138" s="29" t="s">
-        <v>1679</v>
+        <v>1677</v>
       </c>
       <c r="H138" s="29" t="b">
         <v>0</v>
       </c>
       <c r="I138" s="29" t="s">
-        <v>2125</v>
+        <v>2129</v>
       </c>
       <c r="J138" s="29"/>
       <c r="K138" s="29"/>
       <c r="L138" s="29" t="s">
-        <v>2014</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="139" spans="1:12">
       <c r="A139" s="29" t="s">
-        <v>1728</v>
+        <v>1786</v>
       </c>
       <c r="B139" s="29">
         <v>7</v>
       </c>
       <c r="C139" s="29" t="s">
-        <v>630</v>
+        <v>9</v>
       </c>
       <c r="D139" s="29" t="s">
-        <v>270</v>
+        <v>1173</v>
       </c>
       <c r="E139" s="29">
         <v>14</v>
       </c>
       <c r="F139" s="29">
-        <f t="shared" si="4"/>
+        <f>E139*2</f>
         <v>28</v>
       </c>
       <c r="G139" s="29" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
       <c r="H139" s="29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I139" s="29" t="s">
-        <v>2135</v>
+        <v>2125</v>
       </c>
       <c r="J139" s="29"/>
       <c r="K139" s="29"/>
       <c r="L139" s="29" t="s">
-        <v>2080</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="140" spans="1:12">
       <c r="A140" s="29" t="s">
-        <v>1762</v>
+        <v>1728</v>
       </c>
       <c r="B140" s="29">
         <v>7</v>
       </c>
       <c r="C140" s="29" t="s">
-        <v>1854</v>
+        <v>630</v>
       </c>
       <c r="D140" s="29" t="s">
-        <v>1912</v>
+        <v>270</v>
       </c>
       <c r="E140" s="29">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F140" s="29">
-        <f t="shared" si="4"/>
-        <v>26</v>
+        <f>E140*2</f>
+        <v>28</v>
       </c>
       <c r="G140" s="29" t="s">
         <v>1681</v>
@@ -15464,207 +15470,207 @@
         <v>1</v>
       </c>
       <c r="I140" s="29" t="s">
-        <v>2129</v>
+        <v>2135</v>
       </c>
       <c r="J140" s="29"/>
       <c r="K140" s="29"/>
       <c r="L140" s="29" t="s">
-        <v>2053</v>
+        <v>2080</v>
       </c>
     </row>
     <row r="141" spans="1:12">
       <c r="A141" s="29" t="s">
-        <v>1723</v>
+        <v>1762</v>
       </c>
       <c r="B141" s="29">
         <v>7</v>
       </c>
       <c r="C141" s="29" t="s">
-        <v>636</v>
+        <v>1854</v>
       </c>
       <c r="D141" s="29" t="s">
-        <v>277</v>
+        <v>1912</v>
       </c>
       <c r="E141" s="29">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F141" s="29">
-        <f t="shared" si="4"/>
-        <v>28</v>
+        <f>E141*2</f>
+        <v>26</v>
       </c>
       <c r="G141" s="29" t="s">
         <v>1681</v>
       </c>
       <c r="H141" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I141" s="29" t="s">
-        <v>2136</v>
+        <v>2129</v>
       </c>
       <c r="J141" s="29"/>
       <c r="K141" s="29"/>
       <c r="L141" s="29" t="s">
-        <v>2027</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="142" spans="1:12">
       <c r="A142" s="29" t="s">
-        <v>1855</v>
+        <v>1723</v>
       </c>
       <c r="B142" s="29">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C142" s="29" t="s">
-        <v>1593</v>
+        <v>636</v>
       </c>
       <c r="D142" s="29" t="s">
-        <v>2138</v>
+        <v>277</v>
       </c>
       <c r="E142" s="29">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F142" s="29">
-        <f t="shared" si="4"/>
-        <v>30</v>
+        <f>E142*2</f>
+        <v>28</v>
       </c>
       <c r="G142" s="29" t="s">
-        <v>1677</v>
+        <v>1681</v>
       </c>
       <c r="H142" s="29" t="b">
         <v>0</v>
       </c>
       <c r="I142" s="29" t="s">
-        <v>2119</v>
+        <v>2136</v>
       </c>
       <c r="J142" s="29"/>
       <c r="K142" s="29"/>
       <c r="L142" s="29" t="s">
-        <v>1999</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="143" spans="1:12">
       <c r="A143" s="29" t="s">
-        <v>1696</v>
+        <v>1855</v>
       </c>
       <c r="B143" s="29">
         <v>8</v>
       </c>
       <c r="C143" s="29" t="s">
-        <v>656</v>
+        <v>1593</v>
       </c>
       <c r="D143" s="29" t="s">
-        <v>293</v>
+        <v>2138</v>
       </c>
       <c r="E143" s="29">
         <v>15</v>
       </c>
       <c r="F143" s="29">
-        <f t="shared" si="4"/>
+        <f>E143*2</f>
         <v>30</v>
       </c>
       <c r="G143" s="29" t="s">
-        <v>1681</v>
+        <v>1677</v>
       </c>
       <c r="H143" s="29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I143" s="29" t="s">
-        <v>2132</v>
+        <v>2119</v>
       </c>
       <c r="J143" s="29"/>
       <c r="K143" s="29"/>
       <c r="L143" s="29" t="s">
-        <v>2044</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="144" spans="1:12">
       <c r="A144" s="29" t="s">
-        <v>1801</v>
+        <v>1696</v>
       </c>
       <c r="B144" s="29">
         <v>8</v>
       </c>
       <c r="C144" s="29" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="D144" s="29" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="E144" s="29">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F144" s="29">
-        <f t="shared" si="4"/>
-        <v>32</v>
+        <f>E144*2</f>
+        <v>30</v>
       </c>
       <c r="G144" s="29" t="s">
         <v>1681</v>
       </c>
       <c r="H144" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I144" s="29" t="s">
-        <v>2124</v>
+        <v>2132</v>
       </c>
       <c r="J144" s="29"/>
       <c r="K144" s="29"/>
       <c r="L144" s="29" t="s">
-        <v>2022</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="145" spans="1:12">
       <c r="A145" s="29" t="s">
-        <v>1864</v>
+        <v>1801</v>
       </c>
       <c r="B145" s="29">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C145" s="29" t="s">
-        <v>1594</v>
+        <v>660</v>
       </c>
       <c r="D145" s="29" t="s">
-        <v>1905</v>
+        <v>298</v>
       </c>
       <c r="E145" s="29">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F145" s="29">
-        <f t="shared" si="4"/>
-        <v>36</v>
+        <f>E145*2</f>
+        <v>32</v>
       </c>
       <c r="G145" s="29" t="s">
-        <v>1677</v>
+        <v>1681</v>
       </c>
       <c r="H145" s="29" t="b">
         <v>0</v>
       </c>
       <c r="I145" s="29" t="s">
-        <v>2119</v>
+        <v>2124</v>
       </c>
       <c r="J145" s="29"/>
       <c r="K145" s="29"/>
       <c r="L145" s="29" t="s">
-        <v>2038</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="146" spans="1:12">
       <c r="A146" s="29" t="s">
-        <v>1892</v>
+        <v>1864</v>
       </c>
       <c r="B146" s="29">
         <v>9</v>
       </c>
       <c r="C146" s="29" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="D146" s="29" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="E146" s="29">
         <v>18</v>
       </c>
       <c r="F146" s="29">
-        <f t="shared" si="4"/>
+        <f>E146*2</f>
         <v>36</v>
       </c>
       <c r="G146" s="29" t="s">
@@ -15674,68 +15680,68 @@
         <v>0</v>
       </c>
       <c r="I146" s="29" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
       <c r="J146" s="29"/>
       <c r="K146" s="29"/>
       <c r="L146" s="29" t="s">
-        <v>1943</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="147" spans="1:12">
       <c r="A147" s="29" t="s">
-        <v>1779</v>
+        <v>1892</v>
       </c>
       <c r="B147" s="29">
         <v>9</v>
       </c>
       <c r="C147" s="29" t="s">
-        <v>679</v>
+        <v>1595</v>
       </c>
       <c r="D147" s="29" t="s">
-        <v>514</v>
+        <v>1906</v>
       </c>
       <c r="E147" s="29">
         <v>18</v>
       </c>
       <c r="F147" s="29">
-        <f t="shared" si="4"/>
+        <f>E147*2</f>
         <v>36</v>
       </c>
       <c r="G147" s="29" t="s">
-        <v>1681</v>
+        <v>1677</v>
       </c>
       <c r="H147" s="29" t="b">
         <v>0</v>
       </c>
       <c r="I147" s="29" t="s">
-        <v>2122</v>
+        <v>2120</v>
       </c>
       <c r="J147" s="29"/>
       <c r="K147" s="29"/>
       <c r="L147" s="29" t="s">
-        <v>2079</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="148" spans="1:12">
       <c r="A148" s="29" t="s">
-        <v>1764</v>
+        <v>1779</v>
       </c>
       <c r="B148" s="29">
         <v>9</v>
       </c>
       <c r="C148" s="29" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="D148" s="29" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="E148" s="29">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F148" s="29">
-        <f t="shared" si="4"/>
-        <v>40</v>
+        <f>E148*2</f>
+        <v>36</v>
       </c>
       <c r="G148" s="29" t="s">
         <v>1681</v>
@@ -15744,102 +15750,102 @@
         <v>0</v>
       </c>
       <c r="I148" s="29" t="s">
-        <v>2123</v>
+        <v>2122</v>
       </c>
       <c r="J148" s="29"/>
       <c r="K148" s="29"/>
       <c r="L148" s="29" t="s">
-        <v>1933</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="149" spans="1:12">
       <c r="A149" s="29" t="s">
-        <v>1891</v>
+        <v>1764</v>
       </c>
       <c r="B149" s="29">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C149" s="29" t="s">
-        <v>1596</v>
+        <v>682</v>
       </c>
       <c r="D149" s="29" t="s">
-        <v>1907</v>
+        <v>519</v>
       </c>
       <c r="E149" s="29">
         <v>20</v>
       </c>
       <c r="F149" s="29">
-        <f t="shared" si="4"/>
+        <f>E149*2</f>
         <v>40</v>
       </c>
       <c r="G149" s="29" t="s">
-        <v>1677</v>
+        <v>1681</v>
       </c>
       <c r="H149" s="29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I149" s="29" t="s">
-        <v>2120</v>
+        <v>2123</v>
       </c>
       <c r="J149" s="29"/>
       <c r="K149" s="29"/>
       <c r="L149" s="29" t="s">
-        <v>1990</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="150" spans="1:12">
       <c r="A150" s="29" t="s">
-        <v>1881</v>
+        <v>1891</v>
       </c>
       <c r="B150" s="29">
         <v>10</v>
       </c>
       <c r="C150" s="29" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="D150" s="29" t="s">
-        <v>1927</v>
+        <v>1907</v>
       </c>
       <c r="E150" s="29">
         <v>20</v>
       </c>
       <c r="F150" s="29">
-        <f t="shared" si="4"/>
+        <f>E150*2</f>
         <v>40</v>
       </c>
       <c r="G150" s="29" t="s">
         <v>1677</v>
       </c>
       <c r="H150" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I150" s="29" t="s">
-        <v>2127</v>
+        <v>2120</v>
       </c>
       <c r="J150" s="29"/>
       <c r="K150" s="29"/>
       <c r="L150" s="29" t="s">
-        <v>2028</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="151" spans="1:12">
       <c r="A151" s="29" t="s">
-        <v>1812</v>
+        <v>1881</v>
       </c>
       <c r="B151" s="29">
         <v>10</v>
       </c>
       <c r="C151" s="29" t="s">
-        <v>695</v>
+        <v>1597</v>
       </c>
       <c r="D151" s="29" t="s">
-        <v>674</v>
+        <v>1927</v>
       </c>
       <c r="E151" s="29">
         <v>20</v>
       </c>
       <c r="F151" s="29">
-        <f t="shared" si="4"/>
+        <f>E151*2</f>
         <v>40</v>
       </c>
       <c r="G151" s="29" t="s">
@@ -15849,95 +15855,122 @@
         <v>0</v>
       </c>
       <c r="I151" s="29" t="s">
-        <v>2126</v>
+        <v>2127</v>
       </c>
       <c r="J151" s="29"/>
       <c r="K151" s="29"/>
       <c r="L151" s="29" t="s">
-        <v>2019</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="152" spans="1:12">
       <c r="A152" s="29" t="s">
-        <v>1857</v>
-      </c>
-      <c r="B152" s="30" t="s">
-        <v>1399</v>
+        <v>1812</v>
+      </c>
+      <c r="B152" s="29">
+        <v>10</v>
       </c>
       <c r="C152" s="29" t="s">
-        <v>1609</v>
+        <v>695</v>
       </c>
       <c r="D152" s="29" t="s">
-        <v>1924</v>
+        <v>674</v>
       </c>
       <c r="E152" s="29">
         <v>20</v>
       </c>
       <c r="F152" s="29">
-        <f t="shared" si="4"/>
+        <f>E152*2</f>
         <v>40</v>
       </c>
       <c r="G152" s="29" t="s">
-        <v>1680</v>
+        <v>1677</v>
       </c>
       <c r="H152" s="29" t="b">
         <v>0</v>
       </c>
       <c r="I152" s="29" t="s">
-        <v>2119</v>
+        <v>2126</v>
       </c>
       <c r="J152" s="29"/>
       <c r="K152" s="29"/>
       <c r="L152" s="29" t="s">
-        <v>1978</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="153" spans="1:12">
       <c r="A153" s="29" t="s">
-        <v>1784</v>
+        <v>1857</v>
       </c>
       <c r="B153" s="30" t="s">
         <v>1399</v>
       </c>
       <c r="C153" s="29" t="s">
-        <v>1223</v>
+        <v>1609</v>
       </c>
       <c r="D153" s="29" t="s">
-        <v>1232</v>
+        <v>1924</v>
       </c>
       <c r="E153" s="29">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F153" s="29">
-        <f t="shared" si="4"/>
-        <v>36</v>
+        <f>E153*2</f>
+        <v>40</v>
       </c>
       <c r="G153" s="29" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="H153" s="29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I153" s="29" t="s">
-        <v>2125</v>
+        <v>2119</v>
       </c>
       <c r="J153" s="29"/>
       <c r="K153" s="29"/>
       <c r="L153" s="29" t="s">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12">
+      <c r="A154" s="29" t="s">
+        <v>1784</v>
+      </c>
+      <c r="B154" s="30" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C154" s="29" t="s">
+        <v>1223</v>
+      </c>
+      <c r="D154" s="29" t="s">
+        <v>1232</v>
+      </c>
+      <c r="E154" s="29">
+        <v>18</v>
+      </c>
+      <c r="F154" s="29">
+        <f>E154*2</f>
+        <v>36</v>
+      </c>
+      <c r="G154" s="29" t="s">
+        <v>1681</v>
+      </c>
+      <c r="H154" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I154" s="29" t="s">
+        <v>2125</v>
+      </c>
+      <c r="J154" s="29"/>
+      <c r="K154" s="29"/>
+      <c r="L154" s="29" t="s">
         <v>1967</v>
-      </c>
-    </row>
-    <row r="154" spans="1:12">
-      <c r="A154" t="s">
-        <v>1944</v>
-      </c>
-      <c r="I154" t="s">
-        <v>2130</v>
       </c>
     </row>
     <row r="155" spans="1:12">
       <c r="A155" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="I155" t="s">
         <v>2130</v>
@@ -15945,15 +15978,15 @@
     </row>
     <row r="156" spans="1:12">
       <c r="A156" t="s">
-        <v>1695</v>
+        <v>1945</v>
       </c>
       <c r="I156" t="s">
-        <v>2132</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="157" spans="1:12">
       <c r="A157" t="s">
-        <v>1946</v>
+        <v>1695</v>
       </c>
       <c r="I157" t="s">
         <v>2132</v>
@@ -15961,7 +15994,7 @@
     </row>
     <row r="158" spans="1:12">
       <c r="A158" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="I158" t="s">
         <v>2132</v>
@@ -15969,7 +16002,7 @@
     </row>
     <row r="159" spans="1:12">
       <c r="A159" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="I159" t="s">
         <v>2132</v>
@@ -15977,15 +16010,15 @@
     </row>
     <row r="160" spans="1:12">
       <c r="A160" t="s">
-        <v>1951</v>
+        <v>1948</v>
       </c>
       <c r="I160" t="s">
-        <v>2128</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="161" spans="1:9">
       <c r="A161" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="I161" t="s">
         <v>2128</v>
@@ -15993,7 +16026,7 @@
     </row>
     <row r="162" spans="1:9">
       <c r="A162" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="I162" t="s">
         <v>2128</v>
@@ -16001,7 +16034,7 @@
     </row>
     <row r="163" spans="1:9">
       <c r="A163" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="I163" t="s">
         <v>2128</v>
@@ -16009,7 +16042,7 @@
     </row>
     <row r="164" spans="1:9">
       <c r="A164" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="I164" t="s">
         <v>2128</v>
@@ -16017,7 +16050,7 @@
     </row>
     <row r="165" spans="1:9">
       <c r="A165" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="I165" t="s">
         <v>2128</v>
@@ -16025,23 +16058,23 @@
     </row>
     <row r="166" spans="1:9">
       <c r="A166" t="s">
-        <v>1950</v>
+        <v>1956</v>
       </c>
       <c r="I166" t="s">
-        <v>2131</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="167" spans="1:9">
       <c r="A167" t="s">
-        <v>1957</v>
+        <v>1950</v>
       </c>
       <c r="I167" t="s">
-        <v>2133</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="168" spans="1:9">
       <c r="A168" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="I168" t="s">
         <v>2133</v>
@@ -16049,7 +16082,7 @@
     </row>
     <row r="169" spans="1:9">
       <c r="A169" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="I169" t="s">
         <v>2133</v>
@@ -16057,15 +16090,15 @@
     </row>
     <row r="170" spans="1:9">
       <c r="A170" t="s">
-        <v>1722</v>
+        <v>1959</v>
       </c>
       <c r="I170" t="s">
-        <v>2136</v>
+        <v>2133</v>
       </c>
     </row>
     <row r="171" spans="1:9">
       <c r="A171" t="s">
-        <v>1960</v>
+        <v>1722</v>
       </c>
       <c r="I171" t="s">
         <v>2136</v>
@@ -16073,7 +16106,7 @@
     </row>
     <row r="172" spans="1:9">
       <c r="A172" t="s">
-        <v>1962</v>
+        <v>1960</v>
       </c>
       <c r="I172" t="s">
         <v>2136</v>
@@ -16081,7 +16114,7 @@
     </row>
     <row r="173" spans="1:9">
       <c r="A173" t="s">
-        <v>1961</v>
+        <v>1962</v>
       </c>
       <c r="I173" t="s">
         <v>2136</v>
@@ -16089,7 +16122,7 @@
     </row>
     <row r="174" spans="1:9">
       <c r="A174" t="s">
-        <v>1724</v>
+        <v>1961</v>
       </c>
       <c r="I174" t="s">
         <v>2136</v>
@@ -16097,63 +16130,63 @@
     </row>
     <row r="175" spans="1:9">
       <c r="A175" t="s">
-        <v>1963</v>
+        <v>1724</v>
       </c>
       <c r="I175" t="s">
-        <v>2121</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="176" spans="1:9">
       <c r="A176" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="I176" t="s">
-        <v>2134</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="177" spans="1:9">
       <c r="A177" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="I177" t="s">
-        <v>2129</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="178" spans="1:9">
       <c r="A178" t="s">
-        <v>1776</v>
+        <v>1965</v>
       </c>
       <c r="I178" t="s">
-        <v>2122</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="179" spans="1:9">
       <c r="A179" t="s">
-        <v>1808</v>
+        <v>1776</v>
       </c>
       <c r="I179" t="s">
-        <v>2126</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="180" spans="1:9">
       <c r="A180" t="s">
-        <v>1861</v>
+        <v>1808</v>
       </c>
       <c r="I180" t="s">
-        <v>2119</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="181" spans="1:9">
       <c r="A181" t="s">
-        <v>1865</v>
+        <v>1861</v>
       </c>
       <c r="I181" t="s">
-        <v>2118</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="182" spans="1:9">
       <c r="A182" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="I182" t="s">
         <v>2118</v>
@@ -16161,7 +16194,7 @@
     </row>
     <row r="183" spans="1:9">
       <c r="A183" t="s">
-        <v>1868</v>
+        <v>1866</v>
       </c>
       <c r="I183" t="s">
         <v>2118</v>
@@ -16264,17 +16297,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>1404</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
       <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10">
@@ -16283,13 +16316,13 @@
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="36" t="s">
         <v>1406</v>
       </c>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="4" t="s">
@@ -16390,60 +16423,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" s="5" customFormat="1">
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="32" t="s">
         <v>175</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31" t="s">
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31" t="s">
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32" t="s">
         <v>316</v>
       </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31" t="s">
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32" t="s">
         <v>547</v>
       </c>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31" t="s">
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32" t="s">
         <v>819</v>
       </c>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31" t="s">
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32" t="s">
         <v>833</v>
       </c>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31" t="s">
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32" t="s">
         <v>834</v>
       </c>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31" t="s">
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32" t="s">
         <v>835</v>
       </c>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31" t="s">
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32" t="s">
         <v>869</v>
       </c>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
       <c r="AM1" s="11"/>
       <c r="AN1" s="11"/>
       <c r="AO1" s="11"/>
@@ -50875,76 +50908,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" s="5" customFormat="1">
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33" t="s">
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="34" t="s">
         <v>193</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="32" t="s">
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="33" t="s">
         <v>316</v>
       </c>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32" t="s">
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33" t="s">
         <v>547</v>
       </c>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32" t="s">
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33" t="s">
         <v>819</v>
       </c>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32" t="s">
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33" t="s">
         <v>833</v>
       </c>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32" t="s">
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33" t="s">
         <v>834</v>
       </c>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32" t="s">
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33" t="s">
         <v>835</v>
       </c>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="32"/>
-      <c r="AQ1" s="32"/>
-      <c r="AR1" s="32" t="s">
+      <c r="AM1" s="33"/>
+      <c r="AN1" s="33"/>
+      <c r="AO1" s="33"/>
+      <c r="AP1" s="33"/>
+      <c r="AQ1" s="33"/>
+      <c r="AR1" s="33" t="s">
         <v>869</v>
       </c>
-      <c r="AS1" s="32"/>
-      <c r="AT1" s="32"/>
-      <c r="AU1" s="32"/>
-      <c r="AV1" s="32"/>
-      <c r="AW1" s="32"/>
-      <c r="AX1" s="32"/>
-      <c r="AY1" s="32"/>
-      <c r="AZ1" s="32"/>
-      <c r="BA1" s="32"/>
-      <c r="BB1" s="33"/>
+      <c r="AS1" s="33"/>
+      <c r="AT1" s="33"/>
+      <c r="AU1" s="33"/>
+      <c r="AV1" s="33"/>
+      <c r="AW1" s="33"/>
+      <c r="AX1" s="33"/>
+      <c r="AY1" s="33"/>
+      <c r="AZ1" s="33"/>
+      <c r="BA1" s="33"/>
+      <c r="BB1" s="34"/>
     </row>
     <row r="2" spans="1:54">
       <c r="A2" s="4" t="s">

</xml_diff>